<commit_message>
Add linewidth in the preference window 2
</commit_message>
<xml_diff>
--- a/DATA/UKSAF/STO.xlsx
+++ b/DATA/UKSAF/STO.xlsx
@@ -759,6 +759,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -808,7 +811,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="7277100" cy="5095875"/>
+    <ext cx="5648325" cy="4086225"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -822,9 +825,6 @@
       </blipFill>
       <spPr>
         <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -11188,8 +11188,16 @@
           <t>Calculated Fit</t>
         </is>
       </c>
-      <c r="J1" s="31" t="inlineStr"/>
-      <c r="K1" s="31" t="inlineStr"/>
+      <c r="J1" s="31" t="inlineStr">
+        <is>
+          <t>O1s p1</t>
+        </is>
+      </c>
+      <c r="K1" s="31" t="inlineStr">
+        <is>
+          <t>O1s p2</t>
+        </is>
+      </c>
       <c r="L1" s="31" t="inlineStr"/>
       <c r="M1" s="31" t="inlineStr"/>
       <c r="N1" s="31" t="inlineStr"/>
@@ -11324,8 +11332,107 @@
       <c r="F2" t="n">
         <v>545.08</v>
       </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
       <c r="H2" t="n">
         <v>45763.7</v>
+      </c>
+      <c r="I2" t="n">
+        <v>45763.7</v>
+      </c>
+      <c r="J2" t="n">
+        <v>45763.7</v>
+      </c>
+      <c r="K2" t="n">
+        <v>45763.7</v>
+      </c>
+      <c r="X2" s="35" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="Y2" s="36" t="inlineStr">
+        <is>
+          <t>O1s p1</t>
+        </is>
+      </c>
+      <c r="Z2" s="36" t="inlineStr">
+        <is>
+          <t>529.11</t>
+        </is>
+      </c>
+      <c r="AA2" s="36" t="inlineStr">
+        <is>
+          <t>135281</t>
+        </is>
+      </c>
+      <c r="AB2" s="36" t="inlineStr">
+        <is>
+          <t>1.16</t>
+        </is>
+      </c>
+      <c r="AC2" s="36" t="inlineStr">
+        <is>
+          <t>48.36</t>
+        </is>
+      </c>
+      <c r="AD2" s="36" t="inlineStr">
+        <is>
+          <t>167043</t>
+        </is>
+      </c>
+      <c r="AE2" s="36" t="inlineStr"/>
+      <c r="AF2" s="36" t="inlineStr"/>
+      <c r="AG2" s="36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AH2" s="36" t="inlineStr">
+        <is>
+          <t>70.9</t>
+        </is>
+      </c>
+      <c r="AI2" s="36" t="inlineStr">
+        <is>
+          <t>100.0</t>
+        </is>
+      </c>
+      <c r="AJ2" s="36" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AK2" s="36" t="inlineStr">
+        <is>
+          <t>GL (Area)</t>
+        </is>
+      </c>
+      <c r="AL2" s="36" t="inlineStr">
+        <is>
+          <t>Multi-Regions Smart</t>
+        </is>
+      </c>
+      <c r="AM2" s="36" t="inlineStr">
+        <is>
+          <t>525.08</t>
+        </is>
+      </c>
+      <c r="AN2" s="36" t="inlineStr">
+        <is>
+          <t>545.08</t>
+        </is>
+      </c>
+      <c r="AO2" s="36" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AP2" s="37" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -11338,9 +11445,64 @@
       <c r="F3" t="n">
         <v>544.98</v>
       </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
       <c r="H3" t="n">
         <v>46726.9</v>
       </c>
+      <c r="I3" t="n">
+        <v>46726.9</v>
+      </c>
+      <c r="J3" t="n">
+        <v>45763.7</v>
+      </c>
+      <c r="K3" t="n">
+        <v>45763.7</v>
+      </c>
+      <c r="X3" s="38" t="inlineStr"/>
+      <c r="Y3" s="39" t="inlineStr"/>
+      <c r="Z3" s="39" t="inlineStr">
+        <is>
+          <t>525.08,545.08</t>
+        </is>
+      </c>
+      <c r="AA3" s="39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB3" s="39" t="inlineStr">
+        <is>
+          <t>0.3:3.5</t>
+        </is>
+      </c>
+      <c r="AC3" s="39" t="inlineStr">
+        <is>
+          <t>2:80</t>
+        </is>
+      </c>
+      <c r="AD3" s="39" t="inlineStr">
+        <is>
+          <t>1:1e7</t>
+        </is>
+      </c>
+      <c r="AE3" s="39" t="inlineStr"/>
+      <c r="AF3" s="39" t="inlineStr"/>
+      <c r="AG3" s="39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AH3" s="39" t="inlineStr"/>
+      <c r="AI3" s="39" t="inlineStr"/>
+      <c r="AJ3" s="39" t="inlineStr"/>
+      <c r="AK3" s="39" t="inlineStr"/>
+      <c r="AL3" s="39" t="inlineStr"/>
+      <c r="AM3" s="39" t="inlineStr"/>
+      <c r="AN3" s="39" t="inlineStr"/>
+      <c r="AO3" s="39" t="inlineStr"/>
+      <c r="AP3" s="40" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -11352,8 +11514,107 @@
       <c r="F4" t="n">
         <v>544.88</v>
       </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
       <c r="H4" t="n">
         <v>46338.7</v>
+      </c>
+      <c r="I4" t="n">
+        <v>46338.7</v>
+      </c>
+      <c r="J4" t="n">
+        <v>46726.9</v>
+      </c>
+      <c r="K4" t="n">
+        <v>46726.9</v>
+      </c>
+      <c r="X4" s="35" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="Y4" s="36" t="inlineStr">
+        <is>
+          <t>O1s p2</t>
+        </is>
+      </c>
+      <c r="Z4" s="36" t="inlineStr">
+        <is>
+          <t>531.03</t>
+        </is>
+      </c>
+      <c r="AA4" s="36" t="inlineStr">
+        <is>
+          <t>27380</t>
+        </is>
+      </c>
+      <c r="AB4" s="36" t="inlineStr">
+        <is>
+          <t>2.35</t>
+        </is>
+      </c>
+      <c r="AC4" s="36" t="inlineStr">
+        <is>
+          <t>55.48</t>
+        </is>
+      </c>
+      <c r="AD4" s="36" t="inlineStr">
+        <is>
+          <t>68490</t>
+        </is>
+      </c>
+      <c r="AE4" s="36" t="inlineStr"/>
+      <c r="AF4" s="36" t="inlineStr"/>
+      <c r="AG4" s="36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AH4" s="36" t="inlineStr">
+        <is>
+          <t>29.1</t>
+        </is>
+      </c>
+      <c r="AI4" s="36" t="inlineStr">
+        <is>
+          <t>41.0</t>
+        </is>
+      </c>
+      <c r="AJ4" s="36" t="inlineStr">
+        <is>
+          <t>1.92</t>
+        </is>
+      </c>
+      <c r="AK4" s="36" t="inlineStr">
+        <is>
+          <t>GL (Area)</t>
+        </is>
+      </c>
+      <c r="AL4" s="36" t="inlineStr">
+        <is>
+          <t>Multi-Regions Smart</t>
+        </is>
+      </c>
+      <c r="AM4" s="36" t="inlineStr">
+        <is>
+          <t>525.08</t>
+        </is>
+      </c>
+      <c r="AN4" s="36" t="inlineStr">
+        <is>
+          <t>545.08</t>
+        </is>
+      </c>
+      <c r="AO4" s="36" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AP4" s="37" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -11366,9 +11627,64 @@
       <c r="F5" t="n">
         <v>544.78</v>
       </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
       <c r="H5" t="n">
         <v>46687</v>
       </c>
+      <c r="I5" t="n">
+        <v>46687</v>
+      </c>
+      <c r="J5" t="n">
+        <v>46338.7</v>
+      </c>
+      <c r="K5" t="n">
+        <v>46338.7</v>
+      </c>
+      <c r="X5" s="38" t="inlineStr"/>
+      <c r="Y5" s="39" t="inlineStr"/>
+      <c r="Z5" s="39" t="inlineStr">
+        <is>
+          <t>525.08,545.08</t>
+        </is>
+      </c>
+      <c r="AA5" s="39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB5" s="39" t="inlineStr">
+        <is>
+          <t>0.3:3.5</t>
+        </is>
+      </c>
+      <c r="AC5" s="39" t="inlineStr">
+        <is>
+          <t>2:80</t>
+        </is>
+      </c>
+      <c r="AD5" s="39" t="inlineStr">
+        <is>
+          <t>1:1e7</t>
+        </is>
+      </c>
+      <c r="AE5" s="39" t="inlineStr"/>
+      <c r="AF5" s="39" t="inlineStr"/>
+      <c r="AG5" s="39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AH5" s="39" t="inlineStr"/>
+      <c r="AI5" s="39" t="inlineStr"/>
+      <c r="AJ5" s="39" t="inlineStr"/>
+      <c r="AK5" s="39" t="inlineStr"/>
+      <c r="AL5" s="39" t="inlineStr"/>
+      <c r="AM5" s="39" t="inlineStr"/>
+      <c r="AN5" s="39" t="inlineStr"/>
+      <c r="AO5" s="39" t="inlineStr"/>
+      <c r="AP5" s="40" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -11380,8 +11696,20 @@
       <c r="F6" t="n">
         <v>544.6799999999999</v>
       </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
       <c r="H6" t="n">
         <v>46636.4</v>
+      </c>
+      <c r="I6" t="n">
+        <v>46636.4</v>
+      </c>
+      <c r="J6" t="n">
+        <v>46687</v>
+      </c>
+      <c r="K6" t="n">
+        <v>46687</v>
       </c>
     </row>
     <row r="7">
@@ -11394,8 +11722,20 @@
       <c r="F7" t="n">
         <v>544.58</v>
       </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
       <c r="H7" t="n">
         <v>46404.6</v>
+      </c>
+      <c r="I7" t="n">
+        <v>46404.6</v>
+      </c>
+      <c r="J7" t="n">
+        <v>46636.4</v>
+      </c>
+      <c r="K7" t="n">
+        <v>46636.4</v>
       </c>
     </row>
     <row r="8">
@@ -11408,8 +11748,20 @@
       <c r="F8" t="n">
         <v>544.48</v>
       </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
       <c r="H8" t="n">
         <v>47747</v>
+      </c>
+      <c r="I8" t="n">
+        <v>47747</v>
+      </c>
+      <c r="J8" t="n">
+        <v>46404.6</v>
+      </c>
+      <c r="K8" t="n">
+        <v>46404.6</v>
       </c>
     </row>
     <row r="9">
@@ -11422,8 +11774,20 @@
       <c r="F9" t="n">
         <v>544.38</v>
       </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
       <c r="H9" t="n">
         <v>45229.4</v>
+      </c>
+      <c r="I9" t="n">
+        <v>45229.4</v>
+      </c>
+      <c r="J9" t="n">
+        <v>47747</v>
+      </c>
+      <c r="K9" t="n">
+        <v>47747</v>
       </c>
     </row>
     <row r="10">
@@ -11436,8 +11800,20 @@
       <c r="F10" t="n">
         <v>544.28</v>
       </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
       <c r="H10" t="n">
         <v>46400.1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>46400.1</v>
+      </c>
+      <c r="J10" t="n">
+        <v>45229.4</v>
+      </c>
+      <c r="K10" t="n">
+        <v>45229.4</v>
       </c>
     </row>
     <row r="11">
@@ -11450,8 +11826,20 @@
       <c r="F11" t="n">
         <v>544.1799999999999</v>
       </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
       <c r="H11" t="n">
         <v>47015.4</v>
+      </c>
+      <c r="I11" t="n">
+        <v>47015.4</v>
+      </c>
+      <c r="J11" t="n">
+        <v>46400.1</v>
+      </c>
+      <c r="K11" t="n">
+        <v>46400.1</v>
       </c>
     </row>
     <row r="12">
@@ -11464,8 +11852,20 @@
       <c r="F12" t="n">
         <v>544.08</v>
       </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
       <c r="H12" t="n">
         <v>47330.1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>47330.1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>47015.4</v>
+      </c>
+      <c r="K12" t="n">
+        <v>47015.4</v>
       </c>
     </row>
     <row r="13">
@@ -11478,8 +11878,20 @@
       <c r="F13" t="n">
         <v>543.98</v>
       </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
       <c r="H13" t="n">
         <v>47281.4</v>
+      </c>
+      <c r="I13" t="n">
+        <v>47281.4</v>
+      </c>
+      <c r="J13" t="n">
+        <v>47330.1</v>
+      </c>
+      <c r="K13" t="n">
+        <v>47330.1</v>
       </c>
     </row>
     <row r="14">
@@ -11492,8 +11904,20 @@
       <c r="F14" t="n">
         <v>543.88</v>
       </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
       <c r="H14" t="n">
         <v>46775.6</v>
+      </c>
+      <c r="I14" t="n">
+        <v>46775.6</v>
+      </c>
+      <c r="J14" t="n">
+        <v>47281.4</v>
+      </c>
+      <c r="K14" t="n">
+        <v>47281.4</v>
       </c>
     </row>
     <row r="15">
@@ -11506,8 +11930,20 @@
       <c r="F15" t="n">
         <v>543.78</v>
       </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
       <c r="H15" t="n">
         <v>46993.4</v>
+      </c>
+      <c r="I15" t="n">
+        <v>46993.4</v>
+      </c>
+      <c r="J15" t="n">
+        <v>46775.6</v>
+      </c>
+      <c r="K15" t="n">
+        <v>46775.6</v>
       </c>
     </row>
     <row r="16">
@@ -11520,8 +11956,20 @@
       <c r="F16" t="n">
         <v>543.6799999999999</v>
       </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
       <c r="H16" t="n">
         <v>47547.8</v>
+      </c>
+      <c r="I16" t="n">
+        <v>47547.8</v>
+      </c>
+      <c r="J16" t="n">
+        <v>46993.4</v>
+      </c>
+      <c r="K16" t="n">
+        <v>46993.4</v>
       </c>
     </row>
     <row r="17">
@@ -11534,8 +11982,20 @@
       <c r="F17" t="n">
         <v>543.58</v>
       </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
       <c r="H17" t="n">
         <v>47962.4</v>
+      </c>
+      <c r="I17" t="n">
+        <v>47962.4</v>
+      </c>
+      <c r="J17" t="n">
+        <v>47547.8</v>
+      </c>
+      <c r="K17" t="n">
+        <v>47547.8</v>
       </c>
     </row>
     <row r="18">
@@ -11548,8 +12008,20 @@
       <c r="F18" t="n">
         <v>543.48</v>
       </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
       <c r="H18" t="n">
         <v>47990.3</v>
+      </c>
+      <c r="I18" t="n">
+        <v>47990.3</v>
+      </c>
+      <c r="J18" t="n">
+        <v>47962.4</v>
+      </c>
+      <c r="K18" t="n">
+        <v>47962.4</v>
       </c>
     </row>
     <row r="19">
@@ -11562,8 +12034,20 @@
       <c r="F19" t="n">
         <v>543.38</v>
       </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
       <c r="H19" t="n">
         <v>48070.3</v>
+      </c>
+      <c r="I19" t="n">
+        <v>48070.3</v>
+      </c>
+      <c r="J19" t="n">
+        <v>47990.3</v>
+      </c>
+      <c r="K19" t="n">
+        <v>47990.3</v>
       </c>
     </row>
     <row r="20">
@@ -11576,8 +12060,20 @@
       <c r="F20" t="n">
         <v>543.28</v>
       </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
       <c r="H20" t="n">
         <v>48922.9</v>
+      </c>
+      <c r="I20" t="n">
+        <v>48922.9</v>
+      </c>
+      <c r="J20" t="n">
+        <v>48070.3</v>
+      </c>
+      <c r="K20" t="n">
+        <v>48070.3</v>
       </c>
     </row>
     <row r="21">
@@ -11590,8 +12086,20 @@
       <c r="F21" t="n">
         <v>543.1799999999999</v>
       </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
       <c r="H21" t="n">
         <v>47680.8</v>
+      </c>
+      <c r="I21" t="n">
+        <v>47680.8</v>
+      </c>
+      <c r="J21" t="n">
+        <v>48922.9</v>
+      </c>
+      <c r="K21" t="n">
+        <v>48922.9</v>
       </c>
     </row>
     <row r="22">
@@ -11604,8 +12112,20 @@
       <c r="F22" t="n">
         <v>543.08</v>
       </c>
+      <c r="G22" t="n">
+        <v>-7.275957614183426e-12</v>
+      </c>
       <c r="H22" t="n">
         <v>47754.4</v>
+      </c>
+      <c r="I22" t="n">
+        <v>47754.40000000001</v>
+      </c>
+      <c r="J22" t="n">
+        <v>47680.8</v>
+      </c>
+      <c r="K22" t="n">
+        <v>47680.8</v>
       </c>
     </row>
     <row r="23">
@@ -11618,8 +12138,20 @@
       <c r="F23" t="n">
         <v>542.98</v>
       </c>
+      <c r="G23" t="n">
+        <v>-7.275957614183426e-12</v>
+      </c>
       <c r="H23" t="n">
         <v>48211.7</v>
+      </c>
+      <c r="I23" t="n">
+        <v>48211.7</v>
+      </c>
+      <c r="J23" t="n">
+        <v>47754.4</v>
+      </c>
+      <c r="K23" t="n">
+        <v>47754.40000000001</v>
       </c>
     </row>
     <row r="24">
@@ -11632,8 +12164,20 @@
       <c r="F24" t="n">
         <v>542.88</v>
       </c>
+      <c r="G24" t="n">
+        <v>-1.455191522836685e-11</v>
+      </c>
       <c r="H24" t="n">
         <v>47863.3</v>
+      </c>
+      <c r="I24" t="n">
+        <v>47863.30000000002</v>
+      </c>
+      <c r="J24" t="n">
+        <v>48211.7</v>
+      </c>
+      <c r="K24" t="n">
+        <v>48211.7</v>
       </c>
     </row>
     <row r="25">
@@ -11646,8 +12190,20 @@
       <c r="F25" t="n">
         <v>542.78</v>
       </c>
+      <c r="G25" t="n">
+        <v>-2.182787284255028e-11</v>
+      </c>
       <c r="H25" t="n">
         <v>47621.9</v>
+      </c>
+      <c r="I25" t="n">
+        <v>47621.90000000002</v>
+      </c>
+      <c r="J25" t="n">
+        <v>47863.3</v>
+      </c>
+      <c r="K25" t="n">
+        <v>47863.30000000002</v>
       </c>
     </row>
     <row r="26">
@@ -11660,8 +12216,20 @@
       <c r="F26" t="n">
         <v>542.6799999999999</v>
       </c>
+      <c r="G26" t="n">
+        <v>-3.637978807091713e-11</v>
+      </c>
       <c r="H26" t="n">
         <v>46922.5</v>
+      </c>
+      <c r="I26" t="n">
+        <v>46922.50000000004</v>
+      </c>
+      <c r="J26" t="n">
+        <v>47621.9</v>
+      </c>
+      <c r="K26" t="n">
+        <v>47621.90000000002</v>
       </c>
     </row>
     <row r="27">
@@ -11674,8 +12242,20 @@
       <c r="F27" t="n">
         <v>542.58</v>
       </c>
+      <c r="G27" t="n">
+        <v>-5.820766091346741e-11</v>
+      </c>
       <c r="H27" t="n">
         <v>46828.6</v>
+      </c>
+      <c r="I27" t="n">
+        <v>46828.60000000006</v>
+      </c>
+      <c r="J27" t="n">
+        <v>46922.5</v>
+      </c>
+      <c r="K27" t="n">
+        <v>46922.50000000004</v>
       </c>
     </row>
     <row r="28">
@@ -11688,8 +12268,20 @@
       <c r="F28" t="n">
         <v>542.48</v>
       </c>
+      <c r="G28" t="n">
+        <v>-9.458744898438454e-11</v>
+      </c>
       <c r="H28" t="n">
         <v>46541.6</v>
+      </c>
+      <c r="I28" t="n">
+        <v>46541.60000000009</v>
+      </c>
+      <c r="J28" t="n">
+        <v>46828.6</v>
+      </c>
+      <c r="K28" t="n">
+        <v>46828.60000000006</v>
       </c>
     </row>
     <row r="29">
@@ -11702,8 +12294,20 @@
       <c r="F29" t="n">
         <v>542.38</v>
       </c>
+      <c r="G29" t="n">
+        <v>-1.600710675120354e-10</v>
+      </c>
       <c r="H29" t="n">
         <v>46921.1</v>
+      </c>
+      <c r="I29" t="n">
+        <v>46921.10000000016</v>
+      </c>
+      <c r="J29" t="n">
+        <v>46541.6</v>
+      </c>
+      <c r="K29" t="n">
+        <v>46541.60000000009</v>
       </c>
     </row>
     <row r="30">
@@ -11716,8 +12320,20 @@
       <c r="F30" t="n">
         <v>542.28</v>
       </c>
+      <c r="G30" t="n">
+        <v>-2.764863893389702e-10</v>
+      </c>
       <c r="H30" t="n">
         <v>47045.9</v>
+      </c>
+      <c r="I30" t="n">
+        <v>47045.90000000028</v>
+      </c>
+      <c r="J30" t="n">
+        <v>46921.1</v>
+      </c>
+      <c r="K30" t="n">
+        <v>46921.10000000016</v>
       </c>
     </row>
     <row r="31">
@@ -11730,8 +12346,20 @@
       <c r="F31" t="n">
         <v>542.1799999999999</v>
       </c>
+      <c r="G31" t="n">
+        <v>-4.583853296935558e-10</v>
+      </c>
       <c r="H31" t="n">
         <v>47351.3</v>
+      </c>
+      <c r="I31" t="n">
+        <v>47351.30000000046</v>
+      </c>
+      <c r="J31" t="n">
+        <v>47045.9</v>
+      </c>
+      <c r="K31" t="n">
+        <v>47045.90000000028</v>
       </c>
     </row>
     <row r="32">
@@ -11744,8 +12372,20 @@
       <c r="F32" t="n">
         <v>542.08</v>
       </c>
+      <c r="G32" t="n">
+        <v>-7.712515071034431e-10</v>
+      </c>
       <c r="H32" t="n">
         <v>46947.9</v>
+      </c>
+      <c r="I32" t="n">
+        <v>46947.90000000077</v>
+      </c>
+      <c r="J32" t="n">
+        <v>47351.3</v>
+      </c>
+      <c r="K32" t="n">
+        <v>47351.30000000046</v>
       </c>
     </row>
     <row r="33">
@@ -11758,8 +12398,20 @@
       <c r="F33" t="n">
         <v>541.98</v>
       </c>
+      <c r="G33" t="n">
+        <v>-1.280568540096283e-09</v>
+      </c>
       <c r="H33" t="n">
         <v>47201.2</v>
+      </c>
+      <c r="I33" t="n">
+        <v>47201.20000000128</v>
+      </c>
+      <c r="J33" t="n">
+        <v>46947.9</v>
+      </c>
+      <c r="K33" t="n">
+        <v>46947.90000000077</v>
       </c>
     </row>
     <row r="34">
@@ -11772,8 +12424,20 @@
       <c r="F34" t="n">
         <v>541.88</v>
       </c>
+      <c r="G34" t="n">
+        <v>-2.117303665727377e-09</v>
+      </c>
       <c r="H34" t="n">
         <v>47402.3</v>
+      </c>
+      <c r="I34" t="n">
+        <v>47402.30000000212</v>
+      </c>
+      <c r="J34" t="n">
+        <v>47201.2</v>
+      </c>
+      <c r="K34" t="n">
+        <v>47201.20000000128</v>
       </c>
     </row>
     <row r="35">
@@ -11786,8 +12450,20 @@
       <c r="F35" t="n">
         <v>541.78</v>
       </c>
+      <c r="G35" t="n">
+        <v>-3.492459654808044e-09</v>
+      </c>
       <c r="H35" t="n">
         <v>46781.3</v>
+      </c>
+      <c r="I35" t="n">
+        <v>46781.3000000035</v>
+      </c>
+      <c r="J35" t="n">
+        <v>47402.3</v>
+      </c>
+      <c r="K35" t="n">
+        <v>47402.30000000212</v>
       </c>
     </row>
     <row r="36">
@@ -11800,8 +12476,20 @@
       <c r="F36" t="n">
         <v>541.6799999999999</v>
       </c>
+      <c r="G36" t="n">
+        <v>-5.740730557590723e-09</v>
+      </c>
       <c r="H36" t="n">
         <v>47433.4</v>
+      </c>
+      <c r="I36" t="n">
+        <v>47433.40000000574</v>
+      </c>
+      <c r="J36" t="n">
+        <v>46781.3</v>
+      </c>
+      <c r="K36" t="n">
+        <v>46781.3000000035</v>
       </c>
     </row>
     <row r="37">
@@ -11814,8 +12502,20 @@
       <c r="F37" t="n">
         <v>541.58</v>
       </c>
+      <c r="G37" t="n">
+        <v>-9.400537237524986e-09</v>
+      </c>
       <c r="H37" t="n">
         <v>46591.5</v>
+      </c>
+      <c r="I37" t="n">
+        <v>46591.5000000094</v>
+      </c>
+      <c r="J37" t="n">
+        <v>47433.4</v>
+      </c>
+      <c r="K37" t="n">
+        <v>47433.40000000574</v>
       </c>
     </row>
     <row r="38">
@@ -11828,8 +12528,20 @@
       <c r="F38" t="n">
         <v>541.48</v>
       </c>
+      <c r="G38" t="n">
+        <v>-1.530861482024193e-08</v>
+      </c>
       <c r="H38" t="n">
         <v>47057.5</v>
+      </c>
+      <c r="I38" t="n">
+        <v>47057.50000001531</v>
+      </c>
+      <c r="J38" t="n">
+        <v>46591.5</v>
+      </c>
+      <c r="K38" t="n">
+        <v>46591.5000000094</v>
       </c>
     </row>
     <row r="39">
@@ -11842,8 +12554,20 @@
       <c r="F39" t="n">
         <v>541.38</v>
       </c>
+      <c r="G39" t="n">
+        <v>-2.483284333720803e-08</v>
+      </c>
       <c r="H39" t="n">
         <v>46964.3</v>
+      </c>
+      <c r="I39" t="n">
+        <v>46964.30000002484</v>
+      </c>
+      <c r="J39" t="n">
+        <v>47057.5</v>
+      </c>
+      <c r="K39" t="n">
+        <v>47057.50000001531</v>
       </c>
     </row>
     <row r="40">
@@ -11856,8 +12580,20 @@
       <c r="F40" t="n">
         <v>541.28</v>
       </c>
+      <c r="G40" t="n">
+        <v>-4.010507836937904e-08</v>
+      </c>
       <c r="H40" t="n">
         <v>48107.6</v>
+      </c>
+      <c r="I40" t="n">
+        <v>48107.6000000401</v>
+      </c>
+      <c r="J40" t="n">
+        <v>46964.3</v>
+      </c>
+      <c r="K40" t="n">
+        <v>46964.30000002484</v>
       </c>
     </row>
     <row r="41">
@@ -11870,8 +12606,20 @@
       <c r="F41" t="n">
         <v>541.1799999999999</v>
       </c>
+      <c r="G41" t="n">
+        <v>-6.450136424973607e-08</v>
+      </c>
       <c r="H41" t="n">
         <v>47256.7</v>
+      </c>
+      <c r="I41" t="n">
+        <v>47256.7000000645</v>
+      </c>
+      <c r="J41" t="n">
+        <v>48107.6</v>
+      </c>
+      <c r="K41" t="n">
+        <v>48107.60000004011</v>
       </c>
     </row>
     <row r="42">
@@ -11884,8 +12632,20 @@
       <c r="F42" t="n">
         <v>541.08</v>
       </c>
+      <c r="G42" t="n">
+        <v>-1.032894942909479e-07</v>
+      </c>
       <c r="H42" t="n">
         <v>46274.8</v>
+      </c>
+      <c r="I42" t="n">
+        <v>46274.80000010329</v>
+      </c>
+      <c r="J42" t="n">
+        <v>47256.7</v>
+      </c>
+      <c r="K42" t="n">
+        <v>47256.7000000645</v>
       </c>
     </row>
     <row r="43">
@@ -11898,8 +12658,20 @@
       <c r="F43" t="n">
         <v>540.98</v>
       </c>
+      <c r="G43" t="n">
+        <v>-1.646913005970418e-07</v>
+      </c>
       <c r="H43" t="n">
         <v>46851.9</v>
+      </c>
+      <c r="I43" t="n">
+        <v>46851.90000016469</v>
+      </c>
+      <c r="J43" t="n">
+        <v>46274.8</v>
+      </c>
+      <c r="K43" t="n">
+        <v>46274.80000010329</v>
       </c>
     </row>
     <row r="44">
@@ -11912,8 +12684,20 @@
       <c r="F44" t="n">
         <v>540.88</v>
       </c>
+      <c r="G44" t="n">
+        <v>-2.614760887809098e-07</v>
+      </c>
       <c r="H44" t="n">
         <v>46646.7</v>
+      </c>
+      <c r="I44" t="n">
+        <v>46646.70000026147</v>
+      </c>
+      <c r="J44" t="n">
+        <v>46851.9</v>
+      </c>
+      <c r="K44" t="n">
+        <v>46851.9000001647</v>
       </c>
     </row>
     <row r="45">
@@ -11926,8 +12710,20 @@
       <c r="F45" t="n">
         <v>540.78</v>
       </c>
+      <c r="G45" t="n">
+        <v>-4.133617039769888e-07</v>
+      </c>
       <c r="H45" t="n">
         <v>45538.9</v>
+      </c>
+      <c r="I45" t="n">
+        <v>45538.90000041336</v>
+      </c>
+      <c r="J45" t="n">
+        <v>46646.7</v>
+      </c>
+      <c r="K45" t="n">
+        <v>46646.70000026147</v>
       </c>
     </row>
     <row r="46">
@@ -11940,8 +12736,20 @@
       <c r="F46" t="n">
         <v>540.6799999999999</v>
       </c>
+      <c r="G46" t="n">
+        <v>-6.506816134788096e-07</v>
+      </c>
       <c r="H46" t="n">
         <v>46497.2</v>
+      </c>
+      <c r="I46" t="n">
+        <v>46497.20000065068</v>
+      </c>
+      <c r="J46" t="n">
+        <v>45538.9</v>
+      </c>
+      <c r="K46" t="n">
+        <v>45538.90000041337</v>
       </c>
     </row>
     <row r="47">
@@ -11954,8 +12762,20 @@
       <c r="F47" t="n">
         <v>540.58</v>
       </c>
+      <c r="G47" t="n">
+        <v>-1.019900082610548e-06</v>
+      </c>
       <c r="H47" t="n">
         <v>47188.7</v>
+      </c>
+      <c r="I47" t="n">
+        <v>47188.7000010199</v>
+      </c>
+      <c r="J47" t="n">
+        <v>46497.2</v>
+      </c>
+      <c r="K47" t="n">
+        <v>46497.20000065069</v>
       </c>
     </row>
     <row r="48">
@@ -11968,8 +12788,20 @@
       <c r="F48" t="n">
         <v>540.48</v>
       </c>
+      <c r="G48" t="n">
+        <v>-1.591804903000593e-06</v>
+      </c>
       <c r="H48" t="n">
         <v>46594.4</v>
+      </c>
+      <c r="I48" t="n">
+        <v>46594.40000159181</v>
+      </c>
+      <c r="J48" t="n">
+        <v>47188.7</v>
+      </c>
+      <c r="K48" t="n">
+        <v>47188.70000101991</v>
       </c>
     </row>
     <row r="49">
@@ -11982,8 +12814,20 @@
       <c r="F49" t="n">
         <v>540.38</v>
       </c>
+      <c r="G49" t="n">
+        <v>-2.473832864779979e-06</v>
+      </c>
       <c r="H49" t="n">
         <v>45738.4</v>
+      </c>
+      <c r="I49" t="n">
+        <v>45738.40000247383</v>
+      </c>
+      <c r="J49" t="n">
+        <v>46594.4</v>
+      </c>
+      <c r="K49" t="n">
+        <v>46594.40000159183</v>
       </c>
     </row>
     <row r="50">
@@ -11996,8 +12840,20 @@
       <c r="F50" t="n">
         <v>540.28</v>
       </c>
+      <c r="G50" t="n">
+        <v>-3.828252374660224e-06</v>
+      </c>
       <c r="H50" t="n">
         <v>45499.2</v>
+      </c>
+      <c r="I50" t="n">
+        <v>45499.20000382825</v>
+      </c>
+      <c r="J50" t="n">
+        <v>45738.4</v>
+      </c>
+      <c r="K50" t="n">
+        <v>45738.40000247387</v>
       </c>
     </row>
     <row r="51">
@@ -12010,8 +12866,20 @@
       <c r="F51" t="n">
         <v>540.1799999999999</v>
       </c>
+      <c r="G51" t="n">
+        <v>-5.899055395275354e-06</v>
+      </c>
       <c r="H51" t="n">
         <v>45977.5</v>
+      </c>
+      <c r="I51" t="n">
+        <v>45977.50000589906</v>
+      </c>
+      <c r="J51" t="n">
+        <v>45499.2</v>
+      </c>
+      <c r="K51" t="n">
+        <v>45499.20000382831</v>
       </c>
     </row>
     <row r="52">
@@ -12024,8 +12892,20 @@
       <c r="F52" t="n">
         <v>540.08</v>
       </c>
+      <c r="G52" t="n">
+        <v>-9.051451343111694e-06</v>
+      </c>
       <c r="H52" t="n">
         <v>45482.6</v>
+      </c>
+      <c r="I52" t="n">
+        <v>45482.60000905145</v>
+      </c>
+      <c r="J52" t="n">
+        <v>45977.5</v>
+      </c>
+      <c r="K52" t="n">
+        <v>45977.50000589914</v>
       </c>
     </row>
     <row r="53">
@@ -12038,8 +12918,20 @@
       <c r="F53" t="n">
         <v>539.98</v>
       </c>
+      <c r="G53" t="n">
+        <v>-1.382959453621879e-05</v>
+      </c>
       <c r="H53" t="n">
         <v>45679.8</v>
+      </c>
+      <c r="I53" t="n">
+        <v>45679.8000138296</v>
+      </c>
+      <c r="J53" t="n">
+        <v>45482.6</v>
+      </c>
+      <c r="K53" t="n">
+        <v>45482.60000905158</v>
       </c>
     </row>
     <row r="54">
@@ -12052,8 +12944,20 @@
       <c r="F54" t="n">
         <v>539.88</v>
       </c>
+      <c r="G54" t="n">
+        <v>-2.104058512486517e-05</v>
+      </c>
       <c r="H54" t="n">
         <v>44395.1</v>
+      </c>
+      <c r="I54" t="n">
+        <v>44395.10002104058</v>
+      </c>
+      <c r="J54" t="n">
+        <v>45679.8</v>
+      </c>
+      <c r="K54" t="n">
+        <v>45679.80001382979</v>
       </c>
     </row>
     <row r="55">
@@ -12066,8 +12970,20 @@
       <c r="F55" t="n">
         <v>539.78</v>
       </c>
+      <c r="G55" t="n">
+        <v>-3.187614493072033e-05</v>
+      </c>
       <c r="H55" t="n">
         <v>45122.1</v>
+      </c>
+      <c r="I55" t="n">
+        <v>45122.10003187614</v>
+      </c>
+      <c r="J55" t="n">
+        <v>44395.1</v>
+      </c>
+      <c r="K55" t="n">
+        <v>44395.1000210409</v>
       </c>
     </row>
     <row r="56">
@@ -12080,8 +12996,20 @@
       <c r="F56" t="n">
         <v>539.6799999999999</v>
       </c>
+      <c r="G56" t="n">
+        <v>-4.808784433407709e-05</v>
+      </c>
       <c r="H56" t="n">
         <v>44310</v>
+      </c>
+      <c r="I56" t="n">
+        <v>44310.00004808784</v>
+      </c>
+      <c r="J56" t="n">
+        <v>45122.1</v>
+      </c>
+      <c r="K56" t="n">
+        <v>45122.10003187661</v>
       </c>
     </row>
     <row r="57">
@@ -12094,8 +13022,20 @@
       <c r="F57" t="n">
         <v>539.58</v>
       </c>
+      <c r="G57" t="n">
+        <v>-7.223846478154883e-05</v>
+      </c>
       <c r="H57" t="n">
         <v>44337.1</v>
+      </c>
+      <c r="I57" t="n">
+        <v>44337.10007223846</v>
+      </c>
+      <c r="J57" t="n">
+        <v>44310</v>
+      </c>
+      <c r="K57" t="n">
+        <v>44310.00004808854</v>
       </c>
     </row>
     <row r="58">
@@ -12108,8 +13048,20 @@
       <c r="F58" t="n">
         <v>539.48</v>
       </c>
+      <c r="G58" t="n">
+        <v>-0.000108060659840703</v>
+      </c>
       <c r="H58" t="n">
         <v>43303.6</v>
+      </c>
+      <c r="I58" t="n">
+        <v>43303.60010806066</v>
+      </c>
+      <c r="J58" t="n">
+        <v>44337.1</v>
+      </c>
+      <c r="K58" t="n">
+        <v>44337.10007223952</v>
       </c>
     </row>
     <row r="59">
@@ -12122,8 +13074,20 @@
       <c r="F59" t="n">
         <v>539.38</v>
       </c>
+      <c r="G59" t="n">
+        <v>-0.0001609663013368845</v>
+      </c>
       <c r="H59" t="n">
         <v>43176.2</v>
+      </c>
+      <c r="I59" t="n">
+        <v>43176.2001609663</v>
+      </c>
+      <c r="J59" t="n">
+        <v>43303.6</v>
+      </c>
+      <c r="K59" t="n">
+        <v>43303.60010806224</v>
       </c>
     </row>
     <row r="60">
@@ -12136,8 +13100,20 @@
       <c r="F60" t="n">
         <v>539.28</v>
       </c>
+      <c r="G60" t="n">
+        <v>-0.0002387662316323258</v>
+      </c>
       <c r="H60" t="n">
         <v>42995.6</v>
+      </c>
+      <c r="I60" t="n">
+        <v>42995.60023876623</v>
+      </c>
+      <c r="J60" t="n">
+        <v>43176.2</v>
+      </c>
+      <c r="K60" t="n">
+        <v>43176.20016096866</v>
       </c>
     </row>
     <row r="61">
@@ -12150,8 +13126,20 @@
       <c r="F61" t="n">
         <v>539.1799999999999</v>
       </c>
+      <c r="G61" t="n">
+        <v>-0.0003526824511936866</v>
+      </c>
       <c r="H61" t="n">
         <v>42623.1</v>
+      </c>
+      <c r="I61" t="n">
+        <v>42623.10035268245</v>
+      </c>
+      <c r="J61" t="n">
+        <v>42995.6</v>
+      </c>
+      <c r="K61" t="n">
+        <v>42995.60023876972</v>
       </c>
     </row>
     <row r="62">
@@ -12164,8 +13152,20 @@
       <c r="F62" t="n">
         <v>539.08</v>
       </c>
+      <c r="G62" t="n">
+        <v>-0.0005187645947444253</v>
+      </c>
       <c r="H62" t="n">
         <v>43099.4</v>
+      </c>
+      <c r="I62" t="n">
+        <v>43099.4005187646</v>
+      </c>
+      <c r="J62" t="n">
+        <v>42623.1</v>
+      </c>
+      <c r="K62" t="n">
+        <v>42623.10035268761</v>
       </c>
     </row>
     <row r="63">
@@ -12178,8 +13178,20 @@
       <c r="F63" t="n">
         <v>538.98</v>
       </c>
+      <c r="G63" t="n">
+        <v>-0.0007598623487865552</v>
+      </c>
       <c r="H63" t="n">
         <v>42832.8</v>
+      </c>
+      <c r="I63" t="n">
+        <v>42832.80075986235</v>
+      </c>
+      <c r="J63" t="n">
+        <v>43099.4</v>
+      </c>
+      <c r="K63" t="n">
+        <v>43099.40051877218</v>
       </c>
     </row>
     <row r="64">
@@ -12192,8 +13204,20 @@
       <c r="F64" t="n">
         <v>538.88</v>
       </c>
+      <c r="G64" t="n">
+        <v>-0.001108358650526498</v>
+      </c>
       <c r="H64" t="n">
         <v>42906.4</v>
+      </c>
+      <c r="I64" t="n">
+        <v>42906.40110835865</v>
+      </c>
+      <c r="J64" t="n">
+        <v>42832.8</v>
+      </c>
+      <c r="K64" t="n">
+        <v>42832.80075987346</v>
       </c>
     </row>
     <row r="65">
@@ -12206,8 +13230,20 @@
       <c r="F65" t="n">
         <v>538.78</v>
       </c>
+      <c r="G65" t="n">
+        <v>-0.001609938408364542</v>
+      </c>
       <c r="H65" t="n">
         <v>41538.1</v>
+      </c>
+      <c r="I65" t="n">
+        <v>41538.10160993841</v>
+      </c>
+      <c r="J65" t="n">
+        <v>42906.4</v>
+      </c>
+      <c r="K65" t="n">
+        <v>42906.40110837486</v>
       </c>
     </row>
     <row r="66">
@@ -12220,8 +13256,20 @@
       <c r="F66" t="n">
         <v>538.6799999999999</v>
       </c>
+      <c r="G66" t="n">
+        <v>-0.002328759321244434</v>
+      </c>
       <c r="H66" t="n">
         <v>41941.6</v>
+      </c>
+      <c r="I66" t="n">
+        <v>41941.60232875932</v>
+      </c>
+      <c r="J66" t="n">
+        <v>41538.1</v>
+      </c>
+      <c r="K66" t="n">
+        <v>41538.10160996194</v>
       </c>
     </row>
     <row r="67">
@@ -12234,8 +13282,20 @@
       <c r="F67" t="n">
         <v>538.58</v>
       </c>
+      <c r="G67" t="n">
+        <v>-0.003354511572979391</v>
+      </c>
       <c r="H67" t="n">
         <v>40284.7</v>
+      </c>
+      <c r="I67" t="n">
+        <v>40284.70335451157</v>
+      </c>
+      <c r="J67" t="n">
+        <v>41941.6</v>
+      </c>
+      <c r="K67" t="n">
+        <v>41941.60232879337</v>
       </c>
     </row>
     <row r="68">
@@ -12248,8 +13308,20 @@
       <c r="F68" t="n">
         <v>538.48</v>
       </c>
+      <c r="G68" t="n">
+        <v>-0.004812008221051656</v>
+      </c>
       <c r="H68" t="n">
         <v>41792.5</v>
+      </c>
+      <c r="I68" t="n">
+        <v>41792.50481200822</v>
+      </c>
+      <c r="J68" t="n">
+        <v>40284.7</v>
+      </c>
+      <c r="K68" t="n">
+        <v>40284.70335456062</v>
       </c>
     </row>
     <row r="69">
@@ -12262,8 +13334,20 @@
       <c r="F69" t="n">
         <v>538.38</v>
       </c>
+      <c r="G69" t="n">
+        <v>-0.00687414900312433</v>
+      </c>
       <c r="H69" t="n">
         <v>41865.3</v>
+      </c>
+      <c r="I69" t="n">
+        <v>41865.30687414901</v>
+      </c>
+      <c r="J69" t="n">
+        <v>41792.5</v>
+      </c>
+      <c r="K69" t="n">
+        <v>41792.50481207858</v>
       </c>
     </row>
     <row r="70">
@@ -12276,8 +13360,20 @@
       <c r="F70" t="n">
         <v>538.28</v>
       </c>
+      <c r="G70" t="n">
+        <v>-0.009779356521903537</v>
+      </c>
       <c r="H70" t="n">
         <v>40219</v>
+      </c>
+      <c r="I70" t="n">
+        <v>40219.00977935652</v>
+      </c>
+      <c r="J70" t="n">
+        <v>41865.3</v>
+      </c>
+      <c r="K70" t="n">
+        <v>41865.30687424952</v>
       </c>
     </row>
     <row r="71">
@@ -12290,8 +13386,20 @@
       <c r="F71" t="n">
         <v>538.1799999999999</v>
       </c>
+      <c r="G71" t="n">
+        <v>-0.01385491041583009</v>
+      </c>
       <c r="H71" t="n">
         <v>41229.2</v>
+      </c>
+      <c r="I71" t="n">
+        <v>41229.21385491041</v>
+      </c>
+      <c r="J71" t="n">
+        <v>40219</v>
+      </c>
+      <c r="K71" t="n">
+        <v>40219.00977949951</v>
       </c>
     </row>
     <row r="72">
@@ -12304,8 +13412,20 @@
       <c r="F72" t="n">
         <v>538.08</v>
       </c>
+      <c r="G72" t="n">
+        <v>-0.0195480180773302</v>
+      </c>
       <c r="H72" t="n">
         <v>41217.1</v>
+      </c>
+      <c r="I72" t="n">
+        <v>41217.11954801808</v>
+      </c>
+      <c r="J72" t="n">
+        <v>41229.2</v>
+      </c>
+      <c r="K72" t="n">
+        <v>41229.21385511299</v>
       </c>
     </row>
     <row r="73">
@@ -12318,8 +13438,20 @@
       <c r="F73" t="n">
         <v>537.98</v>
       </c>
+      <c r="G73" t="n">
+        <v>-0.02746697851398494</v>
+      </c>
       <c r="H73" t="n">
         <v>40096</v>
+      </c>
+      <c r="I73" t="n">
+        <v>40096.02746697851</v>
+      </c>
+      <c r="J73" t="n">
+        <v>41217.1</v>
+      </c>
+      <c r="K73" t="n">
+        <v>41217.1195483039</v>
       </c>
     </row>
     <row r="74">
@@ -12332,8 +13464,20 @@
       <c r="F74" t="n">
         <v>537.88</v>
       </c>
+      <c r="G74" t="n">
+        <v>-0.03843544294068124</v>
+      </c>
       <c r="H74" t="n">
         <v>41375.3</v>
+      </c>
+      <c r="I74" t="n">
+        <v>41375.33843544294</v>
+      </c>
+      <c r="J74" t="n">
+        <v>40096</v>
+      </c>
+      <c r="K74" t="n">
+        <v>40096.02746738013</v>
       </c>
     </row>
     <row r="75">
@@ -12346,8 +13490,20 @@
       <c r="F75" t="n">
         <v>537.78</v>
       </c>
+      <c r="G75" t="n">
+        <v>-0.05356357645359822</v>
+      </c>
       <c r="H75" t="n">
         <v>42743.3</v>
+      </c>
+      <c r="I75" t="n">
+        <v>42743.35356357646</v>
+      </c>
+      <c r="J75" t="n">
+        <v>41375.3</v>
+      </c>
+      <c r="K75" t="n">
+        <v>41375.33843600493</v>
       </c>
     </row>
     <row r="76">
@@ -12360,8 +13516,20 @@
       <c r="F76" t="n">
         <v>537.6799999999999</v>
       </c>
+      <c r="G76" t="n">
+        <v>-0.07434091082541272</v>
+      </c>
       <c r="H76" t="n">
         <v>41739.3</v>
+      </c>
+      <c r="I76" t="n">
+        <v>41739.37434091083</v>
+      </c>
+      <c r="J76" t="n">
+        <v>42743.3</v>
+      </c>
+      <c r="K76" t="n">
+        <v>42743.35356435964</v>
       </c>
     </row>
     <row r="77">
@@ -12374,8 +13542,20 @@
       <c r="F77" t="n">
         <v>537.58</v>
       </c>
+      <c r="G77" t="n">
+        <v>-0.102756882122776</v>
+      </c>
       <c r="H77" t="n">
         <v>41779.1</v>
+      </c>
+      <c r="I77" t="n">
+        <v>41779.20275688212</v>
+      </c>
+      <c r="J77" t="n">
+        <v>41739.3</v>
+      </c>
+      <c r="K77" t="n">
+        <v>41739.37434199781</v>
       </c>
     </row>
     <row r="78">
@@ -12388,8 +13568,20 @@
       <c r="F78" t="n">
         <v>537.48</v>
       </c>
+      <c r="G78" t="n">
+        <v>-0.1414565063241753</v>
+      </c>
       <c r="H78" t="n">
         <v>42431.9</v>
+      </c>
+      <c r="I78" t="n">
+        <v>42432.04145650633</v>
+      </c>
+      <c r="J78" t="n">
+        <v>41779.1</v>
+      </c>
+      <c r="K78" t="n">
+        <v>41779.20275838458</v>
       </c>
     </row>
     <row r="79">
@@ -12402,8 +13594,20 @@
       <c r="F79" t="n">
         <v>537.38</v>
       </c>
+      <c r="G79" t="n">
+        <v>-0.193940402714361</v>
+      </c>
       <c r="H79" t="n">
         <v>42881</v>
+      </c>
+      <c r="I79" t="n">
+        <v>42881.19394040271</v>
+      </c>
+      <c r="J79" t="n">
+        <v>42431.9</v>
+      </c>
+      <c r="K79" t="n">
+        <v>42432.04145857464</v>
       </c>
     </row>
     <row r="80">
@@ -12416,8 +13620,20 @@
       <c r="F80" t="n">
         <v>537.28</v>
       </c>
+      <c r="G80" t="n">
+        <v>-0.2648204720098875</v>
+      </c>
       <c r="H80" t="n">
         <v>41384.7</v>
+      </c>
+      <c r="I80" t="n">
+        <v>41384.96482047201</v>
+      </c>
+      <c r="J80" t="n">
+        <v>42881</v>
+      </c>
+      <c r="K80" t="n">
+        <v>42881.19394323843</v>
       </c>
     </row>
     <row r="81">
@@ -12430,8 +13646,20 @@
       <c r="F81" t="n">
         <v>537.1799999999999</v>
       </c>
+      <c r="G81" t="n">
+        <v>-0.3601450210844632</v>
+      </c>
       <c r="H81" t="n">
         <v>40732</v>
+      </c>
+      <c r="I81" t="n">
+        <v>40732.36014502108</v>
+      </c>
+      <c r="J81" t="n">
+        <v>41384.7</v>
+      </c>
+      <c r="K81" t="n">
+        <v>41384.9648243441</v>
       </c>
     </row>
     <row r="82">
@@ -12444,8 +13672,20 @@
       <c r="F82" t="n">
         <v>537.08</v>
       </c>
+      <c r="G82" t="n">
+        <v>-0.4878100451969658</v>
+      </c>
       <c r="H82" t="n">
         <v>42223.1</v>
+      </c>
+      <c r="I82" t="n">
+        <v>42223.5878100452</v>
+      </c>
+      <c r="J82" t="n">
+        <v>40732</v>
+      </c>
+      <c r="K82" t="n">
+        <v>40732.36015028697</v>
       </c>
     </row>
     <row r="83">
@@ -12458,8 +13698,20 @@
       <c r="F83" t="n">
         <v>536.98</v>
       </c>
+      <c r="G83" t="n">
+        <v>-0.6580767788909725</v>
+      </c>
       <c r="H83" t="n">
         <v>41680.1</v>
+      </c>
+      <c r="I83" t="n">
+        <v>41680.75807677889</v>
+      </c>
+      <c r="J83" t="n">
+        <v>42223.1</v>
+      </c>
+      <c r="K83" t="n">
+        <v>42223.58781717774</v>
       </c>
     </row>
     <row r="84">
@@ -12472,8 +13724,20 @@
       <c r="F84" t="n">
         <v>536.88</v>
       </c>
+      <c r="G84" t="n">
+        <v>-0.8842195519828238</v>
+      </c>
       <c r="H84" t="n">
         <v>42359.5</v>
+      </c>
+      <c r="I84" t="n">
+        <v>42360.38421955198</v>
+      </c>
+      <c r="J84" t="n">
+        <v>41680.1</v>
+      </c>
+      <c r="K84" t="n">
+        <v>41680.758086401</v>
       </c>
     </row>
     <row r="85">
@@ -12486,8 +13750,20 @@
       <c r="F85" t="n">
         <v>536.78</v>
       </c>
+      <c r="G85" t="n">
+        <v>-1.183332475717179</v>
+      </c>
       <c r="H85" t="n">
         <v>42169.3</v>
+      </c>
+      <c r="I85" t="n">
+        <v>42170.48333247572</v>
+      </c>
+      <c r="J85" t="n">
+        <v>42359.5</v>
+      </c>
+      <c r="K85" t="n">
+        <v>42360.38423248066</v>
       </c>
     </row>
     <row r="86">
@@ -12500,8 +13776,20 @@
       <c r="F86" t="n">
         <v>536.6799999999999</v>
       </c>
+      <c r="G86" t="n">
+        <v>-1.577328566723736</v>
+      </c>
       <c r="H86" t="n">
         <v>42478.2</v>
+      </c>
+      <c r="I86" t="n">
+        <v>42479.77732856672</v>
+      </c>
+      <c r="J86" t="n">
+        <v>42169.3</v>
+      </c>
+      <c r="K86" t="n">
+        <v>42170.4833497779</v>
       </c>
     </row>
     <row r="87">
@@ -12514,8 +13802,20 @@
       <c r="F87" t="n">
         <v>536.58</v>
       </c>
+      <c r="G87" t="n">
+        <v>-2.094170610274887</v>
+      </c>
       <c r="H87" t="n">
         <v>42341</v>
+      </c>
+      <c r="I87" t="n">
+        <v>42343.09417061027</v>
+      </c>
+      <c r="J87" t="n">
+        <v>42478.2</v>
+      </c>
+      <c r="K87" t="n">
+        <v>42479.77735162974</v>
       </c>
     </row>
     <row r="88">
@@ -12528,8 +13828,20 @@
       <c r="F88" t="n">
         <v>536.48</v>
       </c>
+      <c r="G88" t="n">
+        <v>-2.769379371733521</v>
+      </c>
       <c r="H88" t="n">
         <v>42236.1</v>
+      </c>
+      <c r="I88" t="n">
+        <v>42238.86937937173</v>
+      </c>
+      <c r="J88" t="n">
+        <v>42341</v>
+      </c>
+      <c r="K88" t="n">
+        <v>42343.09420123033</v>
       </c>
     </row>
     <row r="89">
@@ -12542,8 +13854,20 @@
       <c r="F89" t="n">
         <v>536.38</v>
       </c>
+      <c r="G89" t="n">
+        <v>-3.647871666093124</v>
+      </c>
       <c r="H89" t="n">
         <v>43978</v>
+      </c>
+      <c r="I89" t="n">
+        <v>43981.64787166609</v>
+      </c>
+      <c r="J89" t="n">
+        <v>42236.1</v>
+      </c>
+      <c r="K89" t="n">
+        <v>42238.8694198644</v>
       </c>
     </row>
     <row r="90">
@@ -12556,8 +13880,20 @@
       <c r="F90" t="n">
         <v>536.28</v>
       </c>
+      <c r="G90" t="n">
+        <v>-4.786188245030644</v>
+      </c>
       <c r="H90" t="n">
         <v>43202.3</v>
+      </c>
+      <c r="I90" t="n">
+        <v>43207.08618824503</v>
+      </c>
+      <c r="J90" t="n">
+        <v>43978</v>
+      </c>
+      <c r="K90" t="n">
+        <v>43981.6479250037</v>
       </c>
     </row>
     <row r="91">
@@ -12570,8 +13906,20 @@
       <c r="F91" t="n">
         <v>536.1799999999999</v>
       </c>
+      <c r="G91" t="n">
+        <v>-6.25517938152916</v>
+      </c>
       <c r="H91" t="n">
         <v>43182.1</v>
+      </c>
+      <c r="I91" t="n">
+        <v>43188.35517938153</v>
+      </c>
+      <c r="J91" t="n">
+        <v>43202.3</v>
+      </c>
+      <c r="K91" t="n">
+        <v>43207.08625822661</v>
       </c>
     </row>
     <row r="92">
@@ -12584,8 +13932,20 @@
       <c r="F92" t="n">
         <v>536.08</v>
       </c>
+      <c r="G92" t="n">
+        <v>-8.143224310282676</v>
+      </c>
       <c r="H92" t="n">
         <v>42938.6</v>
+      </c>
+      <c r="I92" t="n">
+        <v>42946.74322431028</v>
+      </c>
+      <c r="J92" t="n">
+        <v>43182.1</v>
+      </c>
+      <c r="K92" t="n">
+        <v>43188.35527084206</v>
       </c>
     </row>
     <row r="93">
@@ -12598,8 +13958,20 @@
       <c r="F93" t="n">
         <v>535.98</v>
       </c>
+      <c r="G93" t="n">
+        <v>-10.56006916040496</v>
+      </c>
       <c r="H93" t="n">
         <v>42639.4</v>
+      </c>
+      <c r="I93" t="n">
+        <v>42649.96006916041</v>
+      </c>
+      <c r="J93" t="n">
+        <v>42938.6</v>
+      </c>
+      <c r="K93" t="n">
+        <v>42946.74334337699</v>
       </c>
     </row>
     <row r="94">
@@ -12612,8 +13984,20 @@
       <c r="F94" t="n">
         <v>535.88</v>
       </c>
+      <c r="G94" t="n">
+        <v>-13.64137649153417</v>
+      </c>
       <c r="H94" t="n">
         <v>43272.7</v>
+      </c>
+      <c r="I94" t="n">
+        <v>43286.34137649153</v>
+      </c>
+      <c r="J94" t="n">
+        <v>42639.4</v>
+      </c>
+      <c r="K94" t="n">
+        <v>42649.96022356518</v>
       </c>
     </row>
     <row r="95">
@@ -12626,8 +14010,20 @@
       <c r="F95" t="n">
         <v>535.78</v>
       </c>
+      <c r="G95" t="n">
+        <v>-17.55408775607793</v>
+      </c>
       <c r="H95" t="n">
         <v>43237.8</v>
+      </c>
+      <c r="I95" t="n">
+        <v>43255.35408775608</v>
+      </c>
+      <c r="J95" t="n">
+        <v>43272.7</v>
+      </c>
+      <c r="K95" t="n">
+        <v>43286.34157594986</v>
       </c>
     </row>
     <row r="96">
@@ -12640,8 +14036,20 @@
       <c r="F96" t="n">
         <v>535.6799999999999</v>
       </c>
+      <c r="G96" t="n">
+        <v>-22.50270764323068</v>
+      </c>
       <c r="H96" t="n">
         <v>42287.2</v>
+      </c>
+      <c r="I96" t="n">
+        <v>42309.70270764323</v>
+      </c>
+      <c r="J96" t="n">
+        <v>43237.8</v>
+      </c>
+      <c r="K96" t="n">
+        <v>43255.35434442438</v>
       </c>
     </row>
     <row r="97">
@@ -12654,8 +14062,20 @@
       <c r="F97" t="n">
         <v>535.58</v>
       </c>
+      <c r="G97" t="n">
+        <v>-28.73662593372865</v>
+      </c>
       <c r="H97" t="n">
         <v>42514.4</v>
+      </c>
+      <c r="I97" t="n">
+        <v>42543.13662593373</v>
+      </c>
+      <c r="J97" t="n">
+        <v>42287.2</v>
+      </c>
+      <c r="K97" t="n">
+        <v>42309.70303666812</v>
       </c>
     </row>
     <row r="98">
@@ -12668,8 +14088,20 @@
       <c r="F98" t="n">
         <v>535.48</v>
       </c>
+      <c r="G98" t="n">
+        <v>-36.55859775931458</v>
+      </c>
       <c r="H98" t="n">
         <v>43303.1</v>
+      </c>
+      <c r="I98" t="n">
+        <v>43339.65859775931</v>
+      </c>
+      <c r="J98" t="n">
+        <v>42514.4</v>
+      </c>
+      <c r="K98" t="n">
+        <v>42543.13704610829</v>
       </c>
     </row>
     <row r="99">
@@ -12682,8 +14114,20 @@
       <c r="F99" t="n">
         <v>535.38</v>
       </c>
+      <c r="G99" t="n">
+        <v>-46.33450649350561</v>
+      </c>
       <c r="H99" t="n">
         <v>42525.3</v>
+      </c>
+      <c r="I99" t="n">
+        <v>42571.63450649351</v>
+      </c>
+      <c r="J99" t="n">
+        <v>43303.1</v>
+      </c>
+      <c r="K99" t="n">
+        <v>43339.65913230338</v>
       </c>
     </row>
     <row r="100">
@@ -12696,8 +14140,20 @@
       <c r="F100" t="n">
         <v>535.28</v>
       </c>
+      <c r="G100" t="n">
+        <v>-58.50453429396293</v>
+      </c>
       <c r="H100" t="n">
         <v>42309.5</v>
+      </c>
+      <c r="I100" t="n">
+        <v>42368.00453429396</v>
+      </c>
+      <c r="J100" t="n">
+        <v>42525.3</v>
+      </c>
+      <c r="K100" t="n">
+        <v>42571.63518397669</v>
       </c>
     </row>
     <row r="101">
@@ -12710,8 +14166,20 @@
       <c r="F101" t="n">
         <v>535.1799999999999</v>
       </c>
+      <c r="G101" t="n">
+        <v>-73.59586286973354</v>
+      </c>
       <c r="H101" t="n">
         <v>43059.2</v>
+      </c>
+      <c r="I101" t="n">
+        <v>43132.79586286973</v>
+      </c>
+      <c r="J101" t="n">
+        <v>42309.5</v>
+      </c>
+      <c r="K101" t="n">
+        <v>42368.00538972205</v>
       </c>
     </row>
     <row r="102">
@@ -12724,8 +14192,20 @@
       <c r="F102" t="n">
         <v>535.08</v>
       </c>
+      <c r="G102" t="n">
+        <v>-92.23702054644673</v>
+      </c>
       <c r="H102" t="n">
         <v>43043.8</v>
+      </c>
+      <c r="I102" t="n">
+        <v>43136.03702054645</v>
+      </c>
+      <c r="J102" t="n">
+        <v>43059.2</v>
+      </c>
+      <c r="K102" t="n">
+        <v>43132.79693895672</v>
       </c>
     </row>
     <row r="103">
@@ -12738,8 +14218,20 @@
       <c r="F103" t="n">
         <v>534.98</v>
       </c>
+      <c r="G103" t="n">
+        <v>-38.47398019924731</v>
+      </c>
       <c r="H103" t="n">
-        <v>43407.5</v>
+        <v>43330.8</v>
+      </c>
+      <c r="I103" t="n">
+        <v>43445.97398019925</v>
+      </c>
+      <c r="J103" t="n">
+        <v>43043.8</v>
+      </c>
+      <c r="K103" t="n">
+        <v>43136.03836919642</v>
       </c>
     </row>
     <row r="104">
@@ -12752,8 +14244,20 @@
       <c r="F104" t="n">
         <v>534.88</v>
       </c>
+      <c r="G104" t="n">
+        <v>398.6445760386341</v>
+      </c>
       <c r="H104" t="n">
-        <v>43836</v>
+        <v>43294.06732897285</v>
+      </c>
+      <c r="I104" t="n">
+        <v>43437.35542396137</v>
+      </c>
+      <c r="J104" t="n">
+        <v>43330.8</v>
+      </c>
+      <c r="K104" t="n">
+        <v>43445.97566422355</v>
       </c>
     </row>
     <row r="105">
@@ -12766,8 +14270,20 @@
       <c r="F105" t="n">
         <v>534.78</v>
       </c>
+      <c r="G105" t="n">
+        <v>-722.212817634223</v>
+      </c>
       <c r="H105" t="n">
-        <v>42748.9</v>
+        <v>43293.49688392528</v>
+      </c>
+      <c r="I105" t="n">
+        <v>43471.11281763422</v>
+      </c>
+      <c r="J105" t="n">
+        <v>43294.06732897285</v>
+      </c>
+      <c r="K105" t="n">
+        <v>43437.35751905814</v>
       </c>
     </row>
     <row r="106">
@@ -12780,8 +14296,20 @@
       <c r="F106" t="n">
         <v>534.6799999999999</v>
       </c>
+      <c r="G106" t="n">
+        <v>505.4310184660935</v>
+      </c>
       <c r="H106" t="n">
-        <v>44018.3</v>
+        <v>43293.49793826786</v>
+      </c>
+      <c r="I106" t="n">
+        <v>43512.86898153391</v>
+      </c>
+      <c r="J106" t="n">
+        <v>43293.49688392529</v>
+      </c>
+      <c r="K106" t="n">
+        <v>43471.11541465786</v>
       </c>
     </row>
     <row r="107">
@@ -12794,8 +14322,20 @@
       <c r="F107" t="n">
         <v>534.58</v>
       </c>
+      <c r="G107" t="n">
+        <v>-249.5935808420545</v>
+      </c>
       <c r="H107" t="n">
-        <v>43313.7</v>
+        <v>43293.325960628</v>
+      </c>
+      <c r="I107" t="n">
+        <v>43563.29358084205</v>
+      </c>
+      <c r="J107" t="n">
+        <v>43293.49793826787</v>
+      </c>
+      <c r="K107" t="n">
+        <v>43512.87218908274</v>
       </c>
     </row>
     <row r="108">
@@ -12808,8 +14348,20 @@
       <c r="F108" t="n">
         <v>534.48</v>
       </c>
+      <c r="G108" t="n">
+        <v>-177.683550103473</v>
+      </c>
       <c r="H108" t="n">
-        <v>43446</v>
+        <v>43292.63753639476</v>
+      </c>
+      <c r="I108" t="n">
+        <v>43623.68355010347</v>
+      </c>
+      <c r="J108" t="n">
+        <v>43293.32596062805</v>
+      </c>
+      <c r="K108" t="n">
+        <v>43563.2975281922</v>
       </c>
     </row>
     <row r="109">
@@ -12822,8 +14374,20 @@
       <c r="F109" t="n">
         <v>534.38</v>
       </c>
+      <c r="G109" t="n">
+        <v>-84.07349636506115</v>
+      </c>
       <c r="H109" t="n">
-        <v>43612.9</v>
+        <v>43292.47359125551</v>
+      </c>
+      <c r="I109" t="n">
+        <v>43696.97349636506</v>
+      </c>
+      <c r="J109" t="n">
+        <v>43292.63753639491</v>
+      </c>
+      <c r="K109" t="n">
+        <v>43623.68839051547</v>
       </c>
     </row>
     <row r="110">
@@ -12836,8 +14400,20 @@
       <c r="F110" t="n">
         <v>534.28</v>
       </c>
+      <c r="G110" t="n">
+        <v>-337.4379144176564</v>
+      </c>
       <c r="H110" t="n">
-        <v>43447.1</v>
+        <v>43292.03300426409</v>
+      </c>
+      <c r="I110" t="n">
+        <v>43784.53791441765</v>
+      </c>
+      <c r="J110" t="n">
+        <v>43292.473591256</v>
+      </c>
+      <c r="K110" t="n">
+        <v>43696.97941078786</v>
       </c>
     </row>
     <row r="111">
@@ -12850,8 +14426,20 @@
       <c r="F111" t="n">
         <v>534.1799999999999</v>
       </c>
+      <c r="G111" t="n">
+        <v>-487.540788807928</v>
+      </c>
       <c r="H111" t="n">
-        <v>43401.6</v>
+        <v>43291.59256685943</v>
+      </c>
+      <c r="I111" t="n">
+        <v>43889.14078880793</v>
+      </c>
+      <c r="J111" t="n">
+        <v>43292.03300426562</v>
+      </c>
+      <c r="K111" t="n">
+        <v>43784.54511561067</v>
       </c>
     </row>
     <row r="112">
@@ -12864,8 +14452,20 @@
       <c r="F112" t="n">
         <v>534.08</v>
       </c>
+      <c r="G112" t="n">
+        <v>-1262.210552928249</v>
+      </c>
       <c r="H112" t="n">
-        <v>42751.6</v>
+        <v>43291.35180408233</v>
+      </c>
+      <c r="I112" t="n">
+        <v>44013.81055292825</v>
+      </c>
+      <c r="J112" t="n">
+        <v>43291.59256686414</v>
+      </c>
+      <c r="K112" t="n">
+        <v>43889.14952589579</v>
       </c>
     </row>
     <row r="113">
@@ -12878,8 +14478,20 @@
       <c r="F113" t="n">
         <v>533.98</v>
       </c>
+      <c r="G113" t="n">
+        <v>-44.18250092591916</v>
+      </c>
       <c r="H113" t="n">
-        <v>44118</v>
+        <v>43291.74551112639</v>
+      </c>
+      <c r="I113" t="n">
+        <v>44162.18250092592</v>
+      </c>
+      <c r="J113" t="n">
+        <v>43291.3518040966</v>
+      </c>
+      <c r="K113" t="n">
+        <v>44013.82111639445</v>
       </c>
     </row>
     <row r="114">
@@ -12892,8 +14504,20 @@
       <c r="F114" t="n">
         <v>533.88</v>
       </c>
+      <c r="G114" t="n">
+        <v>-655.8551003863686</v>
+      </c>
       <c r="H114" t="n">
-        <v>43680.7</v>
+        <v>43291.47148335023</v>
+      </c>
+      <c r="I114" t="n">
+        <v>44336.55510038637</v>
+      </c>
+      <c r="J114" t="n">
+        <v>43291.74551116869</v>
+      </c>
+      <c r="K114" t="n">
+        <v>44162.19522803816</v>
       </c>
     </row>
     <row r="115">
@@ -12906,8 +14530,20 @@
       <c r="F115" t="n">
         <v>533.78</v>
       </c>
+      <c r="G115" t="n">
+        <v>335.1399882455298</v>
+      </c>
       <c r="H115" t="n">
-        <v>44875.9</v>
+        <v>43290.33462811027</v>
+      </c>
+      <c r="I115" t="n">
+        <v>44540.76001175447</v>
+      </c>
+      <c r="J115" t="n">
+        <v>43291.47148347305</v>
+      </c>
+      <c r="K115" t="n">
+        <v>44336.57038102579</v>
       </c>
     </row>
     <row r="116">
@@ -12920,8 +14556,20 @@
       <c r="F116" t="n">
         <v>533.6799999999999</v>
       </c>
+      <c r="G116" t="n">
+        <v>-742.9310566507629</v>
+      </c>
       <c r="H116" t="n">
-        <v>44036.5</v>
+        <v>43288.49453763908</v>
+      </c>
+      <c r="I116" t="n">
+        <v>44779.43105665076</v>
+      </c>
+      <c r="J116" t="n">
+        <v>43290.33462845969</v>
+      </c>
+      <c r="K116" t="n">
+        <v>44540.77829458612</v>
       </c>
     </row>
     <row r="117">
@@ -12934,8 +14582,20 @@
       <c r="F117" t="n">
         <v>533.58</v>
       </c>
+      <c r="G117" t="n">
+        <v>-295.6779306165627</v>
+      </c>
       <c r="H117" t="n">
-        <v>44762.2</v>
+        <v>43286.32474112064</v>
+      </c>
+      <c r="I117" t="n">
+        <v>45057.87793061656</v>
+      </c>
+      <c r="J117" t="n">
+        <v>43288.49453861304</v>
+      </c>
+      <c r="K117" t="n">
+        <v>44779.45285550803</v>
       </c>
     </row>
     <row r="118">
@@ -12948,8 +14608,20 @@
       <c r="F118" t="n">
         <v>533.48</v>
       </c>
+      <c r="G118" t="n">
+        <v>-984.030313155461</v>
+      </c>
       <c r="H118" t="n">
-        <v>44397.9</v>
+        <v>43284.25246188632</v>
+      </c>
+      <c r="I118" t="n">
+        <v>45381.93031315546</v>
+      </c>
+      <c r="J118" t="n">
+        <v>43286.32474378056</v>
+      </c>
+      <c r="K118" t="n">
+        <v>45057.90383084385</v>
       </c>
     </row>
     <row r="119">
@@ -12962,8 +14634,20 @@
       <c r="F119" t="n">
         <v>533.38</v>
       </c>
+      <c r="G119" t="n">
+        <v>-703.1097601269139</v>
+      </c>
       <c r="H119" t="n">
-        <v>45053.9</v>
+        <v>43281.84039183114</v>
+      </c>
+      <c r="I119" t="n">
+        <v>45757.00976012692</v>
+      </c>
+      <c r="J119" t="n">
+        <v>43284.25246900412</v>
+      </c>
+      <c r="K119" t="n">
+        <v>45381.96097737906</v>
       </c>
     </row>
     <row r="120">
@@ -12976,8 +14660,20 @@
       <c r="F120" t="n">
         <v>533.28</v>
       </c>
+      <c r="G120" t="n">
+        <v>660.2572849672506</v>
+      </c>
       <c r="H120" t="n">
-        <v>46849.7</v>
+        <v>43279.12914457225</v>
+      </c>
+      <c r="I120" t="n">
+        <v>46189.44271503275</v>
+      </c>
+      <c r="J120" t="n">
+        <v>43281.84041049443</v>
+      </c>
+      <c r="K120" t="n">
+        <v>45757.0459323231</v>
       </c>
     </row>
     <row r="121">
@@ -12990,8 +14686,20 @@
       <c r="F121" t="n">
         <v>533.1799999999999</v>
       </c>
+      <c r="G121" t="n">
+        <v>-647.811753878028</v>
+      </c>
       <c r="H121" t="n">
-        <v>46036.1</v>
+        <v>43274.14430490348</v>
+      </c>
+      <c r="I121" t="n">
+        <v>46683.91175387803</v>
+      </c>
+      <c r="J121" t="n">
+        <v>43279.12919252505</v>
+      </c>
+      <c r="K121" t="n">
+        <v>46189.48522042989</v>
       </c>
     </row>
     <row r="122">
@@ -13004,8 +14712,20 @@
       <c r="F122" t="n">
         <v>533.08</v>
       </c>
+      <c r="G122" t="n">
+        <v>625.2965946765544</v>
+      </c>
       <c r="H122" t="n">
-        <v>47874</v>
+        <v>43268.23499660165</v>
+      </c>
+      <c r="I122" t="n">
+        <v>47248.70340532345</v>
+      </c>
+      <c r="J122" t="n">
+        <v>43274.14442564066</v>
+      </c>
+      <c r="K122" t="n">
+        <v>46683.96148928889</v>
       </c>
     </row>
     <row r="123">
@@ -13018,8 +14738,20 @@
       <c r="F123" t="n">
         <v>532.98</v>
       </c>
+      <c r="G123" t="n">
+        <v>45.75588939979207</v>
+      </c>
       <c r="H123" t="n">
-        <v>47936.6</v>
+        <v>43261.34617323051</v>
+      </c>
+      <c r="I123" t="n">
+        <v>47890.84411060021</v>
+      </c>
+      <c r="J123" t="n">
+        <v>43268.23529451419</v>
+      </c>
+      <c r="K123" t="n">
+        <v>47248.76130809931</v>
       </c>
     </row>
     <row r="124">
@@ -13032,8 +14764,20 @@
       <c r="F124" t="n">
         <v>532.88</v>
       </c>
+      <c r="G124" t="n">
+        <v>936.2409400235192</v>
+      </c>
       <c r="H124" t="n">
-        <v>49552.8</v>
+        <v>43252.67226340636</v>
+      </c>
+      <c r="I124" t="n">
+        <v>48616.55905997648</v>
+      </c>
+      <c r="J124" t="n">
+        <v>43261.34689363721</v>
+      </c>
+      <c r="K124" t="n">
+        <v>47890.91108070457</v>
       </c>
     </row>
     <row r="125">
@@ -13046,8 +14790,20 @@
       <c r="F125" t="n">
         <v>532.78</v>
       </c>
+      <c r="G125" t="n">
+        <v>-783.5770068041311</v>
+      </c>
       <c r="H125" t="n">
-        <v>48649.2</v>
+        <v>43242.43040540381</v>
+      </c>
+      <c r="I125" t="n">
+        <v>49432.77700680413</v>
+      </c>
+      <c r="J125" t="n">
+        <v>43252.67397078457</v>
+      </c>
+      <c r="K125" t="n">
+        <v>48616.63578100939</v>
       </c>
     </row>
     <row r="126">
@@ -13060,8 +14816,20 @@
       <c r="F126" t="n">
         <v>532.6799999999999</v>
       </c>
+      <c r="G126" t="n">
+        <v>-542.2238467543648</v>
+      </c>
       <c r="H126" t="n">
-        <v>49804.2</v>
+        <v>43231.51300959419</v>
+      </c>
+      <c r="I126" t="n">
+        <v>50346.42384675436</v>
+      </c>
+      <c r="J126" t="n">
+        <v>43242.43437154361</v>
+      </c>
+      <c r="K126" t="n">
+        <v>49432.86355317487</v>
       </c>
     </row>
     <row r="127">
@@ -13074,8 +14842,20 @@
       <c r="F127" t="n">
         <v>532.58</v>
       </c>
+      <c r="G127" t="n">
+        <v>352.1571042266369</v>
+      </c>
       <c r="H127" t="n">
-        <v>51714.9</v>
+        <v>43220.27522436452</v>
+      </c>
+      <c r="I127" t="n">
+        <v>51362.74289577336</v>
+      </c>
+      <c r="J127" t="n">
+        <v>43231.52204020934</v>
+      </c>
+      <c r="K127" t="n">
+        <v>50346.51884714061</v>
       </c>
     </row>
     <row r="128">
@@ -13088,8 +14868,20 @@
       <c r="F128" t="n">
         <v>532.48</v>
       </c>
+      <c r="G128" t="n">
+        <v>450.0923418693128</v>
+      </c>
       <c r="H128" t="n">
-        <v>52932.4</v>
+        <v>43206.13918608351</v>
+      </c>
+      <c r="I128" t="n">
+        <v>52482.30765813069</v>
+      </c>
+      <c r="J128" t="n">
+        <v>43220.29538035132</v>
+      </c>
+      <c r="K128" t="n">
+        <v>51362.84179508579</v>
       </c>
     </row>
     <row r="129">
@@ -13102,8 +14894,20 @@
       <c r="F129" t="n">
         <v>532.38</v>
       </c>
+      <c r="G129" t="n">
+        <v>-151.7786272437443</v>
+      </c>
       <c r="H129" t="n">
-        <v>53554</v>
+        <v>43189.07724306933</v>
+      </c>
+      <c r="I129" t="n">
+        <v>53705.77862724374</v>
+      </c>
+      <c r="J129" t="n">
+        <v>43206.18328788616</v>
+      </c>
+      <c r="K129" t="n">
+        <v>52482.39918769127</v>
       </c>
     </row>
     <row r="130">
@@ -13116,8 +14920,20 @@
       <c r="F130" t="n">
         <v>532.28</v>
       </c>
+      <c r="G130" t="n">
+        <v>-154.1820615186298</v>
+      </c>
       <c r="H130" t="n">
-        <v>54877.5</v>
+        <v>43170.25119379305</v>
+      </c>
+      <c r="I130" t="n">
+        <v>55031.68206151863</v>
+      </c>
+      <c r="J130" t="n">
+        <v>43189.17184591125</v>
+      </c>
+      <c r="K130" t="n">
+        <v>53705.8377934158</v>
       </c>
     </row>
     <row r="131">
@@ -13130,8 +14946,20 @@
       <c r="F131" t="n">
         <v>532.1799999999999</v>
       </c>
+      <c r="G131" t="n">
+        <v>-60.1486120841364</v>
+      </c>
       <c r="H131" t="n">
-        <v>56392.8</v>
+        <v>43149.52419270402</v>
+      </c>
+      <c r="I131" t="n">
+        <v>56452.94861208414</v>
+      </c>
+      <c r="J131" t="n">
+        <v>43170.45016014502</v>
+      </c>
+      <c r="K131" t="n">
+        <v>55031.65652440283</v>
       </c>
     </row>
     <row r="132">
@@ -13144,8 +14972,20 @@
       <c r="F132" t="n">
         <v>532.08</v>
       </c>
+      <c r="G132" t="n">
+        <v>580.8357964872921</v>
+      </c>
       <c r="H132" t="n">
-        <v>58537.3</v>
+        <v>43126.04476639436</v>
+      </c>
+      <c r="I132" t="n">
+        <v>57956.46420351271</v>
+      </c>
+      <c r="J132" t="n">
+        <v>43149.934507263</v>
+      </c>
+      <c r="K132" t="n">
+        <v>56452.732807258</v>
       </c>
     </row>
     <row r="133">
@@ -13158,8 +14998,20 @@
       <c r="F133" t="n">
         <v>531.98</v>
       </c>
+      <c r="G133" t="n">
+        <v>11.78575910785003</v>
+      </c>
       <c r="H133" t="n">
-        <v>59534.7</v>
+        <v>43099.08631671629</v>
+      </c>
+      <c r="I133" t="n">
+        <v>59522.91424089215</v>
+      </c>
+      <c r="J133" t="n">
+        <v>43126.87452660096</v>
+      </c>
+      <c r="K133" t="n">
+        <v>57955.85127273592</v>
       </c>
     </row>
     <row r="134">
@@ -13172,8 +15024,20 @@
       <c r="F134" t="n">
         <v>531.88</v>
       </c>
+      <c r="G134" t="n">
+        <v>1701.028678326082</v>
+      </c>
       <c r="H134" t="n">
-        <v>62828</v>
+        <v>43069.03805924368</v>
+      </c>
+      <c r="I134" t="n">
+        <v>61126.97132167392</v>
+      </c>
+      <c r="J134" t="n">
+        <v>43100.7319220971</v>
+      </c>
+      <c r="K134" t="n">
+        <v>59521.50874874588</v>
       </c>
     </row>
     <row r="135">
@@ -13186,8 +15050,20 @@
       <c r="F135" t="n">
         <v>531.78</v>
       </c>
+      <c r="G135" t="n">
+        <v>-463.4493773585127</v>
+      </c>
       <c r="H135" t="n">
-        <v>62271</v>
+        <v>43034.95415063726</v>
+      </c>
+      <c r="I135" t="n">
+        <v>62734.44937735851</v>
+      </c>
+      <c r="J135" t="n">
+        <v>43072.23900180178</v>
+      </c>
+      <c r="K135" t="n">
+        <v>61124.03435822032</v>
       </c>
     </row>
     <row r="136">
@@ -13200,8 +15076,20 @@
       <c r="F136" t="n">
         <v>531.6799999999999</v>
       </c>
+      <c r="G136" t="n">
+        <v>305.2976208130494</v>
+      </c>
       <c r="H136" t="n">
-        <v>64611.6</v>
+        <v>42998.26952378461</v>
+      </c>
+      <c r="I136" t="n">
+        <v>64306.30237918695</v>
+      </c>
+      <c r="J136" t="n">
+        <v>43041.06151164749</v>
+      </c>
+      <c r="K136" t="n">
+        <v>62728.62994662328</v>
       </c>
     </row>
     <row r="137">
@@ -13214,8 +15102,20 @@
       <c r="F137" t="n">
         <v>531.58</v>
       </c>
+      <c r="G137" t="n">
+        <v>-426.2910365206917</v>
+      </c>
       <c r="H137" t="n">
-        <v>65370.5</v>
+        <v>42959.71345278985</v>
+      </c>
+      <c r="I137" t="n">
+        <v>65796.79103652069</v>
+      </c>
+      <c r="J137" t="n">
+        <v>43009.70094362812</v>
+      </c>
+      <c r="K137" t="n">
+        <v>64295.18231546394</v>
       </c>
     </row>
     <row r="138">
@@ -13228,8 +15128,20 @@
       <c r="F138" t="n">
         <v>531.48</v>
       </c>
+      <c r="G138" t="n">
+        <v>-899.204707928453</v>
+      </c>
       <c r="H138" t="n">
-        <v>66255.7</v>
+        <v>42918.25065026537</v>
+      </c>
+      <c r="I138" t="n">
+        <v>67154.90470792845</v>
+      </c>
+      <c r="J138" t="n">
+        <v>42980.70613638378</v>
+      </c>
+      <c r="K138" t="n">
+        <v>65776.13189817012</v>
       </c>
     </row>
     <row r="139">
@@ -13242,8 +15154,20 @@
       <c r="F139" t="n">
         <v>531.38</v>
       </c>
+      <c r="G139" t="n">
+        <v>-528.6930517849687</v>
+      </c>
       <c r="H139" t="n">
-        <v>67803.5</v>
+        <v>42875.06241856637</v>
+      </c>
+      <c r="I139" t="n">
+        <v>68332.19305178497</v>
+      </c>
+      <c r="J139" t="n">
+        <v>42956.07838166285</v>
+      </c>
+      <c r="K139" t="n">
+        <v>67117.43069012955</v>
       </c>
     </row>
     <row r="140">
@@ -13256,8 +15180,20 @@
       <c r="F140" t="n">
         <v>531.28</v>
       </c>
+      <c r="G140" t="n">
+        <v>-727.6587362324062</v>
+      </c>
       <c r="H140" t="n">
-        <v>68556.2</v>
+        <v>42829.4759307543</v>
+      </c>
+      <c r="I140" t="n">
+        <v>69283.8587362324</v>
+      </c>
+      <c r="J140" t="n">
+        <v>42941.95585463916</v>
+      </c>
+      <c r="K140" t="n">
+        <v>68265.6706641557</v>
       </c>
     </row>
     <row r="141">
@@ -13270,8 +15206,20 @@
       <c r="F141" t="n">
         <v>531.1799999999999</v>
       </c>
+      <c r="G141" t="n">
+        <v>104.0380866603227</v>
+      </c>
       <c r="H141" t="n">
-        <v>70081.60000000001</v>
+        <v>42781.59914207643</v>
+      </c>
+      <c r="I141" t="n">
+        <v>69977.56191333968</v>
+      </c>
+      <c r="J141" t="n">
+        <v>42945.57979977006</v>
+      </c>
+      <c r="K141" t="n">
+        <v>69168.13963284229</v>
       </c>
     </row>
     <row r="142">
@@ -13284,8 +15232,20 @@
       <c r="F142" t="n">
         <v>531.08</v>
       </c>
+      <c r="G142" t="n">
+        <v>-92.44775579599082</v>
+      </c>
       <c r="H142" t="n">
-        <v>70306.8</v>
+        <v>42731.50971163717</v>
+      </c>
+      <c r="I142" t="n">
+        <v>70399.24775579599</v>
+      </c>
+      <c r="J142" t="n">
+        <v>42979.41512822659</v>
+      </c>
+      <c r="K142" t="n">
+        <v>69780.14010088993</v>
       </c>
     </row>
     <row r="143">
@@ -13298,8 +15258,20 @@
       <c r="F143" t="n">
         <v>530.98</v>
       </c>
+      <c r="G143" t="n">
+        <v>-310.9014919025358</v>
+      </c>
       <c r="H143" t="n">
-        <v>70249.3</v>
+        <v>42679.85878671519</v>
+      </c>
+      <c r="I143" t="n">
+        <v>70560.20149190254</v>
+      </c>
+      <c r="J143" t="n">
+        <v>43062.40522567827</v>
+      </c>
+      <c r="K143" t="n">
+        <v>70068.75097647298</v>
       </c>
     </row>
     <row r="144">
@@ -13312,8 +15284,20 @@
       <c r="F144" t="n">
         <v>530.88</v>
       </c>
+      <c r="G144" t="n">
+        <v>760.7232095465151</v>
+      </c>
       <c r="H144" t="n">
-        <v>71263.39999999999</v>
+        <v>42627.83121676077</v>
+      </c>
+      <c r="I144" t="n">
+        <v>70502.67679045348</v>
+      </c>
+      <c r="J144" t="n">
+        <v>43223.35833675109</v>
+      </c>
+      <c r="K144" t="n">
+        <v>70017.10005155118</v>
       </c>
     </row>
     <row r="145">
@@ -13326,8 +15310,20 @@
       <c r="F145" t="n">
         <v>530.78</v>
       </c>
+      <c r="G145" t="n">
+        <v>1172.280822050714</v>
+      </c>
       <c r="H145" t="n">
-        <v>71474.3</v>
+        <v>42574.73951991515</v>
+      </c>
+      <c r="I145" t="n">
+        <v>70302.01917794929</v>
+      </c>
+      <c r="J145" t="n">
+        <v>43504.52800950218</v>
+      </c>
+      <c r="K145" t="n">
+        <v>69626.37217557426</v>
       </c>
     </row>
     <row r="146">
@@ -13340,8 +15336,20 @@
       <c r="F146" t="n">
         <v>530.6799999999999</v>
       </c>
+      <c r="G146" t="n">
+        <v>-47.49067021388328</v>
+      </c>
       <c r="H146" t="n">
-        <v>70025.3</v>
+        <v>42520.78687618918</v>
+      </c>
+      <c r="I146" t="n">
+        <v>70072.79067021389</v>
+      </c>
+      <c r="J146" t="n">
+        <v>43963.73649931502</v>
+      </c>
+      <c r="K146" t="n">
+        <v>68913.40322200314</v>
       </c>
     </row>
     <row r="147">
@@ -13354,8 +15362,20 @@
       <c r="F147" t="n">
         <v>530.58</v>
       </c>
+      <c r="G147" t="n">
+        <v>581.3152186731022</v>
+      </c>
       <c r="H147" t="n">
-        <v>70553.3</v>
+        <v>42467.86619873066</v>
+      </c>
+      <c r="I147" t="n">
+        <v>69971.9847813269</v>
+      </c>
+      <c r="J147" t="n">
+        <v>44682.54731437931</v>
+      </c>
+      <c r="K147" t="n">
+        <v>67911.39512177851</v>
       </c>
     </row>
     <row r="148">
@@ -13368,8 +15388,20 @@
       <c r="F148" t="n">
         <v>530.48</v>
       </c>
+      <c r="G148" t="n">
+        <v>170.6513273677556</v>
+      </c>
       <c r="H148" t="n">
-        <v>70367.3</v>
+        <v>42415.48581107709</v>
+      </c>
+      <c r="I148" t="n">
+        <v>70196.64867263225</v>
+      </c>
+      <c r="J148" t="n">
+        <v>45773.14884908586</v>
+      </c>
+      <c r="K148" t="n">
+        <v>66667.0462385963</v>
       </c>
     </row>
     <row r="149">
@@ -13382,8 +15414,20 @@
       <c r="F149" t="n">
         <v>530.38</v>
       </c>
+      <c r="G149" t="n">
+        <v>340.2642933787574</v>
+      </c>
       <c r="H149" t="n">
-        <v>71326.8</v>
+        <v>42362.58649456379</v>
+      </c>
+      <c r="I149" t="n">
+        <v>70986.53570662125</v>
+      </c>
+      <c r="J149" t="n">
+        <v>47380.54923744542</v>
+      </c>
+      <c r="K149" t="n">
+        <v>65231.90425645902</v>
       </c>
     </row>
     <row r="150">
@@ -13396,8 +15440,20 @@
       <c r="F150" t="n">
         <v>530.28</v>
       </c>
+      <c r="G150" t="n">
+        <v>657.7240441602044</v>
+      </c>
       <c r="H150" t="n">
-        <v>73281.7</v>
+        <v>42308.37794914078</v>
+      </c>
+      <c r="I150" t="n">
+        <v>72623.97595583979</v>
+      </c>
+      <c r="J150" t="n">
+        <v>49689.91276310062</v>
+      </c>
+      <c r="K150" t="n">
+        <v>63659.49928624312</v>
       </c>
     </row>
     <row r="151">
@@ -13410,8 +15466,20 @@
       <c r="F151" t="n">
         <v>530.1799999999999</v>
       </c>
+      <c r="G151" t="n">
+        <v>-1323.265186365345</v>
+      </c>
       <c r="H151" t="n">
-        <v>74104.60000000001</v>
+        <v>42251.28358778087</v>
+      </c>
+      <c r="I151" t="n">
+        <v>75427.86518636535</v>
+      </c>
+      <c r="J151" t="n">
+        <v>52930.55687999436</v>
+      </c>
+      <c r="K151" t="n">
+        <v>62002.0537451268</v>
       </c>
     </row>
     <row r="152">
@@ -13424,8 +15492,20 @@
       <c r="F152" t="n">
         <v>530.08</v>
       </c>
+      <c r="G152" t="n">
+        <v>-299.0697770389233</v>
+      </c>
       <c r="H152" t="n">
-        <v>79443.39999999999</v>
+        <v>42190.57827608667</v>
+      </c>
+      <c r="I152" t="n">
+        <v>79742.46977703892</v>
+      </c>
+      <c r="J152" t="n">
+        <v>57373.0884193871</v>
+      </c>
+      <c r="K152" t="n">
+        <v>60306.2798867575</v>
       </c>
     </row>
     <row r="153">
@@ -13438,8 +15518,20 @@
       <c r="F153" t="n">
         <v>529.98</v>
       </c>
+      <c r="G153" t="n">
+        <v>-489.7117843189044</v>
+      </c>
       <c r="H153" t="n">
-        <v>85417.10000000001</v>
+        <v>42122.45765303395</v>
+      </c>
+      <c r="I153" t="n">
+        <v>85906.81178431891</v>
+      </c>
+      <c r="J153" t="n">
+        <v>63320.22534413877</v>
+      </c>
+      <c r="K153" t="n">
+        <v>58613.00070811811</v>
       </c>
     </row>
     <row r="154">
@@ -13452,8 +15544,20 @@
       <c r="F154" t="n">
         <v>529.88</v>
       </c>
+      <c r="G154" t="n">
+        <v>506.6240197120205</v>
+      </c>
       <c r="H154" t="n">
-        <v>94714.7</v>
+        <v>42042.06887759222</v>
+      </c>
+      <c r="I154" t="n">
+        <v>94208.07598028798</v>
+      </c>
+      <c r="J154" t="n">
+        <v>71077.13698613137</v>
+      </c>
+      <c r="K154" t="n">
+        <v>56952.2641593773</v>
       </c>
     </row>
     <row r="155">
@@ -13466,8 +15570,20 @@
       <c r="F155" t="n">
         <v>529.78</v>
       </c>
+      <c r="G155" t="n">
+        <v>1321.611119801208</v>
+      </c>
       <c r="H155" t="n">
-        <v>106125</v>
+        <v>41944.85464307328</v>
+      </c>
+      <c r="I155" t="n">
+        <v>104803.3888801988</v>
+      </c>
+      <c r="J155" t="n">
+        <v>80904.94762389499</v>
+      </c>
+      <c r="K155" t="n">
+        <v>55345.2774921462</v>
       </c>
     </row>
     <row r="156">
@@ -13480,8 +15596,20 @@
       <c r="F156" t="n">
         <v>529.6799999999999</v>
       </c>
+      <c r="G156" t="n">
+        <v>983.1865188161319</v>
+      </c>
       <c r="H156" t="n">
-        <v>118586</v>
+        <v>41825.73955765846</v>
+      </c>
+      <c r="I156" t="n">
+        <v>117602.8134811839</v>
+      </c>
+      <c r="J156" t="n">
+        <v>92942.00705314302</v>
+      </c>
+      <c r="K156" t="n">
+        <v>53806.25997368306</v>
       </c>
     </row>
     <row r="157">
@@ -13494,8 +15622,20 @@
       <c r="F157" t="n">
         <v>529.58</v>
       </c>
+      <c r="G157" t="n">
+        <v>-93.30769620556384</v>
+      </c>
       <c r="H157" t="n">
-        <v>132033</v>
+        <v>41681.4472693803</v>
+      </c>
+      <c r="I157" t="n">
+        <v>132126.3076962056</v>
+      </c>
+      <c r="J157" t="n">
+        <v>107086.0148417805</v>
+      </c>
+      <c r="K157" t="n">
+        <v>52342.50010800493</v>
       </c>
     </row>
     <row r="158">
@@ -13508,8 +15648,20 @@
       <c r="F158" t="n">
         <v>529.48</v>
       </c>
+      <c r="G158" t="n">
+        <v>2824.526875278505</v>
+      </c>
       <c r="H158" t="n">
-        <v>150188</v>
+        <v>41507.87936058627</v>
+      </c>
+      <c r="I158" t="n">
+        <v>147363.4731247215</v>
+      </c>
+      <c r="J158" t="n">
+        <v>122849.9446992396</v>
+      </c>
+      <c r="K158" t="n">
+        <v>50957.70727098941</v>
       </c>
     </row>
     <row r="159">
@@ -13522,8 +15674,20 @@
       <c r="F159" t="n">
         <v>529.38</v>
       </c>
+      <c r="G159" t="n">
+        <v>582.0686282922106</v>
+      </c>
       <c r="H159" t="n">
-        <v>162308</v>
+        <v>41301.2644857261</v>
+      </c>
+      <c r="I159" t="n">
+        <v>161725.9313717078</v>
+      </c>
+      <c r="J159" t="n">
+        <v>139220.738343824</v>
+      </c>
+      <c r="K159" t="n">
+        <v>49650.44593130877</v>
       </c>
     </row>
     <row r="160">
@@ -13536,8 +15700,20 @@
       <c r="F160" t="n">
         <v>529.28</v>
       </c>
+      <c r="G160" t="n">
+        <v>-935.0569480507402</v>
+      </c>
       <c r="H160" t="n">
-        <v>172273</v>
+        <v>41065.77627983599</v>
+      </c>
+      <c r="I160" t="n">
+        <v>173208.0569480507</v>
+      </c>
+      <c r="J160" t="n">
+        <v>154610.6964473708</v>
+      </c>
+      <c r="K160" t="n">
+        <v>48416.27032327253</v>
       </c>
     </row>
     <row r="161">
@@ -13550,8 +15726,20 @@
       <c r="F161" t="n">
         <v>529.1799999999999</v>
       </c>
+      <c r="G161" t="n">
+        <v>-3608.703566777025</v>
+      </c>
       <c r="H161" t="n">
-        <v>176202</v>
+        <v>40810.26237048138</v>
+      </c>
+      <c r="I161" t="n">
+        <v>179810.703566777</v>
+      </c>
+      <c r="J161" t="n">
+        <v>167017.3440284331</v>
+      </c>
+      <c r="K161" t="n">
+        <v>47256.20942760705</v>
       </c>
     </row>
     <row r="162">
@@ -13564,8 +15752,20 @@
       <c r="F162" t="n">
         <v>529.08</v>
       </c>
+      <c r="G162" t="n">
+        <v>464.9060077118338</v>
+      </c>
       <c r="H162" t="n">
-        <v>180614</v>
+        <v>40542.32259549104</v>
+      </c>
+      <c r="I162" t="n">
+        <v>180149.0939922882</v>
+      </c>
+      <c r="J162" t="n">
+        <v>174446.4256013185</v>
+      </c>
+      <c r="K162" t="n">
+        <v>46174.22588808442</v>
       </c>
     </row>
     <row r="163">
@@ -13578,8 +15778,20 @@
       <c r="F163" t="n">
         <v>528.98</v>
       </c>
+      <c r="G163" t="n">
+        <v>-388.4209578569862</v>
+      </c>
       <c r="H163" t="n">
-        <v>173583</v>
+        <v>40271.99121800061</v>
+      </c>
+      <c r="I163" t="n">
+        <v>173971.420957857</v>
+      </c>
+      <c r="J163" t="n">
+        <v>175519.1999574963</v>
+      </c>
+      <c r="K163" t="n">
+        <v>45171.88750296588</v>
       </c>
     </row>
     <row r="164">
@@ -13592,8 +15804,20 @@
       <c r="F164" t="n">
         <v>528.88</v>
       </c>
+      <c r="G164" t="n">
+        <v>428.4296197151125</v>
+      </c>
       <c r="H164" t="n">
-        <v>162693</v>
+        <v>40015.18489644155</v>
+      </c>
+      <c r="I164" t="n">
+        <v>162264.5703802849</v>
+      </c>
+      <c r="J164" t="n">
+        <v>169990.5714880583</v>
+      </c>
+      <c r="K164" t="n">
+        <v>44252.51752949896</v>
       </c>
     </row>
     <row r="165">
@@ -13606,8 +15830,20 @@
       <c r="F165" t="n">
         <v>528.78</v>
       </c>
+      <c r="G165" t="n">
+        <v>514.1325739577296</v>
+      </c>
       <c r="H165" t="n">
-        <v>147380</v>
+        <v>39783.83812275406</v>
+      </c>
+      <c r="I165" t="n">
+        <v>146865.8674260423</v>
+      </c>
+      <c r="J165" t="n">
+        <v>158854.4536770904</v>
+      </c>
+      <c r="K165" t="n">
+        <v>43425.00208082695</v>
       </c>
     </row>
     <row r="166">
@@ -13620,8 +15856,20 @@
       <c r="F166" t="n">
         <v>528.6799999999999</v>
       </c>
+      <c r="G166" t="n">
+        <v>247.0854712457949</v>
+      </c>
       <c r="H166" t="n">
-        <v>130094</v>
+        <v>39585.32622655711</v>
+      </c>
+      <c r="I166" t="n">
+        <v>129846.9145287542</v>
+      </c>
+      <c r="J166" t="n">
+        <v>143955.2476505415</v>
+      </c>
+      <c r="K166" t="n">
+        <v>42694.19419861171</v>
       </c>
     </row>
     <row r="167">
@@ -13634,8 +15882,20 @@
       <c r="F167" t="n">
         <v>528.58</v>
       </c>
+      <c r="G167" t="n">
+        <v>-731.3298599744012</v>
+      </c>
       <c r="H167" t="n">
-        <v>112259</v>
+        <v>39422.74478469363</v>
+      </c>
+      <c r="I167" t="n">
+        <v>112990.3298599744</v>
+      </c>
+      <c r="J167" t="n">
+        <v>127371.4870970372</v>
+      </c>
+      <c r="K167" t="n">
+        <v>42060.53176704907</v>
       </c>
     </row>
     <row r="168">
@@ -13648,8 +15908,20 @@
       <c r="F168" t="n">
         <v>528.48</v>
       </c>
+      <c r="G168" t="n">
+        <v>-2485.424383687801</v>
+      </c>
       <c r="H168" t="n">
-        <v>95045.8</v>
+        <v>39295.79536240159</v>
+      </c>
+      <c r="I168" t="n">
+        <v>97531.2243836878</v>
+      </c>
+      <c r="J168" t="n">
+        <v>110892.4419024263</v>
+      </c>
+      <c r="K168" t="n">
+        <v>41520.45330018675</v>
       </c>
     </row>
     <row r="169">
@@ -13662,8 +15934,20 @@
       <c r="F169" t="n">
         <v>528.38</v>
       </c>
+      <c r="G169" t="n">
+        <v>-437.7466859197448</v>
+      </c>
       <c r="H169" t="n">
-        <v>83699.39999999999</v>
+        <v>39198.03925939836</v>
+      </c>
+      <c r="I169" t="n">
+        <v>84137.14668591974</v>
+      </c>
+      <c r="J169" t="n">
+        <v>95759.50519948021</v>
+      </c>
+      <c r="K169" t="n">
+        <v>41067.37445212515</v>
       </c>
     </row>
     <row r="170">
@@ -13676,8 +15960,20 @@
       <c r="F170" t="n">
         <v>528.28</v>
       </c>
+      <c r="G170" t="n">
+        <v>-218.8709065775329</v>
+      </c>
       <c r="H170" t="n">
-        <v>72810.39999999999</v>
+        <v>39122.61355536734</v>
+      </c>
+      <c r="I170" t="n">
+        <v>73029.27090657753</v>
+      </c>
+      <c r="J170" t="n">
+        <v>82646.08243520248</v>
+      </c>
+      <c r="K170" t="n">
+        <v>40688.99757726731</v>
       </c>
     </row>
     <row r="171">
@@ -13690,8 +15986,20 @@
       <c r="F171" t="n">
         <v>528.1799999999999</v>
       </c>
+      <c r="G171" t="n">
+        <v>-1868.759501488552</v>
+      </c>
       <c r="H171" t="n">
-        <v>62269.4</v>
+        <v>39067.9609243497</v>
+      </c>
+      <c r="I171" t="n">
+        <v>64138.15950148855</v>
+      </c>
+      <c r="J171" t="n">
+        <v>71778.74951767594</v>
+      </c>
+      <c r="K171" t="n">
+        <v>40373.05722184319</v>
       </c>
     </row>
     <row r="172">
@@ -13704,8 +16012,20 @@
       <c r="F172" t="n">
         <v>528.08</v>
       </c>
+      <c r="G172" t="n">
+        <v>-615.9254184947713</v>
+      </c>
       <c r="H172" t="n">
-        <v>56610</v>
+        <v>39029.05588560287</v>
+      </c>
+      <c r="I172" t="n">
+        <v>57225.92541849477</v>
+      </c>
+      <c r="J172" t="n">
+        <v>63093.0052534705</v>
+      </c>
+      <c r="K172" t="n">
+        <v>40113.05982202526</v>
       </c>
     </row>
     <row r="173">
@@ -13718,8 +16038,20 @@
       <c r="F173" t="n">
         <v>527.98</v>
       </c>
+      <c r="G173" t="n">
+        <v>1117.228179012563</v>
+      </c>
       <c r="H173" t="n">
-        <v>53099.8</v>
+        <v>38999.10432175895</v>
+      </c>
+      <c r="I173" t="n">
+        <v>51982.57182098744</v>
+      </c>
+      <c r="J173" t="n">
+        <v>56355.43749099684</v>
+      </c>
+      <c r="K173" t="n">
+        <v>39899.50560251482</v>
       </c>
     </row>
     <row r="174">
@@ -13732,8 +16064,20 @@
       <c r="F174" t="n">
         <v>527.88</v>
       </c>
+      <c r="G174" t="n">
+        <v>-151.0931842019199</v>
+      </c>
       <c r="H174" t="n">
-        <v>47942.8</v>
+        <v>38977.32619449216</v>
+      </c>
+      <c r="I174" t="n">
+        <v>48093.89318420192</v>
+      </c>
+      <c r="J174" t="n">
+        <v>51260.0770261848</v>
+      </c>
+      <c r="K174" t="n">
+        <v>39721.57363407123</v>
       </c>
     </row>
     <row r="175">
@@ -13746,8 +16090,20 @@
       <c r="F175" t="n">
         <v>527.78</v>
       </c>
+      <c r="G175" t="n">
+        <v>1496.956628553562</v>
+      </c>
       <c r="H175" t="n">
-        <v>46764.8</v>
+        <v>38961.54252504184</v>
+      </c>
+      <c r="I175" t="n">
+        <v>45267.84337144644</v>
+      </c>
+      <c r="J175" t="n">
+        <v>47496.31991731214</v>
+      </c>
+      <c r="K175" t="n">
+        <v>39574.88315352852</v>
       </c>
     </row>
     <row r="176">
@@ -13760,8 +16116,20 @@
       <c r="F176" t="n">
         <v>527.6799999999999</v>
       </c>
+      <c r="G176" t="n">
+        <v>1879.561721858285</v>
+      </c>
       <c r="H176" t="n">
-        <v>45130.3</v>
+        <v>38948.44961808917</v>
+      </c>
+      <c r="I176" t="n">
+        <v>43250.73827814172</v>
+      </c>
+      <c r="J176" t="n">
+        <v>44775.32136939577</v>
+      </c>
+      <c r="K176" t="n">
+        <v>39454.05463638842</v>
       </c>
     </row>
     <row r="177">
@@ -13774,8 +16142,20 @@
       <c r="F177" t="n">
         <v>527.58</v>
       </c>
+      <c r="G177" t="n">
+        <v>2010.694208376553</v>
+      </c>
       <c r="H177" t="n">
-        <v>43847.2</v>
+        <v>38938.06771602331</v>
+      </c>
+      <c r="I177" t="n">
+        <v>41836.50579162344</v>
+      </c>
+      <c r="J177" t="n">
+        <v>42846.22691397715</v>
+      </c>
+      <c r="K177" t="n">
+        <v>39352.95543762152</v>
       </c>
     </row>
     <row r="178">
@@ -13788,8 +16168,20 @@
       <c r="F178" t="n">
         <v>527.48</v>
       </c>
+      <c r="G178" t="n">
+        <v>1069.883684919252</v>
+      </c>
       <c r="H178" t="n">
-        <v>41931.9</v>
+        <v>38930.65732677122</v>
+      </c>
+      <c r="I178" t="n">
+        <v>40862.01631508075</v>
+      </c>
+      <c r="J178" t="n">
+        <v>41505.45223007422</v>
+      </c>
+      <c r="K178" t="n">
+        <v>39269.11857014409</v>
       </c>
     </row>
     <row r="179">
@@ -13802,8 +16194,20 @@
       <c r="F179" t="n">
         <v>527.38</v>
       </c>
+      <c r="G179" t="n">
+        <v>2174.148991482274</v>
+      </c>
       <c r="H179" t="n">
-        <v>42374.3</v>
+        <v>38924.63364139901</v>
+      </c>
+      <c r="I179" t="n">
+        <v>40200.15100851773</v>
+      </c>
+      <c r="J179" t="n">
+        <v>40592.04381056508</v>
+      </c>
+      <c r="K179" t="n">
+        <v>39200.62889433547</v>
       </c>
     </row>
     <row r="180">
@@ -13816,8 +16220,20 @@
       <c r="F180" t="n">
         <v>527.28</v>
       </c>
+      <c r="G180" t="n">
+        <v>1210.199998068842</v>
+      </c>
       <c r="H180" t="n">
-        <v>40966.8</v>
+        <v>38919.50643059107</v>
+      </c>
+      <c r="I180" t="n">
+        <v>39756.60000193116</v>
+      </c>
+      <c r="J180" t="n">
+        <v>39980.77686030165</v>
+      </c>
+      <c r="K180" t="n">
+        <v>39144.00789221389</v>
       </c>
     </row>
     <row r="181">
@@ -13830,8 +16246,20 @@
       <c r="F181" t="n">
         <v>527.1799999999999</v>
       </c>
+      <c r="G181" t="n">
+        <v>1610.402467280728</v>
+      </c>
       <c r="H181" t="n">
-        <v>41073.7</v>
+        <v>38915.5802920212</v>
+      </c>
+      <c r="I181" t="n">
+        <v>39463.29753271927</v>
+      </c>
+      <c r="J181" t="n">
+        <v>39578.982129433</v>
+      </c>
+      <c r="K181" t="n">
+        <v>39097.12496132364</v>
       </c>
     </row>
     <row r="182">
@@ -13844,8 +16272,20 @@
       <c r="F182" t="n">
         <v>527.08</v>
       </c>
+      <c r="G182" t="n">
+        <v>1674.696021290096</v>
+      </c>
       <c r="H182" t="n">
-        <v>40945.1</v>
+        <v>38911.67945636129</v>
+      </c>
+      <c r="I182" t="n">
+        <v>39270.4039787099</v>
+      </c>
+      <c r="J182" t="n">
+        <v>39320.00824875508</v>
+      </c>
+      <c r="K182" t="n">
+        <v>39058.87048210649</v>
       </c>
     </row>
     <row r="183">
@@ -13858,8 +16298,20 @@
       <c r="F183" t="n">
         <v>526.98</v>
       </c>
+      <c r="G183" t="n">
+        <v>636.5932150541848</v>
+      </c>
       <c r="H183" t="n">
-        <v>39781.8</v>
+        <v>38908.9652351894</v>
+      </c>
+      <c r="I183" t="n">
+        <v>39145.20678494582</v>
+      </c>
+      <c r="J183" t="n">
+        <v>39155.22928249973</v>
+      </c>
+      <c r="K183" t="n">
+        <v>39026.85512058488</v>
       </c>
     </row>
     <row r="184">
@@ -13872,8 +16324,20 @@
       <c r="F184" t="n">
         <v>526.88</v>
       </c>
+      <c r="G184" t="n">
+        <v>-468.4085414456713</v>
+      </c>
       <c r="H184" t="n">
-        <v>38597.2</v>
+        <v>38908.42546227164</v>
+      </c>
+      <c r="I184" t="n">
+        <v>39065.60854144567</v>
+      </c>
+      <c r="J184" t="n">
+        <v>39052.96934104241</v>
+      </c>
+      <c r="K184" t="n">
+        <v>39001.20360438584</v>
       </c>
     </row>
     <row r="185">
@@ -13886,8 +16350,20 @@
       <c r="F185" t="n">
         <v>526.78</v>
       </c>
+      <c r="G185" t="n">
+        <v>458.5848510462311</v>
+      </c>
       <c r="H185" t="n">
-        <v>39472.9</v>
+        <v>38908.18748841507</v>
+      </c>
+      <c r="I185" t="n">
+        <v>39014.31514895377</v>
+      </c>
+      <c r="J185" t="n">
+        <v>38992.01243283903</v>
+      </c>
+      <c r="K185" t="n">
+        <v>38982.02240122837</v>
       </c>
     </row>
     <row r="186">
@@ -13900,8 +16376,20 @@
       <c r="F186" t="n">
         <v>526.6799999999999</v>
       </c>
+      <c r="G186" t="n">
+        <v>255.3751325445119</v>
+      </c>
       <c r="H186" t="n">
-        <v>39235.7</v>
+        <v>38907.36165043546</v>
+      </c>
+      <c r="I186" t="n">
+        <v>38980.32486745549</v>
+      </c>
+      <c r="J186" t="n">
+        <v>38955.81047465323</v>
+      </c>
+      <c r="K186" t="n">
+        <v>38966.69287813712</v>
       </c>
     </row>
     <row r="187">
@@ -13914,8 +16402,20 @@
       <c r="F187" t="n">
         <v>526.58</v>
       </c>
+      <c r="G187" t="n">
+        <v>478.9673818674273</v>
+      </c>
       <c r="H187" t="n">
-        <v>39436.7</v>
+        <v>38906.56304859624</v>
+      </c>
+      <c r="I187" t="n">
+        <v>38957.73261813257</v>
+      </c>
+      <c r="J187" t="n">
+        <v>38933.9902826766</v>
+      </c>
+      <c r="K187" t="n">
+        <v>38953.69683441215</v>
       </c>
     </row>
     <row r="188">
@@ -13928,8 +16428,20 @@
       <c r="F188" t="n">
         <v>526.48</v>
       </c>
+      <c r="G188" t="n">
+        <v>429.45989240372</v>
+      </c>
       <c r="H188" t="n">
-        <v>39371.7</v>
+        <v>38905.63754859154</v>
+      </c>
+      <c r="I188" t="n">
+        <v>38942.24010759628</v>
+      </c>
+      <c r="J188" t="n">
+        <v>38921.17397741864</v>
+      </c>
+      <c r="K188" t="n">
+        <v>38943.12218089963</v>
       </c>
     </row>
     <row r="189">
@@ -13942,8 +16454,20 @@
       <c r="F189" t="n">
         <v>526.38</v>
       </c>
+      <c r="G189" t="n">
+        <v>-253.5671834255772</v>
+      </c>
       <c r="H189" t="n">
-        <v>38678.5</v>
+        <v>38905.41004016042</v>
+      </c>
+      <c r="I189" t="n">
+        <v>38932.06718342558</v>
+      </c>
+      <c r="J189" t="n">
+        <v>38913.50345853759</v>
+      </c>
+      <c r="K189" t="n">
+        <v>38934.37459469984</v>
       </c>
     </row>
     <row r="190">
@@ -13956,8 +16480,20 @@
       <c r="F190" t="n">
         <v>526.28</v>
       </c>
+      <c r="G190" t="n">
+        <v>-23.02739187944826</v>
+      </c>
       <c r="H190" t="n">
-        <v>38902.3</v>
+        <v>38905.62093906668</v>
+      </c>
+      <c r="I190" t="n">
+        <v>38925.32739187945</v>
+      </c>
+      <c r="J190" t="n">
+        <v>38909.56446356878</v>
+      </c>
+      <c r="K190" t="n">
+        <v>38927.91307682855</v>
       </c>
     </row>
     <row r="191">
@@ -13970,8 +16506,20 @@
       <c r="F191" t="n">
         <v>526.1799999999999</v>
       </c>
+      <c r="G191" t="n">
+        <v>-136.0726812858629</v>
+      </c>
       <c r="H191" t="n">
-        <v>38784.4</v>
+        <v>38905.73755910315</v>
+      </c>
+      <c r="I191" t="n">
+        <v>38920.47268128586</v>
+      </c>
+      <c r="J191" t="n">
+        <v>38907.77329779566</v>
+      </c>
+      <c r="K191" t="n">
+        <v>38923.17528349106</v>
       </c>
     </row>
     <row r="192">
@@ -13984,8 +16532,20 @@
       <c r="F192" t="n">
         <v>526.08</v>
       </c>
+      <c r="G192" t="n">
+        <v>27.27986713475548</v>
+      </c>
       <c r="H192" t="n">
-        <v>38944.2</v>
+        <v>38905.81497078711</v>
+      </c>
+      <c r="I192" t="n">
+        <v>38916.92013286524</v>
+      </c>
+      <c r="J192" t="n">
+        <v>38906.83130157884</v>
+      </c>
+      <c r="K192" t="n">
+        <v>38919.37913505302</v>
       </c>
     </row>
     <row r="193">
@@ -13998,8 +16558,20 @@
       <c r="F193" t="n">
         <v>525.98</v>
       </c>
+      <c r="G193" t="n">
+        <v>-36.21539862511418</v>
+      </c>
       <c r="H193" t="n">
-        <v>38878</v>
+        <v>38905.80577174084</v>
+      </c>
+      <c r="I193" t="n">
+        <v>38914.21539862511</v>
+      </c>
+      <c r="J193" t="n">
+        <v>38906.36006210233</v>
+      </c>
+      <c r="K193" t="n">
+        <v>38916.3751943523</v>
       </c>
     </row>
     <row r="194">
@@ -14012,8 +16584,20 @@
       <c r="F194" t="n">
         <v>525.88</v>
       </c>
+      <c r="G194" t="n">
+        <v>-115.1145658445312</v>
+      </c>
       <c r="H194" t="n">
-        <v>38797.2</v>
+        <v>38905.93171834338</v>
+      </c>
+      <c r="I194" t="n">
+        <v>38912.31456584453</v>
+      </c>
+      <c r="J194" t="n">
+        <v>38906.07217353163</v>
+      </c>
+      <c r="K194" t="n">
+        <v>38913.94911511784</v>
       </c>
     </row>
     <row r="195">
@@ -14026,8 +16610,20 @@
       <c r="F195" t="n">
         <v>525.78</v>
       </c>
+      <c r="G195" t="n">
+        <v>-4.846176681036013</v>
+      </c>
       <c r="H195" t="n">
         <v>38493.4</v>
+      </c>
+      <c r="I195" t="n">
+        <v>38498.24617668104</v>
+      </c>
+      <c r="J195" t="n">
+        <v>38906.05938608767</v>
+      </c>
+      <c r="K195" t="n">
+        <v>38912.18698918544</v>
       </c>
     </row>
     <row r="196">
@@ -14040,8 +16636,20 @@
       <c r="F196" t="n">
         <v>525.6799999999999</v>
       </c>
+      <c r="G196" t="n">
+        <v>-3.675506747589679</v>
+      </c>
       <c r="H196" t="n">
         <v>37637.7</v>
+      </c>
+      <c r="I196" t="n">
+        <v>37641.37550674759</v>
+      </c>
+      <c r="J196" t="n">
+        <v>38493.45998825965</v>
+      </c>
+      <c r="K196" t="n">
+        <v>38498.18625822661</v>
       </c>
     </row>
     <row r="197">
@@ -14054,8 +16662,20 @@
       <c r="F197" t="n">
         <v>525.58</v>
       </c>
+      <c r="G197" t="n">
+        <v>-2.781859851471381</v>
+      </c>
       <c r="H197" t="n">
         <v>38219.1</v>
+      </c>
+      <c r="I197" t="n">
+        <v>38221.88185985147</v>
+      </c>
+      <c r="J197" t="n">
+        <v>37637.72763500025</v>
+      </c>
+      <c r="K197" t="n">
+        <v>37641.3479250037</v>
       </c>
     </row>
     <row r="198">
@@ -14068,8 +16688,20 @@
       <c r="F198" t="n">
         <v>525.48</v>
       </c>
+      <c r="G198" t="n">
+        <v>-2.099695838958723</v>
+      </c>
       <c r="H198" t="n">
         <v>39274.4</v>
+      </c>
+      <c r="I198" t="n">
+        <v>39276.49969583896</v>
+      </c>
+      <c r="J198" t="n">
+        <v>38219.11248044304</v>
+      </c>
+      <c r="K198" t="n">
+        <v>38221.86941986441</v>
       </c>
     </row>
     <row r="199">
@@ -14082,8 +16714,20 @@
       <c r="F199" t="n">
         <v>525.38</v>
       </c>
+      <c r="G199" t="n">
+        <v>-1.579726243406185</v>
+      </c>
       <c r="H199" t="n">
         <v>38023.5</v>
+      </c>
+      <c r="I199" t="n">
+        <v>38025.07972624341</v>
+      </c>
+      <c r="J199" t="n">
+        <v>39274.40552521245</v>
+      </c>
+      <c r="K199" t="n">
+        <v>39276.49420123034</v>
       </c>
     </row>
     <row r="200">
@@ -14096,8 +16740,20 @@
       <c r="F200" t="n">
         <v>525.28</v>
       </c>
+      <c r="G200" t="n">
+        <v>-1.184352303826017</v>
+      </c>
       <c r="H200" t="n">
         <v>37119.3</v>
+      </c>
+      <c r="I200" t="n">
+        <v>37120.48435230383</v>
+      </c>
+      <c r="J200" t="n">
+        <v>38023.50239766964</v>
+      </c>
+      <c r="K200" t="n">
+        <v>38025.07735162974</v>
       </c>
     </row>
     <row r="201">
@@ -14110,8 +16766,20 @@
       <c r="F201" t="n">
         <v>525.1799999999999</v>
       </c>
+      <c r="G201" t="n">
+        <v>-0.8846446954412386</v>
+      </c>
       <c r="H201" t="n">
         <v>38762.3</v>
+      </c>
+      <c r="I201" t="n">
+        <v>38763.18464469544</v>
+      </c>
+      <c r="J201" t="n">
+        <v>37119.30101982511</v>
+      </c>
+      <c r="K201" t="n">
+        <v>37120.4833497779</v>
       </c>
     </row>
     <row r="202">
@@ -14124,8 +16792,20 @@
       <c r="F202" t="n">
         <v>525.08</v>
       </c>
+      <c r="G202" t="n">
+        <v>-0.6582504764883197</v>
+      </c>
       <c r="H202" t="n">
         <v>38716.1</v>
+      </c>
+      <c r="I202" t="n">
+        <v>38716.75825047649</v>
+      </c>
+      <c r="J202" t="n">
+        <v>38762.30042514222</v>
+      </c>
+      <c r="K202" t="n">
+        <v>38763.18423248066</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix issues that was solved before
</commit_message>
<xml_diff>
--- a/DATA/UKSAF/STO.xlsx
+++ b/DATA/UKSAF/STO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3072" yWindow="3072" windowWidth="16200" windowHeight="25080" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Ti2p" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sr3d" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="O1s" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="C1s" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Results Table" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ti2p" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sr3d" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="O1s" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="C1s" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results Table" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -20,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -39,15 +39,10 @@
       <sz val="11"/>
     </font>
     <font>
-      <name val="Aptos Narrow"/>
-      <b val="1"/>
-      <sz val="11"/>
-    </font>
-    <font>
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -62,24 +57,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF90EE90"/>
-        <bgColor rgb="FF90EE90"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF90EE90"/>
-        <bgColor rgb="FF90EE90"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="0090EE90"/>
         <bgColor rgb="0090EE90"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="23">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -230,282 +220,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="medium">
         <color auto="1"/>
       </right>
       <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="medium">
@@ -573,93 +294,54 @@
       <top style="thin"/>
       <bottom style="medium"/>
     </border>
-    <border>
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="34" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="35" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="41" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,7 +419,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>3</col>
@@ -752,16 +434,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -770,7 +449,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>3</col>
@@ -781,18 +460,20 @@
     <ext cx="7191375" cy="5095875"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPr id="2" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -803,7 +484,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>3</col>
@@ -814,17 +495,22 @@
     <ext cx="5648325" cy="4086225"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPr id="2" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -833,7 +519,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>3</col>
@@ -844,18 +530,20 @@
     <ext cx="7191375" cy="5095875"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPr id="2" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
-        <a:ln>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
@@ -1195,167 +883,167 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="31" t="inlineStr">
+      <c r="A1" s="13" t="inlineStr">
         <is>
           <t>Binding Energy (E)</t>
         </is>
       </c>
-      <c r="B1" s="31" t="inlineStr">
-        <is>
-          <t>Raw Data</t>
-        </is>
-      </c>
-      <c r="C1" s="31" t="inlineStr"/>
-      <c r="D1" s="31" t="inlineStr"/>
-      <c r="E1" s="31" t="inlineStr"/>
-      <c r="F1" s="31" t="inlineStr">
+      <c r="B1" s="13" t="inlineStr">
+        <is>
+          <t>Intensity</t>
+        </is>
+      </c>
+      <c r="C1" s="13" t="inlineStr"/>
+      <c r="D1" s="13" t="inlineStr"/>
+      <c r="E1" s="13" t="inlineStr"/>
+      <c r="F1" s="13" t="inlineStr">
         <is>
           <t>BE</t>
         </is>
       </c>
-      <c r="G1" s="31" t="inlineStr">
+      <c r="G1" s="13" t="inlineStr">
         <is>
           <t>Residuals</t>
         </is>
       </c>
-      <c r="H1" s="31" t="inlineStr">
+      <c r="H1" s="13" t="inlineStr">
         <is>
           <t>Background</t>
         </is>
       </c>
-      <c r="I1" s="31" t="inlineStr">
+      <c r="I1" s="13" t="inlineStr">
         <is>
           <t>Calculated Fit</t>
         </is>
       </c>
-      <c r="J1" s="31" t="inlineStr">
+      <c r="J1" s="13" t="inlineStr">
         <is>
           <t>Ti2p3/2 p1</t>
         </is>
       </c>
-      <c r="K1" s="31" t="inlineStr">
+      <c r="K1" s="13" t="inlineStr">
         <is>
           <t>Ti2p1/2 p2</t>
         </is>
       </c>
-      <c r="L1" s="31" t="inlineStr"/>
-      <c r="M1" s="31" t="inlineStr"/>
-      <c r="N1" s="31" t="inlineStr"/>
-      <c r="O1" s="31" t="inlineStr"/>
-      <c r="P1" s="31" t="inlineStr"/>
-      <c r="Q1" s="31" t="inlineStr"/>
-      <c r="R1" s="31" t="inlineStr"/>
-      <c r="S1" s="31" t="inlineStr"/>
-      <c r="T1" s="31" t="inlineStr"/>
-      <c r="U1" s="31" t="inlineStr"/>
-      <c r="V1" s="31" t="inlineStr"/>
-      <c r="W1" s="31" t="inlineStr"/>
-      <c r="X1" s="32" t="inlineStr">
+      <c r="L1" s="13" t="inlineStr"/>
+      <c r="M1" s="13" t="inlineStr"/>
+      <c r="N1" s="13" t="inlineStr"/>
+      <c r="O1" s="13" t="inlineStr"/>
+      <c r="P1" s="13" t="inlineStr"/>
+      <c r="Q1" s="13" t="inlineStr"/>
+      <c r="R1" s="13" t="inlineStr"/>
+      <c r="S1" s="13" t="inlineStr"/>
+      <c r="T1" s="13" t="inlineStr"/>
+      <c r="U1" s="13" t="inlineStr"/>
+      <c r="V1" s="13" t="inlineStr"/>
+      <c r="W1" s="13" t="inlineStr"/>
+      <c r="X1" s="14" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="Y1" s="33" t="inlineStr">
+      <c r="Y1" s="15" t="inlineStr">
         <is>
           <t>Peak
 Label</t>
         </is>
       </c>
-      <c r="Z1" s="33" t="inlineStr">
+      <c r="Z1" s="15" t="inlineStr">
         <is>
           <t>Position
 (eV)</t>
         </is>
       </c>
-      <c r="AA1" s="33" t="inlineStr">
+      <c r="AA1" s="15" t="inlineStr">
         <is>
           <t>Height
 (CPS)</t>
         </is>
       </c>
-      <c r="AB1" s="33" t="inlineStr">
+      <c r="AB1" s="15" t="inlineStr">
         <is>
           <t>FWHM
 (eV)</t>
         </is>
       </c>
-      <c r="AC1" s="33" t="inlineStr">
+      <c r="AC1" s="15" t="inlineStr">
         <is>
           <t xml:space="preserve">σ/γ (%)
 L/G 
 </t>
         </is>
       </c>
-      <c r="AD1" s="33" t="inlineStr">
+      <c r="AD1" s="15" t="inlineStr">
         <is>
           <t>Area
 (CPS.eV)</t>
         </is>
       </c>
-      <c r="AE1" s="33" t="inlineStr">
+      <c r="AE1" s="15" t="inlineStr">
         <is>
           <t>σ
 W_g</t>
         </is>
       </c>
-      <c r="AF1" s="33" t="inlineStr">
+      <c r="AF1" s="15" t="inlineStr">
         <is>
           <t>γ
 W_l</t>
         </is>
       </c>
-      <c r="AG1" s="33" t="inlineStr">
+      <c r="AG1" s="15" t="inlineStr">
         <is>
           <t>W_g
 Skew</t>
         </is>
       </c>
-      <c r="AH1" s="33" t="inlineStr">
+      <c r="AH1" s="15" t="inlineStr">
         <is>
           <t>Conc.
 (%)</t>
         </is>
       </c>
-      <c r="AI1" s="33" t="inlineStr">
+      <c r="AI1" s="15" t="inlineStr">
         <is>
           <t>A/Aᴀ</t>
         </is>
       </c>
-      <c r="AJ1" s="33" t="inlineStr">
+      <c r="AJ1" s="15" t="inlineStr">
         <is>
           <t>Split
 (eV)</t>
         </is>
       </c>
-      <c r="AK1" s="33" t="inlineStr">
+      <c r="AK1" s="15" t="inlineStr">
         <is>
           <t>Fitting Model</t>
         </is>
       </c>
-      <c r="AL1" s="33" t="inlineStr">
+      <c r="AL1" s="15" t="inlineStr">
         <is>
           <t>Bkg Type</t>
         </is>
       </c>
-      <c r="AM1" s="33" t="inlineStr">
+      <c r="AM1" s="15" t="inlineStr">
         <is>
           <t>Bkg Low
 (eV)</t>
         </is>
       </c>
-      <c r="AN1" s="33" t="inlineStr">
+      <c r="AN1" s="15" t="inlineStr">
         <is>
           <t>Bkg High
 (eV)</t>
         </is>
       </c>
-      <c r="AO1" s="33" t="inlineStr">
+      <c r="AO1" s="15" t="inlineStr">
         <is>
           <t>Bkg Offset Low
 (CPS)</t>
         </is>
       </c>
-      <c r="AP1" s="34" t="inlineStr">
+      <c r="AP1" s="16" t="inlineStr">
         <is>
           <t>Bkg Offset High
 (CPS)</t>
@@ -1387,97 +1075,97 @@
       <c r="K2" t="n">
         <v>39754.6</v>
       </c>
-      <c r="X2" s="35" t="inlineStr">
+      <c r="X2" s="17" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="Y2" s="36" t="inlineStr">
+      <c r="Y2" s="18" t="inlineStr">
         <is>
           <t>Ti2p3/2 p1</t>
         </is>
       </c>
-      <c r="Z2" s="36" t="inlineStr">
+      <c r="Z2" s="18" t="inlineStr">
         <is>
           <t>458.00</t>
         </is>
       </c>
-      <c r="AA2" s="36" t="inlineStr">
+      <c r="AA2" s="18" t="inlineStr">
         <is>
           <t>88789</t>
         </is>
       </c>
-      <c r="AB2" s="36" t="inlineStr">
+      <c r="AB2" s="18" t="inlineStr">
         <is>
           <t>1.01</t>
         </is>
       </c>
-      <c r="AC2" s="36" t="inlineStr">
+      <c r="AC2" s="18" t="inlineStr">
         <is>
           <t>50.00</t>
         </is>
       </c>
-      <c r="AD2" s="36" t="inlineStr">
+      <c r="AD2" s="18" t="inlineStr">
         <is>
           <t>108142</t>
         </is>
       </c>
-      <c r="AE2" s="36" t="inlineStr">
+      <c r="AE2" s="18" t="inlineStr">
         <is>
           <t>2.16</t>
         </is>
       </c>
-      <c r="AF2" s="36" t="inlineStr">
+      <c r="AF2" s="18" t="inlineStr">
         <is>
           <t>2.16</t>
         </is>
       </c>
-      <c r="AG2" s="36" t="inlineStr">
+      <c r="AG2" s="18" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AH2" s="36" t="inlineStr">
+      <c r="AH2" s="18" t="inlineStr">
         <is>
           <t>64.5</t>
         </is>
       </c>
-      <c r="AI2" s="36" t="inlineStr">
+      <c r="AI2" s="18" t="inlineStr">
         <is>
           <t>100.0</t>
         </is>
       </c>
-      <c r="AJ2" s="36" t="inlineStr">
+      <c r="AJ2" s="18" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="AK2" s="36" t="inlineStr">
+      <c r="AK2" s="18" t="inlineStr">
         <is>
           <t>LA (Area, σ/γ, γ)</t>
         </is>
       </c>
-      <c r="AL2" s="36" t="inlineStr">
+      <c r="AL2" s="18" t="inlineStr">
         <is>
           <t>Multi-Regions Smart</t>
         </is>
       </c>
-      <c r="AM2" s="36" t="inlineStr">
+      <c r="AM2" s="18" t="inlineStr">
         <is>
           <t>448.08</t>
         </is>
       </c>
-      <c r="AN2" s="36" t="inlineStr">
+      <c r="AN2" s="18" t="inlineStr">
         <is>
           <t>475.08</t>
         </is>
       </c>
-      <c r="AO2" s="36" t="inlineStr">
+      <c r="AO2" s="18" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AP2" s="37" t="inlineStr">
+      <c r="AP2" s="19" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1508,57 +1196,57 @@
       <c r="K3" t="n">
         <v>39759.5227141248</v>
       </c>
-      <c r="X3" s="38" t="inlineStr"/>
-      <c r="Y3" s="39" t="inlineStr"/>
-      <c r="Z3" s="39" t="inlineStr">
+      <c r="X3" s="20" t="inlineStr"/>
+      <c r="Y3" s="21" t="inlineStr"/>
+      <c r="Z3" s="21" t="inlineStr">
         <is>
           <t>448.08,475.08</t>
         </is>
       </c>
-      <c r="AA3" s="39" t="inlineStr">
+      <c r="AA3" s="21" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AB3" s="39" t="inlineStr">
+      <c r="AB3" s="21" t="inlineStr">
         <is>
           <t>0.3:3.5</t>
         </is>
       </c>
-      <c r="AC3" s="39" t="inlineStr">
+      <c r="AC3" s="21" t="inlineStr">
         <is>
           <t>Fixed</t>
         </is>
       </c>
-      <c r="AD3" s="39" t="inlineStr">
+      <c r="AD3" s="21" t="inlineStr">
         <is>
           <t>1:1e7</t>
         </is>
       </c>
-      <c r="AE3" s="39" t="inlineStr">
+      <c r="AE3" s="21" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AF3" s="39" t="inlineStr">
+      <c r="AF3" s="21" t="inlineStr">
         <is>
           <t>0.01:10</t>
         </is>
       </c>
-      <c r="AG3" s="39" t="inlineStr">
+      <c r="AG3" s="21" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AH3" s="39" t="inlineStr"/>
-      <c r="AI3" s="39" t="inlineStr"/>
-      <c r="AJ3" s="39" t="inlineStr"/>
-      <c r="AK3" s="39" t="inlineStr"/>
-      <c r="AL3" s="39" t="inlineStr"/>
-      <c r="AM3" s="39" t="inlineStr"/>
-      <c r="AN3" s="39" t="inlineStr"/>
-      <c r="AO3" s="39" t="inlineStr"/>
-      <c r="AP3" s="40" t="inlineStr"/>
+      <c r="AH3" s="21" t="inlineStr"/>
+      <c r="AI3" s="21" t="inlineStr"/>
+      <c r="AJ3" s="21" t="inlineStr"/>
+      <c r="AK3" s="21" t="inlineStr"/>
+      <c r="AL3" s="21" t="inlineStr"/>
+      <c r="AM3" s="21" t="inlineStr"/>
+      <c r="AN3" s="21" t="inlineStr"/>
+      <c r="AO3" s="21" t="inlineStr"/>
+      <c r="AP3" s="22" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1585,97 +1273,97 @@
       <c r="K4" t="n">
         <v>39976.91078309989</v>
       </c>
-      <c r="X4" s="35" t="inlineStr">
+      <c r="X4" s="17" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="Y4" s="36" t="inlineStr">
+      <c r="Y4" s="18" t="inlineStr">
         <is>
           <t>Ti2p1/2 p2</t>
         </is>
       </c>
-      <c r="Z4" s="36" t="inlineStr">
+      <c r="Z4" s="18" t="inlineStr">
         <is>
           <t>463.73</t>
         </is>
       </c>
-      <c r="AA4" s="36" t="inlineStr">
+      <c r="AA4" s="18" t="inlineStr">
         <is>
           <t>25280</t>
         </is>
       </c>
-      <c r="AB4" s="36" t="inlineStr">
+      <c r="AB4" s="18" t="inlineStr">
         <is>
           <t>1.95</t>
         </is>
       </c>
-      <c r="AC4" s="36" t="inlineStr">
+      <c r="AC4" s="18" t="inlineStr">
         <is>
           <t>50.00</t>
         </is>
       </c>
-      <c r="AD4" s="36" t="inlineStr">
+      <c r="AD4" s="18" t="inlineStr">
         <is>
           <t>59478</t>
         </is>
       </c>
-      <c r="AE4" s="36" t="inlineStr">
+      <c r="AE4" s="18" t="inlineStr">
         <is>
           <t>2.16</t>
         </is>
       </c>
-      <c r="AF4" s="36" t="inlineStr">
+      <c r="AF4" s="18" t="inlineStr">
         <is>
           <t>2.16</t>
         </is>
       </c>
-      <c r="AG4" s="36" t="inlineStr">
+      <c r="AG4" s="18" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AH4" s="36" t="inlineStr">
+      <c r="AH4" s="18" t="inlineStr">
         <is>
           <t>35.5</t>
         </is>
       </c>
-      <c r="AI4" s="36" t="inlineStr">
+      <c r="AI4" s="18" t="inlineStr">
         <is>
           <t>55.0</t>
         </is>
       </c>
-      <c r="AJ4" s="36" t="inlineStr">
+      <c r="AJ4" s="18" t="inlineStr">
         <is>
           <t>5.73</t>
         </is>
       </c>
-      <c r="AK4" s="36" t="inlineStr">
+      <c r="AK4" s="18" t="inlineStr">
         <is>
           <t>LA (Area, σ/γ, γ)</t>
         </is>
       </c>
-      <c r="AL4" s="36" t="inlineStr">
+      <c r="AL4" s="18" t="inlineStr">
         <is>
           <t>Multi-Regions Smart</t>
         </is>
       </c>
-      <c r="AM4" s="36" t="inlineStr">
+      <c r="AM4" s="18" t="inlineStr">
         <is>
           <t>448.08</t>
         </is>
       </c>
-      <c r="AN4" s="36" t="inlineStr">
+      <c r="AN4" s="18" t="inlineStr">
         <is>
           <t>475.08</t>
         </is>
       </c>
-      <c r="AO4" s="36" t="inlineStr">
+      <c r="AO4" s="18" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AP4" s="37" t="inlineStr">
+      <c r="AP4" s="19" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1706,57 +1394,57 @@
       <c r="K5" t="n">
         <v>39346.80774419603</v>
       </c>
-      <c r="X5" s="38" t="inlineStr"/>
-      <c r="Y5" s="39" t="inlineStr"/>
-      <c r="Z5" s="39" t="inlineStr">
+      <c r="X5" s="20" t="inlineStr"/>
+      <c r="Y5" s="21" t="inlineStr"/>
+      <c r="Z5" s="21" t="inlineStr">
         <is>
           <t>A+5.7#0.2</t>
         </is>
       </c>
-      <c r="AA5" s="39" t="inlineStr">
+      <c r="AA5" s="21" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AB5" s="39" t="inlineStr">
+      <c r="AB5" s="21" t="inlineStr">
         <is>
           <t>0.3:3.5</t>
         </is>
       </c>
-      <c r="AC5" s="39" t="inlineStr">
+      <c r="AC5" s="21" t="inlineStr">
         <is>
           <t>A*1</t>
         </is>
       </c>
-      <c r="AD5" s="39" t="inlineStr">
+      <c r="AD5" s="21" t="inlineStr">
         <is>
           <t>A*0.5#0.05</t>
         </is>
       </c>
-      <c r="AE5" s="39" t="inlineStr">
+      <c r="AE5" s="21" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AF5" s="39" t="inlineStr">
+      <c r="AF5" s="21" t="inlineStr">
         <is>
           <t>A*1</t>
         </is>
       </c>
-      <c r="AG5" s="39" t="inlineStr">
+      <c r="AG5" s="21" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AH5" s="39" t="inlineStr"/>
-      <c r="AI5" s="39" t="inlineStr"/>
-      <c r="AJ5" s="39" t="inlineStr"/>
-      <c r="AK5" s="39" t="inlineStr"/>
-      <c r="AL5" s="39" t="inlineStr"/>
-      <c r="AM5" s="39" t="inlineStr"/>
-      <c r="AN5" s="39" t="inlineStr"/>
-      <c r="AO5" s="39" t="inlineStr"/>
-      <c r="AP5" s="40" t="inlineStr"/>
+      <c r="AH5" s="21" t="inlineStr"/>
+      <c r="AI5" s="21" t="inlineStr"/>
+      <c r="AJ5" s="21" t="inlineStr"/>
+      <c r="AK5" s="21" t="inlineStr"/>
+      <c r="AL5" s="21" t="inlineStr"/>
+      <c r="AM5" s="21" t="inlineStr"/>
+      <c r="AN5" s="21" t="inlineStr"/>
+      <c r="AO5" s="21" t="inlineStr"/>
+      <c r="AP5" s="22" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -8718,162 +8406,162 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="31" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Binding Energy (E)</t>
         </is>
       </c>
-      <c r="B1" s="31" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Raw Data</t>
         </is>
       </c>
-      <c r="C1" s="31" t="inlineStr"/>
-      <c r="D1" s="31" t="inlineStr"/>
-      <c r="E1" s="31" t="inlineStr"/>
-      <c r="F1" s="31" t="inlineStr">
+      <c r="C1" s="1" t="n"/>
+      <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>BE</t>
         </is>
       </c>
-      <c r="G1" s="31" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Residuals</t>
         </is>
       </c>
-      <c r="H1" s="31" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Background</t>
         </is>
       </c>
-      <c r="I1" s="31" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Calculated Fit</t>
         </is>
       </c>
-      <c r="J1" s="31" t="inlineStr"/>
-      <c r="K1" s="31" t="inlineStr"/>
-      <c r="L1" s="31" t="inlineStr"/>
-      <c r="M1" s="31" t="inlineStr"/>
-      <c r="N1" s="31" t="inlineStr"/>
-      <c r="O1" s="31" t="inlineStr"/>
-      <c r="P1" s="31" t="inlineStr"/>
-      <c r="Q1" s="31" t="inlineStr"/>
-      <c r="R1" s="31" t="inlineStr"/>
-      <c r="S1" s="31" t="inlineStr"/>
-      <c r="T1" s="31" t="inlineStr"/>
-      <c r="U1" s="31" t="inlineStr"/>
-      <c r="V1" s="31" t="inlineStr"/>
-      <c r="W1" s="31" t="inlineStr"/>
-      <c r="X1" s="32" t="inlineStr">
+      <c r="J1" s="1" t="n"/>
+      <c r="K1" s="1" t="n"/>
+      <c r="L1" s="1" t="n"/>
+      <c r="M1" s="1" t="n"/>
+      <c r="N1" s="1" t="n"/>
+      <c r="O1" s="1" t="n"/>
+      <c r="P1" s="1" t="n"/>
+      <c r="Q1" s="1" t="n"/>
+      <c r="R1" s="1" t="n"/>
+      <c r="S1" s="1" t="n"/>
+      <c r="T1" s="1" t="n"/>
+      <c r="U1" s="1" t="n"/>
+      <c r="V1" s="1" t="n"/>
+      <c r="W1" s="1" t="n"/>
+      <c r="X1" s="2" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="Y1" s="33" t="inlineStr">
+      <c r="Y1" s="3" t="inlineStr">
         <is>
           <t>Peak
 Label</t>
         </is>
       </c>
-      <c r="Z1" s="33" t="inlineStr">
+      <c r="Z1" s="3" t="inlineStr">
         <is>
           <t>Position
 (eV)</t>
         </is>
       </c>
-      <c r="AA1" s="33" t="inlineStr">
+      <c r="AA1" s="3" t="inlineStr">
         <is>
           <t>Height
 (CPS)</t>
         </is>
       </c>
-      <c r="AB1" s="33" t="inlineStr">
+      <c r="AB1" s="3" t="inlineStr">
         <is>
           <t>FWHM
 (eV)</t>
         </is>
       </c>
-      <c r="AC1" s="33" t="inlineStr">
+      <c r="AC1" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">σ/γ (%)
 L/G 
 </t>
         </is>
       </c>
-      <c r="AD1" s="33" t="inlineStr">
+      <c r="AD1" s="3" t="inlineStr">
         <is>
           <t>Area
 (CPS.eV)</t>
         </is>
       </c>
-      <c r="AE1" s="33" t="inlineStr">
+      <c r="AE1" s="3" t="inlineStr">
         <is>
           <t>σ
 W_g</t>
         </is>
       </c>
-      <c r="AF1" s="33" t="inlineStr">
+      <c r="AF1" s="3" t="inlineStr">
         <is>
           <t>γ
 W_l</t>
         </is>
       </c>
-      <c r="AG1" s="33" t="inlineStr">
+      <c r="AG1" s="3" t="inlineStr">
         <is>
           <t>W_g
 Skew</t>
         </is>
       </c>
-      <c r="AH1" s="33" t="inlineStr">
+      <c r="AH1" s="3" t="inlineStr">
         <is>
           <t>Conc.
 (%)</t>
         </is>
       </c>
-      <c r="AI1" s="33" t="inlineStr">
+      <c r="AI1" s="3" t="inlineStr">
         <is>
           <t>A/Aᴀ</t>
         </is>
       </c>
-      <c r="AJ1" s="33" t="inlineStr">
+      <c r="AJ1" s="3" t="inlineStr">
         <is>
           <t>Split
 (eV)</t>
         </is>
       </c>
-      <c r="AK1" s="33" t="inlineStr">
+      <c r="AK1" s="3" t="inlineStr">
         <is>
           <t>Fitting Model</t>
         </is>
       </c>
-      <c r="AL1" s="33" t="inlineStr">
+      <c r="AL1" s="3" t="inlineStr">
         <is>
           <t>Bkg Type</t>
         </is>
       </c>
-      <c r="AM1" s="33" t="inlineStr">
+      <c r="AM1" s="3" t="inlineStr">
         <is>
           <t>Bkg Low
 (eV)</t>
         </is>
       </c>
-      <c r="AN1" s="33" t="inlineStr">
+      <c r="AN1" s="3" t="inlineStr">
         <is>
           <t>Bkg High
 (eV)</t>
         </is>
       </c>
-      <c r="AO1" s="33" t="inlineStr">
+      <c r="AO1" s="3" t="inlineStr">
         <is>
           <t>Bkg Offset Low
 (CPS)</t>
         </is>
       </c>
-      <c r="AP1" s="34" t="inlineStr">
+      <c r="AP1" s="4" t="inlineStr">
         <is>
           <t>Bkg Offset High
 (CPS)</t>
@@ -11152,170 +10840,170 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="31" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Binding Energy (E)</t>
         </is>
       </c>
-      <c r="B1" s="31" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Raw Data</t>
         </is>
       </c>
-      <c r="C1" s="31" t="inlineStr"/>
-      <c r="D1" s="31" t="inlineStr"/>
-      <c r="E1" s="31" t="inlineStr"/>
-      <c r="F1" s="31" t="inlineStr">
+      <c r="C1" s="1" t="n"/>
+      <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>BE</t>
         </is>
       </c>
-      <c r="G1" s="31" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Residuals</t>
         </is>
       </c>
-      <c r="H1" s="31" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Background</t>
         </is>
       </c>
-      <c r="I1" s="31" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Calculated Fit</t>
         </is>
       </c>
-      <c r="J1" s="31" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>O1s p1</t>
         </is>
       </c>
-      <c r="K1" s="31" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>O1s p2</t>
         </is>
       </c>
-      <c r="L1" s="31" t="inlineStr"/>
-      <c r="M1" s="31" t="inlineStr"/>
-      <c r="N1" s="31" t="inlineStr"/>
-      <c r="O1" s="31" t="inlineStr"/>
-      <c r="P1" s="31" t="inlineStr"/>
-      <c r="Q1" s="31" t="inlineStr"/>
-      <c r="R1" s="31" t="inlineStr"/>
-      <c r="S1" s="31" t="inlineStr"/>
-      <c r="T1" s="31" t="inlineStr"/>
-      <c r="U1" s="31" t="inlineStr"/>
-      <c r="V1" s="31" t="inlineStr"/>
-      <c r="W1" s="31" t="inlineStr"/>
-      <c r="X1" s="32" t="inlineStr">
+      <c r="L1" s="1" t="n"/>
+      <c r="M1" s="1" t="n"/>
+      <c r="N1" s="1" t="n"/>
+      <c r="O1" s="1" t="n"/>
+      <c r="P1" s="1" t="n"/>
+      <c r="Q1" s="1" t="n"/>
+      <c r="R1" s="1" t="n"/>
+      <c r="S1" s="1" t="n"/>
+      <c r="T1" s="1" t="n"/>
+      <c r="U1" s="1" t="n"/>
+      <c r="V1" s="1" t="n"/>
+      <c r="W1" s="1" t="n"/>
+      <c r="X1" s="2" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="Y1" s="33" t="inlineStr">
+      <c r="Y1" s="3" t="inlineStr">
         <is>
           <t>Peak
 Label</t>
         </is>
       </c>
-      <c r="Z1" s="33" t="inlineStr">
+      <c r="Z1" s="3" t="inlineStr">
         <is>
           <t>Position
 (eV)</t>
         </is>
       </c>
-      <c r="AA1" s="33" t="inlineStr">
+      <c r="AA1" s="3" t="inlineStr">
         <is>
           <t>Height
 (CPS)</t>
         </is>
       </c>
-      <c r="AB1" s="33" t="inlineStr">
+      <c r="AB1" s="3" t="inlineStr">
         <is>
           <t>FWHM
 (eV)</t>
         </is>
       </c>
-      <c r="AC1" s="33" t="inlineStr">
+      <c r="AC1" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">σ/γ (%)
 L/G 
 </t>
         </is>
       </c>
-      <c r="AD1" s="33" t="inlineStr">
+      <c r="AD1" s="3" t="inlineStr">
         <is>
           <t>Area
 (CPS.eV)</t>
         </is>
       </c>
-      <c r="AE1" s="33" t="inlineStr">
+      <c r="AE1" s="3" t="inlineStr">
         <is>
           <t>σ
 W_g</t>
         </is>
       </c>
-      <c r="AF1" s="33" t="inlineStr">
+      <c r="AF1" s="3" t="inlineStr">
         <is>
           <t>γ
 W_l</t>
         </is>
       </c>
-      <c r="AG1" s="33" t="inlineStr">
+      <c r="AG1" s="3" t="inlineStr">
         <is>
           <t>W_g
 Skew</t>
         </is>
       </c>
-      <c r="AH1" s="33" t="inlineStr">
+      <c r="AH1" s="3" t="inlineStr">
         <is>
           <t>Conc.
 (%)</t>
         </is>
       </c>
-      <c r="AI1" s="33" t="inlineStr">
+      <c r="AI1" s="3" t="inlineStr">
         <is>
           <t>A/Aᴀ</t>
         </is>
       </c>
-      <c r="AJ1" s="33" t="inlineStr">
+      <c r="AJ1" s="3" t="inlineStr">
         <is>
           <t>Split
 (eV)</t>
         </is>
       </c>
-      <c r="AK1" s="33" t="inlineStr">
+      <c r="AK1" s="3" t="inlineStr">
         <is>
           <t>Fitting Model</t>
         </is>
       </c>
-      <c r="AL1" s="33" t="inlineStr">
+      <c r="AL1" s="3" t="inlineStr">
         <is>
           <t>Bkg Type</t>
         </is>
       </c>
-      <c r="AM1" s="33" t="inlineStr">
+      <c r="AM1" s="3" t="inlineStr">
         <is>
           <t>Bkg Low
 (eV)</t>
         </is>
       </c>
-      <c r="AN1" s="33" t="inlineStr">
+      <c r="AN1" s="3" t="inlineStr">
         <is>
           <t>Bkg High
 (eV)</t>
         </is>
       </c>
-      <c r="AO1" s="33" t="inlineStr">
+      <c r="AO1" s="3" t="inlineStr">
         <is>
           <t>Bkg Offset Low
 (CPS)</t>
         </is>
       </c>
-      <c r="AP1" s="34" t="inlineStr">
+      <c r="AP1" s="4" t="inlineStr">
         <is>
           <t>Bkg Offset High
 (CPS)</t>
@@ -11347,89 +11035,89 @@
       <c r="K2" t="n">
         <v>45763.7</v>
       </c>
-      <c r="X2" s="35" t="inlineStr">
+      <c r="X2" s="5" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="Y2" s="36" t="inlineStr">
+      <c r="Y2" s="6" t="inlineStr">
         <is>
           <t>O1s p1</t>
         </is>
       </c>
-      <c r="Z2" s="36" t="inlineStr">
+      <c r="Z2" s="6" t="inlineStr">
         <is>
           <t>529.11</t>
         </is>
       </c>
-      <c r="AA2" s="36" t="inlineStr">
+      <c r="AA2" s="6" t="inlineStr">
         <is>
           <t>135281</t>
         </is>
       </c>
-      <c r="AB2" s="36" t="inlineStr">
+      <c r="AB2" s="6" t="inlineStr">
         <is>
           <t>1.16</t>
         </is>
       </c>
-      <c r="AC2" s="36" t="inlineStr">
+      <c r="AC2" s="6" t="inlineStr">
         <is>
           <t>48.36</t>
         </is>
       </c>
-      <c r="AD2" s="36" t="inlineStr">
+      <c r="AD2" s="6" t="inlineStr">
         <is>
           <t>167043</t>
         </is>
       </c>
-      <c r="AE2" s="36" t="inlineStr"/>
-      <c r="AF2" s="36" t="inlineStr"/>
-      <c r="AG2" s="36" t="inlineStr">
+      <c r="AE2" s="6" t="n"/>
+      <c r="AF2" s="6" t="n"/>
+      <c r="AG2" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AH2" s="36" t="inlineStr">
+      <c r="AH2" s="6" t="inlineStr">
         <is>
           <t>70.9</t>
         </is>
       </c>
-      <c r="AI2" s="36" t="inlineStr">
+      <c r="AI2" s="6" t="inlineStr">
         <is>
           <t>100.0</t>
         </is>
       </c>
-      <c r="AJ2" s="36" t="inlineStr">
+      <c r="AJ2" s="6" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="AK2" s="36" t="inlineStr">
+      <c r="AK2" s="6" t="inlineStr">
         <is>
           <t>GL (Area)</t>
         </is>
       </c>
-      <c r="AL2" s="36" t="inlineStr">
+      <c r="AL2" s="6" t="inlineStr">
         <is>
           <t>Multi-Regions Smart</t>
         </is>
       </c>
-      <c r="AM2" s="36" t="inlineStr">
+      <c r="AM2" s="6" t="inlineStr">
         <is>
           <t>525.08</t>
         </is>
       </c>
-      <c r="AN2" s="36" t="inlineStr">
+      <c r="AN2" s="6" t="inlineStr">
         <is>
           <t>545.08</t>
         </is>
       </c>
-      <c r="AO2" s="36" t="inlineStr">
+      <c r="AO2" s="6" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="AP2" s="37" t="inlineStr">
+      <c r="AP2" s="7" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
@@ -11460,49 +11148,49 @@
       <c r="K3" t="n">
         <v>45763.7</v>
       </c>
-      <c r="X3" s="38" t="inlineStr"/>
-      <c r="Y3" s="39" t="inlineStr"/>
-      <c r="Z3" s="39" t="inlineStr">
+      <c r="X3" s="8" t="n"/>
+      <c r="Y3" s="9" t="n"/>
+      <c r="Z3" s="9" t="inlineStr">
         <is>
           <t>525.08,545.08</t>
         </is>
       </c>
-      <c r="AA3" s="39" t="inlineStr">
+      <c r="AA3" s="9" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AB3" s="39" t="inlineStr">
+      <c r="AB3" s="9" t="inlineStr">
         <is>
           <t>0.3:3.5</t>
         </is>
       </c>
-      <c r="AC3" s="39" t="inlineStr">
+      <c r="AC3" s="9" t="inlineStr">
         <is>
           <t>2:80</t>
         </is>
       </c>
-      <c r="AD3" s="39" t="inlineStr">
+      <c r="AD3" s="9" t="inlineStr">
         <is>
           <t>1:1e7</t>
         </is>
       </c>
-      <c r="AE3" s="39" t="inlineStr"/>
-      <c r="AF3" s="39" t="inlineStr"/>
-      <c r="AG3" s="39" t="inlineStr">
+      <c r="AE3" s="9" t="n"/>
+      <c r="AF3" s="9" t="n"/>
+      <c r="AG3" s="9" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AH3" s="39" t="inlineStr"/>
-      <c r="AI3" s="39" t="inlineStr"/>
-      <c r="AJ3" s="39" t="inlineStr"/>
-      <c r="AK3" s="39" t="inlineStr"/>
-      <c r="AL3" s="39" t="inlineStr"/>
-      <c r="AM3" s="39" t="inlineStr"/>
-      <c r="AN3" s="39" t="inlineStr"/>
-      <c r="AO3" s="39" t="inlineStr"/>
-      <c r="AP3" s="40" t="inlineStr"/>
+      <c r="AH3" s="9" t="n"/>
+      <c r="AI3" s="9" t="n"/>
+      <c r="AJ3" s="9" t="n"/>
+      <c r="AK3" s="9" t="n"/>
+      <c r="AL3" s="9" t="n"/>
+      <c r="AM3" s="9" t="n"/>
+      <c r="AN3" s="9" t="n"/>
+      <c r="AO3" s="9" t="n"/>
+      <c r="AP3" s="10" t="n"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -11529,89 +11217,89 @@
       <c r="K4" t="n">
         <v>46726.9</v>
       </c>
-      <c r="X4" s="35" t="inlineStr">
+      <c r="X4" s="5" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="Y4" s="36" t="inlineStr">
+      <c r="Y4" s="6" t="inlineStr">
         <is>
           <t>O1s p2</t>
         </is>
       </c>
-      <c r="Z4" s="36" t="inlineStr">
+      <c r="Z4" s="6" t="inlineStr">
         <is>
           <t>531.03</t>
         </is>
       </c>
-      <c r="AA4" s="36" t="inlineStr">
+      <c r="AA4" s="6" t="inlineStr">
         <is>
           <t>27380</t>
         </is>
       </c>
-      <c r="AB4" s="36" t="inlineStr">
+      <c r="AB4" s="6" t="inlineStr">
         <is>
           <t>2.35</t>
         </is>
       </c>
-      <c r="AC4" s="36" t="inlineStr">
+      <c r="AC4" s="6" t="inlineStr">
         <is>
           <t>55.48</t>
         </is>
       </c>
-      <c r="AD4" s="36" t="inlineStr">
+      <c r="AD4" s="6" t="inlineStr">
         <is>
           <t>68490</t>
         </is>
       </c>
-      <c r="AE4" s="36" t="inlineStr"/>
-      <c r="AF4" s="36" t="inlineStr"/>
-      <c r="AG4" s="36" t="inlineStr">
+      <c r="AE4" s="6" t="n"/>
+      <c r="AF4" s="6" t="n"/>
+      <c r="AG4" s="6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AH4" s="36" t="inlineStr">
+      <c r="AH4" s="6" t="inlineStr">
         <is>
           <t>29.1</t>
         </is>
       </c>
-      <c r="AI4" s="36" t="inlineStr">
+      <c r="AI4" s="6" t="inlineStr">
         <is>
           <t>41.0</t>
         </is>
       </c>
-      <c r="AJ4" s="36" t="inlineStr">
+      <c r="AJ4" s="6" t="inlineStr">
         <is>
           <t>1.92</t>
         </is>
       </c>
-      <c r="AK4" s="36" t="inlineStr">
+      <c r="AK4" s="6" t="inlineStr">
         <is>
           <t>GL (Area)</t>
         </is>
       </c>
-      <c r="AL4" s="36" t="inlineStr">
+      <c r="AL4" s="6" t="inlineStr">
         <is>
           <t>Multi-Regions Smart</t>
         </is>
       </c>
-      <c r="AM4" s="36" t="inlineStr">
+      <c r="AM4" s="6" t="inlineStr">
         <is>
           <t>525.08</t>
         </is>
       </c>
-      <c r="AN4" s="36" t="inlineStr">
+      <c r="AN4" s="6" t="inlineStr">
         <is>
           <t>545.08</t>
         </is>
       </c>
-      <c r="AO4" s="36" t="inlineStr">
+      <c r="AO4" s="6" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="AP4" s="37" t="inlineStr">
+      <c r="AP4" s="7" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
@@ -11642,49 +11330,49 @@
       <c r="K5" t="n">
         <v>46338.7</v>
       </c>
-      <c r="X5" s="38" t="inlineStr"/>
-      <c r="Y5" s="39" t="inlineStr"/>
-      <c r="Z5" s="39" t="inlineStr">
+      <c r="X5" s="8" t="n"/>
+      <c r="Y5" s="9" t="n"/>
+      <c r="Z5" s="9" t="inlineStr">
         <is>
           <t>525.08,545.08</t>
         </is>
       </c>
-      <c r="AA5" s="39" t="inlineStr">
+      <c r="AA5" s="9" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AB5" s="39" t="inlineStr">
+      <c r="AB5" s="9" t="inlineStr">
         <is>
           <t>0.3:3.5</t>
         </is>
       </c>
-      <c r="AC5" s="39" t="inlineStr">
+      <c r="AC5" s="9" t="inlineStr">
         <is>
           <t>2:80</t>
         </is>
       </c>
-      <c r="AD5" s="39" t="inlineStr">
+      <c r="AD5" s="9" t="inlineStr">
         <is>
           <t>1:1e7</t>
         </is>
       </c>
-      <c r="AE5" s="39" t="inlineStr"/>
-      <c r="AF5" s="39" t="inlineStr"/>
-      <c r="AG5" s="39" t="inlineStr">
+      <c r="AE5" s="9" t="n"/>
+      <c r="AF5" s="9" t="n"/>
+      <c r="AG5" s="9" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AH5" s="39" t="inlineStr"/>
-      <c r="AI5" s="39" t="inlineStr"/>
-      <c r="AJ5" s="39" t="inlineStr"/>
-      <c r="AK5" s="39" t="inlineStr"/>
-      <c r="AL5" s="39" t="inlineStr"/>
-      <c r="AM5" s="39" t="inlineStr"/>
-      <c r="AN5" s="39" t="inlineStr"/>
-      <c r="AO5" s="39" t="inlineStr"/>
-      <c r="AP5" s="40" t="inlineStr"/>
+      <c r="AH5" s="9" t="n"/>
+      <c r="AI5" s="9" t="n"/>
+      <c r="AJ5" s="9" t="n"/>
+      <c r="AK5" s="9" t="n"/>
+      <c r="AL5" s="9" t="n"/>
+      <c r="AM5" s="9" t="n"/>
+      <c r="AN5" s="9" t="n"/>
+      <c r="AO5" s="9" t="n"/>
+      <c r="AP5" s="10" t="n"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -16826,162 +16514,162 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="31" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Binding Energy (E)</t>
         </is>
       </c>
-      <c r="B1" s="31" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Raw Data</t>
         </is>
       </c>
-      <c r="C1" s="31" t="inlineStr"/>
-      <c r="D1" s="31" t="inlineStr"/>
-      <c r="E1" s="31" t="inlineStr"/>
-      <c r="F1" s="31" t="inlineStr">
+      <c r="C1" s="1" t="n"/>
+      <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>BE</t>
         </is>
       </c>
-      <c r="G1" s="31" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Residuals</t>
         </is>
       </c>
-      <c r="H1" s="31" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Background</t>
         </is>
       </c>
-      <c r="I1" s="31" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Calculated Fit</t>
         </is>
       </c>
-      <c r="J1" s="31" t="inlineStr"/>
-      <c r="K1" s="31" t="inlineStr"/>
-      <c r="L1" s="31" t="inlineStr"/>
-      <c r="M1" s="31" t="inlineStr"/>
-      <c r="N1" s="31" t="inlineStr"/>
-      <c r="O1" s="31" t="inlineStr"/>
-      <c r="P1" s="31" t="inlineStr"/>
-      <c r="Q1" s="31" t="inlineStr"/>
-      <c r="R1" s="31" t="inlineStr"/>
-      <c r="S1" s="31" t="inlineStr"/>
-      <c r="T1" s="31" t="inlineStr"/>
-      <c r="U1" s="31" t="inlineStr"/>
-      <c r="V1" s="31" t="inlineStr"/>
-      <c r="W1" s="31" t="inlineStr"/>
-      <c r="X1" s="32" t="inlineStr">
+      <c r="J1" s="1" t="n"/>
+      <c r="K1" s="1" t="n"/>
+      <c r="L1" s="1" t="n"/>
+      <c r="M1" s="1" t="n"/>
+      <c r="N1" s="1" t="n"/>
+      <c r="O1" s="1" t="n"/>
+      <c r="P1" s="1" t="n"/>
+      <c r="Q1" s="1" t="n"/>
+      <c r="R1" s="1" t="n"/>
+      <c r="S1" s="1" t="n"/>
+      <c r="T1" s="1" t="n"/>
+      <c r="U1" s="1" t="n"/>
+      <c r="V1" s="1" t="n"/>
+      <c r="W1" s="1" t="n"/>
+      <c r="X1" s="2" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="Y1" s="33" t="inlineStr">
+      <c r="Y1" s="3" t="inlineStr">
         <is>
           <t>Peak
 Label</t>
         </is>
       </c>
-      <c r="Z1" s="33" t="inlineStr">
+      <c r="Z1" s="3" t="inlineStr">
         <is>
           <t>Position
 (eV)</t>
         </is>
       </c>
-      <c r="AA1" s="33" t="inlineStr">
+      <c r="AA1" s="3" t="inlineStr">
         <is>
           <t>Height
 (CPS)</t>
         </is>
       </c>
-      <c r="AB1" s="33" t="inlineStr">
+      <c r="AB1" s="3" t="inlineStr">
         <is>
           <t>FWHM
 (eV)</t>
         </is>
       </c>
-      <c r="AC1" s="33" t="inlineStr">
+      <c r="AC1" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">σ/γ (%)
 L/G 
 </t>
         </is>
       </c>
-      <c r="AD1" s="33" t="inlineStr">
+      <c r="AD1" s="3" t="inlineStr">
         <is>
           <t>Area
 (CPS.eV)</t>
         </is>
       </c>
-      <c r="AE1" s="33" t="inlineStr">
+      <c r="AE1" s="3" t="inlineStr">
         <is>
           <t>σ
 W_g</t>
         </is>
       </c>
-      <c r="AF1" s="33" t="inlineStr">
+      <c r="AF1" s="3" t="inlineStr">
         <is>
           <t>γ
 W_l</t>
         </is>
       </c>
-      <c r="AG1" s="33" t="inlineStr">
+      <c r="AG1" s="3" t="inlineStr">
         <is>
           <t>W_g
 Skew</t>
         </is>
       </c>
-      <c r="AH1" s="33" t="inlineStr">
+      <c r="AH1" s="3" t="inlineStr">
         <is>
           <t>Conc.
 (%)</t>
         </is>
       </c>
-      <c r="AI1" s="33" t="inlineStr">
+      <c r="AI1" s="3" t="inlineStr">
         <is>
           <t>A/Aᴀ</t>
         </is>
       </c>
-      <c r="AJ1" s="33" t="inlineStr">
+      <c r="AJ1" s="3" t="inlineStr">
         <is>
           <t>Split
 (eV)</t>
         </is>
       </c>
-      <c r="AK1" s="33" t="inlineStr">
+      <c r="AK1" s="3" t="inlineStr">
         <is>
           <t>Fitting Model</t>
         </is>
       </c>
-      <c r="AL1" s="33" t="inlineStr">
+      <c r="AL1" s="3" t="inlineStr">
         <is>
           <t>Bkg Type</t>
         </is>
       </c>
-      <c r="AM1" s="33" t="inlineStr">
+      <c r="AM1" s="3" t="inlineStr">
         <is>
           <t>Bkg Low
 (eV)</t>
         </is>
       </c>
-      <c r="AN1" s="33" t="inlineStr">
+      <c r="AN1" s="3" t="inlineStr">
         <is>
           <t>Bkg High
 (eV)</t>
         </is>
       </c>
-      <c r="AO1" s="33" t="inlineStr">
+      <c r="AO1" s="3" t="inlineStr">
         <is>
           <t>Bkg Offset Low
 (CPS)</t>
         </is>
       </c>
-      <c r="AP1" s="34" t="inlineStr">
+      <c r="AP1" s="4" t="inlineStr">
         <is>
           <t>Bkg Offset High
 (CPS)</t>
@@ -19680,7 +19368,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="6" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
@@ -19690,15 +19378,11 @@
     <col width="14" customWidth="1" min="6" max="6"/>
     <col width="15" customWidth="1" min="7" max="7"/>
     <col width="12" customWidth="1" min="8" max="8"/>
-    <col width="6" customWidth="1" min="9" max="9"/>
-    <col width="6" customWidth="1" min="10" max="10"/>
-    <col width="6" customWidth="1" min="11" max="11"/>
-    <col width="6" customWidth="1" min="12" max="12"/>
+    <col width="6" customWidth="1" min="9" max="12"/>
     <col width="8" customWidth="1" min="13" max="13"/>
     <col width="15" customWidth="1" min="14" max="14"/>
     <col width="23" customWidth="1" min="15" max="15"/>
-    <col width="12" customWidth="1" min="16" max="16"/>
-    <col width="12" customWidth="1" min="17" max="17"/>
+    <col width="12" customWidth="1" min="16" max="17"/>
     <col width="10" customWidth="1" min="18" max="18"/>
     <col width="14" customWidth="1" min="19" max="19"/>
     <col width="15" customWidth="1" min="20" max="20"/>
@@ -19710,172 +19394,171 @@
     <col width="17" customWidth="1" min="26" max="26"/>
     <col width="16" customWidth="1" min="27" max="27"/>
     <col width="17" customWidth="1" min="28" max="28"/>
-    <col width="14" customWidth="1" min="29" max="29"/>
-    <col width="14" customWidth="1" min="30" max="30"/>
+    <col width="14" customWidth="1" min="29" max="30"/>
   </cols>
   <sheetData>
     <row r="2">
-      <c r="B2" s="41" t="inlineStr">
+      <c r="B2" s="11" t="inlineStr">
         <is>
           <t>Peak
 Label</t>
         </is>
       </c>
-      <c r="C2" s="41" t="inlineStr">
+      <c r="C2" s="11" t="inlineStr">
         <is>
           <t>Position
 (eV)</t>
         </is>
       </c>
-      <c r="D2" s="41" t="inlineStr">
+      <c r="D2" s="11" t="inlineStr">
         <is>
           <t>Height
 (CPS)</t>
         </is>
       </c>
-      <c r="E2" s="41" t="inlineStr">
+      <c r="E2" s="11" t="inlineStr">
         <is>
           <t>FWHM
 (eV)</t>
         </is>
       </c>
-      <c r="F2" s="41" t="inlineStr">
+      <c r="F2" s="11" t="inlineStr">
         <is>
           <t>L/G 
 σ/γ (%)</t>
         </is>
       </c>
-      <c r="G2" s="41" t="inlineStr">
+      <c r="G2" s="11" t="inlineStr">
         <is>
           <t>Area
 (CPS.eV)</t>
         </is>
       </c>
-      <c r="H2" s="41" t="inlineStr">
+      <c r="H2" s="11" t="inlineStr">
         <is>
           <t>Atomic
 (%)</t>
         </is>
       </c>
-      <c r="I2" s="41" t="inlineStr">
+      <c r="I2" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="J2" s="41" t="inlineStr">
+      <c r="J2" s="11" t="inlineStr">
         <is>
           <t>RSF</t>
         </is>
       </c>
-      <c r="K2" s="41" t="inlineStr">
+      <c r="K2" s="11" t="inlineStr">
         <is>
           <t>TXFN</t>
         </is>
       </c>
-      <c r="L2" s="41" t="inlineStr">
+      <c r="L2" s="11" t="inlineStr">
         <is>
           <t>ECF</t>
         </is>
       </c>
-      <c r="M2" s="41" t="inlineStr">
+      <c r="M2" s="11" t="inlineStr">
         <is>
           <t>Instr.</t>
         </is>
       </c>
-      <c r="N2" s="41" t="inlineStr">
+      <c r="N2" s="11" t="inlineStr">
         <is>
           <t>Fitting Model</t>
         </is>
       </c>
-      <c r="O2" s="41" t="inlineStr">
+      <c r="O2" s="11" t="inlineStr">
         <is>
           <t>Norm. Area
  An (a.u.)</t>
         </is>
       </c>
-      <c r="P2" s="41" t="inlineStr">
+      <c r="P2" s="11" t="inlineStr">
         <is>
           <t>σ or α
 W_g</t>
         </is>
       </c>
-      <c r="Q2" s="41" t="inlineStr">
+      <c r="Q2" s="11" t="inlineStr">
         <is>
           <t>γ or β
 W_l</t>
         </is>
       </c>
-      <c r="R2" s="41" t="inlineStr">
+      <c r="R2" s="11" t="inlineStr">
         <is>
           <t>Bkg Type</t>
         </is>
       </c>
-      <c r="S2" s="41" t="inlineStr">
+      <c r="S2" s="11" t="inlineStr">
         <is>
           <t>Bkg Low
 (eV)</t>
         </is>
       </c>
-      <c r="T2" s="41" t="inlineStr">
+      <c r="T2" s="11" t="inlineStr">
         <is>
           <t>Bkg High
 (eV)</t>
         </is>
       </c>
-      <c r="U2" s="41" t="inlineStr">
+      <c r="U2" s="11" t="inlineStr">
         <is>
           <t>Bkg Offset Low
 (CPS)</t>
         </is>
       </c>
-      <c r="V2" s="41" t="inlineStr">
+      <c r="V2" s="11" t="inlineStr">
         <is>
           <t>Bkg Offset High
 (CPS)</t>
         </is>
       </c>
-      <c r="W2" s="41" t="inlineStr">
+      <c r="W2" s="11" t="inlineStr">
         <is>
           <t>Sheetname</t>
         </is>
       </c>
-      <c r="X2" s="41" t="inlineStr">
+      <c r="X2" s="11" t="inlineStr">
         <is>
           <t>Position
 Constraint</t>
         </is>
       </c>
-      <c r="Y2" s="41" t="inlineStr">
+      <c r="Y2" s="11" t="inlineStr">
         <is>
           <t>Height
 Constraint</t>
         </is>
       </c>
-      <c r="Z2" s="41" t="inlineStr">
+      <c r="Z2" s="11" t="inlineStr">
         <is>
           <t>FWHM
 Constraint</t>
         </is>
       </c>
-      <c r="AA2" s="41" t="inlineStr">
+      <c r="AA2" s="11" t="inlineStr">
         <is>
           <t>L/G
 Constraint</t>
         </is>
       </c>
-      <c r="AB2" s="41" t="inlineStr">
+      <c r="AB2" s="11" t="inlineStr">
         <is>
           <t>Area
 Constraint</t>
         </is>
       </c>
-      <c r="AC2" s="41" t="inlineStr">
+      <c r="AC2" s="11" t="inlineStr">
         <is>
           <t>σ
 Constraint</t>
         </is>
       </c>
-      <c r="AD2" s="41" t="inlineStr">
+      <c r="AD2" s="11" t="inlineStr">
         <is>
           <t>γ
 Constraint</t>

</xml_diff>

<commit_message>
Try Dark theme for Mac Area screen
</commit_message>
<xml_diff>
--- a/DATA/UKSAF/STO.xlsx
+++ b/DATA/UKSAF/STO.xlsx
@@ -605,6 +605,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -621,7 +624,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="5667375" cy="4086225"/>
+    <ext cx="5648325" cy="4086225"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -635,9 +638,6 @@
       </blipFill>
       <spPr>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:prstDash val="solid"/>
-        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -8780,7 +8780,7 @@
       </c>
       <c r="AA2" s="28" t="inlineStr">
         <is>
-          <t>101367</t>
+          <t>101467</t>
         </is>
       </c>
       <c r="AB2" s="28" t="inlineStr">
@@ -8790,12 +8790,12 @@
       </c>
       <c r="AC2" s="28" t="inlineStr">
         <is>
-          <t>60.05</t>
+          <t>60.28</t>
         </is>
       </c>
       <c r="AD2" s="28" t="inlineStr">
         <is>
-          <t>107901</t>
+          <t>108009</t>
         </is>
       </c>
       <c r="AE2" s="28" t="inlineStr"/>
@@ -8807,7 +8807,7 @@
       </c>
       <c r="AH2" s="28" t="inlineStr">
         <is>
-          <t>59.1</t>
+          <t>59.0</t>
         </is>
       </c>
       <c r="AI2" s="28" t="inlineStr">
@@ -8842,12 +8842,12 @@
       </c>
       <c r="AO2" s="28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="AP2" s="29" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -8962,7 +8962,7 @@
       </c>
       <c r="AA4" s="28" t="inlineStr">
         <is>
-          <t>70265</t>
+          <t>70522</t>
         </is>
       </c>
       <c r="AB4" s="28" t="inlineStr">
@@ -8972,12 +8972,12 @@
       </c>
       <c r="AC4" s="28" t="inlineStr">
         <is>
-          <t>60.04</t>
+          <t>60.27</t>
         </is>
       </c>
       <c r="AD4" s="28" t="inlineStr">
         <is>
-          <t>74795</t>
+          <t>75068</t>
         </is>
       </c>
       <c r="AE4" s="28" t="inlineStr"/>
@@ -8989,12 +8989,12 @@
       </c>
       <c r="AH4" s="28" t="inlineStr">
         <is>
-          <t>40.9</t>
+          <t>41.0</t>
         </is>
       </c>
       <c r="AI4" s="28" t="inlineStr">
         <is>
-          <t>69.3</t>
+          <t>69.5</t>
         </is>
       </c>
       <c r="AJ4" s="28" t="inlineStr">
@@ -9024,12 +9024,12 @@
       </c>
       <c r="AO4" s="28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="AP4" s="29" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
@@ -9607,7 +9607,7 @@
         <v>139.78</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>-3.637978807091713e-12</v>
       </c>
       <c r="H25" t="n">
         <v>26444.7</v>
@@ -9659,7 +9659,7 @@
         <v>139.58</v>
       </c>
       <c r="G27" t="n">
-        <v>-1.818989403545856e-11</v>
+        <v>-2.182787284255028e-11</v>
       </c>
       <c r="H27" t="n">
         <v>26023.2</v>
@@ -9685,19 +9685,19 @@
         <v>139.48</v>
       </c>
       <c r="G28" t="n">
-        <v>-6.548361852765083e-11</v>
+        <v>-7.639755494892597e-11</v>
       </c>
       <c r="H28" t="n">
         <v>27069.8</v>
       </c>
       <c r="I28" t="n">
-        <v>27069.80000000006</v>
+        <v>27069.80000000008</v>
       </c>
       <c r="J28" t="n">
         <v>27069.8</v>
       </c>
       <c r="K28" t="n">
-        <v>27069.80000000006</v>
+        <v>27069.80000000008</v>
       </c>
     </row>
     <row r="29">
@@ -9711,19 +9711,19 @@
         <v>139.38</v>
       </c>
       <c r="G29" t="n">
-        <v>-2.110027708113194e-10</v>
+        <v>-2.510205376893282e-10</v>
       </c>
       <c r="H29" t="n">
         <v>26161.8</v>
       </c>
       <c r="I29" t="n">
-        <v>26161.80000000021</v>
+        <v>26161.80000000025</v>
       </c>
       <c r="J29" t="n">
         <v>26161.8</v>
       </c>
       <c r="K29" t="n">
-        <v>26161.80000000021</v>
+        <v>26161.80000000025</v>
       </c>
     </row>
     <row r="30">
@@ -9737,19 +9737,19 @@
         <v>139.28</v>
       </c>
       <c r="G30" t="n">
-        <v>-6.803020369261503e-10</v>
+        <v>-7.967173587530851e-10</v>
       </c>
       <c r="H30" t="n">
         <v>26300.2</v>
       </c>
       <c r="I30" t="n">
-        <v>26300.20000000068</v>
+        <v>26300.2000000008</v>
       </c>
       <c r="J30" t="n">
         <v>26300.2</v>
       </c>
       <c r="K30" t="n">
-        <v>26300.20000000068</v>
+        <v>26300.2000000008</v>
       </c>
     </row>
     <row r="31">
@@ -9763,19 +9763,19 @@
         <v>139.18</v>
       </c>
       <c r="G31" t="n">
-        <v>-2.135493559762836e-09</v>
+        <v>-2.492015482857823e-09</v>
       </c>
       <c r="H31" t="n">
         <v>26179.2</v>
       </c>
       <c r="I31" t="n">
-        <v>26179.20000000214</v>
+        <v>26179.20000000249</v>
       </c>
       <c r="J31" t="n">
         <v>26179.2</v>
       </c>
       <c r="K31" t="n">
-        <v>26179.20000000214</v>
+        <v>26179.20000000249</v>
       </c>
     </row>
     <row r="32">
@@ -9789,19 +9789,19 @@
         <v>139.08</v>
       </c>
       <c r="G32" t="n">
-        <v>-6.566551746800542e-09</v>
+        <v>-7.621565600857139e-09</v>
       </c>
       <c r="H32" t="n">
         <v>25952.4</v>
       </c>
       <c r="I32" t="n">
-        <v>25952.40000000657</v>
+        <v>25952.40000000762</v>
       </c>
       <c r="J32" t="n">
         <v>25952.4</v>
       </c>
       <c r="K32" t="n">
-        <v>25952.40000000657</v>
+        <v>25952.40000000762</v>
       </c>
     </row>
     <row r="33">
@@ -9815,19 +9815,19 @@
         <v>138.98</v>
       </c>
       <c r="G33" t="n">
-        <v>-1.977241481654346e-08</v>
+        <v>-2.281376509927213e-08</v>
       </c>
       <c r="H33" t="n">
         <v>25823.1</v>
       </c>
       <c r="I33" t="n">
-        <v>25823.10000001977</v>
+        <v>25823.10000002281</v>
       </c>
       <c r="J33" t="n">
         <v>25823.1</v>
       </c>
       <c r="K33" t="n">
-        <v>25823.10000001977</v>
+        <v>25823.10000002282</v>
       </c>
     </row>
     <row r="34">
@@ -9841,19 +9841,19 @@
         <v>138.88</v>
       </c>
       <c r="G34" t="n">
-        <v>-5.828769644722342e-08</v>
+        <v>-6.685513653792441e-08</v>
       </c>
       <c r="H34" t="n">
         <v>25796.2</v>
       </c>
       <c r="I34" t="n">
-        <v>25796.20000005829</v>
+        <v>25796.20000006686</v>
       </c>
       <c r="J34" t="n">
         <v>25796.2</v>
       </c>
       <c r="K34" t="n">
-        <v>25796.20000005829</v>
+        <v>25796.20000006686</v>
       </c>
     </row>
     <row r="35">
@@ -9867,19 +9867,19 @@
         <v>138.78</v>
       </c>
       <c r="G35" t="n">
-        <v>-1.682019501458853e-07</v>
+        <v>-1.918087946251035e-07</v>
       </c>
       <c r="H35" t="n">
         <v>25706.9</v>
       </c>
       <c r="I35" t="n">
-        <v>25706.9000001682</v>
+        <v>25706.90000019181</v>
       </c>
       <c r="J35" t="n">
         <v>25706.9</v>
       </c>
       <c r="K35" t="n">
-        <v>25706.9000001682</v>
+        <v>25706.90000019181</v>
       </c>
     </row>
     <row r="36">
@@ -9893,19 +9893,19 @@
         <v>138.68</v>
       </c>
       <c r="G36" t="n">
-        <v>-4.752000677399337e-07</v>
+        <v>-5.387992132455111e-07</v>
       </c>
       <c r="H36" t="n">
         <v>25865.6</v>
       </c>
       <c r="I36" t="n">
-        <v>25865.6000004752</v>
+        <v>25865.6000005388</v>
       </c>
       <c r="J36" t="n">
         <v>25865.6</v>
       </c>
       <c r="K36" t="n">
-        <v>25865.60000047519</v>
+        <v>25865.6000005388</v>
       </c>
     </row>
     <row r="37">
@@ -9919,19 +9919,19 @@
         <v>138.58</v>
       </c>
       <c r="G37" t="n">
-        <v>-1.314339897362515e-06</v>
+        <v>-1.481937943026423e-06</v>
       </c>
       <c r="H37" t="n">
         <v>26150.6</v>
       </c>
       <c r="I37" t="n">
-        <v>26150.60000131434</v>
+        <v>26150.60000148194</v>
       </c>
       <c r="J37" t="n">
         <v>26150.6</v>
       </c>
       <c r="K37" t="n">
-        <v>26150.60000131433</v>
+        <v>26150.60000148194</v>
       </c>
     </row>
     <row r="38">
@@ -9945,19 +9945,19 @@
         <v>138.48</v>
       </c>
       <c r="G38" t="n">
-        <v>-3.559161996236071e-06</v>
+        <v>-3.99112468585372e-06</v>
       </c>
       <c r="H38" t="n">
         <v>25610.5</v>
       </c>
       <c r="I38" t="n">
-        <v>25610.50000355916</v>
+        <v>25610.50000399112</v>
       </c>
       <c r="J38" t="n">
         <v>25610.5</v>
       </c>
       <c r="K38" t="n">
-        <v>25610.50000355915</v>
+        <v>25610.50000399115</v>
       </c>
     </row>
     <row r="39">
@@ -9971,19 +9971,19 @@
         <v>138.38</v>
       </c>
       <c r="G39" t="n">
-        <v>-9.436604159418494e-06</v>
+        <v>-1.052554216585122e-05</v>
       </c>
       <c r="H39" t="n">
         <v>25614.3</v>
       </c>
       <c r="I39" t="n">
-        <v>25614.3000094366</v>
+        <v>25614.30001052554</v>
       </c>
       <c r="J39" t="n">
         <v>25614.3</v>
       </c>
       <c r="K39" t="n">
-        <v>25614.30000943657</v>
+        <v>25614.30001052559</v>
       </c>
     </row>
     <row r="40">
@@ -9997,19 +9997,19 @@
         <v>138.28</v>
       </c>
       <c r="G40" t="n">
-        <v>-2.449806561344303e-05</v>
+        <v>-2.718298128456809e-05</v>
       </c>
       <c r="H40" t="n">
         <v>25482.4</v>
       </c>
       <c r="I40" t="n">
-        <v>25482.40002449807</v>
+        <v>25482.40002718298</v>
       </c>
       <c r="J40" t="n">
         <v>25482.4</v>
       </c>
       <c r="K40" t="n">
-        <v>25482.40002449799</v>
+        <v>25482.40002718311</v>
       </c>
     </row>
     <row r="41">
@@ -10023,19 +10023,19 @@
         <v>138.18</v>
       </c>
       <c r="G41" t="n">
-        <v>-6.227557969396003e-05</v>
+        <v>-6.875037797726691e-05</v>
       </c>
       <c r="H41" t="n">
         <v>25820.7</v>
       </c>
       <c r="I41" t="n">
-        <v>25820.70006227558</v>
+        <v>25820.70006875038</v>
       </c>
       <c r="J41" t="n">
         <v>25820.7</v>
       </c>
       <c r="K41" t="n">
-        <v>25820.70006227539</v>
+        <v>25820.70006875069</v>
       </c>
     </row>
     <row r="42">
@@ -10049,19 +10049,19 @@
         <v>138.08</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.0001550233246234711</v>
+        <v>-0.0001702950066828635</v>
       </c>
       <c r="H42" t="n">
         <v>25337.9</v>
       </c>
       <c r="I42" t="n">
-        <v>25337.90015502333</v>
+        <v>25337.90017029501</v>
       </c>
       <c r="J42" t="n">
         <v>25337.9</v>
       </c>
       <c r="K42" t="n">
-        <v>25337.90015502286</v>
+        <v>25337.90017029579</v>
       </c>
     </row>
     <row r="43">
@@ -10075,19 +10075,19 @@
         <v>137.98</v>
       </c>
       <c r="G43" t="n">
-        <v>-0.0003779153521463741</v>
+        <v>-0.0004131450368731748</v>
       </c>
       <c r="H43" t="n">
         <v>25660.4</v>
       </c>
       <c r="I43" t="n">
-        <v>25660.40037791535</v>
+        <v>25660.40041314504</v>
       </c>
       <c r="J43" t="n">
         <v>25660.40000000001</v>
       </c>
       <c r="K43" t="n">
-        <v>25660.40037791421</v>
+        <v>25660.40041314692</v>
       </c>
     </row>
     <row r="44">
@@ -10101,19 +10101,19 @@
         <v>137.88</v>
       </c>
       <c r="G44" t="n">
-        <v>-0.0009022710291901603</v>
+        <v>-0.0009817563841352239</v>
       </c>
       <c r="H44" t="n">
         <v>25130.5</v>
       </c>
       <c r="I44" t="n">
-        <v>25130.50090227103</v>
+        <v>25130.50098175638</v>
       </c>
       <c r="J44" t="n">
-        <v>25130.50000000001</v>
+        <v>25130.50000000002</v>
       </c>
       <c r="K44" t="n">
-        <v>25130.5009022683</v>
+        <v>25130.50098176086</v>
       </c>
     </row>
     <row r="45">
@@ -10127,19 +10127,19 @@
         <v>137.78</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.002109857858158648</v>
+        <v>-0.002285252725414466</v>
       </c>
       <c r="H45" t="n">
         <v>25320.6</v>
       </c>
       <c r="I45" t="n">
-        <v>25320.60210985786</v>
+        <v>25320.60228525272</v>
       </c>
       <c r="J45" t="n">
-        <v>25320.60000000005</v>
+        <v>25320.60000000006</v>
       </c>
       <c r="K45" t="n">
-        <v>25320.60210985146</v>
+        <v>25320.60228526311</v>
       </c>
     </row>
     <row r="46">
@@ -10153,19 +10153,19 @@
         <v>137.68</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.004832523052755278</v>
+        <v>-0.005211046103795525</v>
       </c>
       <c r="H46" t="n">
         <v>24983.9</v>
       </c>
       <c r="I46" t="n">
-        <v>24983.90483252305</v>
+        <v>24983.90521104611</v>
       </c>
       <c r="J46" t="n">
-        <v>24983.90000000017</v>
+        <v>24983.9000000002</v>
       </c>
       <c r="K46" t="n">
-        <v>24983.90483250835</v>
+        <v>24983.90521106973</v>
       </c>
     </row>
     <row r="47">
@@ -10179,19 +10179,19 @@
         <v>137.58</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.01084257436741609</v>
+        <v>-0.01164150121985585</v>
       </c>
       <c r="H47" t="n">
         <v>25008</v>
       </c>
       <c r="I47" t="n">
-        <v>25008.01084257437</v>
+        <v>25008.01164150122</v>
       </c>
       <c r="J47" t="n">
-        <v>25008.00000000055</v>
+        <v>25008.00000000065</v>
       </c>
       <c r="K47" t="n">
-        <v>25008.01084254121</v>
+        <v>25008.01164155378</v>
       </c>
     </row>
     <row r="48">
@@ -10205,19 +10205,19 @@
         <v>137.48</v>
       </c>
       <c r="G48" t="n">
-        <v>-0.02383221316631534</v>
+        <v>-0.02548133834716282</v>
       </c>
       <c r="H48" t="n">
         <v>24993.3</v>
       </c>
       <c r="I48" t="n">
-        <v>24993.32383221317</v>
+        <v>24993.32548133835</v>
       </c>
       <c r="J48" t="n">
-        <v>24993.30000000175</v>
+        <v>24993.30000000205</v>
       </c>
       <c r="K48" t="n">
-        <v>24993.32383213976</v>
+        <v>24993.32548145278</v>
       </c>
     </row>
     <row r="49">
@@ -10231,19 +10231,19 @@
         <v>137.38</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.05132257025616127</v>
+        <v>-0.05465164764609654</v>
       </c>
       <c r="H49" t="n">
         <v>25038.8</v>
       </c>
       <c r="I49" t="n">
-        <v>25038.85132257026</v>
+        <v>25038.85465164765</v>
       </c>
       <c r="J49" t="n">
-        <v>25038.80000000545</v>
+        <v>25038.80000000633</v>
       </c>
       <c r="K49" t="n">
-        <v>25038.8513224105</v>
+        <v>25038.85465189113</v>
       </c>
     </row>
     <row r="50">
@@ -10257,19 +10257,19 @@
         <v>137.28</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.1082944359477551</v>
+        <v>-0.1148666006592975</v>
       </c>
       <c r="H50" t="n">
         <v>24708.8</v>
       </c>
       <c r="I50" t="n">
-        <v>24708.90829443595</v>
+        <v>24708.91486660066</v>
       </c>
       <c r="J50" t="n">
-        <v>24708.80000001658</v>
+        <v>24708.80000001914</v>
       </c>
       <c r="K50" t="n">
-        <v>24708.90829409377</v>
+        <v>24708.91486710659</v>
       </c>
     </row>
     <row r="51">
@@ -10283,19 +10283,19 @@
         <v>137.18</v>
       </c>
       <c r="G51" t="n">
-        <v>-0.2239250516613538</v>
+        <v>24.53005351460524</v>
       </c>
       <c r="H51" t="n">
-        <v>24696.9</v>
+        <v>24672.13333333333</v>
       </c>
       <c r="I51" t="n">
-        <v>24697.12392505166</v>
+        <v>24672.3699464854</v>
       </c>
       <c r="J51" t="n">
-        <v>24696.9000000494</v>
+        <v>24672.13333339001</v>
       </c>
       <c r="K51" t="n">
-        <v>24697.12392432901</v>
+        <v>24672.3699475103</v>
       </c>
     </row>
     <row r="52">
@@ -10309,19 +10309,19 @@
         <v>137.08</v>
       </c>
       <c r="G52" t="n">
-        <v>-0.4537815537660208</v>
+        <v>-3.985933482799737</v>
       </c>
       <c r="H52" t="n">
-        <v>24663.5</v>
+        <v>24667.00819802785</v>
       </c>
       <c r="I52" t="n">
-        <v>24663.95378155377</v>
+        <v>24667.4859334828</v>
       </c>
       <c r="J52" t="n">
-        <v>24663.50000014404</v>
+        <v>24667.00819819214</v>
       </c>
       <c r="K52" t="n">
-        <v>24663.95378004539</v>
+        <v>24667.48593550229</v>
       </c>
     </row>
     <row r="53">
@@ -10335,19 +10335,19 @@
         <v>136.98</v>
       </c>
       <c r="G53" t="n">
-        <v>-0.9013460488313285</v>
+        <v>-11.9481581258915</v>
       </c>
       <c r="H53" t="n">
-        <v>24656</v>
+        <v>24667.0025905701</v>
       </c>
       <c r="I53" t="n">
-        <v>24656.90134604883</v>
+        <v>24667.94815812589</v>
       </c>
       <c r="J53" t="n">
-        <v>24656.00000041117</v>
+        <v>24667.00259103639</v>
       </c>
       <c r="K53" t="n">
-        <v>24656.90134292767</v>
+        <v>24667.9481619819</v>
       </c>
     </row>
     <row r="54">
@@ -10361,19 +10361,19 @@
         <v>136.88</v>
       </c>
       <c r="G54" t="n">
-        <v>-1.755069610378996</v>
+        <v>-85.84145719955632</v>
       </c>
       <c r="H54" t="n">
-        <v>24583</v>
+        <v>24667.00656006446</v>
       </c>
       <c r="I54" t="n">
-        <v>24584.75506961038</v>
+        <v>24668.84145719956</v>
       </c>
       <c r="J54" t="n">
-        <v>24583.00000114907</v>
+        <v>24667.00656136022</v>
       </c>
       <c r="K54" t="n">
-        <v>24584.7550631845</v>
+        <v>24668.8414642913</v>
       </c>
     </row>
     <row r="55">
@@ -10387,19 +10387,19 @@
         <v>136.78</v>
       </c>
       <c r="G55" t="n">
-        <v>-3.350562330550019</v>
+        <v>-393.9238112547064</v>
       </c>
       <c r="H55" t="n">
-        <v>24276.6</v>
+        <v>24667.0323474314</v>
       </c>
       <c r="I55" t="n">
-        <v>24279.95056233055</v>
+        <v>24670.5238112547</v>
       </c>
       <c r="J55" t="n">
-        <v>24276.60000314396</v>
+        <v>24667.03235095715</v>
       </c>
       <c r="K55" t="n">
-        <v>24279.95054911277</v>
+        <v>24670.52382368879</v>
       </c>
     </row>
     <row r="56">
@@ -10413,19 +10413,19 @@
         <v>136.68</v>
       </c>
       <c r="G56" t="n">
-        <v>-100.4390071489324</v>
+        <v>132.7262302915478</v>
       </c>
       <c r="H56" t="n">
-        <v>24900.56666666667</v>
+        <v>24667.15826383816</v>
       </c>
       <c r="I56" t="n">
-        <v>24906.83900714893</v>
+        <v>24673.67376970845</v>
       </c>
       <c r="J56" t="n">
-        <v>24900.56667508888</v>
+        <v>24667.15827323223</v>
       </c>
       <c r="K56" t="n">
-        <v>24906.8389798683</v>
+        <v>24673.67379009739</v>
       </c>
     </row>
     <row r="57">
@@ -10439,19 +10439,19 @@
         <v>136.58</v>
       </c>
       <c r="G57" t="n">
-        <v>332.8547987293823</v>
+        <v>559.8498043727486</v>
       </c>
       <c r="H57" t="n">
-        <v>24894.62913533802</v>
+        <v>24667.22384272402</v>
       </c>
       <c r="I57" t="n">
-        <v>24906.14520127062</v>
+        <v>24679.15019562725</v>
       </c>
       <c r="J57" t="n">
-        <v>24894.62915742907</v>
+        <v>24667.22386723455</v>
       </c>
       <c r="K57" t="n">
-        <v>24906.14514455544</v>
+        <v>24679.15022563316</v>
       </c>
     </row>
     <row r="58">
@@ -10465,19 +10465,19 @@
         <v>136.48</v>
       </c>
       <c r="G58" t="n">
-        <v>-258.9879532600644</v>
+        <v>-32.15224642790054</v>
       </c>
       <c r="H58" t="n">
-        <v>24894.54732748214</v>
+        <v>24667.03484158406</v>
       </c>
       <c r="I58" t="n">
-        <v>24915.28795326006</v>
+        <v>24688.4522464279</v>
       </c>
       <c r="J58" t="n">
-        <v>24894.54738421927</v>
+        <v>24667.03490421197</v>
       </c>
       <c r="K58" t="n">
-        <v>24915.28783416449</v>
+        <v>24688.45228170067</v>
       </c>
     </row>
     <row r="59">
@@ -10491,19 +10491,19 @@
         <v>136.38</v>
       </c>
       <c r="G59" t="n">
-        <v>-446.6634494853315</v>
+        <v>-220.1276171326463</v>
       </c>
       <c r="H59" t="n">
-        <v>24894.51374319724</v>
+        <v>24666.88659774413</v>
       </c>
       <c r="I59" t="n">
-        <v>24931.16344948533</v>
+        <v>24704.62761713265</v>
       </c>
       <c r="J59" t="n">
-        <v>24894.51388589007</v>
+        <v>24666.88675446344</v>
       </c>
       <c r="K59" t="n">
-        <v>24931.16319660251</v>
+        <v>24704.62763293004</v>
       </c>
     </row>
     <row r="60">
@@ -10517,19 +10517,19 @@
         <v>136.28</v>
       </c>
       <c r="G60" t="n">
-        <v>149.9200752541183</v>
+        <v>375.988135177915</v>
       </c>
       <c r="H60" t="n">
-        <v>24894.72554721501</v>
+        <v>24666.93735574661</v>
       </c>
       <c r="I60" t="n">
-        <v>24958.27992474588</v>
+        <v>24732.21186482209</v>
       </c>
       <c r="J60" t="n">
-        <v>24894.72589864995</v>
+        <v>24666.93773984336</v>
       </c>
       <c r="K60" t="n">
-        <v>24958.27938223124</v>
+        <v>24732.21177909817</v>
       </c>
     </row>
     <row r="61">
@@ -10543,19 +10543,19 @@
         <v>136.18</v>
       </c>
       <c r="G61" t="n">
-        <v>-46.77008266640041</v>
+        <v>178.5013478604451</v>
       </c>
       <c r="H61" t="n">
-        <v>24894.78925955672</v>
+        <v>24666.86782124567</v>
       </c>
       <c r="I61" t="n">
-        <v>25002.9700826664</v>
+        <v>24777.69865213956</v>
       </c>
       <c r="J61" t="n">
-        <v>24894.79010721634</v>
+        <v>24666.86874328218</v>
       </c>
       <c r="K61" t="n">
-        <v>25002.9689097579</v>
+        <v>24777.69823671292</v>
       </c>
     </row>
     <row r="62">
@@ -10569,19 +10569,19 @@
         <v>136.08</v>
       </c>
       <c r="G62" t="n">
-        <v>30.00152366020848</v>
+        <v>254.0373011945594</v>
       </c>
       <c r="H62" t="n">
-        <v>24894.69913285868</v>
+        <v>24666.67341136685</v>
       </c>
       <c r="I62" t="n">
-        <v>25075.49847633979</v>
+        <v>24851.46269880544</v>
       </c>
       <c r="J62" t="n">
-        <v>24894.70113529892</v>
+        <v>24666.67557943383</v>
       </c>
       <c r="K62" t="n">
-        <v>25075.49593032718</v>
+        <v>24851.46137540675</v>
       </c>
     </row>
     <row r="63">
@@ -10595,19 +10595,19 @@
         <v>135.98</v>
       </c>
       <c r="G63" t="n">
-        <v>734.7315796640469</v>
+        <v>956.9911474660912</v>
       </c>
       <c r="H63" t="n">
-        <v>24894.6083463169</v>
+        <v>24666.47819827395</v>
       </c>
       <c r="I63" t="n">
-        <v>25191.36842033595</v>
+        <v>24969.10885253391</v>
       </c>
       <c r="J63" t="n">
-        <v>24894.61297960065</v>
+        <v>24666.48319222357</v>
       </c>
       <c r="K63" t="n">
-        <v>25191.36289485883</v>
+        <v>24969.10524188694</v>
       </c>
     </row>
     <row r="64">
@@ -10621,19 +10621,19 @@
         <v>135.88</v>
       </c>
       <c r="G64" t="n">
-        <v>461.6756996923941</v>
+        <v>681.4102218081462</v>
       </c>
       <c r="H64" t="n">
-        <v>24894.19968064029</v>
+        <v>24666.02494443865</v>
       </c>
       <c r="I64" t="n">
-        <v>25372.72430030761</v>
+        <v>25152.98977819186</v>
       </c>
       <c r="J64" t="n">
-        <v>24894.21018190218</v>
+        <v>24666.03621367567</v>
       </c>
       <c r="K64" t="n">
-        <v>25372.71236041928</v>
+        <v>25152.98073479908</v>
       </c>
     </row>
     <row r="65">
@@ -10647,19 +10647,19 @@
         <v>135.78</v>
       </c>
       <c r="G65" t="n">
-        <v>676.6708834917845</v>
+        <v>892.9886600440768</v>
       </c>
       <c r="H65" t="n">
-        <v>24893.55214993827</v>
+        <v>24665.37783824218</v>
       </c>
       <c r="I65" t="n">
-        <v>25651.82911650822</v>
+        <v>25435.51133995592</v>
       </c>
       <c r="J65" t="n">
-        <v>24893.57546581646</v>
+        <v>24665.40275308979</v>
       </c>
       <c r="K65" t="n">
-        <v>25651.80352103328</v>
+        <v>25435.48994519465</v>
       </c>
     </row>
     <row r="66">
@@ -10673,19 +10673,19 @@
         <v>135.68</v>
       </c>
       <c r="G66" t="n">
-        <v>686.7536837326006</v>
+        <v>898.6287509427493</v>
       </c>
       <c r="H66" t="n">
-        <v>24892.77102107914</v>
+        <v>24664.62211073711</v>
       </c>
       <c r="I66" t="n">
-        <v>26073.9463162674</v>
+        <v>25862.07124905725</v>
       </c>
       <c r="J66" t="n">
-        <v>24892.82173846836</v>
+        <v>24664.67608323047</v>
       </c>
       <c r="K66" t="n">
-        <v>26073.89204808231</v>
+        <v>25862.02274963054</v>
       </c>
     </row>
     <row r="67">
@@ -10699,19 +10699,19 @@
         <v>135.58</v>
       </c>
       <c r="G67" t="n">
-        <v>354.6571137157443</v>
+        <v>560.8964242282127</v>
       </c>
       <c r="H67" t="n">
-        <v>24891.68546797722</v>
+        <v>24663.6193376343</v>
       </c>
       <c r="I67" t="n">
-        <v>26700.94288628425</v>
+        <v>26494.70357577179</v>
       </c>
       <c r="J67" t="n">
-        <v>24891.79356081132</v>
+        <v>24663.73390933783</v>
       </c>
       <c r="K67" t="n">
-        <v>26700.829354867</v>
+        <v>26494.59737286896</v>
       </c>
     </row>
     <row r="68">
@@ -10725,19 +10725,19 @@
         <v>135.48</v>
       </c>
       <c r="G68" t="n">
-        <v>332.8270901576179</v>
+        <v>532.151169513796</v>
       </c>
       <c r="H68" t="n">
-        <v>24890.35894127158</v>
+        <v>24662.4208121315</v>
       </c>
       <c r="I68" t="n">
-        <v>27616.27290984238</v>
+        <v>27416.9488304862</v>
       </c>
       <c r="J68" t="n">
-        <v>24890.58468471638</v>
+        <v>24662.65916274437</v>
       </c>
       <c r="K68" t="n">
-        <v>27616.03897303929</v>
+        <v>27416.72306844352</v>
       </c>
     </row>
     <row r="69">
@@ -10751,19 +10751,19 @@
         <v>135.38</v>
       </c>
       <c r="G69" t="n">
-        <v>-211.3872023410222</v>
+        <v>-20.33854386179883</v>
       </c>
       <c r="H69" t="n">
-        <v>24888.6389861754</v>
+        <v>24660.90278736936</v>
       </c>
       <c r="I69" t="n">
-        <v>28929.28720234102</v>
+        <v>28738.2385438618</v>
       </c>
       <c r="J69" t="n">
-        <v>24889.10100377785</v>
+        <v>24661.38878722521</v>
       </c>
       <c r="K69" t="n">
-        <v>28928.81304100664</v>
+        <v>28737.77117648587</v>
       </c>
     </row>
     <row r="70">
@@ -10777,19 +10777,19 @@
         <v>135.28</v>
       </c>
       <c r="G70" t="n">
-        <v>-62.21899133045372</v>
+        <v>119.1531742164261</v>
       </c>
       <c r="H70" t="n">
-        <v>24886.36608769868</v>
+        <v>24658.93552592162</v>
       </c>
       <c r="I70" t="n">
-        <v>30779.81899133045</v>
+        <v>30598.44682578357</v>
       </c>
       <c r="J70" t="n">
-        <v>24887.29287027592</v>
+        <v>24659.90690303612</v>
       </c>
       <c r="K70" t="n">
-        <v>30778.87449931884</v>
+        <v>30597.50258788775</v>
       </c>
     </row>
     <row r="71">
@@ -10803,19 +10803,19 @@
         <v>135.18</v>
       </c>
       <c r="G71" t="n">
-        <v>-560.7351102063985</v>
+        <v>-390.516074667561</v>
       </c>
       <c r="H71" t="n">
-        <v>24883.1718466034</v>
+        <v>24656.21991522051</v>
       </c>
       <c r="I71" t="n">
-        <v>33340.5351102064</v>
+        <v>33170.31607466756</v>
       </c>
       <c r="J71" t="n">
-        <v>24884.99418208534</v>
+        <v>24658.12330043115</v>
       </c>
       <c r="K71" t="n">
-        <v>33338.68736616999</v>
+        <v>33168.45158687868</v>
       </c>
     </row>
     <row r="72">
@@ -10829,19 +10829,19 @@
         <v>135.08</v>
       </c>
       <c r="G72" t="n">
-        <v>-264.7706989272338</v>
+        <v>-107.3474697287966</v>
       </c>
       <c r="H72" t="n">
-        <v>24878.62046728603</v>
+        <v>24652.40202093919</v>
       </c>
       <c r="I72" t="n">
-        <v>36814.87069892723</v>
+        <v>36657.4474697288</v>
       </c>
       <c r="J72" t="n">
-        <v>24882.13340030307</v>
+        <v>24656.05891709149</v>
       </c>
       <c r="K72" t="n">
-        <v>36811.32191574843</v>
+        <v>36653.84540873786</v>
       </c>
     </row>
     <row r="73">
@@ -10855,19 +10855,19 @@
         <v>134.98</v>
       </c>
       <c r="G73" t="n">
-        <v>-103.7839338999474</v>
+        <v>38.78597678784718</v>
       </c>
       <c r="H73" t="n">
-        <v>24872.1065261805</v>
+        <v>24646.9900169195</v>
       </c>
       <c r="I73" t="n">
-        <v>41424.28393389995</v>
+        <v>41281.71402321215</v>
       </c>
       <c r="J73" t="n">
-        <v>24878.74651965537</v>
+        <v>24653.87988574691</v>
       </c>
       <c r="K73" t="n">
-        <v>41417.59424536196</v>
+        <v>41274.90011585334</v>
       </c>
     </row>
     <row r="74">
@@ -10881,19 +10881,19 @@
         <v>134.88</v>
       </c>
       <c r="G74" t="n">
-        <v>-6.167451255474589</v>
+        <v>118.624065561271</v>
       </c>
       <c r="H74" t="n">
-        <v>24862.70830589002</v>
+        <v>24639.23612834462</v>
       </c>
       <c r="I74" t="n">
-        <v>47374.86745125547</v>
+        <v>47250.07593443873</v>
       </c>
       <c r="J74" t="n">
-        <v>24875.01645117073</v>
+        <v>24651.96801358289</v>
       </c>
       <c r="K74" t="n">
-        <v>47362.49175210547</v>
+        <v>47237.44726225547</v>
       </c>
     </row>
     <row r="75">
@@ -10907,19 +10907,19 @@
         <v>134.78</v>
       </c>
       <c r="G75" t="n">
-        <v>756.2102008324437</v>
+        <v>858.9491362543631</v>
       </c>
       <c r="H75" t="n">
-        <v>24849.60893920939</v>
+        <v>24628.47699128988</v>
       </c>
       <c r="I75" t="n">
-        <v>54788.08979916756</v>
+        <v>54685.35086374564</v>
       </c>
       <c r="J75" t="n">
-        <v>24871.98697563953</v>
+        <v>24651.55696303898</v>
       </c>
       <c r="K75" t="n">
-        <v>54765.62198837045</v>
+        <v>54662.4080249587</v>
       </c>
     </row>
     <row r="76">
@@ -10933,19 +10933,19 @@
         <v>134.68</v>
       </c>
       <c r="G76" t="n">
-        <v>-184.3446500321807</v>
+        <v>-109.6388987957689</v>
       </c>
       <c r="H76" t="n">
-        <v>24831.61933330123</v>
+        <v>24613.7488806858</v>
       </c>
       <c r="I76" t="n">
-        <v>63576.24465003218</v>
+        <v>63501.53889879577</v>
       </c>
       <c r="J76" t="n">
-        <v>24871.53467124509</v>
+        <v>24654.79979739772</v>
       </c>
       <c r="K76" t="n">
-        <v>63536.21324840835</v>
+        <v>63460.66527939703</v>
       </c>
     </row>
     <row r="77">
@@ -10959,19 +10959,19 @@
         <v>134.58</v>
       </c>
       <c r="G77" t="n">
-        <v>410.6264289124665</v>
+        <v>450.3887955897953</v>
       </c>
       <c r="H77" t="n">
-        <v>24808.03455595038</v>
+        <v>24594.48020364359</v>
       </c>
       <c r="I77" t="n">
-        <v>73263.27357108753</v>
+        <v>73223.5112044102</v>
       </c>
       <c r="J77" t="n">
-        <v>24877.89600304213</v>
+        <v>24666.13530823815</v>
       </c>
       <c r="K77" t="n">
-        <v>73193.26718418344</v>
+        <v>73152.07758013647</v>
       </c>
     </row>
     <row r="78">
@@ -10985,19 +10985,19 @@
         <v>134.48</v>
       </c>
       <c r="G78" t="n">
-        <v>710.8247961410816</v>
+        <v>710.4133964409557</v>
       </c>
       <c r="H78" t="n">
-        <v>24778.01963763617</v>
+        <v>24569.99433605436</v>
       </c>
       <c r="I78" t="n">
-        <v>82808.37520385892</v>
+        <v>82808.78660355904</v>
       </c>
       <c r="J78" t="n">
-        <v>24898.02886046728</v>
+        <v>24692.76869671101</v>
       </c>
       <c r="K78" t="n">
-        <v>82688.19278829636</v>
+        <v>82686.27707375004</v>
       </c>
     </row>
     <row r="79">
@@ -11011,19 +11011,19 @@
         <v>134.38</v>
       </c>
       <c r="G79" t="n">
-        <v>693.4946671054349</v>
+        <v>653.9273549218633</v>
       </c>
       <c r="H79" t="n">
-        <v>24740.93265585333</v>
+        <v>24539.77423357409</v>
       </c>
       <c r="I79" t="n">
-        <v>90608.20533289456</v>
+        <v>90647.77264507813</v>
       </c>
       <c r="J79" t="n">
-        <v>24943.31776559377</v>
+        <v>24746.31814560902</v>
       </c>
       <c r="K79" t="n">
-        <v>90405.62434790848</v>
+        <v>90441.52858974879</v>
       </c>
     </row>
     <row r="80">
@@ -11037,19 +11037,19 @@
         <v>134.28</v>
       </c>
       <c r="G80" t="n">
-        <v>-1042.187542271509</v>
+        <v>-1109.856424231111</v>
       </c>
       <c r="H80" t="n">
-        <v>24697.86006666808</v>
+        <v>24504.70554666781</v>
       </c>
       <c r="I80" t="n">
-        <v>94905.28754227152</v>
+        <v>94972.95642423112</v>
       </c>
       <c r="J80" t="n">
-        <v>25033.01482754154</v>
+        <v>24845.95947264163</v>
       </c>
       <c r="K80" t="n">
-        <v>94569.92527543604</v>
+        <v>94632.02076623341</v>
       </c>
     </row>
     <row r="81">
@@ -11063,19 +11063,19 @@
         <v>134.18</v>
       </c>
       <c r="G81" t="n">
-        <v>286.252859031636</v>
+        <v>209.4728408498049</v>
       </c>
       <c r="H81" t="n">
-        <v>24651.44939113206</v>
+        <v>24466.93697786327</v>
       </c>
       <c r="I81" t="n">
-        <v>94582.24714096836</v>
+        <v>94659.0271591502</v>
       </c>
       <c r="J81" t="n">
-        <v>25196.62861638377</v>
+        <v>25020.83275867673</v>
       </c>
       <c r="K81" t="n">
-        <v>94036.8634852816</v>
+        <v>94105.44598470631</v>
       </c>
     </row>
     <row r="82">
@@ -11089,19 +11089,19 @@
         <v>134.08</v>
       </c>
       <c r="G82" t="n">
-        <v>-331.1192930475227</v>
+        <v>-398.6019033565244</v>
       </c>
       <c r="H82" t="n">
-        <v>24604.34702726177</v>
+        <v>24428.61668258791</v>
       </c>
       <c r="I82" t="n">
-        <v>89820.01929304752</v>
+        <v>89887.50190335652</v>
       </c>
       <c r="J82" t="n">
-        <v>25475.6950446576</v>
+        <v>25312.09422438189</v>
       </c>
       <c r="K82" t="n">
-        <v>88948.48450641985</v>
+        <v>89004.31361323496</v>
       </c>
     </row>
     <row r="83">
@@ -11115,19 +11115,19 @@
         <v>133.98</v>
       </c>
       <c r="G83" t="n">
-        <v>-361.6692045980599</v>
+        <v>-409.5962394862145</v>
       </c>
       <c r="H83" t="n">
-        <v>24559.63698219865</v>
+        <v>24392.24715731102</v>
       </c>
       <c r="I83" t="n">
-        <v>82017.36920459806</v>
+        <v>82065.29623948621</v>
       </c>
       <c r="J83" t="n">
-        <v>25928.43371782625</v>
+        <v>25777.46225494104</v>
       </c>
       <c r="K83" t="n">
-        <v>80648.41433938833</v>
+        <v>80680.32914246939</v>
       </c>
     </row>
     <row r="84">
@@ -11141,19 +11141,19 @@
         <v>133.88</v>
       </c>
       <c r="G84" t="n">
-        <v>-192.0690764863684</v>
+        <v>-219.2718542125367</v>
       </c>
       <c r="H84" t="n">
-        <v>24520.03242620261</v>
+        <v>24360.02645054711</v>
       </c>
       <c r="I84" t="n">
-        <v>73053.16907648637</v>
+        <v>73080.37185421254</v>
       </c>
       <c r="J84" t="n">
-        <v>26634.10076528286</v>
+        <v>26495.68480524588</v>
       </c>
       <c r="K84" t="n">
-        <v>70938.97740278592</v>
+        <v>70944.91210902992</v>
       </c>
     </row>
     <row r="85">
@@ -11167,19 +11167,19 @@
         <v>133.78</v>
       </c>
       <c r="G85" t="n">
-        <v>677.5359808538851</v>
+        <v>666.9706596469259</v>
       </c>
       <c r="H85" t="n">
-        <v>24486.31724147462</v>
+        <v>24332.58834655982</v>
       </c>
       <c r="I85" t="n">
-        <v>64550.46401914611</v>
+        <v>64561.02934035307</v>
       </c>
       <c r="J85" t="n">
-        <v>27697.49308924663</v>
+        <v>27571.30157582561</v>
       </c>
       <c r="K85" t="n">
-        <v>61339.20202074437</v>
+        <v>61322.46345734411</v>
       </c>
     </row>
     <row r="86">
@@ -11193,19 +11193,19 @@
         <v>133.68</v>
       </c>
       <c r="G86" t="n">
-        <v>252.6643567696883</v>
+        <v>253.643571180015</v>
       </c>
       <c r="H86" t="n">
-        <v>24458.20250478422</v>
+        <v>24309.69741496748</v>
       </c>
       <c r="I86" t="n">
-        <v>57572.33564323031</v>
+        <v>57571.35642881999</v>
       </c>
       <c r="J86" t="n">
-        <v>29256.52556372027</v>
+        <v>29142.02064913041</v>
       </c>
       <c r="K86" t="n">
-        <v>52773.96428604733</v>
+        <v>52739.13071421302</v>
       </c>
     </row>
     <row r="87">
@@ -11219,19 +11219,19 @@
         <v>133.58</v>
       </c>
       <c r="G87" t="n">
-        <v>21.78739297349966</v>
+        <v>30.51771542183269</v>
       </c>
       <c r="H87" t="n">
-        <v>24434.98838575283</v>
+        <v>24290.78484309785</v>
       </c>
       <c r="I87" t="n">
-        <v>52683.4126070265</v>
+        <v>52674.68228457816</v>
       </c>
       <c r="J87" t="n">
-        <v>31489.62945712797</v>
+        <v>31385.96658206957</v>
       </c>
       <c r="K87" t="n">
-        <v>45628.76197221247</v>
+        <v>45579.55023645869</v>
       </c>
     </row>
     <row r="88">
@@ -11245,19 +11245,19 @@
         <v>133.48</v>
       </c>
       <c r="G88" t="n">
-        <v>-630.1483647235218</v>
+        <v>-615.6530686090919</v>
       </c>
       <c r="H88" t="n">
-        <v>24415.52532528701</v>
+        <v>24274.91662275086</v>
       </c>
       <c r="I88" t="n">
-        <v>50142.54836472352</v>
+        <v>50128.05306860909</v>
       </c>
       <c r="J88" t="n">
-        <v>34621.03018968068</v>
+        <v>34526.97709945189</v>
       </c>
       <c r="K88" t="n">
-        <v>39937.07518020201</v>
+        <v>39875.99509520378</v>
       </c>
     </row>
     <row r="89">
@@ -11271,19 +11271,19 @@
         <v>133.38</v>
       </c>
       <c r="G89" t="n">
-        <v>-755.5581272576164</v>
+        <v>-735.832786751489</v>
       </c>
       <c r="H89" t="n">
-        <v>24398.22957581289</v>
+        <v>24260.80689424658</v>
       </c>
       <c r="I89" t="n">
-        <v>50075.15812725761</v>
+        <v>50055.43278675149</v>
       </c>
       <c r="J89" t="n">
-        <v>38921.66299816815</v>
+        <v>38835.59516951958</v>
       </c>
       <c r="K89" t="n">
-        <v>35551.80266622382</v>
+        <v>35480.59797384302</v>
       </c>
     </row>
     <row r="90">
@@ -11297,19 +11297,19 @@
         <v>133.28</v>
       </c>
       <c r="G90" t="n">
-        <v>134.1769891093281</v>
+        <v>159.4015465158809</v>
       </c>
       <c r="H90" t="n">
-        <v>24381.15908031388</v>
+        <v>24246.87866345391</v>
       </c>
       <c r="I90" t="n">
-        <v>52576.32301089067</v>
+        <v>52551.09845348412</v>
       </c>
       <c r="J90" t="n">
-        <v>44699.78070025179</v>
+        <v>44619.84375152897</v>
       </c>
       <c r="K90" t="n">
-        <v>32257.8336941351</v>
+        <v>32178.03287840137</v>
       </c>
     </row>
     <row r="91">
@@ -11323,19 +11323,19 @@
         <v>133.18</v>
       </c>
       <c r="G91" t="n">
-        <v>-1237.486543679595</v>
+        <v>-1206.444234506744</v>
       </c>
       <c r="H91" t="n">
-        <v>24362.40542865509</v>
+        <v>24231.58445443461</v>
       </c>
       <c r="I91" t="n">
-        <v>57741.3865436796</v>
+        <v>57710.34423450675</v>
       </c>
       <c r="J91" t="n">
-        <v>52270.38887679954</v>
+        <v>52194.90353843783</v>
       </c>
       <c r="K91" t="n">
-        <v>29833.60089435951</v>
+        <v>29746.86267470285</v>
       </c>
     </row>
     <row r="92">
@@ -11349,19 +11349,19 @@
         <v>133.08</v>
       </c>
       <c r="G92" t="n">
-        <v>597.1550216036412</v>
+        <v>633.4058409350982</v>
       </c>
       <c r="H92" t="n">
-        <v>24340.21064968075</v>
+        <v>24213.49681872274</v>
       </c>
       <c r="I92" t="n">
-        <v>65623.04497839636</v>
+        <v>65586.7941590649</v>
       </c>
       <c r="J92" t="n">
-        <v>61884.1302620062</v>
+        <v>61812.39099794308</v>
       </c>
       <c r="K92" t="n">
-        <v>28079.40234713289</v>
+        <v>27987.66487237422</v>
       </c>
     </row>
     <row r="93">
@@ -11375,19 +11375,19 @@
         <v>132.98</v>
       </c>
       <c r="G93" t="n">
-        <v>647.9536434104521</v>
+        <v>686.5358390911133</v>
       </c>
       <c r="H93" t="n">
-        <v>24312.22702620497</v>
+        <v>24190.71111249828</v>
       </c>
       <c r="I93" t="n">
-        <v>76103.14635658955</v>
+        <v>76064.56416090889</v>
       </c>
       <c r="J93" t="n">
-        <v>73589.06516618557</v>
+        <v>73522.62994801336</v>
       </c>
       <c r="K93" t="n">
-        <v>26826.6789532198</v>
+        <v>26732.32583306896</v>
       </c>
     </row>
     <row r="94">
@@ -11401,19 +11401,19 @@
         <v>132.88</v>
       </c>
       <c r="G94" t="n">
-        <v>2043.619607769651</v>
+        <v>2078.460445095989</v>
       </c>
       <c r="H94" t="n">
-        <v>24276.34235399746</v>
+        <v>24161.5158175574</v>
       </c>
       <c r="I94" t="n">
-        <v>88671.08039223035</v>
+        <v>88636.23955490401</v>
       </c>
       <c r="J94" t="n">
-        <v>87008.08575674701</v>
+        <v>86951.72754301279</v>
       </c>
       <c r="K94" t="n">
-        <v>25939.81357752191</v>
+        <v>25845.61408679148</v>
       </c>
     </row>
     <row r="95">
@@ -11427,19 +11427,19 @@
         <v>132.78</v>
       </c>
       <c r="G95" t="n">
-        <v>-248.7084167207504</v>
+        <v>-226.2277776386618</v>
       </c>
       <c r="H95" t="n">
-        <v>24231.47911338804</v>
+        <v>24125.04003019476</v>
       </c>
       <c r="I95" t="n">
-        <v>102143.7084167208</v>
+        <v>102121.2277776387</v>
       </c>
       <c r="J95" t="n">
-        <v>101061.8978540661</v>
+        <v>101023.0106739246</v>
       </c>
       <c r="K95" t="n">
-        <v>25313.87624620783</v>
+        <v>25222.74602111023</v>
       </c>
     </row>
     <row r="96">
@@ -11453,19 +11453,19 @@
         <v>132.68</v>
       </c>
       <c r="G96" t="n">
-        <v>1307.491682667489</v>
+        <v>1309.74664264411</v>
       </c>
       <c r="H96" t="n">
-        <v>24177.33710774131</v>
+        <v>24081.04247596088</v>
       </c>
       <c r="I96" t="n">
-        <v>114491.5083173325</v>
+        <v>114489.2533573559</v>
       </c>
       <c r="J96" t="n">
-        <v>113799.6799349279</v>
+        <v>113785.0382911341</v>
       </c>
       <c r="K96" t="n">
-        <v>24869.85143570986</v>
+        <v>24784.65867536528</v>
       </c>
     </row>
     <row r="97">
@@ -11479,19 +11479,19 @@
         <v>132.58</v>
       </c>
       <c r="G97" t="n">
-        <v>-673.7957443692867</v>
+        <v>-693.6355481594219</v>
       </c>
       <c r="H97" t="n">
-        <v>24114.72501604923</v>
+        <v>24030.18291369104</v>
       </c>
       <c r="I97" t="n">
-        <v>123093.7957443693</v>
+        <v>123113.6355481594</v>
       </c>
       <c r="J97" t="n">
-        <v>122659.034356821</v>
+        <v>122669.5926009213</v>
       </c>
       <c r="K97" t="n">
-        <v>24550.24161549173</v>
+        <v>24473.56583107038</v>
       </c>
     </row>
     <row r="98">
@@ -11505,19 +11505,19 @@
         <v>132.48</v>
       </c>
       <c r="G98" t="n">
-        <v>-1739.986431527112</v>
+        <v>-1774.977651742985</v>
       </c>
       <c r="H98" t="n">
-        <v>24047.19134874745</v>
+        <v>23975.34358392637</v>
       </c>
       <c r="I98" t="n">
-        <v>125646.9864315271</v>
+        <v>125681.977651743</v>
       </c>
       <c r="J98" t="n">
-        <v>125378.6242527797</v>
+        <v>125406.7127884148</v>
       </c>
       <c r="K98" t="n">
-        <v>24316.3306362761</v>
+        <v>24249.92890648864</v>
       </c>
     </row>
     <row r="99">
@@ -11531,19 +11531,19 @@
         <v>132.38</v>
       </c>
       <c r="G99" t="n">
-        <v>175.8825596583483</v>
+        <v>136.9193003296677</v>
       </c>
       <c r="H99" t="n">
-        <v>23978.81794476279</v>
+        <v>23919.83387471831</v>
       </c>
       <c r="I99" t="n">
-        <v>121334.1174403417</v>
+        <v>121373.0806996703</v>
       </c>
       <c r="J99" t="n">
-        <v>121171.4778825501</v>
+        <v>121205.3589966263</v>
       </c>
       <c r="K99" t="n">
-        <v>24142.20315607821</v>
+        <v>24086.90337197004</v>
       </c>
     </row>
     <row r="100">
@@ -11557,19 +11557,19 @@
         <v>132.28</v>
       </c>
       <c r="G100" t="n">
-        <v>707.2885054190556</v>
+        <v>671.7016455352277</v>
       </c>
       <c r="H100" t="n">
-        <v>23913.7758658034</v>
+        <v>23867.03633505091</v>
       </c>
       <c r="I100" t="n">
-        <v>111298.7114945809</v>
+        <v>111334.2983544648</v>
       </c>
       <c r="J100" t="n">
-        <v>111201.9754241038</v>
+        <v>111233.8708025972</v>
       </c>
       <c r="K100" t="n">
-        <v>24011.18175197214</v>
+        <v>23966.8779469553</v>
       </c>
     </row>
     <row r="101">
@@ -11583,19 +11583,19 @@
         <v>132.18</v>
       </c>
       <c r="G101" t="n">
-        <v>-249.3864468783868</v>
+        <v>-281.285420175278</v>
       </c>
       <c r="H101" t="n">
-        <v>23856.6606554243</v>
+        <v>23820.67686757211</v>
       </c>
       <c r="I101" t="n">
-        <v>97953.58644687838</v>
+        <v>97985.48542017528</v>
       </c>
       <c r="J101" t="n">
-        <v>97897.14140849288</v>
+        <v>97926.4012393002</v>
       </c>
       <c r="K101" t="n">
-        <v>23913.67392865775</v>
+        <v>23879.26392698235</v>
       </c>
     </row>
     <row r="102">
@@ -11609,19 +11609,19 @@
         <v>132.08</v>
       </c>
       <c r="G102" t="n">
-        <v>-925.6597141749371</v>
+        <v>-957.7147056969552</v>
       </c>
       <c r="H102" t="n">
-        <v>23809.95874539543</v>
+        <v>23782.76986841113</v>
       </c>
       <c r="I102" t="n">
-        <v>83784.75971417494</v>
+        <v>83816.81470569696</v>
       </c>
       <c r="J102" t="n">
-        <v>83752.46499250027</v>
+        <v>83782.6634440551</v>
       </c>
       <c r="K102" t="n">
-        <v>23842.71354518088</v>
+        <v>23816.51857179659</v>
       </c>
     </row>
     <row r="103">
@@ -11635,19 +11635,19 @@
         <v>131.98</v>
       </c>
       <c r="G103" t="n">
-        <v>286.559499400435</v>
+        <v>250.6245745542692</v>
       </c>
       <c r="H103" t="n">
-        <v>23773.08960537953</v>
+        <v>23752.8430546269</v>
       </c>
       <c r="I103" t="n">
-        <v>70563.34050059956</v>
+        <v>70599.27542544572</v>
       </c>
       <c r="J103" t="n">
-        <v>70545.23319393907</v>
+        <v>70579.88133115084</v>
       </c>
       <c r="K103" t="n">
-        <v>23791.5559246824</v>
+        <v>23771.92293833326</v>
       </c>
     </row>
     <row r="104">
@@ -11661,19 +11661,19 @@
         <v>131.88</v>
       </c>
       <c r="G104" t="n">
-        <v>-353.7160030630839</v>
+        <v>-394.754850777048</v>
       </c>
       <c r="H104" t="n">
-        <v>23744.83692760308</v>
+        <v>23729.90940926529</v>
       </c>
       <c r="I104" t="n">
-        <v>59200.91600306308</v>
+        <v>59241.95485077705</v>
       </c>
       <c r="J104" t="n">
-        <v>59190.97403171952</v>
+        <v>59231.13228299493</v>
       </c>
       <c r="K104" t="n">
-        <v>23755.05098703193</v>
+        <v>23740.49374522175</v>
       </c>
     </row>
     <row r="105">
@@ -11687,19 +11687,19 @@
         <v>131.78</v>
       </c>
       <c r="G105" t="n">
-        <v>-1739.594995339336</v>
+        <v>-1784.374903940181</v>
       </c>
       <c r="H105" t="n">
-        <v>23724.48959734066</v>
+        <v>23713.39173918739</v>
       </c>
       <c r="I105" t="n">
-        <v>49962.49499533934</v>
+        <v>50007.27490394018</v>
       </c>
       <c r="J105" t="n">
-        <v>49957.15466809407</v>
+        <v>50001.33833082646</v>
       </c>
       <c r="K105" t="n">
-        <v>23730.03129520622</v>
+        <v>23719.15189689594</v>
       </c>
     </row>
     <row r="106">
@@ -11713,19 +11713,19 @@
         <v>131.68</v>
       </c>
       <c r="G106" t="n">
-        <v>-1526.451883326525</v>
+        <v>-1572.336718242004</v>
       </c>
       <c r="H106" t="n">
-        <v>23710.27780668882</v>
+        <v>23701.85390738455</v>
       </c>
       <c r="I106" t="n">
-        <v>42738.95188332652</v>
+        <v>42784.836718242</v>
       </c>
       <c r="J106" t="n">
-        <v>42736.14920875139</v>
+        <v>42781.63392924835</v>
       </c>
       <c r="K106" t="n">
-        <v>23713.2265333692</v>
+        <v>23704.92864909956</v>
       </c>
     </row>
     <row r="107">
@@ -11739,19 +11739,19 @@
         <v>131.58</v>
       </c>
       <c r="G107" t="n">
-        <v>-150.9324103755134</v>
+        <v>-195.2469793083073</v>
       </c>
       <c r="H107" t="n">
-        <v>23699.92380288724</v>
+        <v>23693.44766254426</v>
       </c>
       <c r="I107" t="n">
-        <v>37253.33241037551</v>
+        <v>37297.64697930831</v>
       </c>
       <c r="J107" t="n">
-        <v>37251.89793264258</v>
+        <v>37295.94610463686</v>
       </c>
       <c r="K107" t="n">
-        <v>23701.46231404127</v>
+        <v>23695.05724613646</v>
       </c>
     </row>
     <row r="108">
@@ -11765,19 +11765,19 @@
         <v>131.48</v>
       </c>
       <c r="G108" t="n">
-        <v>608.653160428883</v>
+        <v>568.0536250378718</v>
       </c>
       <c r="H108" t="n">
-        <v>23692.09837828275</v>
+        <v>23687.09420494802</v>
       </c>
       <c r="I108" t="n">
-        <v>33184.14683957112</v>
+        <v>33224.74637496213</v>
       </c>
       <c r="J108" t="n">
-        <v>33183.43270248004</v>
+        <v>33223.85617491544</v>
       </c>
       <c r="K108" t="n">
-        <v>23692.88537766005</v>
+        <v>23687.92039909959</v>
       </c>
     </row>
     <row r="109">
@@ -11791,19 +11791,19 @@
         <v>131.38</v>
       </c>
       <c r="G109" t="n">
-        <v>466.6207434179705</v>
+        <v>431.1875002451561</v>
       </c>
       <c r="H109" t="n">
-        <v>23686.41577301983</v>
+        <v>23682.4802160073</v>
       </c>
       <c r="I109" t="n">
-        <v>30226.47925658203</v>
+        <v>30261.91249975484</v>
       </c>
       <c r="J109" t="n">
-        <v>30226.13482679253</v>
+        <v>30261.45257462961</v>
       </c>
       <c r="K109" t="n">
-        <v>23686.8104068247</v>
+        <v>23682.89598571191</v>
       </c>
     </row>
     <row r="110">
@@ -11817,19 +11817,19 @@
         <v>131.28</v>
       </c>
       <c r="G110" t="n">
-        <v>1183.372068384338</v>
+        <v>1153.761831465759</v>
       </c>
       <c r="H110" t="n">
-        <v>23682.23599800055</v>
+        <v>23679.08629121726</v>
       </c>
       <c r="I110" t="n">
-        <v>28116.12793161566</v>
+        <v>28145.73816853424</v>
       </c>
       <c r="J110" t="n">
-        <v>28115.96801238796</v>
+        <v>28145.50308976591</v>
       </c>
       <c r="K110" t="n">
-        <v>23682.42995425574</v>
+        <v>23679.29139283685</v>
       </c>
     </row>
     <row r="111">
@@ -11843,19 +11843,19 @@
         <v>131.18</v>
       </c>
       <c r="G111" t="n">
-        <v>1066.955258060334</v>
+        <v>1043.162073831027</v>
       </c>
       <c r="H111" t="n">
-        <v>23679.05210581873</v>
+        <v>23676.50094053337</v>
       </c>
       <c r="I111" t="n">
-        <v>26636.64474193966</v>
+        <v>26660.43792616897</v>
       </c>
       <c r="J111" t="n">
-        <v>26636.57402409805</v>
+        <v>26660.31872993907</v>
       </c>
       <c r="K111" t="n">
-        <v>23679.14552817515</v>
+        <v>23676.60011016779</v>
       </c>
     </row>
     <row r="112">
@@ -11869,19 +11869,19 @@
         <v>131.08</v>
       </c>
       <c r="G112" t="n">
-        <v>993.2711453534466</v>
+        <v>974.8716051838492</v>
       </c>
       <c r="H112" t="n">
-        <v>23676.75559797291</v>
+        <v>23674.63595776026</v>
       </c>
       <c r="I112" t="n">
-        <v>25617.42885464655</v>
+        <v>25635.82839481615</v>
       </c>
       <c r="J112" t="n">
-        <v>25617.39965797784</v>
+        <v>25635.76823908391</v>
       </c>
       <c r="K112" t="n">
-        <v>23676.79969276784</v>
+        <v>23674.68295080842</v>
       </c>
     </row>
     <row r="113">
@@ -11895,19 +11895,19 @@
         <v>130.98</v>
       </c>
       <c r="G113" t="n">
-        <v>854.2097610407582</v>
+        <v>840.5090029898493</v>
       </c>
       <c r="H113" t="n">
-        <v>23675.09422068701</v>
+        <v>23673.28661119623</v>
       </c>
       <c r="I113" t="n">
-        <v>24927.39023895924</v>
+        <v>24941.09099701015</v>
       </c>
       <c r="J113" t="n">
-        <v>24927.37946022035</v>
+        <v>24941.06066621245</v>
       </c>
       <c r="K113" t="n">
-        <v>23675.11461311599</v>
+        <v>23673.30843293708</v>
       </c>
     </row>
     <row r="114">
@@ -11921,19 +11921,19 @@
         <v>130.88</v>
       </c>
       <c r="G114" t="n">
-        <v>1190.699480351199</v>
+        <v>1180.863519723214</v>
       </c>
       <c r="H114" t="n">
-        <v>23673.74842300855</v>
+        <v>23672.1935673493</v>
       </c>
       <c r="I114" t="n">
-        <v>24468.2005196488</v>
+        <v>24478.03648027679</v>
       </c>
       <c r="J114" t="n">
-        <v>24468.1973789464</v>
+        <v>24478.02114271028</v>
       </c>
       <c r="K114" t="n">
-        <v>23673.75766264093</v>
+        <v>23672.20349633731</v>
       </c>
     </row>
     <row r="115">
@@ -11947,19 +11947,19 @@
         <v>130.78</v>
       </c>
       <c r="G115" t="n">
-        <v>1164.917083053959</v>
+        <v>1158.10659969836</v>
       </c>
       <c r="H115" t="n">
-        <v>23672.55090207247</v>
+        <v>23671.22100965921</v>
       </c>
       <c r="I115" t="n">
-        <v>24167.88291694604</v>
+        <v>24174.69340030164</v>
       </c>
       <c r="J115" t="n">
-        <v>24167.88261842011</v>
+        <v>24174.68559480871</v>
       </c>
       <c r="K115" t="n">
-        <v>23672.55500323089</v>
+        <v>23671.22543597481</v>
       </c>
     </row>
     <row r="116">
@@ -11973,19 +11973,19 @@
         <v>130.68</v>
       </c>
       <c r="G116" t="n">
-        <v>1132.837380159086</v>
+        <v>1128.310554539996</v>
       </c>
       <c r="H116" t="n">
-        <v>23671.53356522193</v>
+        <v>23670.39476882907</v>
       </c>
       <c r="I116" t="n">
-        <v>23974.96261984091</v>
+        <v>23979.48944546</v>
       </c>
       <c r="J116" t="n">
-        <v>23974.96316609849</v>
+        <v>23979.48543773371</v>
       </c>
       <c r="K116" t="n">
-        <v>23671.53534837777</v>
+        <v>23670.39670198246</v>
       </c>
     </row>
     <row r="117">
@@ -11999,19 +11999,19 @@
         <v>130.58</v>
       </c>
       <c r="G117" t="n">
-        <v>1285.653855978009</v>
+        <v>1282.770279881119</v>
       </c>
       <c r="H117" t="n">
-        <v>23670.5801680404</v>
+        <v>23669.62053880833</v>
       </c>
       <c r="I117" t="n">
-        <v>23853.14614402199</v>
+        <v>23856.02972011888</v>
       </c>
       <c r="J117" t="n">
-        <v>23853.14678617804</v>
+        <v>23856.02764190574</v>
       </c>
       <c r="K117" t="n">
-        <v>23670.58092743982</v>
+        <v>23669.62136588178</v>
       </c>
     </row>
     <row r="118">
@@ -12025,19 +12025,19 @@
         <v>130.48</v>
       </c>
       <c r="G118" t="n">
-        <v>467.0312657224385</v>
+        <v>465.3223790697521</v>
       </c>
       <c r="H118" t="n">
-        <v>23669.9083982557</v>
+        <v>23669.07487094035</v>
       </c>
       <c r="I118" t="n">
-        <v>23777.76873427756</v>
+        <v>23779.47762093025</v>
       </c>
       <c r="J118" t="n">
-        <v>23777.76924556894</v>
+        <v>23779.476533315</v>
       </c>
       <c r="K118" t="n">
-        <v>23669.90871500744</v>
+        <v>23669.07521755365</v>
       </c>
     </row>
     <row r="119">
@@ -12051,19 +12051,19 @@
         <v>130.38</v>
       </c>
       <c r="G119" t="n">
-        <v>291.5421231236578</v>
+        <v>290.6773543044037</v>
       </c>
       <c r="H119" t="n">
-        <v>23669.60193866976</v>
+        <v>23668.82567141025</v>
       </c>
       <c r="I119" t="n">
-        <v>23732.15787687634</v>
+        <v>23733.0226456956</v>
       </c>
       <c r="J119" t="n">
-        <v>23732.15822772652</v>
+        <v>23733.02207253802</v>
       </c>
       <c r="K119" t="n">
-        <v>23669.60206806171</v>
+        <v>23668.82581368947</v>
       </c>
     </row>
     <row r="120">
@@ -12077,19 +12077,19 @@
         <v>130.28</v>
       </c>
       <c r="G120" t="n">
-        <v>493.2807954213386</v>
+        <v>492.9689548710485</v>
       </c>
       <c r="H120" t="n">
-        <v>23669.31230302362</v>
+        <v>23668.59023691874</v>
       </c>
       <c r="I120" t="n">
-        <v>23704.91920457866</v>
+        <v>23705.23104512895</v>
       </c>
       <c r="J120" t="n">
-        <v>23704.91942617148</v>
+        <v>23705.23074200091</v>
       </c>
       <c r="K120" t="n">
-        <v>23669.31235478533</v>
+        <v>23668.59029412009</v>
       </c>
     </row>
     <row r="121">
@@ -12103,19 +12103,19 @@
         <v>130.18</v>
       </c>
       <c r="G121" t="n">
-        <v>-75.6431809144342</v>
+        <v>-75.58609490679373</v>
       </c>
       <c r="H121" t="n">
-        <v>23669.1565630603</v>
+        <v>23668.46344911589</v>
       </c>
       <c r="I121" t="n">
-        <v>23689.04318091444</v>
+        <v>23688.9860949068</v>
       </c>
       <c r="J121" t="n">
-        <v>23689.04331330753</v>
+        <v>23688.98593463986</v>
       </c>
       <c r="K121" t="n">
-        <v>23669.15658333705</v>
+        <v>23668.46347163832</v>
       </c>
     </row>
     <row r="122">
@@ -12129,19 +12129,19 @@
         <v>130.08</v>
       </c>
       <c r="G122" t="n">
-        <v>24.44165097839505</v>
+        <v>24.75416686271637</v>
       </c>
       <c r="H122" t="n">
-        <v>23669.1625568296</v>
+        <v>23668.46790508569</v>
       </c>
       <c r="I122" t="n">
-        <v>23680.0583490216</v>
+        <v>23679.74583313728</v>
       </c>
       <c r="J122" t="n">
-        <v>23680.05842489105</v>
+        <v>23679.7457487572</v>
       </c>
       <c r="K122" t="n">
-        <v>23669.16256460735</v>
+        <v>23668.4679137702</v>
       </c>
     </row>
     <row r="123">
@@ -12155,19 +12155,19 @@
         <v>129.98</v>
       </c>
       <c r="G123" t="n">
-        <v>9.398683206756687</v>
+        <v>9.866304806917469</v>
       </c>
       <c r="H123" t="n">
-        <v>23669.14607058957</v>
+        <v>23668.45416354387</v>
       </c>
       <c r="I123" t="n">
-        <v>23675.00131679324</v>
+        <v>23674.53369519308</v>
       </c>
       <c r="J123" t="n">
-        <v>23675.00135882294</v>
+        <v>23674.53365110902</v>
       </c>
       <c r="K123" t="n">
-        <v>23669.14607351071</v>
+        <v>23668.45416682312</v>
       </c>
     </row>
     <row r="124">
@@ -12181,19 +12181,19 @@
         <v>129.88</v>
       </c>
       <c r="G124" t="n">
-        <v>29.08385101882959</v>
+        <v>29.64457475433301</v>
       </c>
       <c r="H124" t="n">
-        <v>23669.13051759025</v>
+        <v>23668.44117492209</v>
       </c>
       <c r="I124" t="n">
-        <v>23672.21614898117</v>
+        <v>23671.65542524567</v>
       </c>
       <c r="J124" t="n">
-        <v>23672.21617159545</v>
+        <v>23671.65540245963</v>
       </c>
       <c r="K124" t="n">
-        <v>23669.13051866442</v>
+        <v>23668.44117613459</v>
       </c>
     </row>
     <row r="125">
@@ -12207,19 +12207,19 @@
         <v>129.78</v>
       </c>
       <c r="G125" t="n">
-        <v>-3.314867990982748</v>
+        <v>-2.699120899920672</v>
       </c>
       <c r="H125" t="n">
-        <v>23669.12051047531</v>
+        <v>23668.43268666447</v>
       </c>
       <c r="I125" t="n">
-        <v>23670.71486799098</v>
+        <v>23670.09912089992</v>
       </c>
       <c r="J125" t="n">
-        <v>23670.71487984418</v>
+        <v>23670.0991092761</v>
       </c>
       <c r="K125" t="n">
-        <v>23669.12051086203</v>
+        <v>23668.43268710345</v>
       </c>
     </row>
     <row r="126">
@@ -12233,19 +12233,19 @@
         <v>129.68</v>
       </c>
       <c r="G126" t="n">
-        <v>-519.4979509566656</v>
+        <v>-518.8171696194695</v>
       </c>
       <c r="H126" t="n">
-        <v>23669.29033280221</v>
+        <v>23668.57007605467</v>
       </c>
       <c r="I126" t="n">
-        <v>23670.09795095666</v>
+        <v>23669.41716961947</v>
       </c>
       <c r="J126" t="n">
-        <v>23670.09795702046</v>
+        <v>23669.41716377829</v>
       </c>
       <c r="K126" t="n">
-        <v>23669.29033293852</v>
+        <v>23668.57007621029</v>
       </c>
     </row>
     <row r="127">
@@ -12259,19 +12259,19 @@
         <v>129.58</v>
       </c>
       <c r="G127" t="n">
-        <v>49.85502736068884</v>
+        <v>50.58350318758676</v>
       </c>
       <c r="H127" t="n">
-        <v>23669.44397097655</v>
+        <v>23668.69436286665</v>
       </c>
       <c r="I127" t="n">
-        <v>23669.84497263931</v>
+        <v>23669.11649681241</v>
       </c>
       <c r="J127" t="n">
-        <v>23669.84497567078</v>
+        <v>23669.1164939251</v>
       </c>
       <c r="K127" t="n">
-        <v>23669.44397102358</v>
+        <v>23668.69436292067</v>
       </c>
     </row>
     <row r="128">
@@ -12285,19 +12285,19 @@
         <v>129.48</v>
       </c>
       <c r="G128" t="n">
-        <v>29.38624241298385</v>
+        <v>30.12036719385287</v>
       </c>
       <c r="H128" t="n">
-        <v>23669.41861514066</v>
+        <v>23668.67343192079</v>
       </c>
       <c r="I128" t="n">
-        <v>23669.61375758702</v>
+        <v>23668.87963280615</v>
       </c>
       <c r="J128" t="n">
-        <v>23669.61375906924</v>
+        <v>23668.87963140381</v>
       </c>
       <c r="K128" t="n">
-        <v>23669.41861515654</v>
+        <v>23668.67343193914</v>
       </c>
     </row>
     <row r="129">
@@ -12311,19 +12311,19 @@
         <v>129.38</v>
       </c>
       <c r="G129" t="n">
-        <v>-96.83347675304321</v>
+        <v>-96.08943194948733</v>
       </c>
       <c r="H129" t="n">
-        <v>23669.44041467013</v>
+        <v>23668.69071265325</v>
       </c>
       <c r="I129" t="n">
-        <v>23669.53347675304</v>
+        <v>23668.78943194949</v>
       </c>
       <c r="J129" t="n">
-        <v>23669.53347746223</v>
+        <v>23668.78943128079</v>
       </c>
       <c r="K129" t="n">
-        <v>23669.44041467538</v>
+        <v>23668.69071265935</v>
       </c>
     </row>
     <row r="130">
@@ -12337,19 +12337,19 @@
         <v>129.28</v>
       </c>
       <c r="G130" t="n">
-        <v>-0.04348736413521692</v>
+        <v>-0.04631681029059109</v>
       </c>
       <c r="H130" t="n">
         <v>23070.3</v>
       </c>
       <c r="I130" t="n">
-        <v>23070.34348736413</v>
+        <v>23070.34631681029</v>
       </c>
       <c r="J130" t="n">
-        <v>23070.34348769629</v>
+        <v>23070.34631649743</v>
       </c>
       <c r="K130" t="n">
-        <v>23070.3000000017</v>
+        <v>23070.30000000199</v>
       </c>
     </row>
     <row r="131">
@@ -12363,19 +12363,19 @@
         <v>129.18</v>
       </c>
       <c r="G131" t="n">
-        <v>-0.01991040254506515</v>
+        <v>-0.02129401750062243</v>
       </c>
       <c r="H131" t="n">
         <v>23261.8</v>
       </c>
       <c r="I131" t="n">
-        <v>23261.81991040254</v>
+        <v>23261.8212940175</v>
       </c>
       <c r="J131" t="n">
-        <v>23261.81991055486</v>
+        <v>23261.82129387395</v>
       </c>
       <c r="K131" t="n">
-        <v>23261.80000000054</v>
+        <v>23261.80000000063</v>
       </c>
     </row>
     <row r="132">
@@ -12389,19 +12389,19 @@
         <v>129.08</v>
       </c>
       <c r="G132" t="n">
-        <v>-0.008930672604037682</v>
+        <v>-0.009592226761014899</v>
       </c>
       <c r="H132" t="n">
         <v>23679.9</v>
       </c>
       <c r="I132" t="n">
-        <v>23679.90893067261</v>
+        <v>23679.90959222676</v>
       </c>
       <c r="J132" t="n">
-        <v>23679.908930741</v>
+        <v>23679.90959216218</v>
       </c>
       <c r="K132" t="n">
-        <v>23679.90000000017</v>
+        <v>23679.9000000002</v>
       </c>
     </row>
     <row r="133">
@@ -12415,19 +12415,19 @@
         <v>128.98</v>
       </c>
       <c r="G133" t="n">
-        <v>-0.003924089454812929</v>
+        <v>-0.004233382718666689</v>
       </c>
       <c r="H133" t="n">
         <v>23737.6</v>
       </c>
       <c r="I133" t="n">
-        <v>23737.60392408945</v>
+        <v>23737.60423338272</v>
       </c>
       <c r="J133" t="n">
-        <v>23737.60392411953</v>
+        <v>23737.60423335424</v>
       </c>
       <c r="K133" t="n">
-        <v>23737.60000000005</v>
+        <v>23737.60000000006</v>
       </c>
     </row>
     <row r="134">
@@ -12441,19 +12441,19 @@
         <v>128.88</v>
       </c>
       <c r="G134" t="n">
-        <v>-0.001688924752670573</v>
+        <v>-0.001830323824833613</v>
       </c>
       <c r="H134" t="n">
         <v>22921.3</v>
       </c>
       <c r="I134" t="n">
-        <v>22921.30168892475</v>
+        <v>22921.30183032382</v>
       </c>
       <c r="J134" t="n">
-        <v>22921.3016889377</v>
+        <v>22921.30183031152</v>
       </c>
       <c r="K134" t="n">
-        <v>22921.30000000001</v>
+        <v>22921.30000000002</v>
       </c>
     </row>
     <row r="135">
@@ -12467,16 +12467,16 @@
         <v>128.78</v>
       </c>
       <c r="G135" t="n">
-        <v>-0.0007119784459064249</v>
+        <v>-0.0007751916491542943</v>
       </c>
       <c r="H135" t="n">
         <v>23216.3</v>
       </c>
       <c r="I135" t="n">
-        <v>23216.30071197845</v>
+        <v>23216.30077519165</v>
       </c>
       <c r="J135" t="n">
-        <v>23216.30071198391</v>
+        <v>23216.30077518644</v>
       </c>
       <c r="K135" t="n">
         <v>23216.3</v>
@@ -12493,16 +12493,16 @@
         <v>128.68</v>
       </c>
       <c r="G136" t="n">
-        <v>-0.0002939538826467469</v>
+        <v>-0.0003215893339074682</v>
       </c>
       <c r="H136" t="n">
         <v>23106.4</v>
       </c>
       <c r="I136" t="n">
-        <v>23106.40029395388</v>
+        <v>23106.40032158934</v>
       </c>
       <c r="J136" t="n">
-        <v>23106.40029395614</v>
+        <v>23106.40032158717</v>
       </c>
       <c r="K136" t="n">
         <v>23106.4</v>
@@ -12519,16 +12519,16 @@
         <v>128.58</v>
       </c>
       <c r="G137" t="n">
-        <v>-0.0001188557034765836</v>
+        <v>-0.0001306707054027356</v>
       </c>
       <c r="H137" t="n">
         <v>23220.2</v>
       </c>
       <c r="I137" t="n">
-        <v>23220.2001188557</v>
+        <v>23220.20013067071</v>
       </c>
       <c r="J137" t="n">
-        <v>23220.20011885662</v>
+        <v>23220.20013066983</v>
       </c>
       <c r="K137" t="n">
         <v>23220.2</v>
@@ -12545,16 +12545,16 @@
         <v>128.48</v>
       </c>
       <c r="G138" t="n">
-        <v>-4.706129402620718e-05</v>
+        <v>-5.200119994697161e-05</v>
       </c>
       <c r="H138" t="n">
         <v>24093.6</v>
       </c>
       <c r="I138" t="n">
-        <v>24093.60004706129</v>
+        <v>24093.6000520012</v>
       </c>
       <c r="J138" t="n">
-        <v>24093.60004706165</v>
+        <v>24093.60005200085</v>
       </c>
       <c r="K138" t="n">
         <v>24093.6</v>
@@ -12571,16 +12571,16 @@
         <v>128.38</v>
       </c>
       <c r="G139" t="n">
-        <v>-1.824680657591671e-05</v>
+        <v>-2.026670699706301e-05</v>
       </c>
       <c r="H139" t="n">
         <v>22379.6</v>
       </c>
       <c r="I139" t="n">
-        <v>22379.60001824681</v>
+        <v>22379.60002026671</v>
       </c>
       <c r="J139" t="n">
-        <v>22379.60001824694</v>
+        <v>22379.60002026657</v>
       </c>
       <c r="K139" t="n">
         <v>22379.6</v>
@@ -12597,16 +12597,16 @@
         <v>128.28</v>
       </c>
       <c r="G140" t="n">
-        <v>-6.927344657015055e-06</v>
+        <v>-7.735092367511243e-06</v>
       </c>
       <c r="H140" t="n">
         <v>23672.7</v>
       </c>
       <c r="I140" t="n">
-        <v>23672.70000692735</v>
+        <v>23672.70000773509</v>
       </c>
       <c r="J140" t="n">
-        <v>23672.7000069274</v>
+        <v>23672.70000773504</v>
       </c>
       <c r="K140" t="n">
         <v>23672.7</v>
@@ -12623,16 +12623,16 @@
         <v>128.18</v>
       </c>
       <c r="G141" t="n">
-        <v>-2.575030521256849e-06</v>
+        <v>-2.890941686928272e-06</v>
       </c>
       <c r="H141" t="n">
         <v>22678.3</v>
       </c>
       <c r="I141" t="n">
-        <v>22678.30000257503</v>
+        <v>22678.30000289094</v>
       </c>
       <c r="J141" t="n">
-        <v>22678.30000257505</v>
+        <v>22678.30000289092</v>
       </c>
       <c r="K141" t="n">
         <v>22678.3</v>
@@ -12649,16 +12649,16 @@
         <v>128.08</v>
       </c>
       <c r="G142" t="n">
-        <v>-9.371615306008607e-07</v>
+        <v>-1.057996996678412e-06</v>
       </c>
       <c r="H142" t="n">
         <v>22925.7</v>
       </c>
       <c r="I142" t="n">
-        <v>22925.70000093716</v>
+        <v>22925.700001058</v>
       </c>
       <c r="J142" t="n">
-        <v>22925.70000093717</v>
+        <v>22925.70000105799</v>
       </c>
       <c r="K142" t="n">
         <v>22925.7</v>
@@ -12675,16 +12675,16 @@
         <v>127.98</v>
       </c>
       <c r="G143" t="n">
-        <v>-3.339227987453341e-07</v>
+        <v>-3.791283234022558e-07</v>
       </c>
       <c r="H143" t="n">
         <v>23234.5</v>
       </c>
       <c r="I143" t="n">
-        <v>23234.50000033392</v>
+        <v>23234.50000037913</v>
       </c>
       <c r="J143" t="n">
-        <v>23234.50000033393</v>
+        <v>23234.50000037912</v>
       </c>
       <c r="K143" t="n">
         <v>23234.5</v>
@@ -12701,16 +12701,16 @@
         <v>127.88</v>
       </c>
       <c r="G144" t="n">
-        <v>-1.164808054454625e-07</v>
+        <v>-1.330226950813085e-07</v>
       </c>
       <c r="H144" t="n">
         <v>23209.9</v>
       </c>
       <c r="I144" t="n">
-        <v>23209.90000011648</v>
+        <v>23209.90000013302</v>
       </c>
       <c r="J144" t="n">
-        <v>23209.90000011648</v>
+        <v>23209.90000013302</v>
       </c>
       <c r="K144" t="n">
         <v>23209.9</v>
@@ -12727,16 +12727,16 @@
         <v>127.78</v>
       </c>
       <c r="G145" t="n">
-        <v>-3.977766027674079e-08</v>
+        <v>-4.569665179587901e-08</v>
       </c>
       <c r="H145" t="n">
         <v>22959.1</v>
       </c>
       <c r="I145" t="n">
-        <v>22959.10000003978</v>
+        <v>22959.1000000457</v>
       </c>
       <c r="J145" t="n">
-        <v>22959.10000003978</v>
+        <v>22959.1000000457</v>
       </c>
       <c r="K145" t="n">
         <v>22959.1</v>
@@ -12753,16 +12753,16 @@
         <v>127.68</v>
       </c>
       <c r="G146" t="n">
-        <v>-1.329681253992021e-08</v>
+        <v>-1.537046045996249e-08</v>
       </c>
       <c r="H146" t="n">
         <v>23204.9</v>
       </c>
       <c r="I146" t="n">
-        <v>23204.9000000133</v>
+        <v>23204.90000001537</v>
       </c>
       <c r="J146" t="n">
-        <v>23204.9000000133</v>
+        <v>23204.90000001537</v>
       </c>
       <c r="K146" t="n">
         <v>23204.9</v>
@@ -12779,16 +12779,16 @@
         <v>127.58</v>
       </c>
       <c r="G147" t="n">
-        <v>-4.351022653281689e-09</v>
+        <v>-5.060428520664573e-09</v>
       </c>
       <c r="H147" t="n">
         <v>22759</v>
       </c>
       <c r="I147" t="n">
-        <v>22759.00000000435</v>
+        <v>22759.00000000506</v>
       </c>
       <c r="J147" t="n">
-        <v>22759.00000000435</v>
+        <v>22759.00000000506</v>
       </c>
       <c r="K147" t="n">
         <v>22759</v>
@@ -12805,16 +12805,16 @@
         <v>127.48</v>
       </c>
       <c r="G148" t="n">
-        <v>-1.393345883116126e-09</v>
+        <v>-1.629814505577087e-09</v>
       </c>
       <c r="H148" t="n">
         <v>23218.7</v>
       </c>
       <c r="I148" t="n">
-        <v>23218.70000000139</v>
+        <v>23218.70000000163</v>
       </c>
       <c r="J148" t="n">
-        <v>23218.70000000139</v>
+        <v>23218.70000000163</v>
       </c>
       <c r="K148" t="n">
         <v>23218.7</v>
@@ -12831,16 +12831,16 @@
         <v>127.38</v>
       </c>
       <c r="G149" t="n">
-        <v>-4.365574568510056e-10</v>
+        <v>-5.129550117999315e-10</v>
       </c>
       <c r="H149" t="n">
         <v>23386.5</v>
       </c>
       <c r="I149" t="n">
-        <v>23386.50000000044</v>
+        <v>23386.50000000051</v>
       </c>
       <c r="J149" t="n">
-        <v>23386.50000000044</v>
+        <v>23386.50000000051</v>
       </c>
       <c r="K149" t="n">
         <v>23386.5</v>
@@ -12857,16 +12857,16 @@
         <v>127.28</v>
       </c>
       <c r="G150" t="n">
-        <v>-1.346052158623934e-10</v>
+        <v>-1.600710675120354e-10</v>
       </c>
       <c r="H150" t="n">
         <v>23184.7</v>
       </c>
       <c r="I150" t="n">
-        <v>23184.70000000014</v>
+        <v>23184.70000000016</v>
       </c>
       <c r="J150" t="n">
-        <v>23184.70000000014</v>
+        <v>23184.70000000016</v>
       </c>
       <c r="K150" t="n">
         <v>23184.7</v>
@@ -12883,16 +12883,16 @@
         <v>127.18</v>
       </c>
       <c r="G151" t="n">
-        <v>-4.001776687800884e-11</v>
+        <v>-4.729372449219227e-11</v>
       </c>
       <c r="H151" t="n">
         <v>22687</v>
       </c>
       <c r="I151" t="n">
-        <v>22687.00000000004</v>
+        <v>22687.00000000005</v>
       </c>
       <c r="J151" t="n">
-        <v>22687.00000000004</v>
+        <v>22687.00000000005</v>
       </c>
       <c r="K151" t="n">
         <v>22687</v>
@@ -12909,16 +12909,16 @@
         <v>127.08</v>
       </c>
       <c r="G152" t="n">
-        <v>-1.091393642127514e-11</v>
+        <v>-1.455191522836685e-11</v>
       </c>
       <c r="H152" t="n">
         <v>22924.4</v>
       </c>
       <c r="I152" t="n">
-        <v>22924.40000000001</v>
+        <v>22924.40000000002</v>
       </c>
       <c r="J152" t="n">
-        <v>22924.40000000001</v>
+        <v>22924.40000000002</v>
       </c>
       <c r="K152" t="n">
         <v>22924.4</v>

</xml_diff>

<commit_message>
Mac: Improve vertical lines
</commit_message>
<xml_diff>
--- a/DATA/UKSAF/STO.xlsx
+++ b/DATA/UKSAF/STO.xlsx
@@ -73,7 +73,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -440,11 +440,17 @@
       <top style="thin"/>
       <bottom style="medium"/>
     </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -506,6 +512,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,7 +651,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="5648325" cy="4086225"/>
+    <ext cx="5657850" cy="4114800"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -638,6 +665,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -668,7 +698,7 @@
       </blipFill>
       <spPr>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
+          <avLst/>
         </a:prstGeom>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
@@ -703,7 +733,7 @@
       </blipFill>
       <spPr>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
+          <avLst/>
         </a:prstGeom>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
@@ -10283,19 +10313,19 @@
         <v>137.18</v>
       </c>
       <c r="G51" t="n">
-        <v>24.53005351460524</v>
+        <v>24.53338684793562</v>
       </c>
       <c r="H51" t="n">
-        <v>24672.13333333333</v>
+        <v>24672.13</v>
       </c>
       <c r="I51" t="n">
-        <v>24672.3699464854</v>
+        <v>24672.36661315207</v>
       </c>
       <c r="J51" t="n">
-        <v>24672.13333339001</v>
+        <v>24672.13000005668</v>
       </c>
       <c r="K51" t="n">
-        <v>24672.3699475103</v>
+        <v>24672.36661417697</v>
       </c>
     </row>
     <row r="52">
@@ -10309,19 +10339,19 @@
         <v>137.08</v>
       </c>
       <c r="G52" t="n">
-        <v>-3.985933482799737</v>
+        <v>-3.98773545494987</v>
       </c>
       <c r="H52" t="n">
-        <v>24667.00819802785</v>
+        <v>24667.01</v>
       </c>
       <c r="I52" t="n">
-        <v>24667.4859334828</v>
+        <v>24667.48773545495</v>
       </c>
       <c r="J52" t="n">
-        <v>24667.00819819214</v>
+        <v>24667.01000016429</v>
       </c>
       <c r="K52" t="n">
-        <v>24667.48593550229</v>
+        <v>24667.48773747444</v>
       </c>
     </row>
     <row r="53">
@@ -10335,19 +10365,19 @@
         <v>136.98</v>
       </c>
       <c r="G53" t="n">
-        <v>-11.9481581258915</v>
+        <v>-11.94556755579106</v>
       </c>
       <c r="H53" t="n">
-        <v>24667.0025905701</v>
+        <v>24667</v>
       </c>
       <c r="I53" t="n">
-        <v>24667.94815812589</v>
+        <v>24667.94556755579</v>
       </c>
       <c r="J53" t="n">
-        <v>24667.00259103639</v>
+        <v>24667.00000046629</v>
       </c>
       <c r="K53" t="n">
-        <v>24667.9481619819</v>
+        <v>24667.9455714118</v>
       </c>
     </row>
     <row r="54">
@@ -10361,19 +10391,19 @@
         <v>136.88</v>
       </c>
       <c r="G54" t="n">
-        <v>-85.84145719955632</v>
+        <v>-85.84489713509538</v>
       </c>
       <c r="H54" t="n">
-        <v>24667.00656006446</v>
+        <v>24667.01</v>
       </c>
       <c r="I54" t="n">
-        <v>24668.84145719956</v>
+        <v>24668.8448971351</v>
       </c>
       <c r="J54" t="n">
-        <v>24667.00656136022</v>
+        <v>24667.01000129576</v>
       </c>
       <c r="K54" t="n">
-        <v>24668.8414642913</v>
+        <v>24668.84490422684</v>
       </c>
     </row>
     <row r="55">
@@ -10387,19 +10417,19 @@
         <v>136.78</v>
       </c>
       <c r="G55" t="n">
-        <v>-393.9238112547064</v>
+        <v>-393.9214638233061</v>
       </c>
       <c r="H55" t="n">
-        <v>24667.0323474314</v>
+        <v>24667.03</v>
       </c>
       <c r="I55" t="n">
-        <v>24670.5238112547</v>
+        <v>24670.5214638233</v>
       </c>
       <c r="J55" t="n">
-        <v>24667.03235095715</v>
+        <v>24667.03000352575</v>
       </c>
       <c r="K55" t="n">
-        <v>24670.52382368879</v>
+        <v>24670.52147625739</v>
       </c>
     </row>
     <row r="56">
@@ -10413,19 +10443,19 @@
         <v>136.68</v>
       </c>
       <c r="G56" t="n">
-        <v>132.7262302915478</v>
+        <v>132.7244941297067</v>
       </c>
       <c r="H56" t="n">
-        <v>24667.15826383816</v>
+        <v>24667.16</v>
       </c>
       <c r="I56" t="n">
-        <v>24673.67376970845</v>
+        <v>24673.67550587029</v>
       </c>
       <c r="J56" t="n">
-        <v>24667.15827323223</v>
+        <v>24667.16000939408</v>
       </c>
       <c r="K56" t="n">
-        <v>24673.67379009739</v>
+        <v>24673.67552625923</v>
       </c>
     </row>
     <row r="57">
@@ -10439,19 +10469,19 @@
         <v>136.58</v>
       </c>
       <c r="G57" t="n">
-        <v>559.8498043727486</v>
+        <v>559.8536470967701</v>
       </c>
       <c r="H57" t="n">
-        <v>24667.22384272402</v>
+        <v>24667.22</v>
       </c>
       <c r="I57" t="n">
-        <v>24679.15019562725</v>
+        <v>24679.14635290323</v>
       </c>
       <c r="J57" t="n">
-        <v>24667.22386723455</v>
+        <v>24667.22002451053</v>
       </c>
       <c r="K57" t="n">
-        <v>24679.15022563316</v>
+        <v>24679.14638290914</v>
       </c>
     </row>
     <row r="58">
@@ -10465,19 +10495,19 @@
         <v>136.48</v>
       </c>
       <c r="G58" t="n">
-        <v>-32.15224642790054</v>
+        <v>-32.14740484383583</v>
       </c>
       <c r="H58" t="n">
-        <v>24667.03484158406</v>
+        <v>24667.03</v>
       </c>
       <c r="I58" t="n">
-        <v>24688.4522464279</v>
+        <v>24688.44740484384</v>
       </c>
       <c r="J58" t="n">
-        <v>24667.03490421197</v>
+        <v>24667.03006262791</v>
       </c>
       <c r="K58" t="n">
-        <v>24688.45228170067</v>
+        <v>24688.4474401166</v>
       </c>
     </row>
     <row r="59">
@@ -10491,19 +10521,19 @@
         <v>136.38</v>
       </c>
       <c r="G59" t="n">
-        <v>-220.1276171326463</v>
+        <v>-220.1310193885147</v>
       </c>
       <c r="H59" t="n">
-        <v>24666.88659774413</v>
+        <v>24666.89</v>
       </c>
       <c r="I59" t="n">
-        <v>24704.62761713265</v>
+        <v>24704.63101938851</v>
       </c>
       <c r="J59" t="n">
-        <v>24666.88675446344</v>
+        <v>24666.89015671931</v>
       </c>
       <c r="K59" t="n">
-        <v>24704.62763293004</v>
+        <v>24704.63103518591</v>
       </c>
     </row>
     <row r="60">
@@ -10517,19 +10547,19 @@
         <v>136.28</v>
       </c>
       <c r="G60" t="n">
-        <v>375.988135177915</v>
+        <v>375.9854909245223</v>
       </c>
       <c r="H60" t="n">
-        <v>24666.93735574661</v>
+        <v>24666.94</v>
       </c>
       <c r="I60" t="n">
-        <v>24732.21186482209</v>
+        <v>24732.21450907548</v>
       </c>
       <c r="J60" t="n">
-        <v>24666.93773984336</v>
+        <v>24666.94038409675</v>
       </c>
       <c r="K60" t="n">
-        <v>24732.21177909817</v>
+        <v>24732.21442335156</v>
       </c>
     </row>
     <row r="61">
@@ -10543,19 +10573,19 @@
         <v>136.18</v>
       </c>
       <c r="G61" t="n">
-        <v>178.5013478604451</v>
+        <v>178.4991691061186</v>
       </c>
       <c r="H61" t="n">
-        <v>24666.86782124567</v>
+        <v>24666.87</v>
       </c>
       <c r="I61" t="n">
-        <v>24777.69865213956</v>
+        <v>24777.70083089388</v>
       </c>
       <c r="J61" t="n">
-        <v>24666.86874328218</v>
+        <v>24666.87092203651</v>
       </c>
       <c r="K61" t="n">
-        <v>24777.69823671292</v>
+        <v>24777.70041546725</v>
       </c>
     </row>
     <row r="62">
@@ -10569,19 +10599,19 @@
         <v>136.08</v>
       </c>
       <c r="G62" t="n">
-        <v>254.0373011945594</v>
+        <v>254.0407125614074</v>
       </c>
       <c r="H62" t="n">
-        <v>24666.67341136685</v>
+        <v>24666.67</v>
       </c>
       <c r="I62" t="n">
-        <v>24851.46269880544</v>
+        <v>24851.45928743859</v>
       </c>
       <c r="J62" t="n">
-        <v>24666.67557943383</v>
+        <v>24666.67216806698</v>
       </c>
       <c r="K62" t="n">
-        <v>24851.46137540675</v>
+        <v>24851.4579640399</v>
       </c>
     </row>
     <row r="63">
@@ -10595,19 +10625,19 @@
         <v>135.98</v>
       </c>
       <c r="G63" t="n">
-        <v>956.9911474660912</v>
+        <v>956.9893457400431</v>
       </c>
       <c r="H63" t="n">
-        <v>24666.47819827395</v>
+        <v>24666.48</v>
       </c>
       <c r="I63" t="n">
-        <v>24969.10885253391</v>
+        <v>24969.11065425996</v>
       </c>
       <c r="J63" t="n">
-        <v>24666.48319222357</v>
+        <v>24666.48499394962</v>
       </c>
       <c r="K63" t="n">
-        <v>24969.10524188694</v>
+        <v>24969.10704361298</v>
       </c>
     </row>
     <row r="64">
@@ -10621,19 +10651,19 @@
         <v>135.88</v>
       </c>
       <c r="G64" t="n">
-        <v>681.4102218081462</v>
+        <v>681.4151662467921</v>
       </c>
       <c r="H64" t="n">
-        <v>24666.02494443865</v>
+        <v>24666.02</v>
       </c>
       <c r="I64" t="n">
-        <v>25152.98977819186</v>
+        <v>25152.98483375321</v>
       </c>
       <c r="J64" t="n">
-        <v>24666.03621367567</v>
+        <v>24666.03126923703</v>
       </c>
       <c r="K64" t="n">
-        <v>25152.98073479908</v>
+        <v>25152.97579036043</v>
       </c>
     </row>
     <row r="65">
@@ -10647,19 +10677,19 @@
         <v>135.78</v>
       </c>
       <c r="G65" t="n">
-        <v>892.9886600440768</v>
+        <v>892.9864982862564</v>
       </c>
       <c r="H65" t="n">
-        <v>24665.37783824218</v>
+        <v>24665.38</v>
       </c>
       <c r="I65" t="n">
-        <v>25435.51133995592</v>
+        <v>25435.51350171374</v>
       </c>
       <c r="J65" t="n">
-        <v>24665.40275308979</v>
+        <v>24665.40491484761</v>
       </c>
       <c r="K65" t="n">
-        <v>25435.48994519465</v>
+        <v>25435.49210695247</v>
       </c>
     </row>
     <row r="66">
@@ -10673,19 +10703,19 @@
         <v>135.68</v>
       </c>
       <c r="G66" t="n">
-        <v>898.6287509427493</v>
+        <v>898.6308616798633</v>
       </c>
       <c r="H66" t="n">
-        <v>24664.62211073711</v>
+        <v>24664.62</v>
       </c>
       <c r="I66" t="n">
-        <v>25862.07124905725</v>
+        <v>25862.06913832014</v>
       </c>
       <c r="J66" t="n">
-        <v>24664.67608323047</v>
+        <v>24664.67397249335</v>
       </c>
       <c r="K66" t="n">
-        <v>25862.02274963054</v>
+        <v>25862.02063889342</v>
       </c>
     </row>
     <row r="67">
@@ -10699,19 +10729,19 @@
         <v>135.58</v>
       </c>
       <c r="G67" t="n">
-        <v>560.8964242282127</v>
+        <v>560.8957618625172</v>
       </c>
       <c r="H67" t="n">
-        <v>24663.6193376343</v>
+        <v>24663.62</v>
       </c>
       <c r="I67" t="n">
-        <v>26494.70357577179</v>
+        <v>26494.70423813748</v>
       </c>
       <c r="J67" t="n">
-        <v>24663.73390933783</v>
+        <v>24663.73457170352</v>
       </c>
       <c r="K67" t="n">
-        <v>26494.59737286896</v>
+        <v>26494.59803523465</v>
       </c>
     </row>
     <row r="68">
@@ -10725,19 +10755,19 @@
         <v>135.48</v>
       </c>
       <c r="G68" t="n">
-        <v>532.151169513796</v>
+        <v>532.1519816452965</v>
       </c>
       <c r="H68" t="n">
-        <v>24662.4208121315</v>
+        <v>24662.42</v>
       </c>
       <c r="I68" t="n">
-        <v>27416.9488304862</v>
+        <v>27416.9480183547</v>
       </c>
       <c r="J68" t="n">
-        <v>24662.65916274437</v>
+        <v>24662.65835061287</v>
       </c>
       <c r="K68" t="n">
-        <v>27416.72306844352</v>
+        <v>27416.72225631202</v>
       </c>
     </row>
     <row r="69">
@@ -10751,19 +10781,19 @@
         <v>135.38</v>
       </c>
       <c r="G69" t="n">
-        <v>-20.33854386179883</v>
+        <v>-20.33575649244449</v>
       </c>
       <c r="H69" t="n">
-        <v>24660.90278736936</v>
+        <v>24660.9</v>
       </c>
       <c r="I69" t="n">
-        <v>28738.2385438618</v>
+        <v>28738.23575649245</v>
       </c>
       <c r="J69" t="n">
-        <v>24661.38878722521</v>
+        <v>24661.38599985585</v>
       </c>
       <c r="K69" t="n">
-        <v>28737.77117648587</v>
+        <v>28737.76838911651</v>
       </c>
     </row>
     <row r="70">
@@ -10777,19 +10807,19 @@
         <v>135.28</v>
       </c>
       <c r="G70" t="n">
-        <v>119.1531742164261</v>
+        <v>119.1487001380483</v>
       </c>
       <c r="H70" t="n">
-        <v>24658.93552592162</v>
+        <v>24658.94</v>
       </c>
       <c r="I70" t="n">
-        <v>30598.44682578357</v>
+        <v>30598.45129986195</v>
       </c>
       <c r="J70" t="n">
-        <v>24659.90690303612</v>
+        <v>24659.9113771145</v>
       </c>
       <c r="K70" t="n">
-        <v>30597.50258788775</v>
+        <v>30597.50706196613</v>
       </c>
     </row>
     <row r="71">
@@ -10803,19 +10833,19 @@
         <v>135.18</v>
       </c>
       <c r="G71" t="n">
-        <v>-390.516074667561</v>
+        <v>-390.5161594470555</v>
       </c>
       <c r="H71" t="n">
-        <v>24656.21991522051</v>
+        <v>24656.22</v>
       </c>
       <c r="I71" t="n">
-        <v>33170.31607466756</v>
+        <v>33170.31615944706</v>
       </c>
       <c r="J71" t="n">
-        <v>24658.12330043115</v>
+        <v>24658.12338521065</v>
       </c>
       <c r="K71" t="n">
-        <v>33168.45158687868</v>
+        <v>33168.45167165816</v>
       </c>
     </row>
     <row r="72">
@@ -10829,19 +10859,19 @@
         <v>135.08</v>
       </c>
       <c r="G72" t="n">
-        <v>-107.3474697287966</v>
+        <v>-107.3454487896015</v>
       </c>
       <c r="H72" t="n">
-        <v>24652.40202093919</v>
+        <v>24652.4</v>
       </c>
       <c r="I72" t="n">
-        <v>36657.4474697288</v>
+        <v>36657.4454487896</v>
       </c>
       <c r="J72" t="n">
-        <v>24656.05891709149</v>
+        <v>24656.0568961523</v>
       </c>
       <c r="K72" t="n">
-        <v>36653.84540873786</v>
+        <v>36653.84338779867</v>
       </c>
     </row>
     <row r="73">
@@ -10855,19 +10885,19 @@
         <v>134.98</v>
       </c>
       <c r="G73" t="n">
-        <v>38.78597678784718</v>
+        <v>38.78599370734446</v>
       </c>
       <c r="H73" t="n">
-        <v>24646.9900169195</v>
+        <v>24646.99</v>
       </c>
       <c r="I73" t="n">
-        <v>41281.71402321215</v>
+        <v>41281.71400629266</v>
       </c>
       <c r="J73" t="n">
-        <v>24653.87988574691</v>
+        <v>24653.87986882741</v>
       </c>
       <c r="K73" t="n">
-        <v>41274.90011585334</v>
+        <v>41274.90009893384</v>
       </c>
     </row>
     <row r="74">
@@ -10881,19 +10911,19 @@
         <v>134.88</v>
       </c>
       <c r="G74" t="n">
-        <v>118.624065561271</v>
+        <v>118.6201939058883</v>
       </c>
       <c r="H74" t="n">
-        <v>24639.23612834462</v>
+        <v>24639.24</v>
       </c>
       <c r="I74" t="n">
-        <v>47250.07593443873</v>
+        <v>47250.07980609411</v>
       </c>
       <c r="J74" t="n">
-        <v>24651.96801358289</v>
+        <v>24651.97188523827</v>
       </c>
       <c r="K74" t="n">
-        <v>47237.44726225547</v>
+        <v>47237.45113391086</v>
       </c>
     </row>
     <row r="75">
@@ -10907,19 +10937,19 @@
         <v>134.78</v>
       </c>
       <c r="G75" t="n">
-        <v>858.9491362543631</v>
+        <v>858.9461275442445</v>
       </c>
       <c r="H75" t="n">
-        <v>24628.47699128988</v>
+        <v>24628.48</v>
       </c>
       <c r="I75" t="n">
-        <v>54685.35086374564</v>
+        <v>54685.35387245576</v>
       </c>
       <c r="J75" t="n">
-        <v>24651.55696303898</v>
+        <v>24651.55997174911</v>
       </c>
       <c r="K75" t="n">
-        <v>54662.4080249587</v>
+        <v>54662.41103366882</v>
       </c>
     </row>
     <row r="76">
@@ -10933,19 +10963,19 @@
         <v>134.68</v>
       </c>
       <c r="G76" t="n">
-        <v>-109.6388987957689</v>
+        <v>-109.6400181099671</v>
       </c>
       <c r="H76" t="n">
-        <v>24613.7488806858</v>
+        <v>24613.75</v>
       </c>
       <c r="I76" t="n">
-        <v>63501.53889879577</v>
+        <v>63501.54001810997</v>
       </c>
       <c r="J76" t="n">
-        <v>24654.79979739772</v>
+        <v>24654.80091671192</v>
       </c>
       <c r="K76" t="n">
-        <v>63460.66527939703</v>
+        <v>63460.66639871123</v>
       </c>
     </row>
     <row r="77">
@@ -10959,19 +10989,19 @@
         <v>134.58</v>
       </c>
       <c r="G77" t="n">
-        <v>450.3887955897953</v>
+        <v>450.3889992333716</v>
       </c>
       <c r="H77" t="n">
-        <v>24594.48020364359</v>
+        <v>24594.48</v>
       </c>
       <c r="I77" t="n">
-        <v>73223.5112044102</v>
+        <v>73223.51100076662</v>
       </c>
       <c r="J77" t="n">
-        <v>24666.13530823815</v>
+        <v>24666.13510459456</v>
       </c>
       <c r="K77" t="n">
-        <v>73152.07758013647</v>
+        <v>73152.07737649287</v>
       </c>
     </row>
     <row r="78">
@@ -10985,19 +11015,19 @@
         <v>134.48</v>
       </c>
       <c r="G78" t="n">
-        <v>710.4133964409557</v>
+        <v>710.4177324953198</v>
       </c>
       <c r="H78" t="n">
-        <v>24569.99433605436</v>
+        <v>24569.99</v>
       </c>
       <c r="I78" t="n">
-        <v>82808.78660355904</v>
+        <v>82808.78226750468</v>
       </c>
       <c r="J78" t="n">
-        <v>24692.76869671101</v>
+        <v>24692.76436065665</v>
       </c>
       <c r="K78" t="n">
-        <v>82686.27707375004</v>
+        <v>82686.27273769568</v>
       </c>
     </row>
     <row r="79">
@@ -11011,19 +11041,19 @@
         <v>134.38</v>
       </c>
       <c r="G79" t="n">
-        <v>653.9273549218633</v>
+        <v>653.9315884959506</v>
       </c>
       <c r="H79" t="n">
-        <v>24539.77423357409</v>
+        <v>24539.77</v>
       </c>
       <c r="I79" t="n">
-        <v>90647.77264507813</v>
+        <v>90647.76841150405</v>
       </c>
       <c r="J79" t="n">
-        <v>24746.31814560902</v>
+        <v>24746.31391203493</v>
       </c>
       <c r="K79" t="n">
-        <v>90441.52858974879</v>
+        <v>90441.5243561747</v>
       </c>
     </row>
     <row r="80">
@@ -11037,19 +11067,19 @@
         <v>134.28</v>
       </c>
       <c r="G80" t="n">
-        <v>-1109.856424231111</v>
+        <v>-1109.860877563304</v>
       </c>
       <c r="H80" t="n">
-        <v>24504.70554666781</v>
+        <v>24504.71</v>
       </c>
       <c r="I80" t="n">
-        <v>94972.95642423112</v>
+        <v>94972.96087756331</v>
       </c>
       <c r="J80" t="n">
-        <v>24845.95947264163</v>
+        <v>24845.96392597381</v>
       </c>
       <c r="K80" t="n">
-        <v>94632.02076623341</v>
+        <v>94632.02521956561</v>
       </c>
     </row>
     <row r="81">
@@ -11063,19 +11093,19 @@
         <v>134.18</v>
       </c>
       <c r="G81" t="n">
-        <v>209.4728408498049</v>
+        <v>209.4698187130853</v>
       </c>
       <c r="H81" t="n">
-        <v>24466.93697786327</v>
+        <v>24466.94</v>
       </c>
       <c r="I81" t="n">
-        <v>94659.0271591502</v>
+        <v>94659.03018128691</v>
       </c>
       <c r="J81" t="n">
-        <v>25020.83275867673</v>
+        <v>25020.83578081346</v>
       </c>
       <c r="K81" t="n">
-        <v>94105.44598470631</v>
+        <v>94105.44900684305</v>
       </c>
     </row>
     <row r="82">
@@ -11089,19 +11119,19 @@
         <v>134.08</v>
       </c>
       <c r="G82" t="n">
-        <v>-398.6019033565244</v>
+        <v>-398.6052207686298</v>
       </c>
       <c r="H82" t="n">
-        <v>24428.61668258791</v>
+        <v>24428.62</v>
       </c>
       <c r="I82" t="n">
-        <v>89887.50190335652</v>
+        <v>89887.50522076862</v>
       </c>
       <c r="J82" t="n">
-        <v>25312.09422438189</v>
+        <v>25312.09754179398</v>
       </c>
       <c r="K82" t="n">
-        <v>89004.31361323496</v>
+        <v>89004.31693064705</v>
       </c>
     </row>
     <row r="83">
@@ -11115,19 +11145,19 @@
         <v>133.98</v>
       </c>
       <c r="G83" t="n">
-        <v>-409.5962394862145</v>
+        <v>-409.5990821751911</v>
       </c>
       <c r="H83" t="n">
-        <v>24392.24715731102</v>
+        <v>24392.25</v>
       </c>
       <c r="I83" t="n">
-        <v>82065.29623948621</v>
+        <v>82065.29908217519</v>
       </c>
       <c r="J83" t="n">
-        <v>25777.46225494104</v>
+        <v>25777.46509763002</v>
       </c>
       <c r="K83" t="n">
-        <v>80680.32914246939</v>
+        <v>80680.33198515838</v>
       </c>
     </row>
     <row r="84">
@@ -11141,19 +11171,19 @@
         <v>133.88</v>
       </c>
       <c r="G84" t="n">
-        <v>-219.2718542125367</v>
+        <v>-219.2754036654369</v>
       </c>
       <c r="H84" t="n">
-        <v>24360.02645054711</v>
+        <v>24360.03</v>
       </c>
       <c r="I84" t="n">
-        <v>73080.37185421254</v>
+        <v>73080.37540366544</v>
       </c>
       <c r="J84" t="n">
-        <v>26495.68480524588</v>
+        <v>26495.68835469878</v>
       </c>
       <c r="K84" t="n">
-        <v>70944.91210902992</v>
+        <v>70944.91565848282</v>
       </c>
     </row>
     <row r="85">
@@ -11167,19 +11197,19 @@
         <v>133.78</v>
       </c>
       <c r="G85" t="n">
-        <v>666.9706596469259</v>
+        <v>666.9690062067384</v>
       </c>
       <c r="H85" t="n">
-        <v>24332.58834655982</v>
+        <v>24332.59</v>
       </c>
       <c r="I85" t="n">
-        <v>64561.02934035307</v>
+        <v>64561.03099379326</v>
       </c>
       <c r="J85" t="n">
-        <v>27571.30157582561</v>
+        <v>27571.30322926579</v>
       </c>
       <c r="K85" t="n">
-        <v>61322.46345734411</v>
+        <v>61322.46511078429</v>
       </c>
     </row>
     <row r="86">
@@ -11193,19 +11223,19 @@
         <v>133.68</v>
       </c>
       <c r="G86" t="n">
-        <v>253.643571180015</v>
+        <v>253.6409861474895</v>
       </c>
       <c r="H86" t="n">
-        <v>24309.69741496748</v>
+        <v>24309.7</v>
       </c>
       <c r="I86" t="n">
-        <v>57571.35642881999</v>
+        <v>57571.35901385251</v>
       </c>
       <c r="J86" t="n">
-        <v>29142.02064913041</v>
+        <v>29142.02323416294</v>
       </c>
       <c r="K86" t="n">
-        <v>52739.13071421302</v>
+        <v>52739.13329924556</v>
       </c>
     </row>
     <row r="87">
@@ -11219,19 +11249,19 @@
         <v>133.58</v>
       </c>
       <c r="G87" t="n">
-        <v>30.51771542183269</v>
+        <v>30.52255851968221</v>
       </c>
       <c r="H87" t="n">
-        <v>24290.78484309785</v>
+        <v>24290.78</v>
       </c>
       <c r="I87" t="n">
-        <v>52674.68228457816</v>
+        <v>52674.67744148031</v>
       </c>
       <c r="J87" t="n">
-        <v>31385.96658206957</v>
+        <v>31385.96173897172</v>
       </c>
       <c r="K87" t="n">
-        <v>45579.55023645869</v>
+        <v>45579.54539336084</v>
       </c>
     </row>
     <row r="88">
@@ -11245,19 +11275,19 @@
         <v>133.48</v>
       </c>
       <c r="G88" t="n">
-        <v>-615.6530686090919</v>
+        <v>-615.6564458582361</v>
       </c>
       <c r="H88" t="n">
-        <v>24274.91662275086</v>
+        <v>24274.92</v>
       </c>
       <c r="I88" t="n">
-        <v>50128.05306860909</v>
+        <v>50128.05644585824</v>
       </c>
       <c r="J88" t="n">
-        <v>34526.97709945189</v>
+        <v>34526.98047670103</v>
       </c>
       <c r="K88" t="n">
-        <v>39875.99509520378</v>
+        <v>39875.99847245292</v>
       </c>
     </row>
     <row r="89">
@@ -11271,19 +11301,19 @@
         <v>133.38</v>
       </c>
       <c r="G89" t="n">
-        <v>-735.832786751489</v>
+        <v>-735.8358925049106</v>
       </c>
       <c r="H89" t="n">
-        <v>24260.80689424658</v>
+        <v>24260.81</v>
       </c>
       <c r="I89" t="n">
-        <v>50055.43278675149</v>
+        <v>50055.43589250491</v>
       </c>
       <c r="J89" t="n">
-        <v>38835.59516951958</v>
+        <v>38835.59827527301</v>
       </c>
       <c r="K89" t="n">
-        <v>35480.59797384302</v>
+        <v>35480.60107959645</v>
       </c>
     </row>
     <row r="90">
@@ -11297,19 +11327,19 @@
         <v>133.28</v>
       </c>
       <c r="G90" t="n">
-        <v>159.4015465158809</v>
+        <v>159.40020996979</v>
       </c>
       <c r="H90" t="n">
-        <v>24246.87866345391</v>
+        <v>24246.88</v>
       </c>
       <c r="I90" t="n">
-        <v>52551.09845348412</v>
+        <v>52551.09979003021</v>
       </c>
       <c r="J90" t="n">
-        <v>44619.84375152897</v>
+        <v>44619.84508807506</v>
       </c>
       <c r="K90" t="n">
-        <v>32178.03287840137</v>
+        <v>32178.03421494746</v>
       </c>
     </row>
     <row r="91">
@@ -11323,19 +11353,19 @@
         <v>133.18</v>
       </c>
       <c r="G91" t="n">
-        <v>-1206.444234506744</v>
+        <v>-1206.439780072142</v>
       </c>
       <c r="H91" t="n">
-        <v>24231.58445443461</v>
+        <v>24231.58</v>
       </c>
       <c r="I91" t="n">
-        <v>57710.34423450675</v>
+        <v>57710.33978007214</v>
       </c>
       <c r="J91" t="n">
-        <v>52194.90353843783</v>
+        <v>52194.89908400322</v>
       </c>
       <c r="K91" t="n">
-        <v>29746.86267470285</v>
+        <v>29746.85822026823</v>
       </c>
     </row>
     <row r="92">
@@ -11349,19 +11379,19 @@
         <v>133.08</v>
       </c>
       <c r="G92" t="n">
-        <v>633.4058409350982</v>
+        <v>633.4026596578333</v>
       </c>
       <c r="H92" t="n">
-        <v>24213.49681872274</v>
+        <v>24213.5</v>
       </c>
       <c r="I92" t="n">
-        <v>65586.7941590649</v>
+        <v>65586.79734034216</v>
       </c>
       <c r="J92" t="n">
-        <v>61812.39099794308</v>
+        <v>61812.39417922033</v>
       </c>
       <c r="K92" t="n">
-        <v>27987.66487237422</v>
+        <v>27987.66805365148</v>
       </c>
     </row>
     <row r="93">
@@ -11375,19 +11405,19 @@
         <v>132.98</v>
       </c>
       <c r="G93" t="n">
-        <v>686.5358390911133</v>
+        <v>686.5369515893981</v>
       </c>
       <c r="H93" t="n">
-        <v>24190.71111249828</v>
+        <v>24190.71</v>
       </c>
       <c r="I93" t="n">
-        <v>76064.56416090889</v>
+        <v>76064.56304841061</v>
       </c>
       <c r="J93" t="n">
-        <v>73522.62994801336</v>
+        <v>73522.62883551508</v>
       </c>
       <c r="K93" t="n">
-        <v>26732.32583306896</v>
+        <v>26732.32472057067</v>
       </c>
     </row>
     <row r="94">
@@ -11401,19 +11431,19 @@
         <v>132.88</v>
       </c>
       <c r="G94" t="n">
-        <v>2078.460445095989</v>
+        <v>2078.456262653388</v>
       </c>
       <c r="H94" t="n">
-        <v>24161.5158175574</v>
+        <v>24161.52</v>
       </c>
       <c r="I94" t="n">
-        <v>88636.23955490401</v>
+        <v>88636.24373734661</v>
       </c>
       <c r="J94" t="n">
-        <v>86951.72754301279</v>
+        <v>86951.73172545539</v>
       </c>
       <c r="K94" t="n">
-        <v>25845.61408679148</v>
+        <v>25845.61826923408</v>
       </c>
     </row>
     <row r="95">
@@ -11427,19 +11457,19 @@
         <v>132.78</v>
       </c>
       <c r="G95" t="n">
-        <v>-226.2277776386618</v>
+        <v>-226.2277474439179</v>
       </c>
       <c r="H95" t="n">
-        <v>24125.04003019476</v>
+        <v>24125.04</v>
       </c>
       <c r="I95" t="n">
-        <v>102121.2277776387</v>
+        <v>102121.2277474439</v>
       </c>
       <c r="J95" t="n">
-        <v>101023.0106739246</v>
+        <v>101023.0106437299</v>
       </c>
       <c r="K95" t="n">
-        <v>25222.74602111023</v>
+        <v>25222.74599091548</v>
       </c>
     </row>
     <row r="96">
@@ -11453,19 +11483,19 @@
         <v>132.68</v>
       </c>
       <c r="G96" t="n">
-        <v>1309.74664264411</v>
+        <v>1309.749118604988</v>
       </c>
       <c r="H96" t="n">
-        <v>24081.04247596088</v>
+        <v>24081.04</v>
       </c>
       <c r="I96" t="n">
-        <v>114489.2533573559</v>
+        <v>114489.250881395</v>
       </c>
       <c r="J96" t="n">
-        <v>113785.0382911341</v>
+        <v>113785.0358151732</v>
       </c>
       <c r="K96" t="n">
-        <v>24784.65867536528</v>
+        <v>24784.65619940441</v>
       </c>
     </row>
     <row r="97">
@@ -11479,19 +11509,19 @@
         <v>132.58</v>
       </c>
       <c r="G97" t="n">
-        <v>-693.6355481594219</v>
+        <v>-693.6326344683766</v>
       </c>
       <c r="H97" t="n">
-        <v>24030.18291369104</v>
+        <v>24030.18</v>
       </c>
       <c r="I97" t="n">
-        <v>123113.6355481594</v>
+        <v>123113.6326344684</v>
       </c>
       <c r="J97" t="n">
-        <v>122669.5926009213</v>
+        <v>122669.5896872303</v>
       </c>
       <c r="K97" t="n">
-        <v>24473.56583107038</v>
+        <v>24473.56291737934</v>
       </c>
     </row>
     <row r="98">
@@ -11505,19 +11535,19 @@
         <v>132.48</v>
       </c>
       <c r="G98" t="n">
-        <v>-1774.977651742985</v>
+        <v>-1774.974067816613</v>
       </c>
       <c r="H98" t="n">
-        <v>23975.34358392637</v>
+        <v>23975.34</v>
       </c>
       <c r="I98" t="n">
-        <v>125681.977651743</v>
+        <v>125681.9740678166</v>
       </c>
       <c r="J98" t="n">
-        <v>125406.7127884148</v>
+        <v>125406.7092044885</v>
       </c>
       <c r="K98" t="n">
-        <v>24249.92890648864</v>
+        <v>24249.92532256227</v>
       </c>
     </row>
     <row r="99">
@@ -11531,19 +11561,19 @@
         <v>132.38</v>
       </c>
       <c r="G99" t="n">
-        <v>136.9193003296677</v>
+        <v>136.9231750479667</v>
       </c>
       <c r="H99" t="n">
-        <v>23919.83387471831</v>
+        <v>23919.83</v>
       </c>
       <c r="I99" t="n">
-        <v>121373.0806996703</v>
+        <v>121373.076824952</v>
       </c>
       <c r="J99" t="n">
-        <v>121205.3589966263</v>
+        <v>121205.355121908</v>
       </c>
       <c r="K99" t="n">
-        <v>24086.90337197004</v>
+        <v>24086.89949725173</v>
       </c>
     </row>
     <row r="100">
@@ -11557,19 +11587,19 @@
         <v>132.28</v>
       </c>
       <c r="G100" t="n">
-        <v>671.7016455352277</v>
+        <v>671.6979805861338</v>
       </c>
       <c r="H100" t="n">
-        <v>23867.03633505091</v>
+        <v>23867.04</v>
       </c>
       <c r="I100" t="n">
-        <v>111334.2983544648</v>
+        <v>111334.3020194139</v>
       </c>
       <c r="J100" t="n">
-        <v>111233.8708025972</v>
+        <v>111233.8744675463</v>
       </c>
       <c r="K100" t="n">
-        <v>23966.8779469553</v>
+        <v>23966.88161190439</v>
       </c>
     </row>
     <row r="101">
@@ -11583,19 +11613,19 @@
         <v>132.18</v>
       </c>
       <c r="G101" t="n">
-        <v>-281.285420175278</v>
+        <v>-281.2885526031605</v>
       </c>
       <c r="H101" t="n">
-        <v>23820.67686757211</v>
+        <v>23820.68</v>
       </c>
       <c r="I101" t="n">
-        <v>97985.48542017528</v>
+        <v>97985.48855260316</v>
       </c>
       <c r="J101" t="n">
-        <v>97926.4012393002</v>
+        <v>97926.4043717281</v>
       </c>
       <c r="K101" t="n">
-        <v>23879.26392698235</v>
+        <v>23879.26705941024</v>
       </c>
     </row>
     <row r="102">
@@ -11609,19 +11639,19 @@
         <v>132.08</v>
       </c>
       <c r="G102" t="n">
-        <v>-957.7147056969552</v>
+        <v>-957.7148372858355</v>
       </c>
       <c r="H102" t="n">
-        <v>23782.76986841113</v>
+        <v>23782.77</v>
       </c>
       <c r="I102" t="n">
-        <v>83816.81470569696</v>
+        <v>83816.81483728584</v>
       </c>
       <c r="J102" t="n">
-        <v>83782.6634440551</v>
+        <v>83782.66357564396</v>
       </c>
       <c r="K102" t="n">
-        <v>23816.51857179659</v>
+        <v>23816.51870338546</v>
       </c>
     </row>
     <row r="103">
@@ -11635,19 +11665,19 @@
         <v>131.98</v>
       </c>
       <c r="G103" t="n">
-        <v>250.6245745542692</v>
+        <v>250.6276291811664</v>
       </c>
       <c r="H103" t="n">
-        <v>23752.8430546269</v>
+        <v>23752.84</v>
       </c>
       <c r="I103" t="n">
-        <v>70599.27542544572</v>
+        <v>70599.27237081883</v>
       </c>
       <c r="J103" t="n">
-        <v>70579.88133115084</v>
+        <v>70579.87827652394</v>
       </c>
       <c r="K103" t="n">
-        <v>23771.92293833326</v>
+        <v>23771.91988370637</v>
       </c>
     </row>
     <row r="104">
@@ -11661,19 +11691,19 @@
         <v>131.88</v>
       </c>
       <c r="G104" t="n">
-        <v>-394.754850777048</v>
+        <v>-394.7554415117556</v>
       </c>
       <c r="H104" t="n">
-        <v>23729.90940926529</v>
+        <v>23729.91</v>
       </c>
       <c r="I104" t="n">
-        <v>59241.95485077705</v>
+        <v>59241.95544151175</v>
       </c>
       <c r="J104" t="n">
-        <v>59231.13228299493</v>
+        <v>59231.13287372964</v>
       </c>
       <c r="K104" t="n">
-        <v>23740.49374522175</v>
+        <v>23740.49433595646</v>
       </c>
     </row>
     <row r="105">
@@ -11687,19 +11717,19 @@
         <v>131.78</v>
       </c>
       <c r="G105" t="n">
-        <v>-1784.374903940181</v>
+        <v>-1784.373164752782</v>
       </c>
       <c r="H105" t="n">
-        <v>23713.39173918739</v>
+        <v>23713.39</v>
       </c>
       <c r="I105" t="n">
-        <v>50007.27490394018</v>
+        <v>50007.27316475278</v>
       </c>
       <c r="J105" t="n">
-        <v>50001.33833082646</v>
+        <v>50001.33659163906</v>
       </c>
       <c r="K105" t="n">
-        <v>23719.15189689594</v>
+        <v>23719.15015770855</v>
       </c>
     </row>
     <row r="106">
@@ -11713,19 +11743,19 @@
         <v>131.68</v>
       </c>
       <c r="G106" t="n">
-        <v>-1572.336718242004</v>
+        <v>-1572.33281085745</v>
       </c>
       <c r="H106" t="n">
-        <v>23701.85390738455</v>
+        <v>23701.85</v>
       </c>
       <c r="I106" t="n">
-        <v>42784.836718242</v>
+        <v>42784.83281085745</v>
       </c>
       <c r="J106" t="n">
-        <v>42781.63392924835</v>
+        <v>42781.63002186379</v>
       </c>
       <c r="K106" t="n">
-        <v>23704.92864909956</v>
+        <v>23704.924741715</v>
       </c>
     </row>
     <row r="107">
@@ -11739,19 +11769,19 @@
         <v>131.58</v>
       </c>
       <c r="G107" t="n">
-        <v>-195.2469793083073</v>
+        <v>-195.2493167640496</v>
       </c>
       <c r="H107" t="n">
-        <v>23693.44766254426</v>
+        <v>23693.45</v>
       </c>
       <c r="I107" t="n">
-        <v>37297.64697930831</v>
+        <v>37297.64931676405</v>
       </c>
       <c r="J107" t="n">
-        <v>37295.94610463686</v>
+        <v>37295.9484420926</v>
       </c>
       <c r="K107" t="n">
-        <v>23695.05724613646</v>
+        <v>23695.0595835922</v>
       </c>
     </row>
     <row r="108">
@@ -11765,19 +11795,19 @@
         <v>131.48</v>
       </c>
       <c r="G108" t="n">
-        <v>568.0536250378718</v>
+        <v>568.0578299858898</v>
       </c>
       <c r="H108" t="n">
-        <v>23687.09420494802</v>
+        <v>23687.09</v>
       </c>
       <c r="I108" t="n">
-        <v>33224.74637496213</v>
+        <v>33224.74217001411</v>
       </c>
       <c r="J108" t="n">
-        <v>33223.85617491544</v>
+        <v>33223.85196996742</v>
       </c>
       <c r="K108" t="n">
-        <v>23687.92039909959</v>
+        <v>23687.91619415157</v>
       </c>
     </row>
     <row r="109">
@@ -11791,19 +11821,19 @@
         <v>131.38</v>
       </c>
       <c r="G109" t="n">
-        <v>431.1875002451561</v>
+        <v>431.1877162524579</v>
       </c>
       <c r="H109" t="n">
-        <v>23682.4802160073</v>
+        <v>23682.48</v>
       </c>
       <c r="I109" t="n">
-        <v>30261.91249975484</v>
+        <v>30261.91228374754</v>
       </c>
       <c r="J109" t="n">
-        <v>30261.45257462961</v>
+        <v>30261.45235862231</v>
       </c>
       <c r="K109" t="n">
-        <v>23682.89598571191</v>
+        <v>23682.89576970461</v>
       </c>
     </row>
     <row r="110">
@@ -11817,19 +11847,19 @@
         <v>131.28</v>
       </c>
       <c r="G110" t="n">
-        <v>1153.761831465759</v>
+        <v>1153.758122683015</v>
       </c>
       <c r="H110" t="n">
-        <v>23679.08629121726</v>
+        <v>23679.09</v>
       </c>
       <c r="I110" t="n">
-        <v>28145.73816853424</v>
+        <v>28145.74187731698</v>
       </c>
       <c r="J110" t="n">
-        <v>28145.50308976591</v>
+        <v>28145.50679854866</v>
       </c>
       <c r="K110" t="n">
-        <v>23679.29139283685</v>
+        <v>23679.29510161959</v>
       </c>
     </row>
     <row r="111">
@@ -11843,19 +11873,19 @@
         <v>131.18</v>
       </c>
       <c r="G111" t="n">
-        <v>1043.162073831027</v>
+        <v>1043.163014364392</v>
       </c>
       <c r="H111" t="n">
-        <v>23676.50094053337</v>
+        <v>23676.5</v>
       </c>
       <c r="I111" t="n">
-        <v>26660.43792616897</v>
+        <v>26660.43698563561</v>
       </c>
       <c r="J111" t="n">
-        <v>26660.31872993907</v>
+        <v>26660.31778940571</v>
       </c>
       <c r="K111" t="n">
-        <v>23676.60011016779</v>
+        <v>23676.59916963443</v>
       </c>
     </row>
     <row r="112">
@@ -11869,19 +11899,19 @@
         <v>131.08</v>
       </c>
       <c r="G112" t="n">
-        <v>974.8716051838492</v>
+        <v>974.8675629441132</v>
       </c>
       <c r="H112" t="n">
-        <v>23674.63595776026</v>
+        <v>23674.64</v>
       </c>
       <c r="I112" t="n">
-        <v>25635.82839481615</v>
+        <v>25635.83243705589</v>
       </c>
       <c r="J112" t="n">
-        <v>25635.76823908391</v>
+        <v>25635.77228132365</v>
       </c>
       <c r="K112" t="n">
-        <v>23674.68295080842</v>
+        <v>23674.68699304816</v>
       </c>
     </row>
     <row r="113">
@@ -11895,19 +11925,19 @@
         <v>130.98</v>
       </c>
       <c r="G113" t="n">
-        <v>840.5090029898493</v>
+        <v>840.5056141860805</v>
       </c>
       <c r="H113" t="n">
-        <v>23673.28661119623</v>
+        <v>23673.29</v>
       </c>
       <c r="I113" t="n">
-        <v>24941.09099701015</v>
+        <v>24941.09438581392</v>
       </c>
       <c r="J113" t="n">
-        <v>24941.06066621245</v>
+        <v>24941.06405501622</v>
       </c>
       <c r="K113" t="n">
-        <v>23673.30843293708</v>
+        <v>23673.31182174085</v>
       </c>
     </row>
     <row r="114">
@@ -11921,19 +11951,19 @@
         <v>130.88</v>
       </c>
       <c r="G114" t="n">
-        <v>1180.863519723214</v>
+        <v>1180.867087072518</v>
       </c>
       <c r="H114" t="n">
-        <v>23672.1935673493</v>
+        <v>23672.19</v>
       </c>
       <c r="I114" t="n">
-        <v>24478.03648027679</v>
+        <v>24478.03291292748</v>
       </c>
       <c r="J114" t="n">
-        <v>24478.02114271028</v>
+        <v>24478.01757536098</v>
       </c>
       <c r="K114" t="n">
-        <v>23672.20349633731</v>
+        <v>23672.19992898801</v>
       </c>
     </row>
     <row r="115">
@@ -11947,19 +11977,19 @@
         <v>130.78</v>
       </c>
       <c r="G115" t="n">
-        <v>1158.10659969836</v>
+        <v>1158.107609357565</v>
       </c>
       <c r="H115" t="n">
-        <v>23671.22100965921</v>
+        <v>23671.22</v>
       </c>
       <c r="I115" t="n">
-        <v>24174.69340030164</v>
+        <v>24174.69239064243</v>
       </c>
       <c r="J115" t="n">
-        <v>24174.68559480871</v>
+        <v>24174.6845851495</v>
       </c>
       <c r="K115" t="n">
-        <v>23671.22543597481</v>
+        <v>23671.2244263156</v>
       </c>
     </row>
     <row r="116">
@@ -11973,19 +12003,19 @@
         <v>130.68</v>
       </c>
       <c r="G116" t="n">
-        <v>1128.310554539996</v>
+        <v>1128.315323369065</v>
       </c>
       <c r="H116" t="n">
-        <v>23670.39476882907</v>
+        <v>23670.39</v>
       </c>
       <c r="I116" t="n">
-        <v>23979.48944546</v>
+        <v>23979.48467663093</v>
       </c>
       <c r="J116" t="n">
-        <v>23979.48543773371</v>
+        <v>23979.48066890464</v>
       </c>
       <c r="K116" t="n">
-        <v>23670.39670198246</v>
+        <v>23670.39193315339</v>
       </c>
     </row>
     <row r="117">
@@ -11999,19 +12029,19 @@
         <v>130.58</v>
       </c>
       <c r="G117" t="n">
-        <v>1282.770279881119</v>
+        <v>1282.770818689452</v>
       </c>
       <c r="H117" t="n">
-        <v>23669.62053880833</v>
+        <v>23669.62</v>
       </c>
       <c r="I117" t="n">
-        <v>23856.02972011888</v>
+        <v>23856.02918131055</v>
       </c>
       <c r="J117" t="n">
-        <v>23856.02764190574</v>
+        <v>23856.02710309741</v>
       </c>
       <c r="K117" t="n">
-        <v>23669.62136588178</v>
+        <v>23669.62082707345</v>
       </c>
     </row>
     <row r="118">
@@ -12025,19 +12055,19 @@
         <v>130.48</v>
       </c>
       <c r="G118" t="n">
-        <v>465.3223790697521</v>
+        <v>465.3272500100975</v>
       </c>
       <c r="H118" t="n">
-        <v>23669.07487094035</v>
+        <v>23669.07</v>
       </c>
       <c r="I118" t="n">
-        <v>23779.47762093025</v>
+        <v>23779.4727499899</v>
       </c>
       <c r="J118" t="n">
-        <v>23779.476533315</v>
+        <v>23779.47166237466</v>
       </c>
       <c r="K118" t="n">
-        <v>23669.07521755365</v>
+        <v>23669.07034661331</v>
       </c>
     </row>
     <row r="119">
@@ -12051,19 +12081,19 @@
         <v>130.38</v>
       </c>
       <c r="G119" t="n">
-        <v>290.6773543044037</v>
+        <v>290.6730257146555</v>
       </c>
       <c r="H119" t="n">
-        <v>23668.82567141025</v>
+        <v>23668.83</v>
       </c>
       <c r="I119" t="n">
-        <v>23733.0226456956</v>
+        <v>23733.02697428535</v>
       </c>
       <c r="J119" t="n">
-        <v>23733.02207253802</v>
+        <v>23733.02640112777</v>
       </c>
       <c r="K119" t="n">
-        <v>23668.82581368947</v>
+        <v>23668.83014227922</v>
       </c>
     </row>
     <row r="120">
@@ -12077,19 +12107,19 @@
         <v>130.28</v>
       </c>
       <c r="G120" t="n">
-        <v>492.9689548710485</v>
+        <v>492.9691917897835</v>
       </c>
       <c r="H120" t="n">
-        <v>23668.59023691874</v>
+        <v>23668.59</v>
       </c>
       <c r="I120" t="n">
-        <v>23705.23104512895</v>
+        <v>23705.23080821022</v>
       </c>
       <c r="J120" t="n">
-        <v>23705.23074200091</v>
+        <v>23705.23050508218</v>
       </c>
       <c r="K120" t="n">
-        <v>23668.59029412009</v>
+        <v>23668.59005720136</v>
       </c>
     </row>
     <row r="121">
@@ -12103,19 +12133,19 @@
         <v>130.18</v>
       </c>
       <c r="G121" t="n">
-        <v>-75.58609490679373</v>
+        <v>-75.5826457909061</v>
       </c>
       <c r="H121" t="n">
-        <v>23668.46344911589</v>
+        <v>23668.46</v>
       </c>
       <c r="I121" t="n">
-        <v>23688.9860949068</v>
+        <v>23688.98264579091</v>
       </c>
       <c r="J121" t="n">
-        <v>23688.98593463986</v>
+        <v>23688.98248552397</v>
       </c>
       <c r="K121" t="n">
-        <v>23668.46347163832</v>
+        <v>23668.46002252243</v>
       </c>
     </row>
     <row r="122">
@@ -12129,19 +12159,19 @@
         <v>130.08</v>
       </c>
       <c r="G122" t="n">
-        <v>24.75416686271637</v>
+        <v>24.75207194840914</v>
       </c>
       <c r="H122" t="n">
-        <v>23668.46790508569</v>
+        <v>23668.47</v>
       </c>
       <c r="I122" t="n">
-        <v>23679.74583313728</v>
+        <v>23679.74792805159</v>
       </c>
       <c r="J122" t="n">
-        <v>23679.7457487572</v>
+        <v>23679.74784367151</v>
       </c>
       <c r="K122" t="n">
-        <v>23668.4679137702</v>
+        <v>23668.4700086845</v>
       </c>
     </row>
     <row r="123">
@@ -12155,19 +12185,19 @@
         <v>129.98</v>
       </c>
       <c r="G123" t="n">
-        <v>9.866304806917469</v>
+        <v>9.870468350789452</v>
       </c>
       <c r="H123" t="n">
-        <v>23668.45416354387</v>
+        <v>23668.45</v>
       </c>
       <c r="I123" t="n">
-        <v>23674.53369519308</v>
+        <v>23674.52953164921</v>
       </c>
       <c r="J123" t="n">
-        <v>23674.53365110902</v>
+        <v>23674.52948756515</v>
       </c>
       <c r="K123" t="n">
-        <v>23668.45416682312</v>
+        <v>23668.45000327925</v>
       </c>
     </row>
     <row r="124">
@@ -12181,19 +12211,19 @@
         <v>129.88</v>
       </c>
       <c r="G124" t="n">
-        <v>29.64457475433301</v>
+        <v>29.64574967641965</v>
       </c>
       <c r="H124" t="n">
-        <v>23668.44117492209</v>
+        <v>23668.44</v>
       </c>
       <c r="I124" t="n">
-        <v>23671.65542524567</v>
+        <v>23671.65425032358</v>
       </c>
       <c r="J124" t="n">
-        <v>23671.65540245963</v>
+        <v>23671.65422753755</v>
       </c>
       <c r="K124" t="n">
-        <v>23668.44117613459</v>
+        <v>23668.4400012125</v>
       </c>
     </row>
     <row r="125">
@@ -12207,19 +12237,19 @@
         <v>129.78</v>
       </c>
       <c r="G125" t="n">
-        <v>-2.699120899920672</v>
+        <v>-2.696434235454944</v>
       </c>
       <c r="H125" t="n">
-        <v>23668.43268666447</v>
+        <v>23668.43</v>
       </c>
       <c r="I125" t="n">
-        <v>23670.09912089992</v>
+        <v>23670.09643423546</v>
       </c>
       <c r="J125" t="n">
-        <v>23670.0991092761</v>
+        <v>23670.09642261163</v>
       </c>
       <c r="K125" t="n">
-        <v>23668.43268710345</v>
+        <v>23668.43000043899</v>
       </c>
     </row>
     <row r="126">
@@ -12233,19 +12263,19 @@
         <v>129.68</v>
       </c>
       <c r="G126" t="n">
-        <v>-518.8171696194695</v>
+        <v>-518.8170935647977</v>
       </c>
       <c r="H126" t="n">
-        <v>23668.57007605467</v>
+        <v>23668.57</v>
       </c>
       <c r="I126" t="n">
-        <v>23669.41716961947</v>
+        <v>23669.4170935648</v>
       </c>
       <c r="J126" t="n">
-        <v>23669.41716377829</v>
+        <v>23669.41708772362</v>
       </c>
       <c r="K126" t="n">
-        <v>23668.57007621029</v>
+        <v>23668.57000015562</v>
       </c>
     </row>
     <row r="127">
@@ -12259,19 +12289,19 @@
         <v>129.58</v>
       </c>
       <c r="G127" t="n">
-        <v>50.58350318758676</v>
+        <v>50.58786605424029</v>
       </c>
       <c r="H127" t="n">
-        <v>23668.69436286665</v>
+        <v>23668.69</v>
       </c>
       <c r="I127" t="n">
-        <v>23669.11649681241</v>
+        <v>23669.11213394576</v>
       </c>
       <c r="J127" t="n">
-        <v>23669.1164939251</v>
+        <v>23669.11213105845</v>
       </c>
       <c r="K127" t="n">
-        <v>23668.69436292067</v>
+        <v>23668.69000005401</v>
       </c>
     </row>
     <row r="128">
@@ -12285,19 +12315,19 @@
         <v>129.48</v>
       </c>
       <c r="G128" t="n">
-        <v>30.12036719385287</v>
+        <v>30.12379911464086</v>
       </c>
       <c r="H128" t="n">
-        <v>23668.67343192079</v>
+        <v>23668.67</v>
       </c>
       <c r="I128" t="n">
-        <v>23668.87963280615</v>
+        <v>23668.87620088536</v>
       </c>
       <c r="J128" t="n">
-        <v>23668.87963140381</v>
+        <v>23668.87619948302</v>
       </c>
       <c r="K128" t="n">
-        <v>23668.67343193914</v>
+        <v>23668.67000001835</v>
       </c>
     </row>
     <row r="129">
@@ -12311,19 +12341,19 @@
         <v>129.38</v>
       </c>
       <c r="G129" t="n">
-        <v>-96.08943194948733</v>
+        <v>-96.08871929624001</v>
       </c>
       <c r="H129" t="n">
-        <v>23668.69071265325</v>
+        <v>23668.69</v>
       </c>
       <c r="I129" t="n">
-        <v>23668.78943194949</v>
+        <v>23668.78871929624</v>
       </c>
       <c r="J129" t="n">
-        <v>23668.78943128079</v>
+        <v>23668.78871862754</v>
       </c>
       <c r="K129" t="n">
-        <v>23668.69071265935</v>
+        <v>23668.69000000611</v>
       </c>
     </row>
     <row r="130">
@@ -21724,13 +21754,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:AD2"/>
+  <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="6" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
@@ -21740,11 +21770,15 @@
     <col width="14" customWidth="1" min="6" max="6"/>
     <col width="15" customWidth="1" min="7" max="7"/>
     <col width="12" customWidth="1" min="8" max="8"/>
-    <col width="6" customWidth="1" min="9" max="12"/>
-    <col width="8" customWidth="1" min="13" max="13"/>
+    <col width="6" customWidth="1" min="9" max="9"/>
+    <col width="6" customWidth="1" min="10" max="10"/>
+    <col width="6" customWidth="1" min="11" max="11"/>
+    <col width="8" customWidth="1" min="12" max="12"/>
+    <col width="13" customWidth="1" min="13" max="13"/>
     <col width="15" customWidth="1" min="14" max="14"/>
     <col width="23" customWidth="1" min="15" max="15"/>
-    <col width="12" customWidth="1" min="16" max="17"/>
+    <col width="12" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="17" max="17"/>
     <col width="10" customWidth="1" min="18" max="18"/>
     <col width="14" customWidth="1" min="19" max="19"/>
     <col width="15" customWidth="1" min="20" max="20"/>
@@ -21756,174 +21790,446 @@
     <col width="17" customWidth="1" min="26" max="26"/>
     <col width="16" customWidth="1" min="27" max="27"/>
     <col width="17" customWidth="1" min="28" max="28"/>
-    <col width="14" customWidth="1" min="29" max="30"/>
+    <col width="14" customWidth="1" min="29" max="29"/>
+    <col width="14" customWidth="1" min="30" max="30"/>
   </cols>
   <sheetData>
+    <row r="1"/>
     <row r="2">
-      <c r="B2" s="11" t="inlineStr">
+      <c r="B2" s="33" t="inlineStr">
         <is>
           <t>Peak
 Label</t>
         </is>
       </c>
-      <c r="C2" s="11" t="inlineStr">
+      <c r="C2" s="33" t="inlineStr">
         <is>
           <t>Position
 (eV)</t>
         </is>
       </c>
-      <c r="D2" s="11" t="inlineStr">
+      <c r="D2" s="33" t="inlineStr">
         <is>
           <t>Height
 (CPS)</t>
         </is>
       </c>
-      <c r="E2" s="11" t="inlineStr">
+      <c r="E2" s="33" t="inlineStr">
         <is>
           <t>FWHM
 (eV)</t>
         </is>
       </c>
-      <c r="F2" s="11" t="inlineStr">
+      <c r="F2" s="33" t="inlineStr">
         <is>
           <t>L/G 
 σ/γ (%)</t>
         </is>
       </c>
-      <c r="G2" s="11" t="inlineStr">
+      <c r="G2" s="33" t="inlineStr">
         <is>
           <t>Area
 (CPS.eV)</t>
         </is>
       </c>
-      <c r="H2" s="11" t="inlineStr">
+      <c r="H2" s="33" t="inlineStr">
         <is>
           <t>Atomic
 (%)</t>
         </is>
       </c>
-      <c r="I2" s="11" t="inlineStr">
+      <c r="I2" s="33" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="J2" s="11" t="inlineStr">
+      <c r="J2" s="33" t="inlineStr">
         <is>
           <t>RSF</t>
         </is>
       </c>
-      <c r="K2" s="11" t="inlineStr">
+      <c r="K2" s="33" t="inlineStr">
         <is>
           <t>TXFN</t>
         </is>
       </c>
-      <c r="L2" s="11" t="inlineStr">
+      <c r="L2" s="33" t="inlineStr">
         <is>
           <t>ECF</t>
         </is>
       </c>
-      <c r="M2" s="11" t="inlineStr">
+      <c r="M2" s="33" t="inlineStr">
         <is>
           <t>Instr.</t>
         </is>
       </c>
-      <c r="N2" s="11" t="inlineStr">
+      <c r="N2" s="33" t="inlineStr">
         <is>
           <t>Fitting Model</t>
         </is>
       </c>
-      <c r="O2" s="11" t="inlineStr">
-        <is>
-          <t>Norm. Area
- An (a.u.)</t>
-        </is>
-      </c>
-      <c r="P2" s="11" t="inlineStr">
+      <c r="O2" s="33" t="inlineStr">
+        <is>
+          <t>Corr. Area
+ Ac (a.u.)</t>
+        </is>
+      </c>
+      <c r="P2" s="33" t="inlineStr">
         <is>
           <t>σ or α
 W_g</t>
         </is>
       </c>
-      <c r="Q2" s="11" t="inlineStr">
+      <c r="Q2" s="33" t="inlineStr">
         <is>
           <t>γ or β
 W_l</t>
         </is>
       </c>
-      <c r="R2" s="11" t="inlineStr">
+      <c r="R2" s="33" t="inlineStr">
         <is>
           <t>Bkg Type</t>
         </is>
       </c>
-      <c r="S2" s="11" t="inlineStr">
+      <c r="S2" s="33" t="inlineStr">
         <is>
           <t>Bkg Low
 (eV)</t>
         </is>
       </c>
-      <c r="T2" s="11" t="inlineStr">
+      <c r="T2" s="33" t="inlineStr">
         <is>
           <t>Bkg High
 (eV)</t>
         </is>
       </c>
-      <c r="U2" s="11" t="inlineStr">
+      <c r="U2" s="33" t="inlineStr">
         <is>
           <t>Bkg Offset Low
 (CPS)</t>
         </is>
       </c>
-      <c r="V2" s="11" t="inlineStr">
+      <c r="V2" s="33" t="inlineStr">
         <is>
           <t>Bkg Offset High
 (CPS)</t>
         </is>
       </c>
-      <c r="W2" s="11" t="inlineStr">
+      <c r="W2" s="33" t="inlineStr">
         <is>
           <t>Sheetname</t>
         </is>
       </c>
-      <c r="X2" s="11" t="inlineStr">
+      <c r="X2" s="33" t="inlineStr">
         <is>
           <t>Position
 Constraint</t>
         </is>
       </c>
-      <c r="Y2" s="11" t="inlineStr">
+      <c r="Y2" s="33" t="inlineStr">
         <is>
           <t>Height
 Constraint</t>
         </is>
       </c>
-      <c r="Z2" s="11" t="inlineStr">
+      <c r="Z2" s="33" t="inlineStr">
         <is>
           <t>FWHM
 Constraint</t>
         </is>
       </c>
-      <c r="AA2" s="11" t="inlineStr">
+      <c r="AA2" s="33" t="inlineStr">
         <is>
           <t>L/G
 Constraint</t>
         </is>
       </c>
-      <c r="AB2" s="11" t="inlineStr">
+      <c r="AB2" s="33" t="inlineStr">
         <is>
           <t>Area
 Constraint</t>
         </is>
       </c>
-      <c r="AC2" s="11" t="inlineStr">
+      <c r="AC2" s="33" t="inlineStr">
         <is>
           <t>σ
 Constraint</t>
         </is>
       </c>
-      <c r="AD2" s="11" t="inlineStr">
+      <c r="AD2" s="33" t="inlineStr">
         <is>
           <t>γ
 Constraint</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="34" t="inlineStr">
+        <is>
+          <t>Sr3d5/2 p1</t>
+        </is>
+      </c>
+      <c r="C3" s="35" t="inlineStr">
+        <is>
+          <t>132.49</t>
+        </is>
+      </c>
+      <c r="D3" s="35" t="inlineStr">
+        <is>
+          <t>101467.39</t>
+        </is>
+      </c>
+      <c r="E3" s="35" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="F3" s="35" t="inlineStr">
+        <is>
+          <t>60.28</t>
+        </is>
+      </c>
+      <c r="G3" s="35" t="inlineStr">
+        <is>
+          <t>108008.69</t>
+        </is>
+      </c>
+      <c r="H3" s="35" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I3" s="35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J3" s="35" t="inlineStr">
+        <is>
+          <t>4.25</t>
+        </is>
+      </c>
+      <c r="K3" s="35" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="L3" s="35" t="inlineStr">
+        <is>
+          <t>TPP-2M</t>
+        </is>
+      </c>
+      <c r="M3" s="35" t="inlineStr">
+        <is>
+          <t>A-ALTHERMO1</t>
+        </is>
+      </c>
+      <c r="N3" s="35" t="inlineStr">
+        <is>
+          <t>GL (Area)</t>
+        </is>
+      </c>
+      <c r="O3" s="35" t="inlineStr">
+        <is>
+          <t>324.68</t>
+        </is>
+      </c>
+      <c r="P3" s="35" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="Q3" s="35" t="inlineStr">
+        <is>
+          <t>0.51</t>
+        </is>
+      </c>
+      <c r="R3" s="35" t="inlineStr"/>
+      <c r="S3" s="35" t="inlineStr">
+        <is>
+          <t>126.08</t>
+        </is>
+      </c>
+      <c r="T3" s="35" t="inlineStr">
+        <is>
+          <t>142.08</t>
+        </is>
+      </c>
+      <c r="U3" s="35" t="inlineStr"/>
+      <c r="V3" s="35" t="inlineStr"/>
+      <c r="W3" s="35" t="inlineStr">
+        <is>
+          <t>Sr3d</t>
+        </is>
+      </c>
+      <c r="X3" s="35" t="inlineStr">
+        <is>
+          <t>126.08,142.08</t>
+        </is>
+      </c>
+      <c r="Y3" s="35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Z3" s="35" t="inlineStr">
+        <is>
+          <t>0.3:3.5</t>
+        </is>
+      </c>
+      <c r="AA3" s="35" t="inlineStr">
+        <is>
+          <t>2:80</t>
+        </is>
+      </c>
+      <c r="AB3" s="35" t="inlineStr">
+        <is>
+          <t>1:1e7</t>
+        </is>
+      </c>
+      <c r="AC3" s="35" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AD3" s="36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="37" t="inlineStr">
+        <is>
+          <t>Sr3d3/2 p2</t>
+        </is>
+      </c>
+      <c r="C4" s="38" t="inlineStr">
+        <is>
+          <t>134.24</t>
+        </is>
+      </c>
+      <c r="D4" s="38" t="inlineStr">
+        <is>
+          <t>70521.91</t>
+        </is>
+      </c>
+      <c r="E4" s="38" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="F4" s="38" t="inlineStr">
+        <is>
+          <t>60.27</t>
+        </is>
+      </c>
+      <c r="G4" s="38" t="inlineStr">
+        <is>
+          <t>75068.25</t>
+        </is>
+      </c>
+      <c r="H4" s="38" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I4" s="38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J4" s="38" t="inlineStr">
+        <is>
+          <t>2.93</t>
+        </is>
+      </c>
+      <c r="K4" s="38" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="L4" s="38" t="inlineStr">
+        <is>
+          <t>TPP-2M</t>
+        </is>
+      </c>
+      <c r="M4" s="38" t="inlineStr">
+        <is>
+          <t>A-ALTHERMO1</t>
+        </is>
+      </c>
+      <c r="N4" s="38" t="inlineStr">
+        <is>
+          <t>GL (Area)</t>
+        </is>
+      </c>
+      <c r="O4" s="38" t="inlineStr">
+        <is>
+          <t>327.86</t>
+        </is>
+      </c>
+      <c r="P4" s="38" t="inlineStr">
+        <is>
+          <t>2.35</t>
+        </is>
+      </c>
+      <c r="Q4" s="38" t="inlineStr">
+        <is>
+          <t>1.02</t>
+        </is>
+      </c>
+      <c r="R4" s="38" t="inlineStr"/>
+      <c r="S4" s="38" t="inlineStr">
+        <is>
+          <t>126.08</t>
+        </is>
+      </c>
+      <c r="T4" s="38" t="inlineStr">
+        <is>
+          <t>142.08</t>
+        </is>
+      </c>
+      <c r="U4" s="38" t="inlineStr"/>
+      <c r="V4" s="38" t="inlineStr"/>
+      <c r="W4" s="38" t="inlineStr">
+        <is>
+          <t>Sr3d</t>
+        </is>
+      </c>
+      <c r="X4" s="38" t="inlineStr">
+        <is>
+          <t>A+1.7#0.2</t>
+        </is>
+      </c>
+      <c r="Y4" s="38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Z4" s="38" t="inlineStr">
+        <is>
+          <t>A*1</t>
+        </is>
+      </c>
+      <c r="AA4" s="38" t="inlineStr">
+        <is>
+          <t>A*1</t>
+        </is>
+      </c>
+      <c r="AB4" s="38" t="inlineStr">
+        <is>
+          <t>A*0.667#0.05</t>
+        </is>
+      </c>
+      <c r="AC4" s="38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AD4" s="39" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Mac: Create highlight when using FileManager 3
</commit_message>
<xml_diff>
--- a/DATA/UKSAF/STO.xlsx
+++ b/DATA/UKSAF/STO.xlsx
@@ -8764,19 +8764,19 @@
         <v>144.08</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>-96.96323344647681</v>
       </c>
       <c r="H2" t="n">
         <v>26049.5</v>
       </c>
       <c r="I2" t="n">
-        <v>26049.5</v>
+        <v>26146.46323344648</v>
       </c>
       <c r="J2" t="n">
-        <v>26049.5</v>
+        <v>26097.23208698448</v>
       </c>
       <c r="K2" t="n">
-        <v>26049.5</v>
+        <v>26098.731146462</v>
       </c>
       <c r="X2" s="32" t="inlineStr">
         <is>
@@ -8790,31 +8790,39 @@
       </c>
       <c r="Z2" s="33" t="inlineStr">
         <is>
-          <t>134.49</t>
+          <t>134.50</t>
         </is>
       </c>
       <c r="AA2" s="33" t="inlineStr">
         <is>
-          <t>101468</t>
+          <t>98665</t>
         </is>
       </c>
       <c r="AB2" s="33" t="inlineStr">
         <is>
-          <t>1.00</t>
+          <t>0.99</t>
         </is>
       </c>
       <c r="AC2" s="33" t="inlineStr">
         <is>
-          <t>60.28</t>
+          <t>22.17</t>
         </is>
       </c>
       <c r="AD2" s="33" t="inlineStr">
         <is>
-          <t>108009</t>
-        </is>
-      </c>
-      <c r="AE2" s="33" t="inlineStr"/>
-      <c r="AF2" s="33" t="inlineStr"/>
+          <t>114445</t>
+        </is>
+      </c>
+      <c r="AE2" s="33" t="inlineStr">
+        <is>
+          <t>0.85</t>
+        </is>
+      </c>
+      <c r="AF2" s="33" t="inlineStr">
+        <is>
+          <t>0.24</t>
+        </is>
+      </c>
       <c r="AG2" s="33" t="inlineStr">
         <is>
           <t>0</t>
@@ -8822,7 +8830,7 @@
       </c>
       <c r="AH2" s="33" t="inlineStr">
         <is>
-          <t>59.0</t>
+          <t>59.2</t>
         </is>
       </c>
       <c r="AI2" s="33" t="inlineStr">
@@ -8837,7 +8845,7 @@
       </c>
       <c r="AK2" s="33" t="inlineStr">
         <is>
-          <t>GL (Area)</t>
+          <t>Voigt (Area, L/G, σ)</t>
         </is>
       </c>
       <c r="AL2" s="33" t="inlineStr">
@@ -8847,22 +8855,22 @@
       </c>
       <c r="AM2" s="33" t="inlineStr">
         <is>
-          <t>126.08</t>
+          <t>128.08</t>
         </is>
       </c>
       <c r="AN2" s="33" t="inlineStr">
         <is>
-          <t>142.08</t>
+          <t>144.08</t>
         </is>
       </c>
       <c r="AO2" s="33" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="AP2" s="34" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.00</t>
         </is>
       </c>
     </row>
@@ -8877,19 +8885,19 @@
         <v>143.98</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>-99.2683372810352</v>
       </c>
       <c r="H3" t="n">
         <v>26437.6</v>
       </c>
       <c r="I3" t="n">
-        <v>26437.6</v>
+        <v>26536.86833728103</v>
       </c>
       <c r="J3" t="n">
-        <v>26437.6</v>
+        <v>26486.34868605289</v>
       </c>
       <c r="K3" t="n">
-        <v>26437.6</v>
+        <v>26488.11965122814</v>
       </c>
       <c r="X3" s="35" t="inlineStr"/>
       <c r="Y3" s="36" t="inlineStr"/>
@@ -8905,7 +8913,7 @@
       </c>
       <c r="AB3" s="36" t="inlineStr">
         <is>
-          <t>0.3:3.5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AC3" s="36" t="inlineStr">
@@ -8918,8 +8926,16 @@
           <t>1:1e7</t>
         </is>
       </c>
-      <c r="AE3" s="36" t="inlineStr"/>
-      <c r="AF3" s="36" t="inlineStr"/>
+      <c r="AE3" s="36" t="inlineStr">
+        <is>
+          <t>0.3:3</t>
+        </is>
+      </c>
+      <c r="AF3" s="36" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="AG3" s="36" t="inlineStr">
         <is>
           <t>0</t>
@@ -8946,19 +8962,19 @@
         <v>143.88</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>-101.6576855512903</v>
       </c>
       <c r="H4" t="n">
         <v>26696.9</v>
       </c>
       <c r="I4" t="n">
-        <v>26696.9</v>
+        <v>26798.55768555129</v>
       </c>
       <c r="J4" t="n">
-        <v>26696.9</v>
+        <v>26746.69815982972</v>
       </c>
       <c r="K4" t="n">
-        <v>26696.9</v>
+        <v>26748.75952572157</v>
       </c>
       <c r="X4" s="32" t="inlineStr">
         <is>
@@ -8977,26 +8993,34 @@
       </c>
       <c r="AA4" s="33" t="inlineStr">
         <is>
-          <t>70522</t>
+          <t>68015</t>
         </is>
       </c>
       <c r="AB4" s="33" t="inlineStr">
         <is>
-          <t>1.00</t>
+          <t>0.99</t>
         </is>
       </c>
       <c r="AC4" s="33" t="inlineStr">
         <is>
-          <t>60.27</t>
+          <t>22.17</t>
         </is>
       </c>
       <c r="AD4" s="33" t="inlineStr">
         <is>
-          <t>75068</t>
-        </is>
-      </c>
-      <c r="AE4" s="33" t="inlineStr"/>
-      <c r="AF4" s="33" t="inlineStr"/>
+          <t>78896</t>
+        </is>
+      </c>
+      <c r="AE4" s="33" t="inlineStr">
+        <is>
+          <t>0.85</t>
+        </is>
+      </c>
+      <c r="AF4" s="33" t="inlineStr">
+        <is>
+          <t>0.24</t>
+        </is>
+      </c>
       <c r="AG4" s="33" t="inlineStr">
         <is>
           <t>0</t>
@@ -9004,22 +9028,22 @@
       </c>
       <c r="AH4" s="33" t="inlineStr">
         <is>
-          <t>41.0</t>
+          <t>40.8</t>
         </is>
       </c>
       <c r="AI4" s="33" t="inlineStr">
         <is>
-          <t>69.5</t>
+          <t>68.9</t>
         </is>
       </c>
       <c r="AJ4" s="33" t="inlineStr">
         <is>
-          <t>1.75</t>
+          <t>1.74</t>
         </is>
       </c>
       <c r="AK4" s="33" t="inlineStr">
         <is>
-          <t>GL (Area)</t>
+          <t>Voigt (Area, L/G, σ)</t>
         </is>
       </c>
       <c r="AL4" s="33" t="inlineStr">
@@ -9029,22 +9053,22 @@
       </c>
       <c r="AM4" s="33" t="inlineStr">
         <is>
-          <t>126.08</t>
+          <t>128.08</t>
         </is>
       </c>
       <c r="AN4" s="33" t="inlineStr">
         <is>
-          <t>142.08</t>
+          <t>144.08</t>
         </is>
       </c>
       <c r="AO4" s="33" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="AP4" s="34" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.00</t>
         </is>
       </c>
     </row>
@@ -9059,19 +9083,19 @@
         <v>143.78</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>-104.1354871006915</v>
       </c>
       <c r="H5" t="n">
         <v>25942.6</v>
       </c>
       <c r="I5" t="n">
-        <v>25942.6</v>
+        <v>26046.73548710069</v>
       </c>
       <c r="J5" t="n">
-        <v>25942.6</v>
+        <v>25993.48194336965</v>
       </c>
       <c r="K5" t="n">
-        <v>25942.6</v>
+        <v>25995.85354373103</v>
       </c>
       <c r="X5" s="35" t="inlineStr"/>
       <c r="Y5" s="36" t="inlineStr"/>
@@ -9082,29 +9106,37 @@
       </c>
       <c r="AA5" s="36" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>A*0.667#0.05</t>
         </is>
       </c>
       <c r="AB5" s="36" t="inlineStr">
         <is>
+          <t>0.3:3.5</t>
+        </is>
+      </c>
+      <c r="AC5" s="36" t="inlineStr">
+        <is>
           <t>A*1</t>
         </is>
       </c>
-      <c r="AC5" s="36" t="inlineStr">
+      <c r="AD5" s="36" t="inlineStr">
+        <is>
+          <t>A*0.667#0.05</t>
+        </is>
+      </c>
+      <c r="AE5" s="36" t="inlineStr">
         <is>
           <t>A*1</t>
         </is>
       </c>
-      <c r="AD5" s="36" t="inlineStr">
-        <is>
-          <t>A*0.667#0.05</t>
-        </is>
-      </c>
-      <c r="AE5" s="36" t="inlineStr"/>
-      <c r="AF5" s="36" t="inlineStr"/>
+      <c r="AF5" s="36" t="inlineStr">
+        <is>
+          <t>A*1</t>
+        </is>
+      </c>
       <c r="AG5" s="36" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>A*1</t>
         </is>
       </c>
       <c r="AH5" s="36" t="inlineStr"/>
@@ -9128,19 +9160,19 @@
         <v>143.68</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>-106.7062202940797</v>
       </c>
       <c r="H6" t="n">
         <v>26565.8</v>
       </c>
       <c r="I6" t="n">
-        <v>26565.8</v>
+        <v>26672.50622029408</v>
       </c>
       <c r="J6" t="n">
-        <v>26565.8</v>
+        <v>26617.80155101709</v>
       </c>
       <c r="K6" t="n">
-        <v>26565.8</v>
+        <v>26620.50466927699</v>
       </c>
     </row>
     <row r="7">
@@ -9154,19 +9186,19 @@
         <v>143.58</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>-109.374654254425</v>
       </c>
       <c r="H7" t="n">
         <v>26089.7</v>
       </c>
       <c r="I7" t="n">
-        <v>26089.7</v>
+        <v>26199.07465425443</v>
       </c>
       <c r="J7" t="n">
-        <v>26089.7</v>
+        <v>26142.85858173036</v>
       </c>
       <c r="K7" t="n">
-        <v>26089.7</v>
+        <v>26145.91607252407</v>
       </c>
     </row>
     <row r="8">
@@ -9180,19 +9212,19 @@
         <v>143.48</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>-112.1458721009694</v>
       </c>
       <c r="H8" t="n">
         <v>26784.6</v>
       </c>
       <c r="I8" t="n">
-        <v>26784.6</v>
+        <v>26896.74587210097</v>
       </c>
       <c r="J8" t="n">
-        <v>26784.6</v>
+        <v>26838.95472482844</v>
       </c>
       <c r="K8" t="n">
-        <v>26784.6</v>
+        <v>26842.39114727253</v>
       </c>
     </row>
     <row r="9">
@@ -9206,19 +9238,19 @@
         <v>143.38</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>-115.0252964096653</v>
       </c>
       <c r="H9" t="n">
         <v>26357.7</v>
       </c>
       <c r="I9" t="n">
-        <v>26357.7</v>
+        <v>26472.72529640967</v>
       </c>
       <c r="J9" t="n">
-        <v>26357.7</v>
+        <v>26413.29176619907</v>
       </c>
       <c r="K9" t="n">
-        <v>26357.7</v>
+        <v>26417.13353021059</v>
       </c>
     </row>
     <row r="10">
@@ -9232,19 +9264,19 @@
         <v>143.28</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>-118.0187171448852</v>
       </c>
       <c r="H10" t="n">
         <v>26256</v>
       </c>
       <c r="I10" t="n">
-        <v>26256</v>
+        <v>26374.01871714489</v>
       </c>
       <c r="J10" t="n">
-        <v>26256</v>
+        <v>26312.87159501099</v>
       </c>
       <c r="K10" t="n">
-        <v>26256</v>
+        <v>26317.14712213389</v>
       </c>
     </row>
     <row r="11">
@@ -9258,19 +9290,19 @@
         <v>143.18</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>-121.1323223436848</v>
       </c>
       <c r="H11" t="n">
         <v>26519.3</v>
       </c>
       <c r="I11" t="n">
-        <v>26519.3</v>
+        <v>26640.43232234368</v>
       </c>
       <c r="J11" t="n">
-        <v>26519.3</v>
+        <v>26577.4962109779</v>
       </c>
       <c r="K11" t="n">
-        <v>26519.3</v>
+        <v>26582.23611136579</v>
       </c>
     </row>
     <row r="12">
@@ -9284,19 +9316,19 @@
         <v>143.08</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>-124.3727318706042</v>
       </c>
       <c r="H12" t="n">
         <v>25948.6</v>
       </c>
       <c r="I12" t="n">
-        <v>25948.6</v>
+        <v>26072.9727318706</v>
       </c>
       <c r="J12" t="n">
-        <v>25948.6</v>
+        <v>26008.16773222655</v>
       </c>
       <c r="K12" t="n">
-        <v>25948.6</v>
+        <v>26013.40499964405</v>
       </c>
     </row>
     <row r="13">
@@ -9310,19 +9342,19 @@
         <v>142.98</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>-127.7470346036389</v>
       </c>
       <c r="H13" t="n">
         <v>26945.3</v>
       </c>
       <c r="I13" t="n">
-        <v>26945.3</v>
+        <v>27073.04703460364</v>
       </c>
       <c r="J13" t="n">
-        <v>26945.3</v>
+        <v>27006.28840382732</v>
       </c>
       <c r="K13" t="n">
-        <v>26945.3</v>
+        <v>27012.05863077632</v>
       </c>
     </row>
     <row r="14">
@@ -9336,19 +9368,19 @@
         <v>142.88</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>-131.2628294606329</v>
       </c>
       <c r="H14" t="n">
         <v>26444</v>
       </c>
       <c r="I14" t="n">
-        <v>26444</v>
+        <v>26575.26282946063</v>
       </c>
       <c r="J14" t="n">
-        <v>26444</v>
+        <v>26506.4606070517</v>
       </c>
       <c r="K14" t="n">
-        <v>26444</v>
+        <v>26512.80222240893</v>
       </c>
     </row>
     <row r="15">
@@ -9362,19 +9394,19 @@
         <v>142.78</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>-134.9282707319871</v>
       </c>
       <c r="H15" t="n">
         <v>26729.6</v>
       </c>
       <c r="I15" t="n">
-        <v>26729.6</v>
+        <v>26864.52827073199</v>
       </c>
       <c r="J15" t="n">
-        <v>26729.6</v>
+        <v>26793.5868694288</v>
       </c>
       <c r="K15" t="n">
-        <v>26729.6</v>
+        <v>26800.54140130319</v>
       </c>
     </row>
     <row r="16">
@@ -9388,19 +9420,19 @@
         <v>142.68</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>-138.7521182506607</v>
       </c>
       <c r="H16" t="n">
         <v>27045.9</v>
       </c>
       <c r="I16" t="n">
-        <v>27045.9</v>
+        <v>27184.65211825066</v>
       </c>
       <c r="J16" t="n">
-        <v>27045.9</v>
+        <v>27111.4698756805</v>
       </c>
       <c r="K16" t="n">
-        <v>27045.9</v>
+        <v>27119.08224257016</v>
       </c>
     </row>
     <row r="17">
@@ -9414,19 +9446,19 @@
         <v>142.58</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>-142.7437930062297</v>
       </c>
       <c r="H17" t="n">
         <v>26274.3</v>
       </c>
       <c r="I17" t="n">
-        <v>26274.3</v>
+        <v>26417.04379300623</v>
       </c>
       <c r="J17" t="n">
-        <v>26274.3</v>
+        <v>26341.51247962456</v>
       </c>
       <c r="K17" t="n">
-        <v>26274.3</v>
+        <v>26349.83131338167</v>
       </c>
     </row>
     <row r="18">
@@ -9440,19 +9472,19 @@
         <v>142.48</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>-146.9134388978528</v>
       </c>
       <c r="H18" t="n">
         <v>25721.7</v>
       </c>
       <c r="I18" t="n">
-        <v>25721.7</v>
+        <v>25868.61343889785</v>
       </c>
       <c r="J18" t="n">
-        <v>25721.7</v>
+        <v>25790.61771714485</v>
       </c>
       <c r="K18" t="n">
-        <v>25721.7</v>
+        <v>25799.695721753</v>
       </c>
     </row>
     <row r="19">
@@ -9466,19 +9498,19 @@
         <v>142.38</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>-151.2719914233639</v>
       </c>
       <c r="H19" t="n">
         <v>26199.6</v>
       </c>
       <c r="I19" t="n">
-        <v>26199.6</v>
+        <v>26350.87199142336</v>
       </c>
       <c r="J19" t="n">
-        <v>26199.6</v>
+        <v>26270.28882033987</v>
       </c>
       <c r="K19" t="n">
-        <v>26199.6</v>
+        <v>26280.18317108349</v>
       </c>
     </row>
     <row r="20">
@@ -9492,19 +9524,19 @@
         <v>142.28</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>-155.8312542219137</v>
       </c>
       <c r="H20" t="n">
         <v>27175.7</v>
       </c>
       <c r="I20" t="n">
-        <v>27175.7</v>
+        <v>27331.53125422191</v>
       </c>
       <c r="J20" t="n">
-        <v>27175.7</v>
+        <v>27248.22923297363</v>
       </c>
       <c r="K20" t="n">
-        <v>27175.7</v>
+        <v>27259.00202124828</v>
       </c>
     </row>
     <row r="21">
@@ -9518,19 +9550,19 @@
         <v>142.18</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>-160.6039845277555</v>
       </c>
       <c r="H21" t="n">
         <v>26142</v>
       </c>
       <c r="I21" t="n">
-        <v>26142</v>
+        <v>26302.60398452776</v>
       </c>
       <c r="J21" t="n">
-        <v>26142</v>
+        <v>26216.44262736813</v>
       </c>
       <c r="K21" t="n">
-        <v>26142</v>
+        <v>26228.16135715962</v>
       </c>
     </row>
     <row r="22">
@@ -9544,19 +9576,19 @@
         <v>142.08</v>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>-165.6039887581355</v>
       </c>
       <c r="H22" t="n">
         <v>26419.9</v>
       </c>
       <c r="I22" t="n">
-        <v>26419.9</v>
+        <v>26585.50398875814</v>
       </c>
       <c r="J22" t="n">
-        <v>26419.9</v>
+        <v>26496.33292289355</v>
       </c>
       <c r="K22" t="n">
-        <v>26419.9</v>
+        <v>26509.07106586459</v>
       </c>
     </row>
     <row r="23">
@@ -9570,19 +9602,19 @@
         <v>141.98</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>-170.8462296526304</v>
       </c>
       <c r="H23" t="n">
         <v>27293.7</v>
       </c>
       <c r="I23" t="n">
-        <v>27293.7</v>
+        <v>27464.54622965263</v>
       </c>
       <c r="J23" t="n">
-        <v>27293.7</v>
+        <v>27372.20430623166</v>
       </c>
       <c r="K23" t="n">
-        <v>27293.7</v>
+        <v>27386.04192342097</v>
       </c>
     </row>
     <row r="24">
@@ -9596,19 +9628,19 @@
         <v>141.88</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>-176.3469466113893</v>
       </c>
       <c r="H24" t="n">
         <v>26191.1</v>
       </c>
       <c r="I24" t="n">
-        <v>26191.1</v>
+        <v>26367.44694661139</v>
       </c>
       <c r="J24" t="n">
-        <v>26191.1</v>
+        <v>26271.76125360998</v>
       </c>
       <c r="K24" t="n">
-        <v>26191.1</v>
+        <v>26286.78569300141</v>
       </c>
     </row>
     <row r="25">
@@ -9622,19 +9654,19 @@
         <v>141.78</v>
       </c>
       <c r="G25" t="n">
-        <v>-3.637978807091713e-12</v>
+        <v>-182.1237911524695</v>
       </c>
       <c r="H25" t="n">
         <v>26444.7</v>
       </c>
       <c r="I25" t="n">
-        <v>26444.7</v>
+        <v>26626.82379115247</v>
       </c>
       <c r="J25" t="n">
-        <v>26444.7</v>
+        <v>26527.60855522942</v>
       </c>
       <c r="K25" t="n">
-        <v>26444.7</v>
+        <v>26543.91523592305</v>
       </c>
     </row>
     <row r="26">
@@ -9648,19 +9680,19 @@
         <v>141.68</v>
       </c>
       <c r="G26" t="n">
-        <v>-7.275957614183426e-12</v>
+        <v>-188.1959797328091</v>
       </c>
       <c r="H26" t="n">
         <v>26393.8</v>
       </c>
       <c r="I26" t="n">
-        <v>26393.80000000001</v>
+        <v>26581.99597973281</v>
       </c>
       <c r="J26" t="n">
-        <v>26393.8</v>
+        <v>26479.05134213674</v>
       </c>
       <c r="K26" t="n">
-        <v>26393.80000000001</v>
+        <v>26496.74463759606</v>
       </c>
     </row>
     <row r="27">
@@ -9674,19 +9706,19 @@
         <v>141.58</v>
       </c>
       <c r="G27" t="n">
-        <v>-2.182787284255028e-11</v>
+        <v>-194.5844665649456</v>
       </c>
       <c r="H27" t="n">
         <v>26023.2</v>
       </c>
       <c r="I27" t="n">
-        <v>26023.20000000002</v>
+        <v>26217.78446656495</v>
       </c>
       <c r="J27" t="n">
-        <v>26023.2</v>
+        <v>26110.8951158266</v>
       </c>
       <c r="K27" t="n">
-        <v>26023.20000000002</v>
+        <v>26130.08935073835</v>
       </c>
     </row>
     <row r="28">
@@ -9700,19 +9732,19 @@
         <v>141.48</v>
       </c>
       <c r="G28" t="n">
-        <v>-7.639755494892597e-11</v>
+        <v>-201.3121395255075</v>
       </c>
       <c r="H28" t="n">
         <v>27069.8</v>
       </c>
       <c r="I28" t="n">
-        <v>27069.80000000008</v>
+        <v>27271.11213952551</v>
       </c>
       <c r="J28" t="n">
-        <v>27069.8</v>
+        <v>27160.04578089525</v>
       </c>
       <c r="K28" t="n">
-        <v>27069.80000000008</v>
+        <v>27180.86635863026</v>
       </c>
     </row>
     <row r="29">
@@ -9726,19 +9758,19 @@
         <v>141.38</v>
       </c>
       <c r="G29" t="n">
-        <v>-2.510205376893282e-10</v>
+        <v>-208.4040428093977</v>
       </c>
       <c r="H29" t="n">
         <v>26161.8</v>
       </c>
       <c r="I29" t="n">
-        <v>26161.80000000025</v>
+        <v>26370.2040428094</v>
       </c>
       <c r="J29" t="n">
-        <v>26161.8</v>
+        <v>26254.70968111219</v>
       </c>
       <c r="K29" t="n">
-        <v>26161.80000000025</v>
+        <v>26277.2943616972</v>
       </c>
     </row>
     <row r="30">
@@ -9752,19 +9784,19 @@
         <v>141.28</v>
       </c>
       <c r="G30" t="n">
-        <v>-7.967173587530851e-10</v>
+        <v>-215.8876306572674</v>
       </c>
       <c r="H30" t="n">
         <v>26300.2</v>
       </c>
       <c r="I30" t="n">
-        <v>26300.2000000008</v>
+        <v>26516.08763065727</v>
       </c>
       <c r="J30" t="n">
-        <v>26300.2</v>
+        <v>26395.89363932579</v>
       </c>
       <c r="K30" t="n">
-        <v>26300.2000000008</v>
+        <v>26420.39399133148</v>
       </c>
     </row>
     <row r="31">
@@ -9778,19 +9810,19 @@
         <v>141.18</v>
       </c>
       <c r="G31" t="n">
-        <v>-2.492015482857823e-09</v>
+        <v>-223.7930572999467</v>
       </c>
       <c r="H31" t="n">
         <v>26179.2</v>
       </c>
       <c r="I31" t="n">
-        <v>26179.20000000249</v>
+        <v>26402.99305729995</v>
       </c>
       <c r="J31" t="n">
-        <v>26179.2</v>
+        <v>26277.80500167743</v>
       </c>
       <c r="K31" t="n">
-        <v>26179.20000000249</v>
+        <v>26304.38805562252</v>
       </c>
     </row>
     <row r="32">
@@ -9804,19 +9836,19 @@
         <v>141.08</v>
       </c>
       <c r="G32" t="n">
-        <v>-7.621565600857139e-09</v>
+        <v>-232.153509256812</v>
       </c>
       <c r="H32" t="n">
         <v>25952.4</v>
       </c>
       <c r="I32" t="n">
-        <v>25952.40000000762</v>
+        <v>26184.55350925681</v>
       </c>
       <c r="J32" t="n">
-        <v>25952.4</v>
+        <v>26054.05168666567</v>
       </c>
       <c r="K32" t="n">
-        <v>25952.40000000762</v>
+        <v>26082.90182259114</v>
       </c>
     </row>
     <row r="33">
@@ -9830,19 +9862,19 @@
         <v>140.98</v>
       </c>
       <c r="G33" t="n">
-        <v>-2.281376509927213e-08</v>
+        <v>-241.0055873394849</v>
       </c>
       <c r="H33" t="n">
         <v>25823.1</v>
       </c>
       <c r="I33" t="n">
-        <v>25823.10000002281</v>
+        <v>26064.10558733948</v>
       </c>
       <c r="J33" t="n">
-        <v>25823.1</v>
+        <v>25927.9422396804</v>
       </c>
       <c r="K33" t="n">
-        <v>25823.10000002282</v>
+        <v>25959.26334765908</v>
       </c>
     </row>
     <row r="34">
@@ -9856,19 +9888,19 @@
         <v>140.88</v>
       </c>
       <c r="G34" t="n">
-        <v>-6.685513653792441e-08</v>
+        <v>-250.3897472030585</v>
       </c>
       <c r="H34" t="n">
         <v>25796.2</v>
       </c>
       <c r="I34" t="n">
-        <v>25796.20000006686</v>
+        <v>26046.58974720306</v>
       </c>
       <c r="J34" t="n">
-        <v>25796.2</v>
+        <v>25904.38589371726</v>
       </c>
       <c r="K34" t="n">
-        <v>25796.20000006686</v>
+        <v>25938.4038534858</v>
       </c>
     </row>
     <row r="35">
@@ -9882,19 +9914,19 @@
         <v>140.78</v>
       </c>
       <c r="G35" t="n">
-        <v>-1.918087946251035e-07</v>
+        <v>-260.3508091273579</v>
       </c>
       <c r="H35" t="n">
         <v>25706.9</v>
       </c>
       <c r="I35" t="n">
-        <v>25706.90000019181</v>
+        <v>25967.25080912736</v>
       </c>
       <c r="J35" t="n">
-        <v>25706.9</v>
+        <v>25818.59263708902</v>
       </c>
       <c r="K35" t="n">
-        <v>25706.90000019181</v>
+        <v>25855.55817203834</v>
       </c>
     </row>
     <row r="36">
@@ -9908,19 +9940,19 @@
         <v>140.68</v>
       </c>
       <c r="G36" t="n">
-        <v>-5.387992132455111e-07</v>
+        <v>-270.9385499926611</v>
       </c>
       <c r="H36" t="n">
         <v>25865.6</v>
       </c>
       <c r="I36" t="n">
-        <v>25865.6000005388</v>
+        <v>26136.53854999266</v>
       </c>
       <c r="J36" t="n">
-        <v>25865.6</v>
+        <v>25980.97328907436</v>
       </c>
       <c r="K36" t="n">
-        <v>25865.6000005388</v>
+        <v>26021.1652609183</v>
       </c>
     </row>
     <row r="37">
@@ -9934,19 +9966,19 @@
         <v>140.58</v>
       </c>
       <c r="G37" t="n">
-        <v>-1.481937943026423e-06</v>
+        <v>-282.2083932600071</v>
       </c>
       <c r="H37" t="n">
         <v>26150.6</v>
       </c>
       <c r="I37" t="n">
-        <v>26150.60000148194</v>
+        <v>26432.80839326001</v>
       </c>
       <c r="J37" t="n">
-        <v>26150.6</v>
+        <v>26269.83958458934</v>
       </c>
       <c r="K37" t="n">
-        <v>26150.60000148194</v>
+        <v>26313.56880867067</v>
       </c>
     </row>
     <row r="38">
@@ -9960,19 +9992,19 @@
         <v>140.48</v>
       </c>
       <c r="G38" t="n">
-        <v>-3.99112468585372e-06</v>
+        <v>-294.222216334656</v>
       </c>
       <c r="H38" t="n">
         <v>25610.5</v>
       </c>
       <c r="I38" t="n">
-        <v>25610.50000399112</v>
+        <v>25904.72221633466</v>
       </c>
       <c r="J38" t="n">
-        <v>25610.5</v>
+        <v>25733.80426913777</v>
       </c>
       <c r="K38" t="n">
-        <v>25610.50000399115</v>
+        <v>25781.41794719689</v>
       </c>
     </row>
     <row r="39">
@@ -9986,19 +10018,19 @@
         <v>140.38</v>
       </c>
       <c r="G39" t="n">
-        <v>-1.052554216585122e-05</v>
+        <v>-307.049299192804</v>
       </c>
       <c r="H39" t="n">
         <v>25614.3</v>
       </c>
       <c r="I39" t="n">
-        <v>25614.30001052554</v>
+        <v>25921.3492991928</v>
       </c>
       <c r="J39" t="n">
-        <v>25614.3</v>
+        <v>25741.88120549766</v>
       </c>
       <c r="K39" t="n">
-        <v>25614.30001052559</v>
+        <v>25793.76809369514</v>
       </c>
     </row>
     <row r="40">
@@ -10012,19 +10044,19 @@
         <v>140.28</v>
       </c>
       <c r="G40" t="n">
-        <v>-2.718298128456809e-05</v>
+        <v>-320.7674438661379</v>
       </c>
       <c r="H40" t="n">
         <v>25482.4</v>
       </c>
       <c r="I40" t="n">
-        <v>25482.40002718298</v>
+        <v>25803.16744386614</v>
       </c>
       <c r="J40" t="n">
-        <v>25482.4</v>
+        <v>25614.48549383839</v>
       </c>
       <c r="K40" t="n">
-        <v>25482.40002718311</v>
+        <v>25671.08195002775</v>
       </c>
     </row>
     <row r="41">
@@ -10038,19 +10070,19 @@
         <v>140.18</v>
       </c>
       <c r="G41" t="n">
-        <v>-6.875037797726691e-05</v>
+        <v>-335.4643016818191</v>
       </c>
       <c r="H41" t="n">
         <v>25820.7</v>
       </c>
       <c r="I41" t="n">
-        <v>25820.70006875038</v>
+        <v>26156.16430168182</v>
       </c>
       <c r="J41" t="n">
-        <v>25820.7</v>
+        <v>25957.53360724484</v>
       </c>
       <c r="K41" t="n">
-        <v>25820.70006875069</v>
+        <v>26019.33069443698</v>
       </c>
     </row>
     <row r="42">
@@ -10064,19 +10096,19 @@
         <v>140.08</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.0001702950066828635</v>
+        <v>-351.2389545550868</v>
       </c>
       <c r="H42" t="n">
         <v>25337.9</v>
       </c>
       <c r="I42" t="n">
-        <v>25337.90017029501</v>
+        <v>25689.13895455509</v>
       </c>
       <c r="J42" t="n">
-        <v>25337.9</v>
+        <v>25479.74354495973</v>
       </c>
       <c r="K42" t="n">
-        <v>25337.90017029579</v>
+        <v>25547.29540959536</v>
       </c>
     </row>
     <row r="43">
@@ -10090,19 +10122,19 @@
         <v>139.98</v>
       </c>
       <c r="G43" t="n">
-        <v>-0.0004131450368731748</v>
+        <v>-368.2038088215413</v>
       </c>
       <c r="H43" t="n">
         <v>25660.4</v>
       </c>
       <c r="I43" t="n">
-        <v>25660.40041314504</v>
+        <v>26028.60380882154</v>
       </c>
       <c r="J43" t="n">
-        <v>25660.40000000001</v>
+        <v>25807.53500605453</v>
       </c>
       <c r="K43" t="n">
-        <v>25660.40041314692</v>
+        <v>25881.46880276702</v>
       </c>
     </row>
     <row r="44">
@@ -10116,19 +10148,19 @@
         <v>139.88</v>
       </c>
       <c r="G44" t="n">
-        <v>-0.0009817563841352239</v>
+        <v>-386.4868760325517</v>
       </c>
       <c r="H44" t="n">
         <v>25130.5</v>
       </c>
       <c r="I44" t="n">
-        <v>25130.50098175638</v>
+        <v>25516.98687603255</v>
       </c>
       <c r="J44" t="n">
-        <v>25130.50000000002</v>
+        <v>25283.22958671748</v>
       </c>
       <c r="K44" t="n">
-        <v>25130.50098176086</v>
+        <v>25364.25728931507</v>
       </c>
     </row>
     <row r="45">
@@ -10142,19 +10174,19 @@
         <v>139.78</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.002285252725414466</v>
+        <v>-406.2345361533007</v>
       </c>
       <c r="H45" t="n">
         <v>25320.6</v>
       </c>
       <c r="I45" t="n">
-        <v>25320.60228525272</v>
+        <v>25726.8345361533</v>
       </c>
       <c r="J45" t="n">
-        <v>25320.60000000006</v>
+        <v>25479.25100492106</v>
       </c>
       <c r="K45" t="n">
-        <v>25320.60228526311</v>
+        <v>25568.18353123224</v>
       </c>
     </row>
     <row r="46">
@@ -10168,19 +10200,19 @@
         <v>139.68</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.005211046103795525</v>
+        <v>-427.6149065753707</v>
       </c>
       <c r="H46" t="n">
         <v>24983.9</v>
       </c>
       <c r="I46" t="n">
-        <v>24983.90521104611</v>
+        <v>25411.51490657537</v>
       </c>
       <c r="J46" t="n">
-        <v>24983.9000000002</v>
+        <v>25148.82535692297</v>
       </c>
       <c r="K46" t="n">
-        <v>24983.90521106973</v>
+        <v>25246.5895496524</v>
       </c>
     </row>
     <row r="47">
@@ -10194,19 +10226,19 @@
         <v>139.58</v>
       </c>
       <c r="G47" t="n">
-        <v>-0.01164150121985585</v>
+        <v>-450.8219779640494</v>
       </c>
       <c r="H47" t="n">
         <v>25008</v>
       </c>
       <c r="I47" t="n">
-        <v>25008.01164150122</v>
+        <v>25458.82197796405</v>
       </c>
       <c r="J47" t="n">
-        <v>25008.00000000065</v>
+        <v>25179.58141089177</v>
       </c>
       <c r="K47" t="n">
-        <v>25008.01164155378</v>
+        <v>25287.24056707228</v>
       </c>
     </row>
     <row r="48">
@@ -10220,19 +10252,19 @@
         <v>139.48</v>
       </c>
       <c r="G48" t="n">
-        <v>-0.02548133834716282</v>
+        <v>-476.0807290745179</v>
       </c>
       <c r="H48" t="n">
         <v>24993.3</v>
       </c>
       <c r="I48" t="n">
-        <v>24993.32548133835</v>
+        <v>25469.38072907452</v>
       </c>
       <c r="J48" t="n">
-        <v>24993.30000000205</v>
+        <v>25171.95094396428</v>
       </c>
       <c r="K48" t="n">
-        <v>24993.32548145278</v>
+        <v>25290.72978511024</v>
       </c>
     </row>
     <row r="49">
@@ -10246,19 +10278,19 @@
         <v>139.38</v>
       </c>
       <c r="G49" t="n">
-        <v>-0.05465164764609654</v>
+        <v>-503.6535029696497</v>
       </c>
       <c r="H49" t="n">
         <v>25038.8</v>
       </c>
       <c r="I49" t="n">
-        <v>25038.85465164765</v>
+        <v>25542.45350296965</v>
       </c>
       <c r="J49" t="n">
-        <v>25038.80000000633</v>
+        <v>25224.96913028162</v>
       </c>
       <c r="K49" t="n">
-        <v>25038.85465189113</v>
+        <v>25356.28437268802</v>
       </c>
     </row>
     <row r="50">
@@ -10272,19 +10304,19 @@
         <v>139.28</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.1148666006592975</v>
+        <v>-533.8480250174216</v>
       </c>
       <c r="H50" t="n">
         <v>24708.8</v>
       </c>
       <c r="I50" t="n">
-        <v>24708.91486660066</v>
+        <v>25242.64802501742</v>
       </c>
       <c r="J50" t="n">
-        <v>24708.80000001914</v>
+        <v>24902.97498906843</v>
       </c>
       <c r="K50" t="n">
-        <v>24708.91486710659</v>
+        <v>25048.47303594899</v>
       </c>
     </row>
     <row r="51">
@@ -10298,19 +10330,19 @@
         <v>139.18</v>
       </c>
       <c r="G51" t="n">
-        <v>24.53338684793562</v>
+        <v>-567.0275814788693</v>
       </c>
       <c r="H51" t="n">
-        <v>24672.13</v>
+        <v>24696.9</v>
       </c>
       <c r="I51" t="n">
-        <v>24672.36661315207</v>
+        <v>25263.92758147887</v>
       </c>
       <c r="J51" t="n">
-        <v>24672.13000005668</v>
+        <v>24899.61190368708</v>
       </c>
       <c r="K51" t="n">
-        <v>24672.36661417697</v>
+        <v>25061.21567779179</v>
       </c>
     </row>
     <row r="52">
@@ -10324,19 +10356,19 @@
         <v>139.08</v>
       </c>
       <c r="G52" t="n">
-        <v>-3.98773545494987</v>
+        <v>-603.6240763027854</v>
       </c>
       <c r="H52" t="n">
-        <v>24667.01</v>
+        <v>24663.5</v>
       </c>
       <c r="I52" t="n">
-        <v>24667.48773545495</v>
+        <v>25267.12407630279</v>
       </c>
       <c r="J52" t="n">
-        <v>24667.01000016429</v>
+        <v>24875.32822490681</v>
       </c>
       <c r="K52" t="n">
-        <v>24667.48773747444</v>
+        <v>25055.29585139597</v>
       </c>
     </row>
     <row r="53">
@@ -10350,19 +10382,19 @@
         <v>138.98</v>
       </c>
       <c r="G53" t="n">
-        <v>-11.94556755579106</v>
+        <v>-644.1549744357217</v>
       </c>
       <c r="H53" t="n">
-        <v>24667</v>
+        <v>24656</v>
       </c>
       <c r="I53" t="n">
-        <v>24667.94556755579</v>
+        <v>25300.15497443572</v>
       </c>
       <c r="J53" t="n">
-        <v>24667.00000046629</v>
+        <v>24877.57797449437</v>
       </c>
       <c r="K53" t="n">
-        <v>24667.9455714118</v>
+        <v>25078.57699994135</v>
       </c>
     </row>
     <row r="54">
@@ -10376,19 +10408,19 @@
         <v>138.88</v>
       </c>
       <c r="G54" t="n">
-        <v>-85.84489713509538</v>
+        <v>-689.245573861579</v>
       </c>
       <c r="H54" t="n">
-        <v>24667.01</v>
+        <v>24583</v>
       </c>
       <c r="I54" t="n">
-        <v>24668.8448971351</v>
+        <v>25272.24557386158</v>
       </c>
       <c r="J54" t="n">
-        <v>24667.01000129577</v>
+        <v>24815.02166881158</v>
       </c>
       <c r="K54" t="n">
-        <v>24668.84490422684</v>
+        <v>25040.22390505</v>
       </c>
     </row>
     <row r="55">
@@ -10402,19 +10434,19 @@
         <v>138.78</v>
       </c>
       <c r="G55" t="n">
-        <v>-393.9214638233061</v>
+        <v>-739.6587120696386</v>
       </c>
       <c r="H55" t="n">
-        <v>24667.03</v>
+        <v>24276.6</v>
       </c>
       <c r="I55" t="n">
-        <v>24670.5214638233</v>
+        <v>25016.25871206964</v>
       </c>
       <c r="J55" t="n">
-        <v>24667.03000352578</v>
+        <v>24519.82728659916</v>
       </c>
       <c r="K55" t="n">
-        <v>24670.52147625739</v>
+        <v>24773.03142547048</v>
       </c>
     </row>
     <row r="56">
@@ -10428,19 +10460,19 @@
         <v>138.68</v>
       </c>
       <c r="G56" t="n">
-        <v>132.7244941297067</v>
+        <v>-796.3350568703099</v>
       </c>
       <c r="H56" t="n">
-        <v>24667.16</v>
+        <v>24806.4</v>
       </c>
       <c r="I56" t="n">
-        <v>24673.67550587029</v>
+        <v>25602.73505687031</v>
       </c>
       <c r="J56" t="n">
-        <v>24667.16000939417</v>
+        <v>25061.67141079864</v>
       </c>
       <c r="K56" t="n">
-        <v>24673.67552625923</v>
+        <v>25347.46364607167</v>
       </c>
     </row>
     <row r="57">
@@ -10454,19 +10486,19 @@
         <v>138.58</v>
       </c>
       <c r="G57" t="n">
-        <v>559.8536470967701</v>
+        <v>-414.7155002998697</v>
       </c>
       <c r="H57" t="n">
-        <v>24667.22</v>
+        <v>24793.26666666667</v>
       </c>
       <c r="I57" t="n">
-        <v>24679.14635290323</v>
+        <v>25653.71550029987</v>
       </c>
       <c r="J57" t="n">
-        <v>24667.22002451077</v>
+        <v>25061.50724813849</v>
       </c>
       <c r="K57" t="n">
-        <v>24679.14638290914</v>
+        <v>25385.47491882805</v>
       </c>
     </row>
     <row r="58">
@@ -10480,19 +10512,19 @@
         <v>138.48</v>
       </c>
       <c r="G58" t="n">
-        <v>-32.14740484383583</v>
+        <v>-1065.022005916664</v>
       </c>
       <c r="H58" t="n">
-        <v>24667.03</v>
+        <v>24787.83526981912</v>
       </c>
       <c r="I58" t="n">
-        <v>24688.44740484384</v>
+        <v>25721.32200591666</v>
       </c>
       <c r="J58" t="n">
-        <v>24667.03006262852</v>
+        <v>25070.06817591052</v>
       </c>
       <c r="K58" t="n">
-        <v>24688.4474401166</v>
+        <v>25439.08909982527</v>
       </c>
     </row>
     <row r="59">
@@ -10506,19 +10538,19 @@
         <v>138.38</v>
       </c>
       <c r="G59" t="n">
-        <v>-220.1310193885147</v>
+        <v>-1320.605393583977</v>
       </c>
       <c r="H59" t="n">
-        <v>24666.89</v>
+        <v>24787.74245502336</v>
       </c>
       <c r="I59" t="n">
-        <v>24704.63101938851</v>
+        <v>25805.10539358398</v>
       </c>
       <c r="J59" t="n">
-        <v>24666.89015672086</v>
+        <v>25085.10244036208</v>
       </c>
       <c r="K59" t="n">
-        <v>24704.63103518591</v>
+        <v>25507.74540824525</v>
       </c>
     </row>
     <row r="60">
@@ -10532,19 +10564,19 @@
         <v>138.28</v>
       </c>
       <c r="G60" t="n">
-        <v>375.9854909245223</v>
+        <v>-794.2645669755475</v>
       </c>
       <c r="H60" t="n">
-        <v>24666.94</v>
+        <v>24787.87173367169</v>
       </c>
       <c r="I60" t="n">
-        <v>24732.21450907548</v>
+        <v>25902.46456697555</v>
       </c>
       <c r="J60" t="n">
-        <v>24666.94038410054</v>
+        <v>25101.62096159845</v>
       </c>
       <c r="K60" t="n">
-        <v>24732.21442335156</v>
+        <v>25588.71533904879</v>
       </c>
     </row>
     <row r="61">
@@ -10558,19 +10590,19 @@
         <v>138.18</v>
       </c>
       <c r="G61" t="n">
-        <v>178.4991691061186</v>
+        <v>-1060.233034401597</v>
       </c>
       <c r="H61" t="n">
-        <v>24666.87</v>
+        <v>24787.86595343672</v>
       </c>
       <c r="I61" t="n">
-        <v>24777.70083089388</v>
+        <v>26016.4330344016</v>
       </c>
       <c r="J61" t="n">
-        <v>24666.87092204559</v>
+        <v>25119.41260150493</v>
       </c>
       <c r="K61" t="n">
-        <v>24777.70041546725</v>
+        <v>25684.88638633339</v>
       </c>
     </row>
     <row r="62">
@@ -10584,19 +10616,19 @@
         <v>138.08</v>
       </c>
       <c r="G62" t="n">
-        <v>254.0407125614074</v>
+        <v>-1046.22516804537</v>
       </c>
       <c r="H62" t="n">
-        <v>24666.67</v>
+        <v>24787.71989566484</v>
       </c>
       <c r="I62" t="n">
-        <v>24851.45928743859</v>
+        <v>26151.72516804537</v>
       </c>
       <c r="J62" t="n">
-        <v>24666.67216808835</v>
+        <v>25138.6401613638</v>
       </c>
       <c r="K62" t="n">
-        <v>24851.4579640399</v>
+        <v>25800.80490234641</v>
       </c>
     </row>
     <row r="63">
@@ -10610,19 +10642,19 @@
         <v>137.98</v>
       </c>
       <c r="G63" t="n">
-        <v>956.9893457400431</v>
+        <v>-389.2155017653677</v>
       </c>
       <c r="H63" t="n">
-        <v>24666.48</v>
+        <v>24787.57313408063</v>
       </c>
       <c r="I63" t="n">
-        <v>24969.11065425996</v>
+        <v>26315.31550176537</v>
       </c>
       <c r="J63" t="n">
-        <v>24666.48499399883</v>
+        <v>25159.63739886654</v>
       </c>
       <c r="K63" t="n">
-        <v>24969.10704361298</v>
+        <v>25943.25123697946</v>
       </c>
     </row>
     <row r="64">
@@ -10636,19 +10668,19 @@
         <v>137.88</v>
       </c>
       <c r="G64" t="n">
-        <v>681.4151662467921</v>
+        <v>-682.8745610208716</v>
       </c>
       <c r="H64" t="n">
-        <v>24666.02</v>
+        <v>24787.13654767668</v>
       </c>
       <c r="I64" t="n">
-        <v>25152.98483375321</v>
+        <v>26517.27456102087</v>
       </c>
       <c r="J64" t="n">
-        <v>24666.03126934809</v>
+        <v>25182.3406600044</v>
       </c>
       <c r="K64" t="n">
-        <v>25152.97579036043</v>
+        <v>26122.07044869316</v>
       </c>
     </row>
     <row r="65">
@@ -10662,19 +10694,19 @@
         <v>137.78</v>
       </c>
       <c r="G65" t="n">
-        <v>892.9864982862564</v>
+        <v>-445.6095253809253</v>
       </c>
       <c r="H65" t="n">
-        <v>24665.38</v>
+        <v>24786.48219507026</v>
       </c>
       <c r="I65" t="n">
-        <v>25435.51350171374</v>
+        <v>26774.10952538093</v>
       </c>
       <c r="J65" t="n">
-        <v>24665.40491509316</v>
+        <v>25207.08509985794</v>
       </c>
       <c r="K65" t="n">
-        <v>25435.49210695247</v>
+        <v>26353.50662059324</v>
       </c>
     </row>
     <row r="66">
@@ -10688,19 +10720,19 @@
         <v>137.68</v>
       </c>
       <c r="G66" t="n">
-        <v>898.6308616798633</v>
+        <v>-352.2540540929622</v>
       </c>
       <c r="H66" t="n">
-        <v>24664.62</v>
+        <v>24785.70596930254</v>
       </c>
       <c r="I66" t="n">
-        <v>25862.06913832014</v>
+        <v>27112.95405409296</v>
       </c>
       <c r="J66" t="n">
-        <v>24664.67397302527</v>
+        <v>25234.27526597932</v>
       </c>
       <c r="K66" t="n">
-        <v>25862.02063889342</v>
+        <v>26664.38475741618</v>
       </c>
     </row>
     <row r="67">
@@ -10714,19 +10746,19 @@
         <v>137.58</v>
       </c>
       <c r="G67" t="n">
-        <v>560.8957618625172</v>
+        <v>-523.3200170261989</v>
       </c>
       <c r="H67" t="n">
-        <v>24663.62</v>
+        <v>24784.65222572482</v>
       </c>
       <c r="I67" t="n">
-        <v>26494.70423813748</v>
+        <v>27578.9200170262</v>
       </c>
       <c r="J67" t="n">
-        <v>24663.73457283267</v>
+        <v>25264.11971392738</v>
       </c>
       <c r="K67" t="n">
-        <v>26494.59803523465</v>
+        <v>27099.45252882363</v>
       </c>
     </row>
     <row r="68">
@@ -10740,19 +10772,19 @@
         <v>137.48</v>
       </c>
       <c r="G68" t="n">
-        <v>532.1519816452965</v>
+        <v>-298.2244993401</v>
       </c>
       <c r="H68" t="n">
-        <v>24662.42</v>
+        <v>24783.37872862409</v>
       </c>
       <c r="I68" t="n">
-        <v>27416.9480183547</v>
+        <v>28247.3244993401</v>
       </c>
       <c r="J68" t="n">
-        <v>24662.65835296192</v>
+        <v>25297.10864957656</v>
       </c>
       <c r="K68" t="n">
-        <v>27416.72225631202</v>
+        <v>27733.59457838763</v>
       </c>
     </row>
     <row r="69">
@@ -10766,19 +10798,19 @@
         <v>137.38</v>
       </c>
       <c r="G69" t="n">
-        <v>-20.33575649244449</v>
+        <v>-521.1782366739208</v>
       </c>
       <c r="H69" t="n">
-        <v>24660.9</v>
+        <v>24781.74649038786</v>
       </c>
       <c r="I69" t="n">
-        <v>28738.23575649245</v>
+        <v>29239.07823667392</v>
       </c>
       <c r="J69" t="n">
-        <v>24661.38600464559</v>
+        <v>25333.62006690957</v>
       </c>
       <c r="K69" t="n">
-        <v>28737.76838911651</v>
+        <v>28687.20466015222</v>
       </c>
     </row>
     <row r="70">
@@ -10792,19 +10824,19 @@
         <v>137.28</v>
       </c>
       <c r="G70" t="n">
-        <v>119.1487001380483</v>
+        <v>-20.00712573503552</v>
       </c>
       <c r="H70" t="n">
-        <v>24658.94</v>
+        <v>24779.60997660406</v>
       </c>
       <c r="I70" t="n">
-        <v>30598.45129986195</v>
+        <v>30737.60712573503</v>
       </c>
       <c r="J70" t="n">
-        <v>24659.91138668783</v>
+        <v>25374.1311071873</v>
       </c>
       <c r="K70" t="n">
-        <v>30597.50706196613</v>
+        <v>30143.0859951518</v>
       </c>
     </row>
     <row r="71">
@@ -10818,19 +10850,19 @@
         <v>137.18</v>
       </c>
       <c r="G71" t="n">
-        <v>-390.5161594470555</v>
+        <v>-218.2300479432743</v>
       </c>
       <c r="H71" t="n">
-        <v>24656.22</v>
+        <v>24776.63329238767</v>
       </c>
       <c r="I71" t="n">
-        <v>33170.31615944706</v>
+        <v>32998.03004794328</v>
       </c>
       <c r="J71" t="n">
-        <v>24658.1234039693</v>
+        <v>25419.06203735647</v>
       </c>
       <c r="K71" t="n">
-        <v>33168.45167165816</v>
+        <v>32355.60130297447</v>
       </c>
     </row>
     <row r="72">
@@ -10844,19 +10876,19 @@
         <v>137.08</v>
       </c>
       <c r="G72" t="n">
-        <v>-107.3454487896015</v>
+        <v>215.1414679670925</v>
       </c>
       <c r="H72" t="n">
-        <v>24652.4</v>
+        <v>24772.41904972702</v>
       </c>
       <c r="I72" t="n">
-        <v>36657.4454487896</v>
+        <v>36334.95853203291</v>
       </c>
       <c r="J72" t="n">
-        <v>24656.05693219255</v>
+        <v>25468.94213365525</v>
       </c>
       <c r="K72" t="n">
-        <v>36653.84338779867</v>
+        <v>35638.43544810468</v>
       </c>
     </row>
     <row r="73">
@@ -10870,19 +10902,19 @@
         <v>136.98</v>
       </c>
       <c r="G73" t="n">
-        <v>38.78599370734446</v>
+        <v>249.1941239978478</v>
       </c>
       <c r="H73" t="n">
-        <v>24646.99</v>
+        <v>24766.41512503193</v>
       </c>
       <c r="I73" t="n">
-        <v>41281.71400629266</v>
+        <v>41071.30587600215</v>
       </c>
       <c r="J73" t="n">
-        <v>24653.87993672997</v>
+        <v>25524.3665169214</v>
       </c>
       <c r="K73" t="n">
-        <v>41274.90009893384</v>
+        <v>40313.35448411269</v>
       </c>
     </row>
     <row r="74">
@@ -10896,19 +10928,19 @@
         <v>136.88</v>
       </c>
       <c r="G74" t="n">
-        <v>118.6201939058883</v>
+        <v>-69.12478306514822</v>
       </c>
       <c r="H74" t="n">
-        <v>24639.24</v>
+        <v>24757.78139103813</v>
       </c>
       <c r="I74" t="n">
-        <v>47250.07980609411</v>
+        <v>47437.82478306515</v>
       </c>
       <c r="J74" t="n">
-        <v>24651.97201071636</v>
+        <v>25585.9318729531</v>
       </c>
       <c r="K74" t="n">
-        <v>47237.45113391086</v>
+        <v>46609.67430115017</v>
       </c>
     </row>
     <row r="75">
@@ -10922,19 +10954,19 @@
         <v>136.78</v>
       </c>
       <c r="G75" t="n">
-        <v>858.9461275442445</v>
+        <v>110.4806636909925</v>
       </c>
       <c r="H75" t="n">
-        <v>24628.48</v>
+        <v>24745.773001035</v>
       </c>
       <c r="I75" t="n">
-        <v>54685.35387245576</v>
+        <v>55433.81933630901</v>
       </c>
       <c r="J75" t="n">
-        <v>24651.56019921194</v>
+        <v>25654.71685000229</v>
       </c>
       <c r="K75" t="n">
-        <v>54662.41103366882</v>
+        <v>54524.87548734173</v>
       </c>
     </row>
     <row r="76">
@@ -10948,19 +10980,19 @@
         <v>136.68</v>
       </c>
       <c r="G76" t="n">
-        <v>-109.6400181099671</v>
+        <v>-1296.391852625668</v>
       </c>
       <c r="H76" t="n">
-        <v>24613.75</v>
+        <v>24729.30657343539</v>
       </c>
       <c r="I76" t="n">
-        <v>63501.54001810997</v>
+        <v>64688.29185262567</v>
       </c>
       <c r="J76" t="n">
-        <v>24654.80132128598</v>
+        <v>25731.98859147292</v>
       </c>
       <c r="K76" t="n">
-        <v>63460.66639871123</v>
+        <v>63685.60983458813</v>
       </c>
     </row>
     <row r="77">
@@ -10974,19 +11006,19 @@
         <v>136.58</v>
       </c>
       <c r="G77" t="n">
-        <v>450.3889992333716</v>
+        <v>-716.4119039887737</v>
       </c>
       <c r="H77" t="n">
-        <v>24594.48</v>
+        <v>24707.7397387742</v>
       </c>
       <c r="I77" t="n">
-        <v>73223.51100076662</v>
+        <v>74390.31190398877</v>
       </c>
       <c r="J77" t="n">
-        <v>24666.13581078578</v>
+        <v>25820.19183904751</v>
       </c>
       <c r="K77" t="n">
-        <v>73152.07737649287</v>
+        <v>73277.85980371544</v>
       </c>
     </row>
     <row r="78">
@@ -11000,19 +11032,19 @@
         <v>136.48</v>
       </c>
       <c r="G78" t="n">
-        <v>710.4177324953198</v>
+        <v>166.604966561179</v>
       </c>
       <c r="H78" t="n">
-        <v>24569.99</v>
+        <v>24680.31182194132</v>
       </c>
       <c r="I78" t="n">
-        <v>82808.78226750468</v>
+        <v>83352.59503343882</v>
       </c>
       <c r="J78" t="n">
-        <v>24692.76557064966</v>
+        <v>25922.71529363791</v>
       </c>
       <c r="K78" t="n">
-        <v>82686.27273769568</v>
+        <v>82110.19156174222</v>
       </c>
     </row>
     <row r="79">
@@ -11026,19 +11058,19 @@
         <v>136.38</v>
       </c>
       <c r="G79" t="n">
-        <v>653.9315884959506</v>
+        <v>1065.600124475735</v>
       </c>
       <c r="H79" t="n">
-        <v>24539.77</v>
+        <v>24646.43950944506</v>
       </c>
       <c r="I79" t="n">
-        <v>90647.76841150405</v>
+        <v>90236.09987552426</v>
       </c>
       <c r="J79" t="n">
-        <v>24746.31594761214</v>
+        <v>26044.71750922274</v>
       </c>
       <c r="K79" t="n">
-        <v>90441.5243561747</v>
+        <v>88837.82187574658</v>
       </c>
     </row>
     <row r="80">
@@ -11052,19 +11084,19 @@
         <v>136.28</v>
       </c>
       <c r="G80" t="n">
-        <v>-1109.860877563304</v>
+        <v>-26.08085490638041</v>
       </c>
       <c r="H80" t="n">
-        <v>24504.71</v>
+        <v>24607.11514140031</v>
       </c>
       <c r="I80" t="n">
-        <v>94972.96087756331</v>
+        <v>93889.18085490639</v>
       </c>
       <c r="J80" t="n">
-        <v>24845.96728917491</v>
+        <v>26195.43057239637</v>
       </c>
       <c r="K80" t="n">
-        <v>94632.02521956561</v>
+        <v>92300.86542391033</v>
       </c>
     </row>
     <row r="81">
@@ -11078,19 +11110,19 @@
         <v>136.18</v>
       </c>
       <c r="G81" t="n">
-        <v>209.4698187130853</v>
+        <v>1184.378334206063</v>
       </c>
       <c r="H81" t="n">
-        <v>24466.94</v>
+        <v>24564.75233465225</v>
       </c>
       <c r="I81" t="n">
-        <v>94659.03018128691</v>
+        <v>93684.12166579394</v>
       </c>
       <c r="J81" t="n">
-        <v>25020.84123968956</v>
+        <v>26389.61348903899</v>
       </c>
       <c r="K81" t="n">
-        <v>94105.44900684305</v>
+        <v>91859.26051140721</v>
       </c>
     </row>
     <row r="82">
@@ -11104,19 +11136,19 @@
         <v>136.08</v>
       </c>
       <c r="G82" t="n">
-        <v>-398.6052207686298</v>
+        <v>-228.3806591400935</v>
       </c>
       <c r="H82" t="n">
-        <v>24428.62</v>
+        <v>24521.76385515688</v>
       </c>
       <c r="I82" t="n">
-        <v>89887.50522076862</v>
+        <v>89717.28065914009</v>
       </c>
       <c r="J82" t="n">
-        <v>25312.10624883707</v>
+        <v>26649.04193861639</v>
       </c>
       <c r="K82" t="n">
-        <v>89004.31693064705</v>
+        <v>87590.00257568057</v>
       </c>
     </row>
     <row r="83">
@@ -11130,19 +11162,19 @@
         <v>135.98</v>
       </c>
       <c r="G83" t="n">
-        <v>-409.5990821751911</v>
+        <v>-1135.537547534856</v>
       </c>
       <c r="H83" t="n">
-        <v>24392.25</v>
+        <v>24480.96099986324</v>
       </c>
       <c r="I83" t="n">
-        <v>82065.29908217519</v>
+        <v>82791.23754753485</v>
       </c>
       <c r="J83" t="n">
-        <v>25777.47874950795</v>
+        <v>27008.14071672294</v>
       </c>
       <c r="K83" t="n">
-        <v>80680.33198515838</v>
+        <v>80264.05783067514</v>
       </c>
     </row>
     <row r="84">
@@ -11156,19 +11188,19 @@
         <v>135.88</v>
       </c>
       <c r="G84" t="n">
-        <v>-219.2754036654369</v>
+        <v>-1326.690558937684</v>
       </c>
       <c r="H84" t="n">
-        <v>24360.03</v>
+        <v>24444.81524063781</v>
       </c>
       <c r="I84" t="n">
-        <v>73080.37540366544</v>
+        <v>74187.79055893769</v>
       </c>
       <c r="J84" t="n">
-        <v>26495.70940251092</v>
+        <v>27522.28884691905</v>
       </c>
       <c r="K84" t="n">
-        <v>70944.91565848282</v>
+        <v>71110.31695265645</v>
       </c>
     </row>
     <row r="85">
@@ -11182,19 +11214,19 @@
         <v>135.78</v>
       </c>
       <c r="G85" t="n">
-        <v>666.9690062067384</v>
+        <v>-106.5138081083278</v>
       </c>
       <c r="H85" t="n">
-        <v>24332.59</v>
+        <v>24414.03995661348</v>
       </c>
       <c r="I85" t="n">
-        <v>64561.03099379326</v>
+        <v>65334.51380810833</v>
       </c>
       <c r="J85" t="n">
-        <v>27571.33514814808</v>
+        <v>28280.92455035566</v>
       </c>
       <c r="K85" t="n">
-        <v>61322.46511078429</v>
+        <v>61467.62921436614</v>
       </c>
     </row>
     <row r="86">
@@ -11208,19 +11240,19 @@
         <v>135.68</v>
       </c>
       <c r="G86" t="n">
-        <v>253.6409861474895</v>
+        <v>320.3733693067916</v>
       </c>
       <c r="H86" t="n">
-        <v>24309.7</v>
+        <v>24388.37124275643</v>
       </c>
       <c r="I86" t="n">
-        <v>57571.35901385251</v>
+        <v>57504.62663069321</v>
       </c>
       <c r="J86" t="n">
-        <v>29142.07085874269</v>
+        <v>29429.10339071073</v>
       </c>
       <c r="K86" t="n">
-        <v>52739.13329924556</v>
+        <v>52463.89448273891</v>
       </c>
     </row>
     <row r="87">
@@ -11234,19 +11266,19 @@
         <v>135.58</v>
       </c>
       <c r="G87" t="n">
-        <v>30.52255851968221</v>
+        <v>1055.930026061935</v>
       </c>
       <c r="H87" t="n">
-        <v>24290.78</v>
+        <v>24367.17065298516</v>
       </c>
       <c r="I87" t="n">
-        <v>52674.67744148031</v>
+        <v>51649.26997393806</v>
       </c>
       <c r="J87" t="n">
-        <v>31386.03166497465</v>
+        <v>31192.76193748649</v>
       </c>
       <c r="K87" t="n">
-        <v>45579.54539336084</v>
+        <v>44823.67868943673</v>
       </c>
     </row>
     <row r="88">
@@ -11260,19 +11292,19 @@
         <v>135.48</v>
       </c>
       <c r="G88" t="n">
-        <v>-615.6564458582361</v>
+        <v>1128.055205924509</v>
       </c>
       <c r="H88" t="n">
-        <v>24274.92</v>
+        <v>24349.38965781612</v>
       </c>
       <c r="I88" t="n">
-        <v>50128.05644585824</v>
+        <v>48384.34479407549</v>
       </c>
       <c r="J88" t="n">
-        <v>34527.08151507288</v>
+        <v>33898.52926897626</v>
       </c>
       <c r="K88" t="n">
-        <v>39875.99847245292</v>
+        <v>38835.20518291536</v>
       </c>
     </row>
     <row r="89">
@@ -11286,19 +11318,19 @@
         <v>135.38</v>
       </c>
       <c r="G89" t="n">
-        <v>-735.8358925049106</v>
+        <v>1241.385169820678</v>
       </c>
       <c r="H89" t="n">
-        <v>24260.81</v>
+        <v>24333.58419394548</v>
       </c>
       <c r="I89" t="n">
-        <v>50055.43589250491</v>
+        <v>48078.21483017932</v>
       </c>
       <c r="J89" t="n">
-        <v>38835.74191594707</v>
+        <v>37971.34719464639</v>
       </c>
       <c r="K89" t="n">
-        <v>35480.60107959645</v>
+        <v>34440.45182947841</v>
       </c>
     </row>
     <row r="90">
@@ -11312,19 +11344,19 @@
         <v>135.28</v>
       </c>
       <c r="G90" t="n">
-        <v>159.40020996979</v>
+        <v>1764.106699024007</v>
       </c>
       <c r="H90" t="n">
-        <v>24246.88</v>
+        <v>24317.98338551542</v>
       </c>
       <c r="I90" t="n">
-        <v>52551.09979003021</v>
+        <v>50946.39330097599</v>
       </c>
       <c r="J90" t="n">
-        <v>44620.0458722225</v>
+        <v>43885.61472450303</v>
       </c>
       <c r="K90" t="n">
-        <v>32178.03421494746</v>
+        <v>31378.76196198839</v>
       </c>
     </row>
     <row r="91">
@@ -11338,19 +11370,19 @@
         <v>135.18</v>
       </c>
       <c r="G91" t="n">
-        <v>-1206.439780072142</v>
+        <v>-565.4298046886906</v>
       </c>
       <c r="H91" t="n">
-        <v>24231.58</v>
+        <v>24300.84819403032</v>
       </c>
       <c r="I91" t="n">
-        <v>57710.33978007214</v>
+        <v>57069.32980468869</v>
       </c>
       <c r="J91" t="n">
-        <v>52195.17467428463</v>
+        <v>52048.87936553021</v>
       </c>
       <c r="K91" t="n">
-        <v>29746.85822026823</v>
+        <v>29321.2986331888</v>
       </c>
     </row>
     <row r="92">
@@ -11364,19 +11396,19 @@
         <v>135.08</v>
       </c>
       <c r="G92" t="n">
-        <v>633.4026596578333</v>
+        <v>-78.48313718389545</v>
       </c>
       <c r="H92" t="n">
-        <v>24213.5</v>
+        <v>24280.57562375942</v>
       </c>
       <c r="I92" t="n">
-        <v>65586.79734034216</v>
+        <v>66298.68313718389</v>
       </c>
       <c r="J92" t="n">
-        <v>61812.76473215064</v>
+        <v>62617.62581131772</v>
       </c>
       <c r="K92" t="n">
-        <v>27987.66805365148</v>
+        <v>27961.63294962559</v>
       </c>
     </row>
     <row r="93">
@@ -11390,19 +11422,19 @@
         <v>134.98</v>
       </c>
       <c r="G93" t="n">
-        <v>686.5369515893981</v>
+        <v>-1336.005216361489</v>
       </c>
       <c r="H93" t="n">
-        <v>24190.71</v>
+        <v>24255.0257887832</v>
       </c>
       <c r="I93" t="n">
-        <v>76064.56304841061</v>
+        <v>78087.10521636149</v>
       </c>
       <c r="J93" t="n">
-        <v>73523.11502234267</v>
+        <v>75284.90207293362</v>
       </c>
       <c r="K93" t="n">
-        <v>26732.32472057067</v>
+        <v>27057.22893221107</v>
       </c>
     </row>
     <row r="94">
@@ -11416,19 +11448,19 @@
         <v>134.88</v>
       </c>
       <c r="G94" t="n">
-        <v>2078.456262653388</v>
+        <v>-626.27239658701</v>
       </c>
       <c r="H94" t="n">
-        <v>24161.52</v>
+        <v>24222.27453657212</v>
       </c>
       <c r="I94" t="n">
-        <v>88636.24373734661</v>
+        <v>91340.97239658701</v>
       </c>
       <c r="J94" t="n">
-        <v>86952.35054942501</v>
+        <v>89126.39694964378</v>
       </c>
       <c r="K94" t="n">
-        <v>25845.61826923408</v>
+        <v>26436.84998351534</v>
       </c>
     </row>
     <row r="95">
@@ -11442,19 +11474,19 @@
         <v>134.78</v>
       </c>
       <c r="G95" t="n">
-        <v>-226.2277474439179</v>
+        <v>-2519.763375652721</v>
       </c>
       <c r="H95" t="n">
-        <v>24125.04</v>
+        <v>24181.34142671293</v>
       </c>
       <c r="I95" t="n">
-        <v>102121.2277474439</v>
+        <v>104414.7633756527</v>
       </c>
       <c r="J95" t="n">
-        <v>101023.7685056026</v>
+        <v>102606.5927852684</v>
       </c>
       <c r="K95" t="n">
-        <v>25222.74599091548</v>
+        <v>25989.51201709724</v>
       </c>
     </row>
     <row r="96">
@@ -11468,19 +11500,19 @@
         <v>134.68</v>
       </c>
       <c r="G96" t="n">
-        <v>1309.749118604988</v>
+        <v>471.6606431593827</v>
       </c>
       <c r="H96" t="n">
-        <v>24081.04</v>
+        <v>24131.95397749292</v>
       </c>
       <c r="I96" t="n">
-        <v>114489.250881395</v>
+        <v>115327.3393568406</v>
       </c>
       <c r="J96" t="n">
-        <v>113785.9198858151</v>
+        <v>113812.0404798648</v>
       </c>
       <c r="K96" t="n">
-        <v>24784.65619940441</v>
+        <v>25647.25285446877</v>
       </c>
     </row>
     <row r="97">
@@ -11494,19 +11526,19 @@
         <v>134.58</v>
       </c>
       <c r="G97" t="n">
-        <v>-693.6326344683766</v>
+        <v>234.409748845821</v>
       </c>
       <c r="H97" t="n">
-        <v>24030.18</v>
+        <v>24074.85126550225</v>
       </c>
       <c r="I97" t="n">
-        <v>123113.6326344684</v>
+        <v>122185.5902511542</v>
       </c>
       <c r="J97" t="n">
-        <v>122670.5618201374</v>
+        <v>120890.1009069149</v>
       </c>
       <c r="K97" t="n">
-        <v>24473.56291737934</v>
+        <v>25370.34060974157</v>
       </c>
     </row>
     <row r="98">
@@ -11520,19 +11552,19 @@
         <v>134.48</v>
       </c>
       <c r="G98" t="n">
-        <v>-1774.974067816613</v>
+        <v>220.8424487655429</v>
       </c>
       <c r="H98" t="n">
-        <v>23975.34</v>
+        <v>24013.26971418188</v>
       </c>
       <c r="I98" t="n">
-        <v>125681.9740678166</v>
+        <v>123686.1575512345</v>
       </c>
       <c r="J98" t="n">
-        <v>125407.708853332</v>
+        <v>122561.540454168</v>
       </c>
       <c r="K98" t="n">
-        <v>24249.92532256227</v>
+        <v>25137.88681124837</v>
       </c>
     </row>
     <row r="99">
@@ -11546,19 +11578,19 @@
         <v>134.38</v>
       </c>
       <c r="G99" t="n">
-        <v>136.9231750479667</v>
+        <v>2015.08246201271</v>
       </c>
       <c r="H99" t="n">
-        <v>23919.83</v>
+        <v>23950.92875000304</v>
       </c>
       <c r="I99" t="n">
-        <v>121373.076824952</v>
+        <v>119494.9175379873</v>
       </c>
       <c r="J99" t="n">
-        <v>121206.3139117128</v>
+        <v>118506.9163036886</v>
       </c>
       <c r="K99" t="n">
-        <v>24086.89949725173</v>
+        <v>24938.92998430175</v>
       </c>
     </row>
     <row r="100">
@@ -11572,19 +11604,19 @@
         <v>134.28</v>
       </c>
       <c r="G100" t="n">
-        <v>671.6979805861338</v>
+        <v>1661.881736187235</v>
       </c>
       <c r="H100" t="n">
-        <v>23867.04</v>
+        <v>23891.62969337086</v>
       </c>
       <c r="I100" t="n">
-        <v>111334.3020194139</v>
+        <v>110344.1182638128</v>
       </c>
       <c r="J100" t="n">
-        <v>111234.7355044792</v>
+        <v>109467.7547690439</v>
       </c>
       <c r="K100" t="n">
-        <v>23966.88161190439</v>
+        <v>24767.99318813972</v>
       </c>
     </row>
     <row r="101">
@@ -11598,19 +11630,19 @@
         <v>134.18</v>
       </c>
       <c r="G101" t="n">
-        <v>-281.2885526031605</v>
+        <v>-96.42990470498626</v>
       </c>
       <c r="H101" t="n">
-        <v>23820.68</v>
+        <v>23839.56017913263</v>
       </c>
       <c r="I101" t="n">
-        <v>97985.48855260316</v>
+        <v>97800.62990470498</v>
       </c>
       <c r="J101" t="n">
-        <v>97927.13471483838</v>
+        <v>97017.06223867928</v>
       </c>
       <c r="K101" t="n">
-        <v>23879.26705941024</v>
+        <v>24623.12784515832</v>
       </c>
     </row>
     <row r="102">
@@ -11624,19 +11656,19 @@
         <v>134.08</v>
       </c>
       <c r="G102" t="n">
-        <v>-957.7148372858355</v>
+        <v>-942.0061377134552</v>
       </c>
       <c r="H102" t="n">
-        <v>23782.77</v>
+        <v>23796.9847774121</v>
       </c>
       <c r="I102" t="n">
-        <v>83816.81483728584</v>
+        <v>83801.10613771346</v>
       </c>
       <c r="J102" t="n">
-        <v>83783.25489985356</v>
+        <v>83095.73368762934</v>
       </c>
       <c r="K102" t="n">
-        <v>23816.51870338546</v>
+        <v>24502.35722749622</v>
       </c>
     </row>
     <row r="103">
@@ -11650,19 +11682,19 @@
         <v>133.98</v>
       </c>
       <c r="G103" t="n">
-        <v>250.6276291811664</v>
+        <v>703.2200727947493</v>
       </c>
       <c r="H103" t="n">
-        <v>23752.84</v>
+        <v>23763.37321787141</v>
       </c>
       <c r="I103" t="n">
-        <v>70599.27237081883</v>
+        <v>70146.67992720524</v>
       </c>
       <c r="J103" t="n">
-        <v>70580.33977669914</v>
+        <v>69507.94669263913</v>
       </c>
       <c r="K103" t="n">
-        <v>23771.91988370637</v>
+        <v>24402.10645243752</v>
       </c>
     </row>
     <row r="104">
@@ -11676,19 +11708,19 @@
         <v>133.88</v>
       </c>
       <c r="G104" t="n">
-        <v>-394.7554415117556</v>
+        <v>708.957805372338</v>
       </c>
       <c r="H104" t="n">
-        <v>23729.91</v>
+        <v>23737.61663691072</v>
       </c>
       <c r="I104" t="n">
-        <v>59241.95544151175</v>
+        <v>58138.24219462766</v>
       </c>
       <c r="J104" t="n">
-        <v>59231.48275322617</v>
+        <v>57556.84539532336</v>
       </c>
       <c r="K104" t="n">
-        <v>23740.49433595646</v>
+        <v>24319.01343621501</v>
       </c>
     </row>
     <row r="105">
@@ -11702,19 +11734,19 @@
         <v>133.78</v>
       </c>
       <c r="G105" t="n">
-        <v>-1784.373164752782</v>
+        <v>-215.3835018315804</v>
       </c>
       <c r="H105" t="n">
-        <v>23713.39</v>
+        <v>23719.06675256386</v>
       </c>
       <c r="I105" t="n">
-        <v>50007.27316475278</v>
+        <v>48438.28350183158</v>
       </c>
       <c r="J105" t="n">
-        <v>50001.59567041928</v>
+        <v>47906.62872561142</v>
       </c>
       <c r="K105" t="n">
-        <v>23719.15015770855</v>
+        <v>24250.72152878402</v>
       </c>
     </row>
     <row r="106">
@@ -11728,19 +11760,19 @@
         <v>133.68</v>
       </c>
       <c r="G106" t="n">
-        <v>-1572.33281085745</v>
+        <v>73.04115389852086</v>
       </c>
       <c r="H106" t="n">
-        <v>23701.85</v>
+        <v>23706.11003627524</v>
       </c>
       <c r="I106" t="n">
-        <v>42784.83281085745</v>
+        <v>41139.45884610148</v>
       </c>
       <c r="J106" t="n">
-        <v>42781.81806112801</v>
+        <v>40651.2724296469</v>
       </c>
       <c r="K106" t="n">
-        <v>23704.924741715</v>
+        <v>24194.29645272982</v>
       </c>
     </row>
     <row r="107">
@@ -11754,19 +11786,19 @@
         <v>133.58</v>
       </c>
       <c r="G107" t="n">
-        <v>-195.2493167640496</v>
+        <v>1147.641553659581</v>
       </c>
       <c r="H107" t="n">
-        <v>23693.45</v>
+        <v>23696.67011461664</v>
       </c>
       <c r="I107" t="n">
-        <v>37297.64931676405</v>
+        <v>35954.75844634042</v>
       </c>
       <c r="J107" t="n">
-        <v>37296.08250044106</v>
+        <v>35504.80438436779</v>
       </c>
       <c r="K107" t="n">
-        <v>23695.0595835922</v>
+        <v>24146.62417658928</v>
       </c>
     </row>
     <row r="108">
@@ -11780,19 +11812,19 @@
         <v>133.48</v>
       </c>
       <c r="G108" t="n">
-        <v>568.0578299858898</v>
+        <v>1365.424542574819</v>
       </c>
       <c r="H108" t="n">
-        <v>23687.09</v>
+        <v>23689.5353966002</v>
       </c>
       <c r="I108" t="n">
-        <v>33224.74217001411</v>
+        <v>32427.37545742518</v>
       </c>
       <c r="J108" t="n">
-        <v>33223.94595877136</v>
+        <v>32011.24420940931</v>
       </c>
       <c r="K108" t="n">
-        <v>23687.91619415157</v>
+        <v>24105.66664461608</v>
       </c>
     </row>
     <row r="109">
@@ -11806,19 +11838,19 @@
         <v>133.38</v>
       </c>
       <c r="G109" t="n">
-        <v>431.1877162524579</v>
+        <v>602.9443829475786</v>
       </c>
       <c r="H109" t="n">
-        <v>23682.48</v>
+        <v>23684.3542444981</v>
       </c>
       <c r="I109" t="n">
-        <v>30261.91228374754</v>
+        <v>30090.15561705242</v>
       </c>
       <c r="J109" t="n">
-        <v>30261.51719716448</v>
+        <v>29704.10374303221</v>
       </c>
       <c r="K109" t="n">
-        <v>23682.89576970461</v>
+        <v>24070.40611851831</v>
       </c>
     </row>
     <row r="110">
@@ -11832,19 +11864,19 @@
         <v>133.28</v>
       </c>
       <c r="G110" t="n">
-        <v>1153.758122683015</v>
+        <v>747.1173357875123</v>
       </c>
       <c r="H110" t="n">
-        <v>23679.09</v>
+        <v>23680.54318015062</v>
       </c>
       <c r="I110" t="n">
-        <v>28145.74187731698</v>
+        <v>28552.38266421249</v>
       </c>
       <c r="J110" t="n">
-        <v>28145.55081696645</v>
+        <v>28193.209209247</v>
       </c>
       <c r="K110" t="n">
-        <v>23679.29510161959</v>
+        <v>24039.7166351161</v>
       </c>
     </row>
     <row r="111">
@@ -11858,19 +11890,19 @@
         <v>133.18</v>
       </c>
       <c r="G111" t="n">
-        <v>1043.163014364392</v>
+        <v>176.2346717100263</v>
       </c>
       <c r="H111" t="n">
-        <v>23676.5</v>
+        <v>23677.64005669981</v>
       </c>
       <c r="I111" t="n">
-        <v>26660.43698563561</v>
+        <v>27527.36532828997</v>
       </c>
       <c r="J111" t="n">
-        <v>26660.34719618613</v>
+        <v>27192.31527835809</v>
       </c>
       <c r="K111" t="n">
-        <v>23676.59916963443</v>
+        <v>24012.6901066317</v>
       </c>
     </row>
     <row r="112">
@@ -11884,19 +11916,19 @@
         <v>133.08</v>
       </c>
       <c r="G112" t="n">
-        <v>974.8675629441132</v>
+        <v>-212.8046614977029</v>
       </c>
       <c r="H112" t="n">
-        <v>23674.64</v>
+        <v>23675.54595813705</v>
       </c>
       <c r="I112" t="n">
-        <v>25635.83243705589</v>
+        <v>26823.5046614977</v>
       </c>
       <c r="J112" t="n">
-        <v>25635.79160910787</v>
+        <v>26510.19266491025</v>
       </c>
       <c r="K112" t="n">
-        <v>23674.68699304816</v>
+        <v>23988.85795472451</v>
       </c>
     </row>
     <row r="113">
@@ -11910,19 +11942,19 @@
         <v>132.98</v>
       </c>
       <c r="G113" t="n">
-        <v>840.5056141860805</v>
+        <v>-538.8332173180679</v>
       </c>
       <c r="H113" t="n">
-        <v>23673.29</v>
+        <v>23674.03089548006</v>
       </c>
       <c r="I113" t="n">
-        <v>24941.09438581392</v>
+        <v>26320.43321731807</v>
       </c>
       <c r="J113" t="n">
-        <v>24941.07654946323</v>
+        <v>26026.78269118753</v>
       </c>
       <c r="K113" t="n">
-        <v>23673.31182174085</v>
+        <v>23967.68142161059</v>
       </c>
     </row>
     <row r="114">
@@ -11936,19 +11968,19 @@
         <v>132.88</v>
       </c>
       <c r="G114" t="n">
-        <v>1180.867087072518</v>
+        <v>-286.4508553114429</v>
       </c>
       <c r="H114" t="n">
-        <v>23672.19</v>
+        <v>23672.80355545774</v>
       </c>
       <c r="I114" t="n">
-        <v>24478.03291292748</v>
+        <v>25945.35085531144</v>
       </c>
       <c r="J114" t="n">
-        <v>24478.02551713097</v>
+        <v>25669.54491823434</v>
       </c>
       <c r="K114" t="n">
-        <v>23672.19992898801</v>
+        <v>23948.60949253485</v>
       </c>
     </row>
     <row r="115">
@@ -11962,19 +11994,19 @@
         <v>132.78</v>
       </c>
       <c r="G115" t="n">
-        <v>1158.107609357565</v>
+        <v>-322.0966948510577</v>
       </c>
       <c r="H115" t="n">
-        <v>23671.22</v>
+        <v>23671.71143256843</v>
       </c>
       <c r="I115" t="n">
-        <v>24174.69239064243</v>
+        <v>25654.89669485106</v>
       </c>
       <c r="J115" t="n">
-        <v>24174.68954700493</v>
+        <v>25395.33829221049</v>
       </c>
       <c r="K115" t="n">
-        <v>23671.2244263156</v>
+        <v>23931.269835209</v>
       </c>
     </row>
     <row r="116">
@@ -11988,19 +12020,19 @@
         <v>132.68</v>
       </c>
       <c r="G116" t="n">
-        <v>1128.315323369065</v>
+        <v>-315.2330377818471</v>
       </c>
       <c r="H116" t="n">
-        <v>23670.39</v>
+        <v>23670.78361648917</v>
       </c>
       <c r="I116" t="n">
-        <v>23979.48467663093</v>
+        <v>25423.03303778185</v>
       </c>
       <c r="J116" t="n">
-        <v>23979.4837151233</v>
+        <v>25178.31228507199</v>
       </c>
       <c r="K116" t="n">
-        <v>23670.39193315339</v>
+        <v>23915.50436919902</v>
       </c>
     </row>
     <row r="117">
@@ -12014,19 +12046,19 @@
         <v>132.58</v>
       </c>
       <c r="G117" t="n">
-        <v>1282.770818689452</v>
+        <v>-94.60726761785918</v>
       </c>
       <c r="H117" t="n">
-        <v>23669.62</v>
+        <v>23669.914128815</v>
       </c>
       <c r="I117" t="n">
-        <v>23856.02918131055</v>
+        <v>25233.40726761786</v>
       </c>
       <c r="J117" t="n">
-        <v>23856.02894021788</v>
+        <v>25002.274513727</v>
       </c>
       <c r="K117" t="n">
-        <v>23669.62082707345</v>
+        <v>23901.04688270585</v>
       </c>
     </row>
     <row r="118">
@@ -12040,19 +12072,19 @@
         <v>132.48</v>
       </c>
       <c r="G118" t="n">
-        <v>465.3272500100975</v>
+        <v>-830.8355382013688</v>
       </c>
       <c r="H118" t="n">
-        <v>23669.07</v>
+        <v>23669.3014146235</v>
       </c>
       <c r="I118" t="n">
-        <v>23779.4727499899</v>
+        <v>25075.63553820137</v>
       </c>
       <c r="J118" t="n">
-        <v>23779.47275042952</v>
+        <v>24856.97899989589</v>
       </c>
       <c r="K118" t="n">
-        <v>23669.07034661331</v>
+        <v>23887.95795292898</v>
       </c>
     </row>
     <row r="119">
@@ -12066,19 +12098,19 @@
         <v>132.38</v>
       </c>
       <c r="G119" t="n">
-        <v>290.6730257146555</v>
+        <v>-918.87805086968</v>
       </c>
       <c r="H119" t="n">
-        <v>23668.83</v>
+        <v>23669.02172925921</v>
       </c>
       <c r="I119" t="n">
-        <v>23733.02697428535</v>
+        <v>24942.57805086968</v>
       </c>
       <c r="J119" t="n">
-        <v>23733.02703381033</v>
+        <v>24735.40512892543</v>
       </c>
       <c r="K119" t="n">
-        <v>23668.83014227922</v>
+        <v>23876.19465120346</v>
       </c>
     </row>
     <row r="120">
@@ -12092,19 +12124,19 @@
         <v>132.28</v>
       </c>
       <c r="G120" t="n">
-        <v>492.9691917897835</v>
+        <v>-630.5911882236287</v>
       </c>
       <c r="H120" t="n">
-        <v>23668.59</v>
+        <v>23668.75737358506</v>
       </c>
       <c r="I120" t="n">
-        <v>23705.23080821022</v>
+        <v>24828.79118822363</v>
       </c>
       <c r="J120" t="n">
-        <v>23705.23086618978</v>
+        <v>24632.21277015438</v>
       </c>
       <c r="K120" t="n">
-        <v>23668.59005720136</v>
+        <v>23865.33579165431</v>
       </c>
     </row>
     <row r="121">
@@ -12118,19 +12150,19 @@
         <v>132.18</v>
       </c>
       <c r="G121" t="n">
-        <v>-75.5826457909061</v>
+        <v>-1117.216483235821</v>
       </c>
       <c r="H121" t="n">
-        <v>23668.46</v>
+        <v>23668.61508943584</v>
       </c>
       <c r="I121" t="n">
-        <v>23688.98264579091</v>
+        <v>24730.61648323582</v>
       </c>
       <c r="J121" t="n">
-        <v>23688.98268778171</v>
+        <v>24543.83368502096</v>
       </c>
       <c r="K121" t="n">
-        <v>23668.46002252243</v>
+        <v>23855.3978876507</v>
       </c>
     </row>
     <row r="122">
@@ -12144,19 +12176,19 @@
         <v>132.08</v>
       </c>
       <c r="G122" t="n">
-        <v>24.75207194840914</v>
+        <v>-940.7390229528864</v>
       </c>
       <c r="H122" t="n">
-        <v>23668.47</v>
+        <v>23668.62023915951</v>
       </c>
       <c r="I122" t="n">
-        <v>23679.74792805159</v>
+        <v>24645.23902295289</v>
       </c>
       <c r="J122" t="n">
-        <v>23679.74795481941</v>
+        <v>24467.53193500809</v>
       </c>
       <c r="K122" t="n">
-        <v>23668.4700086845</v>
+        <v>23846.3273271043</v>
       </c>
     </row>
     <row r="123">
@@ -12170,19 +12202,19 @@
         <v>131.98</v>
       </c>
       <c r="G123" t="n">
-        <v>9.870468350789452</v>
+        <v>-885.9022905927195</v>
       </c>
       <c r="H123" t="n">
-        <v>23668.45</v>
+        <v>23668.6048858602</v>
       </c>
       <c r="I123" t="n">
-        <v>23674.52953164921</v>
+        <v>24570.30229059272</v>
       </c>
       <c r="J123" t="n">
-        <v>23674.52954748105</v>
+        <v>24401.02038033774</v>
       </c>
       <c r="K123" t="n">
-        <v>23668.45000327925</v>
+        <v>23837.88679611519</v>
       </c>
     </row>
     <row r="124">
@@ -12196,19 +12228,19 @@
         <v>131.88</v>
       </c>
       <c r="G124" t="n">
-        <v>29.64574967641965</v>
+        <v>-802.8116507647028</v>
       </c>
       <c r="H124" t="n">
-        <v>23668.44</v>
+        <v>23668.59038542026</v>
       </c>
       <c r="I124" t="n">
-        <v>23671.65425032358</v>
+        <v>24504.1116507647</v>
       </c>
       <c r="J124" t="n">
-        <v>23671.65425921511</v>
+        <v>24342.66554193562</v>
       </c>
       <c r="K124" t="n">
-        <v>23668.4400012125</v>
+        <v>23830.03649424934</v>
       </c>
     </row>
     <row r="125">
@@ -12222,19 +12254,19 @@
         <v>131.78</v>
       </c>
       <c r="G125" t="n">
-        <v>-2.696434235454944</v>
+        <v>-777.9060548093039</v>
       </c>
       <c r="H125" t="n">
-        <v>23668.43</v>
+        <v>23668.58094109892</v>
       </c>
       <c r="I125" t="n">
-        <v>23670.09643423546</v>
+        <v>24445.30605480931</v>
       </c>
       <c r="J125" t="n">
-        <v>23670.09643903493</v>
+        <v>24291.16045682243</v>
       </c>
       <c r="K125" t="n">
-        <v>23668.43000043899</v>
+        <v>23822.72653908579</v>
       </c>
     </row>
     <row r="126">
@@ -12248,19 +12280,19 @@
         <v>131.68</v>
       </c>
       <c r="G126" t="n">
-        <v>-518.8170935647977</v>
+        <v>-1242.344441766549</v>
       </c>
       <c r="H126" t="n">
-        <v>23668.57</v>
+        <v>23668.7354269795</v>
       </c>
       <c r="I126" t="n">
-        <v>23669.4170935648</v>
+        <v>24392.94444176655</v>
       </c>
       <c r="J126" t="n">
-        <v>23669.41709607203</v>
+        <v>24245.61204442104</v>
       </c>
       <c r="K126" t="n">
-        <v>23668.57000015562</v>
+        <v>23816.067824325</v>
       </c>
     </row>
     <row r="127">
@@ -12274,19 +12306,19 @@
         <v>131.58</v>
       </c>
       <c r="G127" t="n">
-        <v>50.58786605424029</v>
+        <v>-626.2521282984635</v>
       </c>
       <c r="H127" t="n">
-        <v>23668.69</v>
+        <v>23668.87513901928</v>
       </c>
       <c r="I127" t="n">
-        <v>23669.11213394576</v>
+        <v>24345.95212829846</v>
       </c>
       <c r="J127" t="n">
-        <v>23669.11213521873</v>
+        <v>24204.98831047669</v>
       </c>
       <c r="K127" t="n">
-        <v>23668.69000005401</v>
+        <v>23809.83895684106</v>
       </c>
     </row>
     <row r="128">
@@ -12300,19 +12332,19 @@
         <v>131.48</v>
       </c>
       <c r="G128" t="n">
-        <v>30.12379911464086</v>
+        <v>-604.4437132187886</v>
       </c>
       <c r="H128" t="n">
-        <v>23668.67</v>
+        <v>23668.85167499625</v>
       </c>
       <c r="I128" t="n">
-        <v>23668.87620088536</v>
+        <v>24303.44371321879</v>
       </c>
       <c r="J128" t="n">
-        <v>23668.8762015152</v>
+        <v>24168.44194093758</v>
       </c>
       <c r="K128" t="n">
-        <v>23668.67000001835</v>
+        <v>23803.85344727746</v>
       </c>
     </row>
     <row r="129">
@@ -12326,19 +12358,19 @@
         <v>131.38</v>
       </c>
       <c r="G129" t="n">
-        <v>-96.08871929624001</v>
+        <v>-692.3138177325272</v>
       </c>
       <c r="H129" t="n">
-        <v>23668.69</v>
+        <v>23668.87120990136</v>
       </c>
       <c r="I129" t="n">
-        <v>23668.78871929624</v>
+        <v>24265.01381773253</v>
       </c>
       <c r="J129" t="n">
-        <v>23668.78871960046</v>
+        <v>24135.60162837742</v>
       </c>
       <c r="K129" t="n">
-        <v>23668.69000000611</v>
+        <v>23798.28339925648</v>
       </c>
     </row>
     <row r="130">
@@ -12352,19 +12384,19 @@
         <v>131.28</v>
       </c>
       <c r="G130" t="n">
-        <v>-0.04631681029059109</v>
+        <v>-561.2172098631818</v>
       </c>
       <c r="H130" t="n">
         <v>23070.3</v>
       </c>
       <c r="I130" t="n">
-        <v>23070.34631681029</v>
+        <v>23631.51720986318</v>
       </c>
       <c r="J130" t="n">
-        <v>23070.3463169539</v>
+        <v>23507.35269681553</v>
       </c>
       <c r="K130" t="n">
-        <v>23070.30000000199</v>
+        <v>23194.46451304765</v>
       </c>
     </row>
     <row r="131">
@@ -12378,19 +12410,19 @@
         <v>131.18</v>
       </c>
       <c r="G131" t="n">
-        <v>-0.02129401750062243</v>
+        <v>-529.3849604180105</v>
       </c>
       <c r="H131" t="n">
         <v>23261.8</v>
       </c>
       <c r="I131" t="n">
-        <v>23261.8212940175</v>
+        <v>23791.18496041801</v>
       </c>
       <c r="J131" t="n">
-        <v>23261.82129408381</v>
+        <v>23671.95368641951</v>
       </c>
       <c r="K131" t="n">
-        <v>23261.80000000063</v>
+        <v>23381.03127399849</v>
       </c>
     </row>
     <row r="132">
@@ -12404,19 +12436,19 @@
         <v>131.08</v>
       </c>
       <c r="G132" t="n">
-        <v>-0.009592226761014899</v>
+        <v>-500.2804810544221</v>
       </c>
       <c r="H132" t="n">
         <v>23679.9</v>
       </c>
       <c r="I132" t="n">
-        <v>23679.90959222676</v>
+        <v>24180.18048105442</v>
       </c>
       <c r="J132" t="n">
-        <v>23679.90959225672</v>
+        <v>24065.59276020662</v>
       </c>
       <c r="K132" t="n">
-        <v>23679.9000000002</v>
+        <v>23794.48772084781</v>
       </c>
     </row>
     <row r="133">
@@ -12430,19 +12462,19 @@
         <v>130.98</v>
       </c>
       <c r="G133" t="n">
-        <v>-0.004233382718666689</v>
+        <v>-473.5920599024903</v>
       </c>
       <c r="H133" t="n">
         <v>23737.6</v>
       </c>
       <c r="I133" t="n">
-        <v>23737.60423338272</v>
+        <v>24211.19205990249</v>
       </c>
       <c r="J133" t="n">
-        <v>23737.60423339596</v>
+        <v>24100.98055768735</v>
       </c>
       <c r="K133" t="n">
-        <v>23737.60000000006</v>
+        <v>23847.81150221514</v>
       </c>
     </row>
     <row r="134">
@@ -12456,19 +12488,19 @@
         <v>130.88</v>
       </c>
       <c r="G134" t="n">
-        <v>-0.001830323824833613</v>
+        <v>-449.0522792998527</v>
       </c>
       <c r="H134" t="n">
         <v>22921.3</v>
       </c>
       <c r="I134" t="n">
-        <v>22921.30183032382</v>
+        <v>23370.35227929985</v>
       </c>
       <c r="J134" t="n">
-        <v>22921.30183032956</v>
+        <v>23264.26988783507</v>
       </c>
       <c r="K134" t="n">
-        <v>22921.30000000002</v>
+        <v>23027.38239146478</v>
       </c>
     </row>
     <row r="135">
@@ -12482,19 +12514,19 @@
         <v>130.78</v>
       </c>
       <c r="G135" t="n">
-        <v>-0.0007751916491542943</v>
+        <v>-426.4305306039969</v>
       </c>
       <c r="H135" t="n">
         <v>23216.3</v>
       </c>
       <c r="I135" t="n">
-        <v>23216.30077519165</v>
+        <v>23642.730530604</v>
       </c>
       <c r="J135" t="n">
-        <v>23216.30077519408</v>
+        <v>23540.54848283155</v>
       </c>
       <c r="K135" t="n">
-        <v>23216.3</v>
+        <v>23318.48204777244</v>
       </c>
     </row>
     <row r="136">
@@ -12508,19 +12540,19 @@
         <v>130.68</v>
       </c>
       <c r="G136" t="n">
-        <v>-0.0003215893339074682</v>
+        <v>-405.5269877090905</v>
       </c>
       <c r="H136" t="n">
         <v>23106.4</v>
       </c>
       <c r="I136" t="n">
-        <v>23106.40032158934</v>
+        <v>23511.92698770909</v>
       </c>
       <c r="J136" t="n">
-        <v>23106.40032159034</v>
+        <v>23413.43317961073</v>
       </c>
       <c r="K136" t="n">
-        <v>23106.4</v>
+        <v>23204.89380809836</v>
       </c>
     </row>
     <row r="137">
@@ -12534,19 +12566,19 @@
         <v>130.58</v>
       </c>
       <c r="G137" t="n">
-        <v>-0.0001306707054027356</v>
+        <v>-386.1677186674679</v>
       </c>
       <c r="H137" t="n">
         <v>23220.2</v>
       </c>
       <c r="I137" t="n">
-        <v>23220.20013067071</v>
+        <v>23606.36771866747</v>
       </c>
       <c r="J137" t="n">
-        <v>23220.20013067112</v>
+        <v>23511.365213106</v>
       </c>
       <c r="K137" t="n">
-        <v>23220.2</v>
+        <v>23315.20250556147</v>
       </c>
     </row>
     <row r="138">
@@ -12560,19 +12592,19 @@
         <v>130.48</v>
       </c>
       <c r="G138" t="n">
-        <v>-5.200119994697161e-05</v>
+        <v>-368.2006929616728</v>
       </c>
       <c r="H138" t="n">
         <v>24093.6</v>
       </c>
       <c r="I138" t="n">
-        <v>24093.6000520012</v>
+        <v>24461.80069296167</v>
       </c>
       <c r="J138" t="n">
-        <v>24093.60005200136</v>
+        <v>24370.10638252379</v>
       </c>
       <c r="K138" t="n">
-        <v>24093.6</v>
+        <v>24185.29431043788</v>
       </c>
     </row>
     <row r="139">
@@ -12586,19 +12618,19 @@
         <v>130.38</v>
       </c>
       <c r="G139" t="n">
-        <v>-2.026670699706301e-05</v>
+        <v>-351.4924992672204</v>
       </c>
       <c r="H139" t="n">
         <v>22379.6</v>
       </c>
       <c r="I139" t="n">
-        <v>22379.60002026671</v>
+        <v>22731.09249926722</v>
       </c>
       <c r="J139" t="n">
-        <v>22379.60002026677</v>
+        <v>22642.53590866078</v>
       </c>
       <c r="K139" t="n">
-        <v>22379.6</v>
+        <v>22468.15659060644</v>
       </c>
     </row>
     <row r="140">
@@ -12612,19 +12644,19 @@
         <v>130.28</v>
       </c>
       <c r="G140" t="n">
-        <v>-7.735092367511243e-06</v>
+        <v>-335.9256310164455</v>
       </c>
       <c r="H140" t="n">
         <v>23672.7</v>
       </c>
       <c r="I140" t="n">
-        <v>23672.70000773509</v>
+        <v>24008.62563101645</v>
       </c>
       <c r="J140" t="n">
-        <v>23672.70000773511</v>
+        <v>23923.04784225686</v>
       </c>
       <c r="K140" t="n">
-        <v>23672.7</v>
+        <v>23758.27778875959</v>
       </c>
     </row>
     <row r="141">
@@ -12638,19 +12670,19 @@
         <v>130.18</v>
       </c>
       <c r="G141" t="n">
-        <v>-2.890941686928272e-06</v>
+        <v>-321.3962288764269</v>
       </c>
       <c r="H141" t="n">
         <v>22678.3</v>
       </c>
       <c r="I141" t="n">
-        <v>22678.30000289094</v>
+        <v>22999.69622887643</v>
       </c>
       <c r="J141" t="n">
-        <v>22678.30000289095</v>
+        <v>22916.9489147685</v>
       </c>
       <c r="K141" t="n">
-        <v>22678.3</v>
+        <v>22761.04731410793</v>
       </c>
     </row>
     <row r="142">
@@ -12664,19 +12696,19 @@
         <v>130.08</v>
       </c>
       <c r="G142" t="n">
-        <v>-1.057996996678412e-06</v>
+        <v>-307.8121932926297</v>
       </c>
       <c r="H142" t="n">
         <v>22925.7</v>
       </c>
       <c r="I142" t="n">
-        <v>22925.700001058</v>
+        <v>23233.51219329263</v>
       </c>
       <c r="J142" t="n">
-        <v>22925.700001058</v>
+        <v>23153.45674664354</v>
       </c>
       <c r="K142" t="n">
-        <v>22925.7</v>
+        <v>23005.75544664909</v>
       </c>
     </row>
     <row r="143">
@@ -12690,19 +12722,19 @@
         <v>129.98</v>
       </c>
       <c r="G143" t="n">
-        <v>-3.791283234022558e-07</v>
+        <v>-295.0915985790853</v>
       </c>
       <c r="H143" t="n">
         <v>23234.5</v>
       </c>
       <c r="I143" t="n">
-        <v>23234.50000037913</v>
+        <v>23529.59159857909</v>
       </c>
       <c r="J143" t="n">
-        <v>23234.50000037913</v>
+        <v>23452.09834622289</v>
       </c>
       <c r="K143" t="n">
-        <v>23234.5</v>
+        <v>23311.9932523562</v>
       </c>
     </row>
     <row r="144">
@@ -12716,19 +12748,19 @@
         <v>129.88</v>
       </c>
       <c r="G144" t="n">
-        <v>-1.330226950813085e-07</v>
+        <v>-283.1613541261831</v>
       </c>
       <c r="H144" t="n">
         <v>23209.9</v>
       </c>
       <c r="I144" t="n">
-        <v>23209.90000013302</v>
+        <v>23493.06135412618</v>
       </c>
       <c r="J144" t="n">
-        <v>23209.90000013302</v>
+        <v>23418.00884624538</v>
       </c>
       <c r="K144" t="n">
-        <v>23209.9</v>
+        <v>23284.95250788081</v>
       </c>
     </row>
     <row r="145">
@@ -12742,19 +12774,19 @@
         <v>129.78</v>
       </c>
       <c r="G145" t="n">
-        <v>-4.569665179587901e-08</v>
+        <v>-271.9560692111118</v>
       </c>
       <c r="H145" t="n">
         <v>22959.1</v>
       </c>
       <c r="I145" t="n">
-        <v>22959.1000000457</v>
+        <v>23231.05606921111</v>
       </c>
       <c r="J145" t="n">
-        <v>22959.1000000457</v>
+        <v>23158.33043564538</v>
       </c>
       <c r="K145" t="n">
-        <v>22959.1</v>
+        <v>23031.82563356572</v>
       </c>
     </row>
     <row r="146">
@@ -12768,19 +12800,19 @@
         <v>129.68</v>
       </c>
       <c r="G146" t="n">
-        <v>-1.537046045996249e-08</v>
+        <v>-261.4170864106891</v>
       </c>
       <c r="H146" t="n">
         <v>23204.9</v>
       </c>
       <c r="I146" t="n">
-        <v>23204.90000001537</v>
+        <v>23466.31708641069</v>
       </c>
       <c r="J146" t="n">
-        <v>23204.90000001537</v>
+        <v>23395.81145267803</v>
       </c>
       <c r="K146" t="n">
-        <v>23204.9</v>
+        <v>23275.40563373266</v>
       </c>
     </row>
     <row r="147">
@@ -12794,19 +12826,19 @@
         <v>129.58</v>
       </c>
       <c r="G147" t="n">
-        <v>-5.060428520664573e-09</v>
+        <v>-251.4916553039366</v>
       </c>
       <c r="H147" t="n">
         <v>22759</v>
       </c>
       <c r="I147" t="n">
-        <v>22759.00000000506</v>
+        <v>23010.49165530394</v>
       </c>
       <c r="J147" t="n">
-        <v>22759.00000000506</v>
+        <v>22942.10561195094</v>
       </c>
       <c r="K147" t="n">
-        <v>22759</v>
+        <v>22827.386043353</v>
       </c>
     </row>
     <row r="148">
@@ -12820,19 +12852,19 @@
         <v>129.48</v>
       </c>
       <c r="G148" t="n">
-        <v>-1.629814505577087e-09</v>
+        <v>-242.1322234372892</v>
       </c>
       <c r="H148" t="n">
         <v>23218.7</v>
       </c>
       <c r="I148" t="n">
-        <v>23218.70000000163</v>
+        <v>23460.83222343729</v>
       </c>
       <c r="J148" t="n">
-        <v>23218.70000000163</v>
+        <v>23394.47134310608</v>
       </c>
       <c r="K148" t="n">
-        <v>23218.7</v>
+        <v>23285.06088033121</v>
       </c>
     </row>
     <row r="149">
@@ -12846,19 +12878,19 @@
         <v>129.38</v>
       </c>
       <c r="G149" t="n">
-        <v>-5.129550117999315e-10</v>
+        <v>-233.2958257287828</v>
       </c>
       <c r="H149" t="n">
         <v>23386.5</v>
       </c>
       <c r="I149" t="n">
-        <v>23386.50000000051</v>
+        <v>23619.79582572878</v>
       </c>
       <c r="J149" t="n">
-        <v>23386.50000000051</v>
+        <v>23555.37122299467</v>
       </c>
       <c r="K149" t="n">
-        <v>23386.5</v>
+        <v>23450.92460273411</v>
       </c>
     </row>
     <row r="150">
@@ -12872,19 +12904,19 @@
         <v>129.28</v>
       </c>
       <c r="G150" t="n">
-        <v>-1.600710675120354e-10</v>
+        <v>-224.9435568482622</v>
       </c>
       <c r="H150" t="n">
         <v>23184.7</v>
       </c>
       <c r="I150" t="n">
-        <v>23184.70000000016</v>
+        <v>23409.64355684826</v>
       </c>
       <c r="J150" t="n">
-        <v>23184.70000000016</v>
+        <v>23347.07148646142</v>
       </c>
       <c r="K150" t="n">
-        <v>23184.7</v>
+        <v>23247.27207038684</v>
       </c>
     </row>
     <row r="151">
@@ -12898,19 +12930,19 @@
         <v>129.18</v>
       </c>
       <c r="G151" t="n">
-        <v>-4.729372449219227e-11</v>
+        <v>-217.0401138133457</v>
       </c>
       <c r="H151" t="n">
         <v>22687</v>
       </c>
       <c r="I151" t="n">
-        <v>22687.00000000005</v>
+        <v>22904.04011381335</v>
       </c>
       <c r="J151" t="n">
-        <v>22687.00000000005</v>
+        <v>22843.24160348106</v>
       </c>
       <c r="K151" t="n">
-        <v>22687</v>
+        <v>22747.79851033229</v>
       </c>
     </row>
     <row r="152">
@@ -12924,19 +12956,19 @@
         <v>129.08</v>
       </c>
       <c r="G152" t="n">
-        <v>-1.455191522836685e-11</v>
+        <v>-209.5533982242305</v>
       </c>
       <c r="H152" t="n">
         <v>22924.4</v>
       </c>
       <c r="I152" t="n">
-        <v>22924.40000000002</v>
+        <v>23133.95339822423</v>
       </c>
       <c r="J152" t="n">
-        <v>22924.40000000002</v>
+        <v>23074.85391250952</v>
       </c>
       <c r="K152" t="n">
-        <v>22924.4</v>
+        <v>22983.49948571472</v>
       </c>
     </row>
     <row r="153">
@@ -12950,19 +12982,19 @@
         <v>128.98</v>
       </c>
       <c r="G153" t="n">
-        <v>-3.637978807091713e-12</v>
+        <v>-202.4541693340652</v>
       </c>
       <c r="H153" t="n">
         <v>22643.1</v>
       </c>
       <c r="I153" t="n">
-        <v>22643.1</v>
+        <v>22845.55416933406</v>
       </c>
       <c r="J153" t="n">
-        <v>22643.1</v>
+        <v>22788.08330162985</v>
       </c>
       <c r="K153" t="n">
-        <v>22643.1</v>
+        <v>22700.57086770422</v>
       </c>
     </row>
     <row r="154">
@@ -12976,19 +13008,19 @@
         <v>128.88</v>
       </c>
       <c r="G154" t="n">
-        <v>0</v>
+        <v>-195.7157405981816</v>
       </c>
       <c r="H154" t="n">
         <v>22647.9</v>
       </c>
       <c r="I154" t="n">
-        <v>22647.9</v>
+        <v>22843.61574059818</v>
       </c>
       <c r="J154" t="n">
-        <v>22647.9</v>
+        <v>22787.70693047195</v>
       </c>
       <c r="K154" t="n">
-        <v>22647.9</v>
+        <v>22703.80881012623</v>
       </c>
     </row>
     <row r="155">
@@ -13002,19 +13034,19 @@
         <v>128.78</v>
       </c>
       <c r="G155" t="n">
-        <v>0</v>
+        <v>-189.3137135309662</v>
       </c>
       <c r="H155" t="n">
         <v>23050.9</v>
       </c>
       <c r="I155" t="n">
-        <v>23050.9</v>
+        <v>23240.21371353097</v>
       </c>
       <c r="J155" t="n">
-        <v>23050.9</v>
+        <v>23185.80398702941</v>
       </c>
       <c r="K155" t="n">
-        <v>23050.9</v>
+        <v>23105.30972650156</v>
       </c>
     </row>
     <row r="156">
@@ -13028,19 +13060,19 @@
         <v>128.68</v>
       </c>
       <c r="G156" t="n">
-        <v>0</v>
+        <v>-183.2257436747313</v>
       </c>
       <c r="H156" t="n">
         <v>22933.5</v>
       </c>
       <c r="I156" t="n">
-        <v>22933.5</v>
+        <v>23116.72574367473</v>
       </c>
       <c r="J156" t="n">
-        <v>22933.5</v>
+        <v>23063.75547443664</v>
       </c>
       <c r="K156" t="n">
-        <v>22933.5</v>
+        <v>22986.4702692381</v>
       </c>
     </row>
     <row r="157">
@@ -13054,19 +13086,19 @@
         <v>128.58</v>
       </c>
       <c r="G157" t="n">
-        <v>0</v>
+        <v>-177.4313342910355</v>
       </c>
       <c r="H157" t="n">
         <v>23251.9</v>
       </c>
       <c r="I157" t="n">
-        <v>23251.9</v>
+        <v>23429.33133429104</v>
       </c>
       <c r="J157" t="n">
-        <v>23251.9</v>
+        <v>23377.74402354469</v>
       </c>
       <c r="K157" t="n">
-        <v>23251.9</v>
+        <v>23303.48731074635</v>
       </c>
     </row>
     <row r="158">
@@ -13080,19 +13112,19 @@
         <v>128.48</v>
       </c>
       <c r="G158" t="n">
-        <v>0</v>
+        <v>-171.9116540533032</v>
       </c>
       <c r="H158" t="n">
         <v>22359.8</v>
       </c>
       <c r="I158" t="n">
-        <v>22359.8</v>
+        <v>22531.7116540533</v>
       </c>
       <c r="J158" t="n">
-        <v>22359.8</v>
+        <v>22481.45372777565</v>
       </c>
       <c r="K158" t="n">
-        <v>22359.8</v>
+        <v>22410.05792627765</v>
       </c>
     </row>
     <row r="159">
@@ -13106,19 +13138,19 @@
         <v>128.38</v>
       </c>
       <c r="G159" t="n">
-        <v>0</v>
+        <v>-166.6493755763731</v>
       </c>
       <c r="H159" t="n">
         <v>23047.9</v>
       </c>
       <c r="I159" t="n">
-        <v>23047.9</v>
+        <v>23214.54937557637</v>
       </c>
       <c r="J159" t="n">
-        <v>23047.9</v>
+        <v>23165.56999726892</v>
       </c>
       <c r="K159" t="n">
-        <v>23047.9</v>
+        <v>23096.87937830745</v>
       </c>
     </row>
     <row r="160">
@@ -13132,19 +13164,19 @@
         <v>128.28</v>
       </c>
       <c r="G160" t="n">
-        <v>0</v>
+        <v>-161.6285320834686</v>
       </c>
       <c r="H160" t="n">
         <v>22819.4</v>
       </c>
       <c r="I160" t="n">
-        <v>22819.4</v>
+        <v>22981.02853208347</v>
       </c>
       <c r="J160" t="n">
-        <v>22819.4</v>
+        <v>22933.27942977707</v>
       </c>
       <c r="K160" t="n">
-        <v>22819.4</v>
+        <v>22867.1491023064</v>
       </c>
     </row>
     <row r="161">
@@ -13158,19 +13190,19 @@
         <v>128.18</v>
       </c>
       <c r="G161" t="n">
-        <v>0</v>
+        <v>-156.8343899010106</v>
       </c>
       <c r="H161" t="n">
         <v>22415.3</v>
       </c>
       <c r="I161" t="n">
-        <v>22415.3</v>
+        <v>22572.13438990101</v>
       </c>
       <c r="J161" t="n">
-        <v>22415.3</v>
+        <v>22525.56969614132</v>
       </c>
       <c r="K161" t="n">
-        <v>22415.3</v>
+        <v>22461.86469375969</v>
       </c>
     </row>
     <row r="162">
@@ -13184,19 +13216,19 @@
         <v>128.08</v>
       </c>
       <c r="G162" t="n">
-        <v>0</v>
+        <v>-152.2533347996723</v>
       </c>
       <c r="H162" t="n">
         <v>23032.4</v>
       </c>
       <c r="I162" t="n">
-        <v>23032.4</v>
+        <v>23184.65333479967</v>
       </c>
       <c r="J162" t="n">
-        <v>23032.4</v>
+        <v>23139.22943848868</v>
       </c>
       <c r="K162" t="n">
-        <v>23032.4</v>
+        <v>23077.82389631099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mac: Change description of peaks
</commit_message>
<xml_diff>
--- a/DATA/UKSAF/STO.xlsx
+++ b/DATA/UKSAF/STO.xlsx
@@ -680,7 +680,7 @@
       <row>5</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="5686425" cy="4124325"/>
+    <ext cx="5619750" cy="4076700"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -20550,485 +20550,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:AD4"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="6" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="11" customWidth="1" min="5" max="5"/>
-    <col width="14" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="12" customWidth="1" min="8" max="8"/>
-    <col width="6" customWidth="1" min="9" max="9"/>
-    <col width="6" customWidth="1" min="10" max="10"/>
-    <col width="6" customWidth="1" min="11" max="11"/>
-    <col width="8" customWidth="1" min="12" max="12"/>
-    <col width="13" customWidth="1" min="13" max="13"/>
-    <col width="15" customWidth="1" min="14" max="14"/>
-    <col width="23" customWidth="1" min="15" max="15"/>
-    <col width="12" customWidth="1" min="16" max="16"/>
-    <col width="12" customWidth="1" min="17" max="17"/>
-    <col width="10" customWidth="1" min="18" max="18"/>
-    <col width="14" customWidth="1" min="19" max="19"/>
-    <col width="15" customWidth="1" min="20" max="20"/>
-    <col width="22" customWidth="1" min="21" max="21"/>
-    <col width="23" customWidth="1" min="22" max="22"/>
-    <col width="11" customWidth="1" min="23" max="23"/>
-    <col width="21" customWidth="1" min="24" max="24"/>
-    <col width="19" customWidth="1" min="25" max="25"/>
-    <col width="17" customWidth="1" min="26" max="26"/>
-    <col width="16" customWidth="1" min="27" max="27"/>
-    <col width="17" customWidth="1" min="28" max="28"/>
-    <col width="14" customWidth="1" min="29" max="29"/>
-    <col width="14" customWidth="1" min="30" max="30"/>
-  </cols>
-  <sheetData>
-    <row r="2">
-      <c r="B2" s="38" t="inlineStr">
-        <is>
-          <t>Peak
-Label</t>
-        </is>
-      </c>
-      <c r="C2" s="38" t="inlineStr">
-        <is>
-          <t>Position
-(eV)</t>
-        </is>
-      </c>
-      <c r="D2" s="38" t="inlineStr">
-        <is>
-          <t>Height
-(CPS)</t>
-        </is>
-      </c>
-      <c r="E2" s="38" t="inlineStr">
-        <is>
-          <t>FWHM
-(eV)</t>
-        </is>
-      </c>
-      <c r="F2" s="38" t="inlineStr">
-        <is>
-          <t>L/G 
-σ/γ (%)</t>
-        </is>
-      </c>
-      <c r="G2" s="38" t="inlineStr">
-        <is>
-          <t>Area
-(CPS.eV)</t>
-        </is>
-      </c>
-      <c r="H2" s="38" t="inlineStr">
-        <is>
-          <t>Atomic
-(%)</t>
-        </is>
-      </c>
-      <c r="I2" s="38" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="J2" s="38" t="inlineStr">
-        <is>
-          <t>RSF</t>
-        </is>
-      </c>
-      <c r="K2" s="38" t="inlineStr">
-        <is>
-          <t>TXFN</t>
-        </is>
-      </c>
-      <c r="L2" s="38" t="inlineStr">
-        <is>
-          <t>ECF</t>
-        </is>
-      </c>
-      <c r="M2" s="38" t="inlineStr">
-        <is>
-          <t>Instr.</t>
-        </is>
-      </c>
-      <c r="N2" s="38" t="inlineStr">
-        <is>
-          <t>Fitting Model</t>
-        </is>
-      </c>
-      <c r="O2" s="38" t="inlineStr">
-        <is>
-          <t>Corr. Area
- Ac (a.u.)</t>
-        </is>
-      </c>
-      <c r="P2" s="38" t="inlineStr">
-        <is>
-          <t>σ or α
-W_g</t>
-        </is>
-      </c>
-      <c r="Q2" s="38" t="inlineStr">
-        <is>
-          <t>γ or β
-W_l</t>
-        </is>
-      </c>
-      <c r="R2" s="38" t="inlineStr">
-        <is>
-          <t>Bkg Type</t>
-        </is>
-      </c>
-      <c r="S2" s="38" t="inlineStr">
-        <is>
-          <t>Bkg Low
-(eV)</t>
-        </is>
-      </c>
-      <c r="T2" s="38" t="inlineStr">
-        <is>
-          <t>Bkg High
-(eV)</t>
-        </is>
-      </c>
-      <c r="U2" s="38" t="inlineStr">
-        <is>
-          <t>Bkg Offset Low
-(CPS)</t>
-        </is>
-      </c>
-      <c r="V2" s="38" t="inlineStr">
-        <is>
-          <t>Bkg Offset High
-(CPS)</t>
-        </is>
-      </c>
-      <c r="W2" s="38" t="inlineStr">
-        <is>
-          <t>Sheetname</t>
-        </is>
-      </c>
-      <c r="X2" s="38" t="inlineStr">
-        <is>
-          <t>Position
-Constraint</t>
-        </is>
-      </c>
-      <c r="Y2" s="38" t="inlineStr">
-        <is>
-          <t>Height
-Constraint</t>
-        </is>
-      </c>
-      <c r="Z2" s="38" t="inlineStr">
-        <is>
-          <t>FWHM
-Constraint</t>
-        </is>
-      </c>
-      <c r="AA2" s="38" t="inlineStr">
-        <is>
-          <t>L/G
-Constraint</t>
-        </is>
-      </c>
-      <c r="AB2" s="38" t="inlineStr">
-        <is>
-          <t>Area
-Constraint</t>
-        </is>
-      </c>
-      <c r="AC2" s="38" t="inlineStr">
-        <is>
-          <t>σ
-Constraint</t>
-        </is>
-      </c>
-      <c r="AD2" s="38" t="inlineStr">
-        <is>
-          <t>γ
-Constraint</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" s="39" t="inlineStr">
-        <is>
-          <t>Sr3d5/2 p1</t>
-        </is>
-      </c>
-      <c r="C3" s="40" t="inlineStr">
-        <is>
-          <t>132.49</t>
-        </is>
-      </c>
-      <c r="D3" s="40" t="inlineStr">
-        <is>
-          <t>101467.39</t>
-        </is>
-      </c>
-      <c r="E3" s="40" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="F3" s="40" t="inlineStr">
-        <is>
-          <t>60.28</t>
-        </is>
-      </c>
-      <c r="G3" s="40" t="inlineStr">
-        <is>
-          <t>108008.69</t>
-        </is>
-      </c>
-      <c r="H3" s="40" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="I3" s="40" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J3" s="40" t="inlineStr">
-        <is>
-          <t>4.25</t>
-        </is>
-      </c>
-      <c r="K3" s="40" t="inlineStr">
-        <is>
-          <t>1.00</t>
-        </is>
-      </c>
-      <c r="L3" s="40" t="inlineStr">
-        <is>
-          <t>TPP-2M</t>
-        </is>
-      </c>
-      <c r="M3" s="40" t="inlineStr">
-        <is>
-          <t>A-ALTHERMO1</t>
-        </is>
-      </c>
-      <c r="N3" s="40" t="inlineStr">
-        <is>
-          <t>GL (Area)</t>
-        </is>
-      </c>
-      <c r="O3" s="40" t="inlineStr">
-        <is>
-          <t>324.68</t>
-        </is>
-      </c>
-      <c r="P3" s="40" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="Q3" s="40" t="inlineStr">
-        <is>
-          <t>0.51</t>
-        </is>
-      </c>
-      <c r="R3" s="40" t="inlineStr"/>
-      <c r="S3" s="40" t="inlineStr">
-        <is>
-          <t>126.08</t>
-        </is>
-      </c>
-      <c r="T3" s="40" t="inlineStr">
-        <is>
-          <t>142.08</t>
-        </is>
-      </c>
-      <c r="U3" s="40" t="inlineStr"/>
-      <c r="V3" s="40" t="inlineStr"/>
-      <c r="W3" s="40" t="inlineStr">
-        <is>
-          <t>Sr3d</t>
-        </is>
-      </c>
-      <c r="X3" s="40" t="inlineStr">
-        <is>
-          <t>126.08,142.08</t>
-        </is>
-      </c>
-      <c r="Y3" s="40" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Z3" s="40" t="inlineStr">
-        <is>
-          <t>0.3:3.5</t>
-        </is>
-      </c>
-      <c r="AA3" s="40" t="inlineStr">
-        <is>
-          <t>2:80</t>
-        </is>
-      </c>
-      <c r="AB3" s="40" t="inlineStr">
-        <is>
-          <t>1:1e7</t>
-        </is>
-      </c>
-      <c r="AC3" s="40" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AD3" s="41" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="42" t="inlineStr">
-        <is>
-          <t>Sr3d3/2 p2</t>
-        </is>
-      </c>
-      <c r="C4" s="43" t="inlineStr">
-        <is>
-          <t>134.24</t>
-        </is>
-      </c>
-      <c r="D4" s="43" t="inlineStr">
-        <is>
-          <t>70521.91</t>
-        </is>
-      </c>
-      <c r="E4" s="43" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="F4" s="43" t="inlineStr">
-        <is>
-          <t>60.27</t>
-        </is>
-      </c>
-      <c r="G4" s="43" t="inlineStr">
-        <is>
-          <t>75068.25</t>
-        </is>
-      </c>
-      <c r="H4" s="43" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="I4" s="43" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J4" s="43" t="inlineStr">
-        <is>
-          <t>2.93</t>
-        </is>
-      </c>
-      <c r="K4" s="43" t="inlineStr">
-        <is>
-          <t>1.00</t>
-        </is>
-      </c>
-      <c r="L4" s="43" t="inlineStr">
-        <is>
-          <t>TPP-2M</t>
-        </is>
-      </c>
-      <c r="M4" s="43" t="inlineStr">
-        <is>
-          <t>A-ALTHERMO1</t>
-        </is>
-      </c>
-      <c r="N4" s="43" t="inlineStr">
-        <is>
-          <t>GL (Area)</t>
-        </is>
-      </c>
-      <c r="O4" s="43" t="inlineStr">
-        <is>
-          <t>327.86</t>
-        </is>
-      </c>
-      <c r="P4" s="43" t="inlineStr">
-        <is>
-          <t>2.35</t>
-        </is>
-      </c>
-      <c r="Q4" s="43" t="inlineStr">
-        <is>
-          <t>1.02</t>
-        </is>
-      </c>
-      <c r="R4" s="43" t="inlineStr"/>
-      <c r="S4" s="43" t="inlineStr">
-        <is>
-          <t>126.08</t>
-        </is>
-      </c>
-      <c r="T4" s="43" t="inlineStr">
-        <is>
-          <t>142.08</t>
-        </is>
-      </c>
-      <c r="U4" s="43" t="inlineStr"/>
-      <c r="V4" s="43" t="inlineStr"/>
-      <c r="W4" s="43" t="inlineStr">
-        <is>
-          <t>Sr3d</t>
-        </is>
-      </c>
-      <c r="X4" s="43" t="inlineStr">
-        <is>
-          <t>A+1.7#0.2</t>
-        </is>
-      </c>
-      <c r="Y4" s="43" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Z4" s="43" t="inlineStr">
-        <is>
-          <t>A*1</t>
-        </is>
-      </c>
-      <c r="AA4" s="43" t="inlineStr">
-        <is>
-          <t>A*1</t>
-        </is>
-      </c>
-      <c r="AB4" s="43" t="inlineStr">
-        <is>
-          <t>A*0.667#0.05</t>
-        </is>
-      </c>
-      <c r="AC4" s="43" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AD4" s="44" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -21279,7 +20808,7 @@
       <c r="AF2" s="33" t="inlineStr"/>
       <c r="AG2" s="33" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="AH2" s="33" t="inlineStr">
@@ -21362,7 +20891,7 @@
       </c>
       <c r="AA3" s="36" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1:1e7</t>
         </is>
       </c>
       <c r="AB3" s="36" t="inlineStr">
@@ -21384,7 +20913,7 @@
       <c r="AF3" s="36" t="inlineStr"/>
       <c r="AG3" s="36" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.01:2</t>
         </is>
       </c>
       <c r="AH3" s="36" t="inlineStr"/>
@@ -21460,7 +20989,7 @@
       <c r="AF4" s="33" t="inlineStr"/>
       <c r="AG4" s="33" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="AH4" s="33" t="inlineStr">
@@ -21543,7 +21072,7 @@
       </c>
       <c r="AA5" s="36" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>A*0.667#0.05</t>
         </is>
       </c>
       <c r="AB5" s="36" t="inlineStr">
@@ -21565,7 +21094,7 @@
       <c r="AF5" s="36" t="inlineStr"/>
       <c r="AG5" s="36" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>A*1</t>
         </is>
       </c>
       <c r="AH5" s="36" t="inlineStr"/>

</xml_diff>

<commit_message>
Mac: Fix error with Tab popup message
</commit_message>
<xml_diff>
--- a/DATA/UKSAF/STO.xlsx
+++ b/DATA/UKSAF/STO.xlsx
@@ -790,7 +790,7 @@
       </blipFill>
       <spPr>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
+          <avLst/>
         </a:prstGeom>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
@@ -20580,7 +20580,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE9"/>
+  <dimension ref="B2:AE9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20621,7 +20621,6 @@
     <col width="6" customWidth="1" min="31" max="31"/>
   </cols>
   <sheetData>
-    <row r="1"/>
     <row r="2">
       <c r="B2" s="46" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Mac: Change STO file
</commit_message>
<xml_diff>
--- a/DATA/UKSAF/STO.xlsx
+++ b/DATA/UKSAF/STO.xlsx
@@ -20785,19 +20785,19 @@
         <v>143.08</v>
       </c>
       <c r="G2" t="n">
-        <v>-81.56472396294339</v>
+        <v>-147.4491697849226</v>
       </c>
       <c r="H2" t="n">
         <v>26049.5</v>
       </c>
       <c r="I2" t="n">
-        <v>26131.06472396294</v>
+        <v>26196.94916978492</v>
       </c>
       <c r="J2" t="n">
-        <v>26090.5824903156</v>
+        <v>26122.3592094007</v>
       </c>
       <c r="K2" t="n">
-        <v>26089.98225537745</v>
+        <v>26124.09048832685</v>
       </c>
       <c r="X2" s="32" t="inlineStr">
         <is>
@@ -20811,27 +20811,27 @@
       </c>
       <c r="Z2" s="33" t="inlineStr">
         <is>
-          <t>133.51</t>
+          <t>133.50</t>
         </is>
       </c>
       <c r="AA2" s="33" t="inlineStr">
         <is>
-          <t>97020</t>
+          <t>99974</t>
         </is>
       </c>
       <c r="AB2" s="33" t="inlineStr">
         <is>
-          <t>0.83</t>
+          <t>0.98</t>
         </is>
       </c>
       <c r="AC2" s="33" t="inlineStr">
         <is>
-          <t>22.56</t>
+          <t>27.93</t>
         </is>
       </c>
       <c r="AD2" s="33" t="inlineStr">
         <is>
-          <t>94916</t>
+          <t>118146</t>
         </is>
       </c>
       <c r="AE2" s="33" t="inlineStr"/>
@@ -20843,7 +20843,7 @@
       </c>
       <c r="AH2" s="33" t="inlineStr">
         <is>
-          <t>60.0</t>
+          <t>59.3</t>
         </is>
       </c>
       <c r="AI2" s="33" t="inlineStr">
@@ -20868,22 +20868,22 @@
       </c>
       <c r="AM2" s="33" t="inlineStr">
         <is>
-          <t>129.08</t>
+          <t>127.08</t>
         </is>
       </c>
       <c r="AN2" s="33" t="inlineStr">
         <is>
-          <t>145.08</t>
+          <t>143.08</t>
         </is>
       </c>
       <c r="AO2" s="33" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>-285.30</t>
         </is>
       </c>
       <c r="AP2" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>-715.80</t>
         </is>
       </c>
     </row>
@@ -20898,25 +20898,25 @@
         <v>142.98</v>
       </c>
       <c r="G3" t="n">
-        <v>-83.48100408152459</v>
+        <v>-150.9223702109521</v>
       </c>
       <c r="H3" t="n">
         <v>26437.6</v>
       </c>
       <c r="I3" t="n">
-        <v>26521.08100408152</v>
+        <v>26588.52237021095</v>
       </c>
       <c r="J3" t="n">
-        <v>26479.5530339006</v>
+        <v>26512.0003134132</v>
       </c>
       <c r="K3" t="n">
-        <v>26479.12799188242</v>
+        <v>26514.12259846262</v>
       </c>
       <c r="X3" s="35" t="inlineStr"/>
       <c r="Y3" s="36" t="inlineStr"/>
       <c r="Z3" s="36" t="inlineStr">
         <is>
-          <t>129.08,145.08</t>
+          <t>127.08,143.08</t>
         </is>
       </c>
       <c r="AA3" s="36" t="inlineStr">
@@ -20966,19 +20966,19 @@
         <v>142.88</v>
       </c>
       <c r="G4" t="n">
-        <v>-85.46624139469714</v>
+        <v>-154.5208917711498</v>
       </c>
       <c r="H4" t="n">
         <v>26696.9</v>
       </c>
       <c r="I4" t="n">
-        <v>26782.3662413947</v>
+        <v>26851.42089177115</v>
       </c>
       <c r="J4" t="n">
-        <v>26739.7515254551</v>
+        <v>26772.89078988059</v>
       </c>
       <c r="K4" t="n">
-        <v>26739.51473759221</v>
+        <v>26775.43065781859</v>
       </c>
       <c r="X4" s="32" t="inlineStr">
         <is>
@@ -20992,27 +20992,27 @@
       </c>
       <c r="Z4" s="33" t="inlineStr">
         <is>
-          <t>135.21</t>
+          <t>135.24</t>
         </is>
       </c>
       <c r="AA4" s="33" t="inlineStr">
         <is>
-          <t>64712</t>
+          <t>68635</t>
         </is>
       </c>
       <c r="AB4" s="33" t="inlineStr">
         <is>
-          <t>0.83</t>
+          <t>0.98</t>
         </is>
       </c>
       <c r="AC4" s="33" t="inlineStr">
         <is>
-          <t>22.56</t>
+          <t>27.93</t>
         </is>
       </c>
       <c r="AD4" s="33" t="inlineStr">
         <is>
-          <t>63309</t>
+          <t>81110</t>
         </is>
       </c>
       <c r="AE4" s="33" t="inlineStr"/>
@@ -21024,17 +21024,17 @@
       </c>
       <c r="AH4" s="33" t="inlineStr">
         <is>
-          <t>40.0</t>
+          <t>40.7</t>
         </is>
       </c>
       <c r="AI4" s="33" t="inlineStr">
         <is>
-          <t>66.7</t>
+          <t>68.7</t>
         </is>
       </c>
       <c r="AJ4" s="33" t="inlineStr">
         <is>
-          <t>1.70</t>
+          <t>1.74</t>
         </is>
       </c>
       <c r="AK4" s="33" t="inlineStr">
@@ -21049,22 +21049,22 @@
       </c>
       <c r="AM4" s="33" t="inlineStr">
         <is>
-          <t>129.08</t>
+          <t>127.08</t>
         </is>
       </c>
       <c r="AN4" s="33" t="inlineStr">
         <is>
-          <t>145.08</t>
+          <t>143.08</t>
         </is>
       </c>
       <c r="AO4" s="33" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>-285.30</t>
         </is>
       </c>
       <c r="AP4" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>-715.80</t>
         </is>
       </c>
     </row>
@@ -21079,19 +21079,19 @@
         <v>142.78</v>
       </c>
       <c r="G5" t="n">
-        <v>-87.52381476600931</v>
+        <v>-158.2508918354761</v>
       </c>
       <c r="H5" t="n">
         <v>25942.6</v>
       </c>
       <c r="I5" t="n">
-        <v>26030.12381476601</v>
+        <v>26100.85089183547</v>
       </c>
       <c r="J5" t="n">
-        <v>25986.37917341389</v>
+        <v>26020.23276853836</v>
       </c>
       <c r="K5" t="n">
-        <v>25986.34466293364</v>
+        <v>26023.21869405798</v>
       </c>
       <c r="X5" s="35" t="inlineStr"/>
       <c r="Y5" s="36" t="inlineStr"/>
@@ -21147,19 +21147,19 @@
         <v>142.68</v>
       </c>
       <c r="G6" t="n">
-        <v>-89.6573143992282</v>
+        <v>-162.1189139180133</v>
       </c>
       <c r="H6" t="n">
         <v>26565.8</v>
       </c>
       <c r="I6" t="n">
-        <v>26655.45731439923</v>
+        <v>26727.91891391801</v>
       </c>
       <c r="J6" t="n">
-        <v>26610.53725219311</v>
+        <v>26645.12849509623</v>
       </c>
       <c r="K6" t="n">
-        <v>26610.72008369231</v>
+        <v>26648.59100501586</v>
       </c>
     </row>
     <row r="7">
@@ -21173,19 +21173,19 @@
         <v>142.58</v>
       </c>
       <c r="G7" t="n">
-        <v>-91.87055803370822</v>
+        <v>-166.1319173400916</v>
       </c>
       <c r="H7" t="n">
         <v>26089.7</v>
       </c>
       <c r="I7" t="n">
-        <v>26181.57055803371</v>
+        <v>26255.83191734009</v>
       </c>
       <c r="J7" t="n">
-        <v>26135.42710655788</v>
+        <v>26170.78033889232</v>
       </c>
       <c r="K7" t="n">
-        <v>26135.84347284013</v>
+        <v>26174.75218070819</v>
       </c>
     </row>
     <row r="8">
@@ -21199,19 +21199,19 @@
         <v>142.48</v>
       </c>
       <c r="G8" t="n">
-        <v>-94.16760861750663</v>
+        <v>-170.2973096058304</v>
       </c>
       <c r="H8" t="n">
         <v>26784.6</v>
       </c>
       <c r="I8" t="n">
-        <v>26878.76760861751</v>
+        <v>26954.89730960583</v>
       </c>
       <c r="J8" t="n">
-        <v>26831.35015633091</v>
+        <v>26867.49080114267</v>
       </c>
       <c r="K8" t="n">
-        <v>26832.01747349997</v>
+        <v>26872.00712745809</v>
       </c>
     </row>
     <row r="9">
@@ -21225,19 +21225,19 @@
         <v>142.38</v>
       </c>
       <c r="G9" t="n">
-        <v>-96.55279361545763</v>
+        <v>-174.6229817791573</v>
       </c>
       <c r="H9" t="n">
         <v>26357.7</v>
       </c>
       <c r="I9" t="n">
-        <v>26454.25279361546</v>
+        <v>26532.32298177916</v>
       </c>
       <c r="J9" t="n">
-        <v>26405.50790147259</v>
+        <v>26442.46252383946</v>
       </c>
       <c r="K9" t="n">
-        <v>26406.44491317357</v>
+        <v>26447.56109437482</v>
       </c>
     </row>
     <row r="10">
@@ -21251,19 +21251,19 @@
         <v>142.28</v>
       </c>
       <c r="G10" t="n">
-        <v>-99.03072612865071</v>
+        <v>-179.1173471866896</v>
       </c>
       <c r="H10" t="n">
         <v>26256</v>
       </c>
       <c r="I10" t="n">
-        <v>26355.03072612865</v>
+        <v>26435.11734718669</v>
       </c>
       <c r="J10" t="n">
-        <v>26304.90192756644</v>
+        <v>26342.6982993569</v>
       </c>
       <c r="K10" t="n">
-        <v>26306.12881937551</v>
+        <v>26348.41970245092</v>
       </c>
     </row>
     <row r="11">
@@ -21277,19 +21277,19 @@
         <v>142.18</v>
       </c>
       <c r="G11" t="n">
-        <v>-101.6063280234303</v>
+        <v>-183.7893838110322</v>
       </c>
       <c r="H11" t="n">
         <v>26519.3</v>
       </c>
       <c r="I11" t="n">
-        <v>26620.90632802343</v>
+        <v>26703.08938381103</v>
       </c>
       <c r="J11" t="n">
-        <v>26569.3339117474</v>
+        <v>26608.00108082982</v>
       </c>
       <c r="K11" t="n">
-        <v>26570.87243683395</v>
+        <v>26614.3889765772</v>
       </c>
     </row>
     <row r="12">
@@ -21303,19 +21303,19 @@
         <v>142.08</v>
       </c>
       <c r="G12" t="n">
-        <v>-104.2848552931173</v>
+        <v>-188.6486807848232</v>
       </c>
       <c r="H12" t="n">
         <v>25948.6</v>
       </c>
       <c r="I12" t="n">
-        <v>26052.88485529312</v>
+        <v>26137.24868078482</v>
       </c>
       <c r="J12" t="n">
-        <v>25999.80562911415</v>
+        <v>26039.37399337662</v>
       </c>
       <c r="K12" t="n">
-        <v>26001.67924643995</v>
+        <v>26046.47538081411</v>
       </c>
     </row>
     <row r="13">
@@ -21329,19 +21329,19 @@
         <v>141.98</v>
       </c>
       <c r="G13" t="n">
-        <v>-107.0719259039797</v>
+        <v>-193.7054894483808</v>
       </c>
       <c r="H13" t="n">
         <v>26945.3</v>
       </c>
       <c r="I13" t="n">
-        <v>27052.37192590398</v>
+        <v>27139.00548944838</v>
       </c>
       <c r="J13" t="n">
-        <v>26997.71895967113</v>
+        <v>27038.22034624597</v>
       </c>
       <c r="K13" t="n">
-        <v>26999.95298615143</v>
+        <v>27046.08585730286</v>
       </c>
     </row>
     <row r="14">
@@ -21355,19 +21355,19 @@
         <v>141.88</v>
       </c>
       <c r="G14" t="n">
-        <v>-109.9735504094861</v>
+        <v>-198.9707794935202</v>
       </c>
       <c r="H14" t="n">
         <v>26444</v>
       </c>
       <c r="I14" t="n">
-        <v>26553.97355040949</v>
+        <v>26642.97077949352</v>
       </c>
       <c r="J14" t="n">
-        <v>26497.6758958509</v>
+        <v>26539.14364597521</v>
       </c>
       <c r="K14" t="n">
-        <v>26500.29767408501</v>
+        <v>26547.82786925132</v>
       </c>
     </row>
     <row r="15">
@@ -21381,19 +21381,19 @@
         <v>141.78</v>
       </c>
       <c r="G15" t="n">
-        <v>-112.9961656543383</v>
+        <v>-204.4563007849902</v>
       </c>
       <c r="H15" t="n">
         <v>26729.6</v>
       </c>
       <c r="I15" t="n">
-        <v>26842.59616565434</v>
+        <v>26934.05630078499</v>
       </c>
       <c r="J15" t="n">
-        <v>26784.57855067281</v>
+        <v>26827.0476106575</v>
       </c>
       <c r="K15" t="n">
-        <v>26787.61763406133</v>
+        <v>26836.60944848843</v>
       </c>
     </row>
     <row r="16">
@@ -21407,19 +21407,19 @@
         <v>141.68</v>
       </c>
       <c r="G16" t="n">
-        <v>-116.1466719324526</v>
+        <v>-210.1746515297564</v>
       </c>
       <c r="H16" t="n">
         <v>27045.9</v>
       </c>
       <c r="I16" t="n">
-        <v>27162.04667193245</v>
+        <v>27256.07465152976</v>
       </c>
       <c r="J16" t="n">
-        <v>27102.22916660023</v>
+        <v>27145.73618542601</v>
       </c>
       <c r="K16" t="n">
-        <v>27105.71752390573</v>
+        <v>27156.23924814989</v>
       </c>
     </row>
     <row r="17">
@@ -21433,19 +21433,19 @@
         <v>141.58</v>
       </c>
       <c r="G17" t="n">
-        <v>-119.4324740125485</v>
+        <v>-216.139353555358</v>
       </c>
       <c r="H17" t="n">
         <v>26274.3</v>
       </c>
       <c r="I17" t="n">
-        <v>26393.73247401255</v>
+        <v>26490.43935355536</v>
       </c>
       <c r="J17" t="n">
-        <v>26332.03012516554</v>
+        <v>26376.6135592748</v>
       </c>
       <c r="K17" t="n">
-        <v>26336.00236684886</v>
+        <v>26388.12660113587</v>
       </c>
     </row>
     <row r="18">
@@ -21459,19 +21459,19 @@
         <v>141.48</v>
       </c>
       <c r="G18" t="n">
-        <v>-122.8615265018452</v>
+        <v>-222.3649355633206</v>
       </c>
       <c r="H18" t="n">
         <v>25721.7</v>
       </c>
       <c r="I18" t="n">
-        <v>25844.56152650185</v>
+        <v>25944.06493556332</v>
       </c>
       <c r="J18" t="n">
-        <v>25780.88395743968</v>
+        <v>25826.58418334994</v>
       </c>
       <c r="K18" t="n">
-        <v>25785.37758642071</v>
+        <v>25839.18158507391</v>
       </c>
     </row>
     <row r="19">
@@ -21485,19 +21485,19 @@
         <v>141.38</v>
       </c>
       <c r="G19" t="n">
-        <v>-126.4423840842355</v>
+        <v>-228.8670253447744</v>
       </c>
       <c r="H19" t="n">
         <v>26199.6</v>
       </c>
       <c r="I19" t="n">
-        <v>26326.04238408423</v>
+        <v>26428.46702534477</v>
       </c>
       <c r="J19" t="n">
-        <v>26260.29335543207</v>
+        <v>26307.15279085931</v>
       </c>
       <c r="K19" t="n">
-        <v>26265.34904528881</v>
+        <v>26320.91509462515</v>
       </c>
     </row>
     <row r="20">
@@ -21511,19 +21511,19 @@
         <v>141.28</v>
       </c>
       <c r="G20" t="n">
-        <v>-130.1842572455134</v>
+        <v>-235.6624520859368</v>
       </c>
       <c r="H20" t="n">
         <v>27175.7</v>
       </c>
       <c r="I20" t="n">
-        <v>27305.88425724551</v>
+        <v>27411.36245208594</v>
       </c>
       <c r="J20" t="n">
-        <v>27237.96118451651</v>
+        <v>27286.02441876663</v>
       </c>
       <c r="K20" t="n">
-        <v>27243.62308855753</v>
+        <v>27301.03892209647</v>
       </c>
     </row>
     <row r="21">
@@ -21537,19 +21537,19 @@
         <v>141.18</v>
       </c>
       <c r="G21" t="n">
-        <v>-134.0970741868296</v>
+        <v>-242.7693600540551</v>
       </c>
       <c r="H21" t="n">
         <v>26142</v>
       </c>
       <c r="I21" t="n">
-        <v>26276.09707418683</v>
+        <v>26384.76936005406</v>
       </c>
       <c r="J21" t="n">
-        <v>26205.89049698968</v>
+        <v>26255.2044314546</v>
       </c>
       <c r="K21" t="n">
-        <v>26212.20659212286</v>
+        <v>26271.56584746381</v>
       </c>
     </row>
     <row r="22">
@@ -21563,19 +21563,19 @@
         <v>141.08</v>
       </c>
       <c r="G22" t="n">
-        <v>-138.1915497305927</v>
+        <v>-250.2073351442305</v>
       </c>
       <c r="H22" t="n">
         <v>26419.9</v>
       </c>
       <c r="I22" t="n">
-        <v>26558.09154973059</v>
+        <v>26670.10733514423</v>
       </c>
       <c r="J22" t="n">
-        <v>26485.48454688191</v>
+        <v>26536.09854656383</v>
       </c>
       <c r="K22" t="n">
-        <v>26492.50701676753</v>
+        <v>26553.90973908087</v>
       </c>
     </row>
     <row r="23">
@@ -21589,19 +21589,19 @@
         <v>140.98</v>
       </c>
       <c r="G23" t="n">
-        <v>-142.4792621433735</v>
+        <v>-257.9975459890629</v>
       </c>
       <c r="H23" t="n">
         <v>27293.7</v>
       </c>
       <c r="I23" t="n">
-        <v>27436.17926214337</v>
+        <v>27551.69754598906</v>
       </c>
       <c r="J23" t="n">
-        <v>27361.04680615385</v>
+        <v>27413.0128632388</v>
       </c>
       <c r="K23" t="n">
-        <v>27368.83246878714</v>
+        <v>27432.38566654363</v>
       </c>
     </row>
     <row r="24">
@@ -21615,19 +21615,19 @@
         <v>140.88</v>
       </c>
       <c r="G24" t="n">
-        <v>-146.9727389411128</v>
+        <v>-266.162901591968</v>
       </c>
       <c r="H24" t="n">
         <v>26191.1</v>
       </c>
       <c r="I24" t="n">
-        <v>26338.07273894111</v>
+        <v>26457.26290159197</v>
       </c>
       <c r="J24" t="n">
-        <v>26260.28098242906</v>
+        <v>26313.65389304024</v>
       </c>
       <c r="K24" t="n">
-        <v>26268.89176806253</v>
+        <v>26334.71002741211</v>
       </c>
     </row>
     <row r="25">
@@ -21641,19 +21641,19 @@
         <v>140.78</v>
       </c>
       <c r="G25" t="n">
-        <v>-151.6855529069253</v>
+        <v>-274.7282277488339</v>
       </c>
       <c r="H25" t="n">
         <v>26444.7</v>
       </c>
       <c r="I25" t="n">
-        <v>26596.38555290693</v>
+        <v>26719.42822774883</v>
       </c>
       <c r="J25" t="n">
-        <v>26515.79103843131</v>
+        <v>26570.628593815</v>
       </c>
       <c r="K25" t="n">
-        <v>26525.29452464033</v>
+        <v>26593.50068976325</v>
       </c>
     </row>
     <row r="26">
@@ -21667,19 +21667,19 @@
         <v>140.68</v>
       </c>
       <c r="G26" t="n">
-        <v>-156.6324297459978</v>
+        <v>-283.7204648798142</v>
       </c>
       <c r="H26" t="n">
         <v>26393.8</v>
       </c>
       <c r="I26" t="n">
-        <v>26550.432429746</v>
+        <v>26677.52046487981</v>
       </c>
       <c r="J26" t="n">
-        <v>26466.88121331592</v>
+        <v>26523.2444068508</v>
       </c>
       <c r="K26" t="n">
-        <v>26477.35122505622</v>
+        <v>26548.07715286907</v>
       </c>
     </row>
     <row r="27">
@@ -21693,19 +21693,19 @@
         <v>140.58</v>
       </c>
       <c r="G27" t="n">
-        <v>-161.829369031002</v>
+        <v>-293.1688903141549</v>
       </c>
       <c r="H27" t="n">
         <v>26023.2</v>
       </c>
       <c r="I27" t="n">
-        <v>26185.029369031</v>
+        <v>26316.36889031416</v>
       </c>
       <c r="J27" t="n">
-        <v>26098.3560461091</v>
+        <v>26156.30929768437</v>
       </c>
       <c r="K27" t="n">
-        <v>26109.87332984087</v>
+        <v>26183.26072867466</v>
       </c>
     </row>
     <row r="28">
@@ -21719,19 +21719,19 @@
         <v>140.48</v>
       </c>
       <c r="G28" t="n">
-        <v>-167.2937803621862</v>
+        <v>-303.1053685688203</v>
       </c>
       <c r="H28" t="n">
         <v>27069.8</v>
       </c>
       <c r="I28" t="n">
-        <v>27237.09378036219</v>
+        <v>27372.90536856882</v>
       </c>
       <c r="J28" t="n">
-        <v>27147.12040149632</v>
+        <v>27206.73180097875</v>
       </c>
       <c r="K28" t="n">
-        <v>27159.77338389146</v>
+        <v>27235.97474720103</v>
       </c>
     </row>
     <row r="29">
@@ -21745,19 +21745,19 @@
         <v>140.38</v>
       </c>
       <c r="G29" t="n">
-        <v>-173.044636987488</v>
+        <v>-313.5646337520411</v>
       </c>
       <c r="H29" t="n">
         <v>26161.8</v>
       </c>
       <c r="I29" t="n">
-        <v>26334.84463698749</v>
+        <v>26475.36463375204</v>
       </c>
       <c r="J29" t="n">
-        <v>26241.37949823223</v>
+        <v>26302.72106993915</v>
       </c>
       <c r="K29" t="n">
-        <v>26255.26514168162</v>
+        <v>26334.44478953439</v>
       </c>
     </row>
     <row r="30">
@@ -21771,19 +21771,19 @@
         <v>140.28</v>
       </c>
       <c r="G30" t="n">
-        <v>-179.1026495102706</v>
+        <v>-324.5846089251136</v>
       </c>
       <c r="H30" t="n">
         <v>26300.2</v>
       </c>
       <c r="I30" t="n">
-        <v>26479.30264951027</v>
+        <v>26624.78460892511</v>
       </c>
       <c r="J30" t="n">
-        <v>26382.13894048109</v>
+        <v>26445.28693079888</v>
       </c>
       <c r="K30" t="n">
-        <v>26397.36370962848</v>
+        <v>26479.698952704</v>
       </c>
     </row>
     <row r="31">
@@ -21797,19 +21797,19 @@
         <v>140.18</v>
       </c>
       <c r="G31" t="n">
-        <v>-185.4904627682772</v>
+        <v>-336.2067680935252</v>
       </c>
       <c r="H31" t="n">
         <v>26179.2</v>
       </c>
       <c r="I31" t="n">
-        <v>26364.69046276828</v>
+        <v>26515.40676809353</v>
       </c>
       <c r="J31" t="n">
-        <v>26263.60475243738</v>
+        <v>26328.63994297732</v>
       </c>
       <c r="K31" t="n">
-        <v>26280.28570835068</v>
+        <v>26365.96815151743</v>
       </c>
     </row>
     <row r="32">
@@ -21823,19 +21823,19 @@
         <v>140.08</v>
       </c>
       <c r="G32" t="n">
-        <v>-192.2328795139256</v>
+        <v>-348.4765475012209</v>
       </c>
       <c r="H32" t="n">
         <v>25952.4</v>
       </c>
       <c r="I32" t="n">
-        <v>26144.63287951393</v>
+        <v>26300.87654750122</v>
       </c>
       <c r="J32" t="n">
-        <v>26039.38341662489</v>
+        <v>26106.3914655937</v>
       </c>
       <c r="K32" t="n">
-        <v>26057.64945804922</v>
+        <v>26146.88646334357</v>
       </c>
     </row>
     <row r="33">
@@ -21849,19 +21849,19 @@
         <v>139.98</v>
       </c>
       <c r="G33" t="n">
-        <v>-199.3571151822471</v>
+        <v>-361.4438141060527</v>
       </c>
       <c r="H33" t="n">
         <v>25823.1</v>
       </c>
       <c r="I33" t="n">
-        <v>26022.45711518225</v>
+        <v>26184.54381410605</v>
       </c>
       <c r="J33" t="n">
-        <v>25912.7819163267</v>
+        <v>25981.85373111424</v>
       </c>
       <c r="K33" t="n">
-        <v>25932.77519084498</v>
+        <v>26025.79152294376</v>
       </c>
     </row>
     <row r="34">
@@ -21875,19 +21875,19 @@
         <v>139.88</v>
       </c>
       <c r="G34" t="n">
-        <v>-206.8930888245995</v>
+        <v>-375.1634005656888</v>
       </c>
       <c r="H34" t="n">
         <v>25796.2</v>
       </c>
       <c r="I34" t="n">
-        <v>26003.0930888246</v>
+        <v>26171.36340056569</v>
       </c>
       <c r="J34" t="n">
-        <v>25888.70778266282</v>
+        <v>25959.93992701877</v>
       </c>
       <c r="K34" t="n">
-        <v>25910.58529463438</v>
+        <v>26007.62497579434</v>
       </c>
     </row>
     <row r="35">
@@ -21901,19 +21901,19 @@
         <v>139.78</v>
       </c>
       <c r="G35" t="n">
-        <v>-214.8737562443384</v>
+        <v>-389.695717818362</v>
       </c>
       <c r="H35" t="n">
         <v>25706.9</v>
       </c>
       <c r="I35" t="n">
-        <v>25921.77375624434</v>
+        <v>26096.59571781836</v>
       </c>
       <c r="J35" t="n">
-        <v>25802.36914690532</v>
+        <v>25875.86428649823</v>
       </c>
       <c r="K35" t="n">
-        <v>25826.30459390919</v>
+        <v>25927.63299997363</v>
       </c>
     </row>
     <row r="36">
@@ -21927,19 +21927,19 @@
         <v>139.68</v>
       </c>
       <c r="G36" t="n">
-        <v>-223.3354925344902</v>
+        <v>-405.1074584732814</v>
       </c>
       <c r="H36" t="n">
         <v>25865.6</v>
       </c>
       <c r="I36" t="n">
-        <v>26088.93549253449</v>
+        <v>26270.70745847328</v>
       </c>
       <c r="J36" t="n">
-        <v>25964.17479870689</v>
+        <v>26040.04218934027</v>
       </c>
       <c r="K36" t="n">
-        <v>25990.36067406519</v>
+        <v>26096.26690867107</v>
       </c>
     </row>
     <row r="37">
@@ -21953,19 +21953,19 @@
         <v>139.58</v>
       </c>
       <c r="G37" t="n">
-        <v>-232.3185326376661</v>
+        <v>-421.472406821762</v>
       </c>
       <c r="H37" t="n">
         <v>26150.6</v>
       </c>
       <c r="I37" t="n">
-        <v>26382.91853263766</v>
+        <v>26572.07240682176</v>
       </c>
       <c r="J37" t="n">
-        <v>26252.4342510176</v>
+        <v>26330.79027432895</v>
       </c>
       <c r="K37" t="n">
-        <v>26281.08425704436</v>
+        <v>26391.88384780375</v>
       </c>
     </row>
     <row r="38">
@@ -21979,19 +21979,19 @@
         <v>139.48</v>
       </c>
       <c r="G38" t="n">
-        <v>-241.8674802869427</v>
+        <v>-438.8723744564122</v>
       </c>
       <c r="H38" t="n">
         <v>25610.5</v>
       </c>
       <c r="I38" t="n">
-        <v>25852.36748028694</v>
+        <v>26049.37237445641</v>
       </c>
       <c r="J38" t="n">
-        <v>25715.75781258128</v>
+        <v>25796.7265646816</v>
       </c>
       <c r="K38" t="n">
-        <v>25747.10963777861</v>
+        <v>25863.14760620441</v>
       </c>
     </row>
     <row r="39">
@@ -22005,19 +22005,19 @@
         <v>139.38</v>
       </c>
       <c r="G39" t="n">
-        <v>-252.0318978256619</v>
+        <v>-457.3982843875165</v>
       </c>
       <c r="H39" t="n">
         <v>25614.3</v>
       </c>
       <c r="I39" t="n">
-        <v>25866.33189782566</v>
+        <v>26071.69828438752</v>
       </c>
       <c r="J39" t="n">
-        <v>25723.15666903798</v>
+        <v>25806.87060827586</v>
       </c>
       <c r="K39" t="n">
-        <v>25757.47519290592</v>
+        <v>25879.12955951771</v>
       </c>
     </row>
     <row r="40">
@@ -22031,19 +22031,19 @@
         <v>139.28</v>
       </c>
       <c r="G40" t="n">
-        <v>-262.8669920463944</v>
+        <v>-477.1514313602929</v>
       </c>
       <c r="H40" t="n">
         <v>25482.4</v>
       </c>
       <c r="I40" t="n">
-        <v>25745.2669920464</v>
+        <v>25959.55143136029</v>
       </c>
       <c r="J40" t="n">
-        <v>25595.04297381827</v>
+        <v>25681.64363468862</v>
       </c>
       <c r="K40" t="n">
-        <v>25632.62397571387</v>
+        <v>25760.30977348642</v>
       </c>
     </row>
     <row r="41">
@@ -22057,19 +22057,19 @@
         <v>139.18</v>
       </c>
       <c r="G41" t="n">
-        <v>-274.4344144691422</v>
+        <v>-498.2449520424016</v>
       </c>
       <c r="H41" t="n">
         <v>25820.7</v>
       </c>
       <c r="I41" t="n">
-        <v>26095.13441446914</v>
+        <v>26318.9449520424</v>
       </c>
       <c r="J41" t="n">
-        <v>25937.3299502013</v>
+        <v>26026.96873138436</v>
       </c>
       <c r="K41" t="n">
-        <v>25978.50441435814</v>
+        <v>26112.67829795987</v>
       </c>
     </row>
     <row r="42">
@@ -22083,19 +22083,19 @@
         <v>139.08</v>
       </c>
       <c r="G42" t="n">
-        <v>-286.8031985692141</v>
+        <v>-520.8055461795193</v>
       </c>
       <c r="H42" t="n">
         <v>25337.9</v>
       </c>
       <c r="I42" t="n">
-        <v>25624.70319856922</v>
+        <v>25858.70554617952</v>
       </c>
       <c r="J42" t="n">
-        <v>25458.73200612877</v>
+        <v>25551.57104176119</v>
       </c>
       <c r="K42" t="n">
-        <v>25503.87113427475</v>
+        <v>25645.03669001448</v>
       </c>
     </row>
     <row r="43">
@@ -22109,19 +22109,19 @@
         <v>138.98</v>
       </c>
       <c r="G43" t="n">
-        <v>-300.0508615922772</v>
+        <v>-544.9754991090085</v>
       </c>
       <c r="H43" t="n">
         <v>25660.4</v>
       </c>
       <c r="I43" t="n">
-        <v>25960.45086159228</v>
+        <v>26205.37549910901</v>
       </c>
       <c r="J43" t="n">
-        <v>25785.66486362583</v>
+        <v>25881.87798820039</v>
       </c>
       <c r="K43" t="n">
-        <v>25835.18593057204</v>
+        <v>25983.89981343085</v>
       </c>
     </row>
     <row r="44">
@@ -22135,19 +22135,19 @@
         <v>138.88</v>
       </c>
       <c r="G44" t="n">
-        <v>-314.2647050539563</v>
+        <v>-570.9150677052021</v>
       </c>
       <c r="H44" t="n">
         <v>25130.5</v>
       </c>
       <c r="I44" t="n">
-        <v>25444.76470505396</v>
+        <v>25701.4150677052</v>
       </c>
       <c r="J44" t="n">
-        <v>25260.44570498765</v>
+        <v>25360.21952378214</v>
       </c>
       <c r="K44" t="n">
-        <v>25314.81892234108</v>
+        <v>25471.69797293861</v>
       </c>
     </row>
     <row r="45">
@@ -22161,19 +22161,19 @@
         <v>138.78</v>
       </c>
       <c r="G45" t="n">
-        <v>-329.5433562053404</v>
+        <v>-598.8053065952881</v>
       </c>
       <c r="H45" t="n">
         <v>25320.6</v>
       </c>
       <c r="I45" t="n">
-        <v>25650.14335620534</v>
+        <v>25919.40530659529</v>
       </c>
       <c r="J45" t="n">
-        <v>25455.49333825488</v>
+        <v>25559.02841694329</v>
       </c>
       <c r="K45" t="n">
-        <v>25515.24992864279</v>
+        <v>25680.97945579289</v>
       </c>
     </row>
     <row r="46">
@@ -22187,19 +22187,19 @@
         <v>138.68</v>
       </c>
       <c r="G46" t="n">
-        <v>-345.9986031728185</v>
+        <v>75.78190308710691</v>
       </c>
       <c r="H46" t="n">
-        <v>24983.9</v>
+        <v>24279.26666666667</v>
       </c>
       <c r="I46" t="n">
-        <v>25329.89860317282</v>
+        <v>24908.11809691289</v>
       </c>
       <c r="J46" t="n">
-        <v>25124.02838493558</v>
+        <v>24526.90724074811</v>
       </c>
       <c r="K46" t="n">
-        <v>25189.77011592201</v>
+        <v>24660.48023794563</v>
       </c>
     </row>
     <row r="47">
@@ -22213,19 +22213,19 @@
         <v>138.58</v>
       </c>
       <c r="G47" t="n">
-        <v>-363.7575898452305</v>
+        <v>76.1164334356472</v>
       </c>
       <c r="H47" t="n">
-        <v>25008</v>
+        <v>24270.59673606777</v>
       </c>
       <c r="I47" t="n">
-        <v>25371.75758984523</v>
+        <v>24931.88356656435</v>
       </c>
       <c r="J47" t="n">
-        <v>25153.6734934503</v>
+        <v>24527.9921420463</v>
       </c>
       <c r="K47" t="n">
-        <v>25226.0839794451</v>
+        <v>24674.49103791459</v>
       </c>
     </row>
     <row r="48">
@@ -22239,19 +22239,19 @@
         <v>138.48</v>
       </c>
       <c r="G48" t="n">
-        <v>-382.9654538167488</v>
+        <v>26.80657731125029</v>
       </c>
       <c r="H48" t="n">
-        <v>24993.3</v>
+        <v>24270.11552277</v>
       </c>
       <c r="I48" t="n">
-        <v>25376.26545381675</v>
+        <v>24966.49342268875</v>
       </c>
       <c r="J48" t="n">
-        <v>25144.85358239867</v>
+        <v>24537.85176772598</v>
       </c>
       <c r="K48" t="n">
-        <v>25224.7117379708</v>
+        <v>24698.76023211993</v>
       </c>
     </row>
     <row r="49">
@@ -22265,19 +22265,19 @@
         <v>138.38</v>
       </c>
       <c r="G49" t="n">
-        <v>-403.788513067142</v>
+        <v>34.74206662172219</v>
       </c>
       <c r="H49" t="n">
-        <v>25038.8</v>
+        <v>24269.62808213724</v>
       </c>
       <c r="I49" t="n">
-        <v>25442.58851306714</v>
+        <v>25004.05793337828</v>
       </c>
       <c r="J49" t="n">
-        <v>25196.59611849325</v>
+        <v>24548.33890305723</v>
       </c>
       <c r="K49" t="n">
-        <v>25284.79224248994</v>
+        <v>24725.35036059772</v>
       </c>
     </row>
     <row r="50">
@@ -22291,19 +22291,19 @@
         <v>138.28</v>
       </c>
       <c r="G50" t="n">
-        <v>-426.41813630053</v>
+        <v>-336.1246273528195</v>
       </c>
       <c r="H50" t="n">
-        <v>24708.8</v>
+        <v>24269.13085242916</v>
       </c>
       <c r="I50" t="n">
-        <v>25135.21813630053</v>
+        <v>25044.92462735282</v>
       </c>
       <c r="J50" t="n">
-        <v>24873.2314349082</v>
+        <v>24559.50265838537</v>
       </c>
       <c r="K50" t="n">
-        <v>24970.78652820715</v>
+        <v>24754.55628212683</v>
       </c>
     </row>
     <row r="51">
@@ -22317,19 +22317,19 @@
         <v>138.18</v>
       </c>
       <c r="G51" t="n">
-        <v>-451.0754703486782</v>
+        <v>-392.7036844257163</v>
       </c>
       <c r="H51" t="n">
-        <v>24696.9</v>
+        <v>24268.72843941786</v>
       </c>
       <c r="I51" t="n">
-        <v>25147.97547034868</v>
+        <v>25089.60368442572</v>
       </c>
       <c r="J51" t="n">
-        <v>24868.39309688198</v>
+        <v>24571.50587836198</v>
       </c>
       <c r="K51" t="n">
-        <v>24976.48217633138</v>
+        <v>24786.82994013768</v>
       </c>
     </row>
     <row r="52">
@@ -22343,19 +22343,19 @@
         <v>138.08</v>
       </c>
       <c r="G52" t="n">
-        <v>-478.0172490776786</v>
+        <v>-475.0839037351798</v>
       </c>
       <c r="H52" t="n">
-        <v>24663.5</v>
+        <v>24268.43903021374</v>
       </c>
       <c r="I52" t="n">
-        <v>25141.51724907768</v>
+        <v>25138.58390373518</v>
       </c>
       <c r="J52" t="n">
-        <v>24842.51832273874</v>
+        <v>24584.43127407206</v>
       </c>
       <c r="K52" t="n">
-        <v>24962.49870194838</v>
+        <v>24822.5956127132</v>
       </c>
     </row>
     <row r="53">
@@ -22369,19 +22369,19 @@
         <v>137.98</v>
       </c>
       <c r="G53" t="n">
-        <v>-507.5429764346154</v>
+        <v>-536.3158329654871</v>
       </c>
       <c r="H53" t="n">
-        <v>24656</v>
+        <v>24268.16449751587</v>
       </c>
       <c r="I53" t="n">
-        <v>25163.54297643462</v>
+        <v>25192.31583296549</v>
       </c>
       <c r="J53" t="n">
-        <v>24843.04847011072</v>
+        <v>24598.25235560997</v>
       </c>
       <c r="K53" t="n">
-        <v>24976.49425082906</v>
+        <v>24862.23221357238</v>
       </c>
     </row>
     <row r="54">
@@ -22395,19 +22395,19 @@
         <v>137.88</v>
       </c>
       <c r="G54" t="n">
-        <v>-540.0038681573133</v>
+        <v>-668.4410996875631</v>
       </c>
       <c r="H54" t="n">
-        <v>24583</v>
+        <v>24267.90354261339</v>
       </c>
       <c r="I54" t="n">
-        <v>25123.00386815731</v>
+        <v>25251.44109968756</v>
       </c>
       <c r="J54" t="n">
-        <v>24778.62959912295</v>
+        <v>24613.04753302859</v>
       </c>
       <c r="K54" t="n">
-        <v>24927.37397793446</v>
+        <v>24906.30166557264</v>
       </c>
     </row>
     <row r="55">
@@ -22421,19 +22421,19 @@
         <v>137.78</v>
       </c>
       <c r="G55" t="n">
-        <v>-575.8140615609482</v>
+        <v>-1040.131183722209</v>
       </c>
       <c r="H55" t="n">
-        <v>24276.6</v>
+        <v>24267.67016361184</v>
       </c>
       <c r="I55" t="n">
-        <v>24852.41406156095</v>
+        <v>25316.73118372221</v>
       </c>
       <c r="J55" t="n">
-        <v>24481.41312673508</v>
+        <v>24628.91969573027</v>
       </c>
       <c r="K55" t="n">
-        <v>24647.60060283514</v>
+        <v>24955.4865620468</v>
       </c>
     </row>
     <row r="56">
@@ -22447,19 +22447,19 @@
         <v>137.68</v>
       </c>
       <c r="G56" t="n">
-        <v>-615.4647742894558</v>
+        <v>-582.7809912688608</v>
       </c>
       <c r="H56" t="n">
-        <v>24806.4</v>
+        <v>24267.5614041612</v>
       </c>
       <c r="I56" t="n">
-        <v>25421.86477428946</v>
+        <v>25389.18099126886</v>
       </c>
       <c r="J56" t="n">
-        <v>25021.05658943832</v>
+        <v>24646.06525408752</v>
       </c>
       <c r="K56" t="n">
-        <v>25207.20780573309</v>
+        <v>25010.68244821588</v>
       </c>
     </row>
     <row r="57">
@@ -22473,19 +22473,19 @@
         <v>137.58</v>
       </c>
       <c r="G57" t="n">
-        <v>-213.812331797777</v>
+        <v>-230.6609243262574</v>
       </c>
       <c r="H57" t="n">
-        <v>24793.27</v>
+        <v>24267.37573543593</v>
       </c>
       <c r="I57" t="n">
-        <v>25452.81233179778</v>
+        <v>25469.66092432626</v>
       </c>
       <c r="J57" t="n">
-        <v>25018.49453522931</v>
+        <v>24664.3940306315</v>
       </c>
       <c r="K57" t="n">
-        <v>25227.58736292824</v>
+        <v>25072.64838163305</v>
       </c>
     </row>
     <row r="58">
@@ -22499,19 +22499,19 @@
         <v>137.48</v>
       </c>
       <c r="G58" t="n">
-        <v>-840.2913260155001</v>
+        <v>-902.9221103615855</v>
       </c>
       <c r="H58" t="n">
-        <v>24787.84</v>
+        <v>24266.87219964616</v>
       </c>
       <c r="I58" t="n">
-        <v>25496.5913260155</v>
+        <v>25559.22211036158</v>
       </c>
       <c r="J58" t="n">
-        <v>25024.42957042011</v>
+        <v>24683.79017121546</v>
       </c>
       <c r="K58" t="n">
-        <v>25260.0012586179</v>
+        <v>25142.31039451995</v>
       </c>
     </row>
     <row r="59">
@@ -22525,19 +22525,19 @@
         <v>137.38</v>
       </c>
       <c r="G59" t="n">
-        <v>-1067.184695997315</v>
+        <v>-1175.314975035089</v>
       </c>
       <c r="H59" t="n">
-        <v>24787.74</v>
+        <v>24266.42054387253</v>
       </c>
       <c r="I59" t="n">
-        <v>25551.68469599732</v>
+        <v>25659.81497503509</v>
       </c>
       <c r="J59" t="n">
-        <v>25036.57359264644</v>
+        <v>24704.76435647314</v>
       </c>
       <c r="K59" t="n">
-        <v>25302.85053246762</v>
+        <v>25221.47798934589</v>
       </c>
     </row>
     <row r="60">
@@ -22551,19 +22551,19 @@
         <v>137.28</v>
       </c>
       <c r="G60" t="n">
-        <v>-505.8334761672522</v>
+        <v>-665.4182678102625</v>
       </c>
       <c r="H60" t="n">
-        <v>24787.87</v>
+        <v>24266.21636391018</v>
       </c>
       <c r="I60" t="n">
-        <v>25614.03347616725</v>
+        <v>25773.61826781026</v>
       </c>
       <c r="J60" t="n">
-        <v>25049.91924873437</v>
+        <v>24727.67139655773</v>
       </c>
       <c r="K60" t="n">
-        <v>25351.98356989358</v>
+        <v>25312.17071434627</v>
       </c>
     </row>
     <row r="61">
@@ -22577,19 +22577,19 @@
         <v>137.18</v>
       </c>
       <c r="G61" t="n">
-        <v>-728.3611452782534</v>
+        <v>-946.6314490976656</v>
       </c>
       <c r="H61" t="n">
-        <v>24787.87</v>
+        <v>24265.86106008803</v>
       </c>
       <c r="I61" t="n">
-        <v>25684.56114527825</v>
+        <v>25902.83144909767</v>
       </c>
       <c r="J61" t="n">
-        <v>25064.21166530986</v>
+        <v>24752.2930892424</v>
       </c>
       <c r="K61" t="n">
-        <v>25408.21872028111</v>
+        <v>25416.40764989552</v>
       </c>
     </row>
     <row r="62">
@@ -22603,19 +22603,19 @@
         <v>137.08</v>
       </c>
       <c r="G62" t="n">
-        <v>-659.35360250952</v>
+        <v>-945.5895853061265</v>
       </c>
       <c r="H62" t="n">
-        <v>24787.72</v>
+        <v>24265.34975896525</v>
       </c>
       <c r="I62" t="n">
-        <v>25764.85360250952</v>
+        <v>26051.08958530613</v>
       </c>
       <c r="J62" t="n">
-        <v>25079.55051175861</v>
+        <v>24778.829592138</v>
       </c>
       <c r="K62" t="n">
-        <v>25473.02220992573</v>
+        <v>25537.6188560904</v>
       </c>
     </row>
     <row r="63">
@@ -22629,19 +22629,19 @@
         <v>136.98</v>
       </c>
       <c r="G63" t="n">
-        <v>68.97607271560628</v>
+        <v>-298.002893539433</v>
       </c>
       <c r="H63" t="n">
-        <v>24787.57</v>
+        <v>24264.83547033734</v>
       </c>
       <c r="I63" t="n">
-        <v>25857.12392728439</v>
+        <v>26224.10289353943</v>
       </c>
       <c r="J63" t="n">
-        <v>25096.22247012538</v>
+        <v>24807.66769913946</v>
       </c>
       <c r="K63" t="n">
-        <v>25548.47043161503</v>
+        <v>25681.28080428822</v>
       </c>
     </row>
     <row r="64">
@@ -22655,19 +22655,19 @@
         <v>136.88</v>
       </c>
       <c r="G64" t="n">
-        <v>-129.4830141715793</v>
+        <v>-596.3742627470929</v>
       </c>
       <c r="H64" t="n">
-        <v>24787.14</v>
+        <v>24263.99772715311</v>
       </c>
       <c r="I64" t="n">
-        <v>25963.88301417158</v>
+        <v>26430.77426274709</v>
       </c>
       <c r="J64" t="n">
-        <v>25114.10420580053</v>
+        <v>24838.75441983809</v>
       </c>
       <c r="K64" t="n">
-        <v>25636.91760815596</v>
+        <v>25856.02897133622</v>
       </c>
     </row>
     <row r="65">
@@ -22681,19 +22681,19 @@
         <v>136.78</v>
       </c>
       <c r="G65" t="n">
-        <v>239.177686738607</v>
+        <v>-358.87218837818</v>
       </c>
       <c r="H65" t="n">
-        <v>24786.48</v>
+        <v>24262.91721385765</v>
       </c>
       <c r="I65" t="n">
-        <v>26089.32231326139</v>
+        <v>26687.37218837818</v>
       </c>
       <c r="J65" t="n">
-        <v>25133.42595775014</v>
+        <v>24872.47755770869</v>
       </c>
       <c r="K65" t="n">
-        <v>25742.37494092048</v>
+        <v>26077.82484812009</v>
       </c>
     </row>
     <row r="66">
@@ -22707,19 +22707,19 @@
         <v>136.68</v>
       </c>
       <c r="G66" t="n">
-        <v>520.1474496745977</v>
+        <v>-262.1912957378263</v>
       </c>
       <c r="H66" t="n">
-        <v>24785.71</v>
+        <v>24261.69911272375</v>
       </c>
       <c r="I66" t="n">
-        <v>26240.5525503254</v>
+        <v>27022.89129573783</v>
       </c>
       <c r="J66" t="n">
-        <v>25154.51589946801</v>
+        <v>24909.2962575657</v>
       </c>
       <c r="K66" t="n">
-        <v>25871.74496517751</v>
+        <v>26375.30930311094</v>
       </c>
     </row>
     <row r="67">
@@ -22733,19 +22733,19 @@
         <v>136.58</v>
       </c>
       <c r="G67" t="n">
-        <v>624.8797408173123</v>
+        <v>-432.1530169218822</v>
       </c>
       <c r="H67" t="n">
-        <v>24784.65</v>
+        <v>24260.17123390361</v>
       </c>
       <c r="I67" t="n">
-        <v>26430.72025918269</v>
+        <v>27487.75301692188</v>
       </c>
       <c r="J67" t="n">
-        <v>25177.43546431353</v>
+        <v>24949.44789485205</v>
       </c>
       <c r="K67" t="n">
-        <v>26037.93274807715</v>
+        <v>26798.49456491139</v>
       </c>
     </row>
     <row r="68">
@@ -22759,19 +22759,19 @@
         <v>136.48</v>
       </c>
       <c r="G68" t="n">
-        <v>1262.074543058287</v>
+        <v>-217.5803986307801</v>
       </c>
       <c r="H68" t="n">
-        <v>24783.38</v>
+        <v>24258.39649102921</v>
       </c>
       <c r="I68" t="n">
-        <v>26687.02545694171</v>
+        <v>28166.68039863078</v>
       </c>
       <c r="J68" t="n">
-        <v>25202.54588496215</v>
+        <v>24993.4712617816</v>
       </c>
       <c r="K68" t="n">
-        <v>26267.85700506934</v>
+        <v>27431.62840858764</v>
       </c>
     </row>
     <row r="69">
@@ -22785,19 +22785,19 @@
         <v>136.38</v>
       </c>
       <c r="G69" t="n">
-        <v>1653.495803802398</v>
+        <v>-474.3437010405396</v>
       </c>
       <c r="H69" t="n">
-        <v>24781.75</v>
+        <v>24256.21957606118</v>
       </c>
       <c r="I69" t="n">
-        <v>27064.4041961976</v>
+        <v>29192.24370104054</v>
       </c>
       <c r="J69" t="n">
-        <v>25230.02627121758</v>
+        <v>25041.76641141674</v>
       </c>
       <c r="K69" t="n">
-        <v>26616.12453744821</v>
+        <v>28406.7266861544</v>
       </c>
     </row>
     <row r="70">
@@ -22811,19 +22811,19 @@
         <v>136.28</v>
       </c>
       <c r="G70" t="n">
-        <v>3048.741277079807</v>
+        <v>-38.38701688474976</v>
       </c>
       <c r="H70" t="n">
-        <v>24779.61</v>
+        <v>24253.47627788911</v>
       </c>
       <c r="I70" t="n">
-        <v>27668.85872292019</v>
+        <v>30755.98701688475</v>
       </c>
       <c r="J70" t="n">
-        <v>25260.11365025705</v>
+        <v>25094.82026473033</v>
       </c>
       <c r="K70" t="n">
-        <v>27188.35028992937</v>
+        <v>29914.6837357951</v>
       </c>
     </row>
     <row r="71">
@@ -22837,19 +22837,19 @@
         <v>136.18</v>
       </c>
       <c r="G71" t="n">
-        <v>4092.107172393193</v>
+        <v>-328.106517867127</v>
       </c>
       <c r="H71" t="n">
-        <v>24776.63</v>
+        <v>24249.79091213277</v>
       </c>
       <c r="I71" t="n">
-        <v>28687.69282760681</v>
+        <v>33107.90651786713</v>
       </c>
       <c r="J71" t="n">
-        <v>25292.93552817408</v>
+        <v>25153.02432006955</v>
       </c>
       <c r="K71" t="n">
-        <v>28171.38006116985</v>
+        <v>32204.7303461613</v>
       </c>
     </row>
     <row r="72">
@@ -22863,19 +22863,19 @@
         <v>136.08</v>
       </c>
       <c r="G72" t="n">
-        <v>6133.153740292481</v>
+        <v>15.2054471838419</v>
       </c>
       <c r="H72" t="n">
-        <v>24772.42</v>
+        <v>24244.71838881297</v>
       </c>
       <c r="I72" t="n">
-        <v>30416.94625970752</v>
+        <v>36534.89455281616</v>
       </c>
       <c r="J72" t="n">
-        <v>25328.64571527792</v>
+        <v>25216.84217392903</v>
       </c>
       <c r="K72" t="n">
-        <v>29860.70902189286</v>
+        <v>35562.85224478443</v>
       </c>
     </row>
     <row r="73">
@@ -22889,19 +22889,19 @@
         <v>135.98</v>
       </c>
       <c r="G73" t="n">
-        <v>8057.774512221367</v>
+        <v>10.98983901194879</v>
       </c>
       <c r="H73" t="n">
-        <v>24766.42</v>
+        <v>24237.63967018666</v>
       </c>
       <c r="I73" t="n">
-        <v>33262.72548777863</v>
+        <v>41309.51016098805</v>
       </c>
       <c r="J73" t="n">
-        <v>25367.33441019013</v>
+        <v>25286.73729875178</v>
       </c>
       <c r="K73" t="n">
-        <v>32661.79238730944</v>
+        <v>40260.5279225381</v>
       </c>
     </row>
     <row r="74">
@@ -22915,19 +22915,19 @@
         <v>135.88</v>
       </c>
       <c r="G74" t="n">
-        <v>9683.181160550834</v>
+        <v>-240.486087600977</v>
       </c>
       <c r="H74" t="n">
-        <v>24757.78</v>
+        <v>24227.61826560828</v>
       </c>
       <c r="I74" t="n">
-        <v>37685.51883944916</v>
+        <v>47609.18608760097</v>
       </c>
       <c r="J74" t="n">
-        <v>25408.93389033406</v>
+        <v>25363.07140998605</v>
       </c>
       <c r="K74" t="n">
-        <v>37034.33501135988</v>
+        <v>46473.89319514461</v>
       </c>
     </row>
     <row r="75">
@@ -22941,19 +22941,19 @@
         <v>135.78</v>
       </c>
       <c r="G75" t="n">
-        <v>11479.06558485878</v>
+        <v>125.6691488157085</v>
       </c>
       <c r="H75" t="n">
-        <v>24745.77</v>
+        <v>24213.82027477426</v>
       </c>
       <c r="I75" t="n">
-        <v>44065.23441514123</v>
+        <v>55418.63085118429</v>
       </c>
       <c r="J75" t="n">
-        <v>25453.66166323259</v>
+        <v>25446.58085880724</v>
       </c>
       <c r="K75" t="n">
-        <v>43357.29650165702</v>
+        <v>54186.08621387219</v>
       </c>
     </row>
     <row r="76">
@@ -22967,19 +22967,19 @@
         <v>135.68</v>
       </c>
       <c r="G76" t="n">
-        <v>10895.72752791201</v>
+        <v>-1044.273110955946</v>
       </c>
       <c r="H76" t="n">
-        <v>24729.31</v>
+        <v>24195.0424483002</v>
       </c>
       <c r="I76" t="n">
-        <v>52496.17247208799</v>
+        <v>64436.17311095595</v>
       </c>
       <c r="J76" t="n">
-        <v>25501.59371646691</v>
+        <v>25537.98592480601</v>
       </c>
       <c r="K76" t="n">
-        <v>51723.82088619232</v>
+        <v>63093.50992830192</v>
       </c>
     </row>
     <row r="77">
@@ -22993,19 +22993,19 @@
         <v>135.58</v>
       </c>
       <c r="G77" t="n">
-        <v>11102.19104225641</v>
+        <v>-333.9010530837113</v>
       </c>
       <c r="H77" t="n">
-        <v>24707.74</v>
+        <v>24170.56926247515</v>
       </c>
       <c r="I77" t="n">
-        <v>62571.70895774358</v>
+        <v>74007.80105308371</v>
       </c>
       <c r="J77" t="n">
-        <v>25553.49192469826</v>
+        <v>25638.97789138934</v>
       </c>
       <c r="K77" t="n">
-        <v>61725.86330245735</v>
+        <v>72539.74098919696</v>
       </c>
     </row>
     <row r="78">
@@ -23019,19 +23019,19 @@
         <v>135.48</v>
       </c>
       <c r="G78" t="n">
-        <v>10280.89930837728</v>
+        <v>419.6849089021271</v>
       </c>
       <c r="H78" t="n">
-        <v>24680.31</v>
+        <v>24139.55535317079</v>
       </c>
       <c r="I78" t="n">
-        <v>73238.30069162272</v>
+        <v>83099.51509109787</v>
       </c>
       <c r="J78" t="n">
-        <v>25610.37293796627</v>
+        <v>25751.83581697066</v>
       </c>
       <c r="K78" t="n">
-        <v>72308.11667008666</v>
+        <v>81487.64791501428</v>
       </c>
     </row>
     <row r="79">
@@ -23045,19 +23045,19 @@
         <v>135.38</v>
       </c>
       <c r="G79" t="n">
-        <v>8515.992764648472</v>
+        <v>954.9103250145999</v>
       </c>
       <c r="H79" t="n">
-        <v>24646.44</v>
+        <v>24101.36449068717</v>
       </c>
       <c r="I79" t="n">
-        <v>82785.70723535153</v>
+        <v>90346.7896749854</v>
       </c>
       <c r="J79" t="n">
-        <v>25673.88499330872</v>
+        <v>25880.22868716476</v>
       </c>
       <c r="K79" t="n">
-        <v>81758.11677608042</v>
+        <v>88568.3900744483</v>
       </c>
     </row>
     <row r="80">
@@ -23071,19 +23071,19 @@
         <v>135.28</v>
       </c>
       <c r="G80" t="n">
-        <v>4785.489860374015</v>
+        <v>-448.2646820274531</v>
       </c>
       <c r="H80" t="n">
-        <v>24607.12</v>
+        <v>24057.11422926274</v>
       </c>
       <c r="I80" t="n">
-        <v>89077.61013962599</v>
+        <v>94311.36468202746</v>
       </c>
       <c r="J80" t="n">
-        <v>25747.90625100891</v>
+        <v>26031.71213236988</v>
       </c>
       <c r="K80" t="n">
-        <v>87936.66259005821</v>
+        <v>92337.25884266369</v>
       </c>
     </row>
     <row r="81">
@@ -23097,19 +23097,19 @@
         <v>135.18</v>
       </c>
       <c r="G81" t="n">
-        <v>4574.634539979059</v>
+        <v>809.115553890384</v>
       </c>
       <c r="H81" t="n">
-        <v>24564.75</v>
+        <v>24009.49022922284</v>
       </c>
       <c r="I81" t="n">
-        <v>90293.86546002094</v>
+        <v>94059.38444610962</v>
       </c>
       <c r="J81" t="n">
-        <v>25838.78609134764</v>
+        <v>26219.47797009807</v>
       </c>
       <c r="K81" t="n">
-        <v>89019.66555333097</v>
+        <v>91849.88556622883</v>
       </c>
     </row>
     <row r="82">
@@ -23123,19 +23123,19 @@
         <v>135.08</v>
       </c>
       <c r="G82" t="n">
-        <v>3421.595467541745</v>
+        <v>-239.2863041538221</v>
       </c>
       <c r="H82" t="n">
-        <v>24521.76</v>
+        <v>23961.17823651893</v>
       </c>
       <c r="I82" t="n">
-        <v>86067.30453245825</v>
+        <v>89728.18630415382</v>
       </c>
       <c r="J82" t="n">
-        <v>25954.89337816945</v>
+        <v>26464.53754670743</v>
       </c>
       <c r="K82" t="n">
-        <v>84634.0191337569</v>
+        <v>87225.28281794238</v>
       </c>
     </row>
     <row r="83">
@@ -23149,19 +23149,19 @@
         <v>134.98</v>
       </c>
       <c r="G83" t="n">
-        <v>3874.851737302597</v>
+        <v>-800.4941224317445</v>
       </c>
       <c r="H83" t="n">
-        <v>24480.96</v>
+        <v>23915.3066026128</v>
       </c>
       <c r="I83" t="n">
-        <v>77780.8482626974</v>
+        <v>82456.19412243174</v>
       </c>
       <c r="J83" t="n">
-        <v>26109.20688344545</v>
+        <v>26802.92599587788</v>
       </c>
       <c r="K83" t="n">
-        <v>76152.47193104547</v>
+        <v>79568.97562618672</v>
       </c>
     </row>
     <row r="84">
@@ -23175,19 +23175,19 @@
         <v>134.88</v>
       </c>
       <c r="G84" t="n">
-        <v>5263.453035629092</v>
+        <v>-910.3065523035766</v>
       </c>
       <c r="H84" t="n">
-        <v>24444.82</v>
+        <v>23874.62060459255</v>
       </c>
       <c r="I84" t="n">
-        <v>67597.64696437091</v>
+        <v>73771.40655230358</v>
       </c>
       <c r="J84" t="n">
-        <v>26323.81450207759</v>
+        <v>27295.96963063289</v>
       </c>
       <c r="K84" t="n">
-        <v>65718.55085209172</v>
+        <v>70350.39217390463</v>
       </c>
     </row>
     <row r="85">
@@ -23201,19 +23201,19 @@
         <v>134.78</v>
       </c>
       <c r="G85" t="n">
-        <v>7737.486084247263</v>
+        <v>140.1619977827868</v>
       </c>
       <c r="H85" t="n">
-        <v>24414.04</v>
+        <v>23839.91390638598</v>
       </c>
       <c r="I85" t="n">
-        <v>57490.51391575274</v>
+        <v>65087.83800221721</v>
       </c>
       <c r="J85" t="n">
-        <v>26639.65439967579</v>
+        <v>28044.86469063379</v>
       </c>
       <c r="K85" t="n">
-        <v>55264.8261059651</v>
+        <v>60883.1537462831</v>
       </c>
     </row>
     <row r="86">
@@ -23227,19 +23227,19 @@
         <v>134.68</v>
       </c>
       <c r="G86" t="n">
-        <v>8957.917240185634</v>
+        <v>297.0852744690856</v>
       </c>
       <c r="H86" t="n">
-        <v>24388.37</v>
+        <v>23810.8947209701</v>
       </c>
       <c r="I86" t="n">
-        <v>48867.08275981437</v>
+        <v>57527.91472553091</v>
       </c>
       <c r="J86" t="n">
-        <v>27138.57116243066</v>
+        <v>29211.51040907225</v>
       </c>
       <c r="K86" t="n">
-        <v>46116.83355279429</v>
+        <v>52127.50248034927</v>
       </c>
     </row>
     <row r="87">
@@ -23253,19 +23253,19 @@
         <v>134.58</v>
       </c>
       <c r="G87" t="n">
-        <v>10164.7160172049</v>
+        <v>790.0524703199771</v>
       </c>
       <c r="H87" t="n">
-        <v>24367.17</v>
+        <v>23786.85354710593</v>
       </c>
       <c r="I87" t="n">
-        <v>42540.4839827951</v>
+        <v>51915.14752968002</v>
       </c>
       <c r="J87" t="n">
-        <v>27978.49375647372</v>
+        <v>31038.00755892611</v>
       </c>
       <c r="K87" t="n">
-        <v>38929.13349794877</v>
+        <v>44664.1430686315</v>
       </c>
     </row>
     <row r="88">
@@ -23279,19 +23279,19 @@
         <v>134.48</v>
       </c>
       <c r="G88" t="n">
-        <v>10639.47550269544</v>
+        <v>694.1590207966437</v>
       </c>
       <c r="H88" t="n">
-        <v>24349.39</v>
+        <v>23766.62254641343</v>
       </c>
       <c r="I88" t="n">
-        <v>38872.92449730456</v>
+        <v>48818.24097920336</v>
       </c>
       <c r="J88" t="n">
-        <v>29438.99704250679</v>
+        <v>33854.37404891378</v>
       </c>
       <c r="K88" t="n">
-        <v>33783.30864641229</v>
+        <v>38730.59600467066</v>
       </c>
     </row>
     <row r="89">
@@ -23305,19 +23305,19 @@
         <v>134.38</v>
       </c>
       <c r="G89" t="n">
-        <v>11305.50230455114</v>
+        <v>712.4446502949941</v>
       </c>
       <c r="H89" t="n">
-        <v>24333.58</v>
+        <v>23748.59198887889</v>
       </c>
       <c r="I89" t="n">
-        <v>38014.09769544886</v>
+        <v>48607.155349705</v>
       </c>
       <c r="J89" t="n">
-        <v>31962.23930436466</v>
+        <v>38061.13300739953</v>
       </c>
       <c r="K89" t="n">
-        <v>30385.44623999967</v>
+        <v>34294.6884307342</v>
       </c>
     </row>
     <row r="90">
@@ -23331,19 +23331,19 @@
         <v>134.28</v>
       </c>
       <c r="G90" t="n">
-        <v>12588.61193347346</v>
+        <v>1217.652575671607</v>
       </c>
       <c r="H90" t="n">
-        <v>24317.98</v>
+        <v>23730.78637919238</v>
       </c>
       <c r="I90" t="n">
-        <v>40121.88806652654</v>
+        <v>51492.84742432839</v>
       </c>
       <c r="J90" t="n">
-        <v>36155.18220386736</v>
+        <v>44072.88424501078</v>
       </c>
       <c r="K90" t="n">
-        <v>28284.71215814159</v>
+        <v>31150.80029911123</v>
       </c>
     </row>
     <row r="91">
@@ -23357,19 +23357,19 @@
         <v>134.18</v>
       </c>
       <c r="G91" t="n">
-        <v>11057.55804419371</v>
+        <v>-1018.542652055869</v>
       </c>
       <c r="H91" t="n">
-        <v>24300.85</v>
+        <v>23711.26659516591</v>
       </c>
       <c r="I91" t="n">
-        <v>45446.34195580629</v>
+        <v>57522.44265205587</v>
       </c>
       <c r="J91" t="n">
-        <v>42706.57640626142</v>
+        <v>52217.31744920356</v>
       </c>
       <c r="K91" t="n">
-        <v>27040.66535877576</v>
+        <v>29016.4261813831</v>
       </c>
     </row>
     <row r="92">
@@ -23383,19 +23383,19 @@
         <v>134.08</v>
       </c>
       <c r="G92" t="n">
-        <v>12007.34356013157</v>
+        <v>-298.4727983798948</v>
       </c>
       <c r="H92" t="n">
-        <v>24280.58</v>
+        <v>23688.24477740759</v>
       </c>
       <c r="I92" t="n">
-        <v>54212.85643986843</v>
+        <v>66518.67279837989</v>
       </c>
       <c r="J92" t="n">
-        <v>52184.06468893807</v>
+        <v>62599.3093526244</v>
       </c>
       <c r="K92" t="n">
-        <v>26309.45279289301</v>
+        <v>27607.63120211365</v>
       </c>
     </row>
     <row r="93">
@@ -23409,19 +23409,19 @@
         <v>133.98</v>
       </c>
       <c r="G93" t="n">
-        <v>10418.73168573197</v>
+        <v>-1230.028411335763</v>
       </c>
       <c r="H93" t="n">
-        <v>24255.03</v>
+        <v>23659.33643716058</v>
       </c>
       <c r="I93" t="n">
-        <v>66332.36831426804</v>
+        <v>77981.12841133577</v>
       </c>
       <c r="J93" t="n">
-        <v>64726.77320339935</v>
+        <v>74957.25385282602</v>
       </c>
       <c r="K93" t="n">
-        <v>25860.7461354742</v>
+        <v>26683.22583631853</v>
       </c>
     </row>
     <row r="94">
@@ -23435,19 +23435,19 @@
         <v>133.88</v>
       </c>
       <c r="G94" t="n">
-        <v>9657.02134982706</v>
+        <v>-273.3017879428517</v>
       </c>
       <c r="H94" t="n">
-        <v>24222.27</v>
+        <v>23622.40047294605</v>
       </c>
       <c r="I94" t="n">
-        <v>81057.67865017294</v>
+        <v>90988.00178794285</v>
       </c>
       <c r="J94" t="n">
-        <v>79721.99683280398</v>
+        <v>88548.14871889887</v>
       </c>
       <c r="K94" t="n">
-        <v>25558.12003507909</v>
+        <v>26062.26232173021</v>
       </c>
     </row>
     <row r="95">
@@ -23461,19 +23461,19 @@
         <v>133.78</v>
       </c>
       <c r="G95" t="n">
-        <v>5160.095128206376</v>
+        <v>-2234.005892268789</v>
       </c>
       <c r="H95" t="n">
-        <v>24181.34</v>
+        <v>23576.349037702</v>
       </c>
       <c r="I95" t="n">
-        <v>96734.90487179362</v>
+        <v>104129.0058922688</v>
       </c>
       <c r="J95" t="n">
-        <v>95587.72217226357</v>
+        <v>102083.2126717261</v>
       </c>
       <c r="K95" t="n">
-        <v>25328.74061670958</v>
+        <v>25622.14635314</v>
       </c>
     </row>
     <row r="96">
@@ -23487,19 +23487,19 @@
         <v>133.68</v>
       </c>
       <c r="G96" t="n">
-        <v>5037.627026255897</v>
+        <v>292.4749688581651</v>
       </c>
       <c r="H96" t="n">
-        <v>24131.95</v>
+        <v>23520.88382786206</v>
       </c>
       <c r="I96" t="n">
-        <v>110761.3729737441</v>
+        <v>115506.5250311418</v>
       </c>
       <c r="J96" t="n">
-        <v>109757.10268907</v>
+        <v>113741.1019453441</v>
       </c>
       <c r="K96" t="n">
-        <v>25136.48256103069</v>
+        <v>25286.30739699761</v>
       </c>
     </row>
     <row r="97">
@@ -23513,19 +23513,19 @@
         <v>133.58</v>
       </c>
       <c r="G97" t="n">
-        <v>2508.238319247161</v>
+        <v>-520.6218537333916</v>
       </c>
       <c r="H97" t="n">
-        <v>24074.85</v>
+        <v>23456.82798241478</v>
       </c>
       <c r="I97" t="n">
-        <v>119911.7616807528</v>
+        <v>122940.6218537334</v>
       </c>
       <c r="J97" t="n">
-        <v>119022.1893201777</v>
+        <v>121386.8435674175</v>
       </c>
       <c r="K97" t="n">
-        <v>24964.71377459226</v>
+        <v>25010.60417948982</v>
       </c>
     </row>
     <row r="98">
@@ -23539,19 +23539,19 @@
         <v>133.48</v>
       </c>
       <c r="G98" t="n">
-        <v>2464.786897380705</v>
+        <v>-710.6360194476147</v>
       </c>
       <c r="H98" t="n">
-        <v>24013.27</v>
+        <v>23387.77094996308</v>
       </c>
       <c r="I98" t="n">
-        <v>121442.2131026193</v>
+        <v>124617.6360194476</v>
       </c>
       <c r="J98" t="n">
-        <v>120647.8340218842</v>
+        <v>123232.1756122969</v>
       </c>
       <c r="K98" t="n">
-        <v>24807.94596211309</v>
+        <v>24773.22779435893</v>
       </c>
     </row>
     <row r="99">
@@ -23565,19 +23565,19 @@
         <v>133.38</v>
       </c>
       <c r="G99" t="n">
-        <v>6721.409666247884</v>
+        <v>1485.597162367121</v>
       </c>
       <c r="H99" t="n">
-        <v>23950.93</v>
+        <v>23317.84817039809</v>
       </c>
       <c r="I99" t="n">
-        <v>114788.5903337521</v>
+        <v>120024.4028376329</v>
       </c>
       <c r="J99" t="n">
-        <v>114074.7305494668</v>
+        <v>118778.0624544752</v>
       </c>
       <c r="K99" t="n">
-        <v>24665.06673351792</v>
+        <v>24564.18458277292</v>
       </c>
     </row>
     <row r="100">
@@ -23591,19 +23591,19 @@
         <v>133.28</v>
       </c>
       <c r="G100" t="n">
-        <v>10000.47947275442</v>
+        <v>1732.538203689779</v>
       </c>
       <c r="H100" t="n">
-        <v>23891.63</v>
+        <v>23251.27706427683</v>
       </c>
       <c r="I100" t="n">
-        <v>102005.5205272456</v>
+        <v>110273.4617963102</v>
       </c>
       <c r="J100" t="n">
-        <v>101360.5706532065</v>
+        <v>109145.0708173719</v>
       </c>
       <c r="K100" t="n">
-        <v>24536.81785352017</v>
+        <v>24379.66452047916</v>
       </c>
     </row>
     <row r="101">
@@ -23617,19 +23617,19 @@
         <v>133.18</v>
       </c>
       <c r="G101" t="n">
-        <v>11399.18383074032</v>
+        <v>299.0577066347614</v>
       </c>
       <c r="H101" t="n">
-        <v>23839.56</v>
+        <v>23192.70973639133</v>
       </c>
       <c r="I101" t="n">
-        <v>86305.01616925967</v>
+        <v>97405.14229336524</v>
       </c>
       <c r="J101" t="n">
-        <v>85719.54156864621</v>
+        <v>96378.37199812694</v>
       </c>
       <c r="K101" t="n">
-        <v>24425.22450885197</v>
+        <v>24219.47750112756</v>
       </c>
     </row>
     <row r="102">
@@ -23643,19 +23643,19 @@
         <v>133.08</v>
       </c>
       <c r="G102" t="n">
-        <v>12275.04091005051</v>
+        <v>-619.4066308412148</v>
       </c>
       <c r="H102" t="n">
-        <v>23796.98</v>
+        <v>23144.68814635215</v>
       </c>
       <c r="I102" t="n">
-        <v>70584.0590899495</v>
+        <v>83478.50663084122</v>
       </c>
       <c r="J102" t="n">
-        <v>70050.27564842698</v>
+        <v>82540.2087830291</v>
       </c>
       <c r="K102" t="n">
-        <v>24330.9051415469</v>
+        <v>24082.98469757122</v>
       </c>
     </row>
     <row r="103">
@@ -23669,19 +23669,19 @@
         <v>132.98</v>
       </c>
       <c r="G103" t="n">
-        <v>14021.37155440384</v>
+        <v>741.5928337207733</v>
       </c>
       <c r="H103" t="n">
-        <v>23763.37</v>
+        <v>23106.65426004829</v>
       </c>
       <c r="I103" t="n">
-        <v>56828.52844559615</v>
+        <v>70108.30716627922</v>
       </c>
       <c r="J103" t="n">
-        <v>56339.9482836584</v>
+        <v>69247.60761248809</v>
       </c>
       <c r="K103" t="n">
-        <v>24252.04966928912</v>
+        <v>23967.35375686607</v>
       </c>
     </row>
     <row r="104">
@@ -23695,19 +23695,19 @@
         <v>132.88</v>
       </c>
       <c r="G104" t="n">
-        <v>12828.60733589139</v>
+        <v>490.599166789485</v>
       </c>
       <c r="H104" t="n">
-        <v>23737.62</v>
+        <v>23077.38218801484</v>
       </c>
       <c r="I104" t="n">
-        <v>46018.59266410861</v>
+        <v>58356.60083321051</v>
       </c>
       <c r="J104" t="n">
-        <v>45569.76393885198</v>
+        <v>57564.35989312951</v>
       </c>
       <c r="K104" t="n">
-        <v>24186.51509706278</v>
+        <v>23869.62415938352</v>
       </c>
     </row>
     <row r="105">
@@ -23721,19 +23721,19 @@
         <v>132.78</v>
       </c>
       <c r="G105" t="n">
-        <v>9946.257602409358</v>
+        <v>-535.5975089164567</v>
       </c>
       <c r="H105" t="n">
-        <v>23719.07</v>
+        <v>23056.15000669238</v>
       </c>
       <c r="I105" t="n">
-        <v>38276.64239759064</v>
+        <v>48758.49750891646</v>
       </c>
       <c r="J105" t="n">
-        <v>37862.95037883291</v>
+        <v>48026.95365226395</v>
       </c>
       <c r="K105" t="n">
-        <v>24132.80469758468</v>
+        <v>23787.69574867812</v>
       </c>
     </row>
     <row r="106">
@@ -23747,19 +23747,19 @@
         <v>132.68</v>
       </c>
       <c r="G106" t="n">
-        <v>8050.591893963137</v>
+        <v>-195.3476995438614</v>
       </c>
       <c r="H106" t="n">
-        <v>23706.11</v>
+        <v>23041.17569469801</v>
       </c>
       <c r="I106" t="n">
-        <v>33161.90810603686</v>
+        <v>41407.84769954386</v>
       </c>
       <c r="J106" t="n">
-        <v>32779.42040000063</v>
+        <v>40730.36069530147</v>
       </c>
       <c r="K106" t="n">
-        <v>24088.62477975184</v>
+        <v>23718.6651828854</v>
       </c>
     </row>
     <row r="107">
@@ -23773,19 +23773,19 @@
         <v>132.58</v>
       </c>
       <c r="G107" t="n">
-        <v>7103.91908570494</v>
+        <v>1014.376741196109</v>
       </c>
       <c r="H107" t="n">
-        <v>23696.67</v>
+        <v>23030.15004990677</v>
       </c>
       <c r="I107" t="n">
-        <v>29998.48091429506</v>
+        <v>36088.02325880389</v>
       </c>
       <c r="J107" t="n">
-        <v>29643.82592135834</v>
+        <v>35458.87800450102</v>
       </c>
       <c r="K107" t="n">
-        <v>24051.34246801386</v>
+        <v>23659.29815362755</v>
       </c>
     </row>
     <row r="108">
@@ -23799,19 +23799,19 @@
         <v>132.48</v>
       </c>
       <c r="G108" t="n">
-        <v>5665.839917441335</v>
+        <v>1375.151857357534</v>
       </c>
       <c r="H108" t="n">
-        <v>23689.54</v>
+        <v>23021.71087988172</v>
       </c>
       <c r="I108" t="n">
-        <v>28126.96008255867</v>
+        <v>32417.64814264247</v>
       </c>
       <c r="J108" t="n">
-        <v>27797.23078545594</v>
+        <v>31831.89981751545</v>
       </c>
       <c r="K108" t="n">
-        <v>24019.28114648034</v>
+        <v>23607.46223268421</v>
       </c>
     </row>
     <row r="109">
@@ -23825,19 +23825,19 @@
         <v>132.38</v>
       </c>
       <c r="G109" t="n">
-        <v>3659.62282828668</v>
+        <v>717.9045956399677</v>
       </c>
       <c r="H109" t="n">
-        <v>23684.35</v>
+        <v>23015.45607132985</v>
       </c>
       <c r="I109" t="n">
-        <v>27033.47717171332</v>
+        <v>29975.19540436003</v>
       </c>
       <c r="J109" t="n">
-        <v>26726.15427689579</v>
+        <v>29428.54499393664</v>
       </c>
       <c r="K109" t="n">
-        <v>23991.68150508323</v>
+        <v>23562.10955288914</v>
       </c>
     </row>
     <row r="110">
@@ -23851,19 +23851,19 @@
         <v>132.28</v>
       </c>
       <c r="G110" t="n">
-        <v>2924.46676211568</v>
+        <v>918.1144763769626</v>
       </c>
       <c r="H110" t="n">
-        <v>23680.54</v>
+        <v>23010.7376435812</v>
       </c>
       <c r="I110" t="n">
-        <v>26375.03323788432</v>
+        <v>28381.38552362304</v>
       </c>
       <c r="J110" t="n">
-        <v>26087.92316639442</v>
+        <v>27870.07865377862</v>
       </c>
       <c r="K110" t="n">
-        <v>23967.65677171679</v>
+        <v>23522.0475406183</v>
       </c>
     </row>
     <row r="111">
@@ -23877,19 +23877,19 @@
         <v>132.18</v>
       </c>
       <c r="G111" t="n">
-        <v>1754.360196107977</v>
+        <v>364.5336519851335</v>
       </c>
       <c r="H111" t="n">
-        <v>23677.64</v>
+        <v>23007.03805037983</v>
       </c>
       <c r="I111" t="n">
-        <v>25949.23980389202</v>
+        <v>27339.06634801487</v>
       </c>
       <c r="J111" t="n">
-        <v>25680.42418845623</v>
+        <v>26859.81042254122</v>
       </c>
       <c r="K111" t="n">
-        <v>23946.46111160922</v>
+        <v>23486.29690857145</v>
       </c>
     </row>
     <row r="112">
@@ -23903,19 +23903,19 @@
         <v>132.08</v>
       </c>
       <c r="G112" t="n">
-        <v>962.6943767606426</v>
+        <v>-28.30056289857748</v>
       </c>
       <c r="H112" t="n">
-        <v>23675.55</v>
+        <v>23004.24266008168</v>
       </c>
       <c r="I112" t="n">
-        <v>25648.00562323936</v>
+        <v>26639.00056289858</v>
       </c>
       <c r="J112" t="n">
-        <v>25395.79984289108</v>
+        <v>26188.89645963996</v>
       </c>
       <c r="K112" t="n">
-        <v>23927.76044570311</v>
+        <v>23454.34957654734</v>
       </c>
     </row>
     <row r="113">
@@ -23929,19 +23929,19 @@
         <v>131.98</v>
       </c>
       <c r="G113" t="n">
-        <v>364.4351786999287</v>
+        <v>-364.0100308202018</v>
       </c>
       <c r="H113" t="n">
-        <v>23674.03</v>
+        <v>23002.09621081664</v>
       </c>
       <c r="I113" t="n">
-        <v>25417.16482130007</v>
+        <v>26145.6100308202</v>
       </c>
       <c r="J113" t="n">
-        <v>25180.0837314748</v>
+        <v>25722.09547662278</v>
       </c>
       <c r="K113" t="n">
-        <v>23911.11513190745</v>
+        <v>23425.61344956775</v>
       </c>
     </row>
     <row r="114">
@@ -23955,19 +23955,19 @@
         <v>131.88</v>
       </c>
       <c r="G114" t="n">
-        <v>428.6938469923552</v>
+        <v>-117.9511374985887</v>
       </c>
       <c r="H114" t="n">
-        <v>23672.8</v>
+        <v>23000.27392565144</v>
       </c>
       <c r="I114" t="n">
-        <v>25230.20615300765</v>
+        <v>25776.85113749859</v>
       </c>
       <c r="J114" t="n">
-        <v>25006.93560716623</v>
+        <v>25377.65351493757</v>
       </c>
       <c r="K114" t="n">
-        <v>23896.07409202189</v>
+        <v>23399.47410393483</v>
       </c>
     </row>
     <row r="115">
@@ -23981,19 +23981,19 @@
         <v>131.78</v>
       </c>
       <c r="G115" t="n">
-        <v>259.0385750166461</v>
+        <v>-152.8439196473228</v>
       </c>
       <c r="H115" t="n">
-        <v>23671.71</v>
+        <v>22998.60388776983</v>
       </c>
       <c r="I115" t="n">
-        <v>25073.76142498335</v>
+        <v>25485.64391964732</v>
       </c>
       <c r="J115" t="n">
-        <v>24863.13449382208</v>
+        <v>25108.74073614763</v>
       </c>
       <c r="K115" t="n">
-        <v>23882.34006875776</v>
+        <v>23375.5095025123</v>
       </c>
     </row>
     <row r="116">
@@ -24007,19 +24007,19 @@
         <v>131.68</v>
       </c>
       <c r="G116" t="n">
-        <v>167.3216312162513</v>
+        <v>-137.9889494714953</v>
       </c>
       <c r="H116" t="n">
-        <v>23670.78</v>
+        <v>22997.11670792633</v>
       </c>
       <c r="I116" t="n">
-        <v>24940.47836878375</v>
+        <v>25245.78894947149</v>
       </c>
       <c r="J116" t="n">
-        <v>24741.4553907453</v>
+        <v>24889.37456590213</v>
       </c>
       <c r="K116" t="n">
-        <v>23869.80577228675</v>
+        <v>23353.53340457795</v>
       </c>
     </row>
     <row r="117">
@@ -24033,19 +24033,19 @@
         <v>131.58</v>
       </c>
       <c r="G117" t="n">
-        <v>313.2385572265084</v>
+        <v>96.40476015530294</v>
       </c>
       <c r="H117" t="n">
-        <v>23669.91</v>
+        <v>22995.69536887771</v>
       </c>
       <c r="I117" t="n">
-        <v>24825.56144277349</v>
+        <v>25042.3952398447</v>
       </c>
       <c r="J117" t="n">
-        <v>24637.21321344618</v>
+        <v>24704.852739522</v>
       </c>
       <c r="K117" t="n">
-        <v>23858.2607315663</v>
+        <v>23333.24007106022</v>
       </c>
     </row>
     <row r="118">
@@ -24059,19 +24059,19 @@
         <v>131.48</v>
       </c>
       <c r="G118" t="n">
-        <v>-481.0688035468738</v>
+        <v>-622.1630938380913</v>
       </c>
       <c r="H118" t="n">
-        <v>23669.3</v>
+        <v>22994.55862520924</v>
       </c>
       <c r="I118" t="n">
-        <v>24725.86880354687</v>
+        <v>24866.96309383809</v>
       </c>
       <c r="J118" t="n">
-        <v>24547.36234776885</v>
+        <v>24546.84039426616</v>
       </c>
       <c r="K118" t="n">
-        <v>23847.80870755637</v>
+        <v>23314.68342232909</v>
       </c>
     </row>
     <row r="119">
@@ -24085,19 +24085,19 @@
         <v>131.38</v>
       </c>
       <c r="G119" t="n">
-        <v>-615.2251959912574</v>
+        <v>-690.3121216840518</v>
       </c>
       <c r="H119" t="n">
-        <v>23669.02</v>
+        <v>22993.79290818832</v>
       </c>
       <c r="I119" t="n">
-        <v>24638.92519599126</v>
+        <v>24714.01212168405</v>
       </c>
       <c r="J119" t="n">
-        <v>24469.5116743862</v>
+        <v>24410.00160505836</v>
       </c>
       <c r="K119" t="n">
-        <v>23838.4355570767</v>
+        <v>23297.80542465495</v>
       </c>
     </row>
     <row r="120">
@@ -24111,19 +24111,19 @@
         <v>131.28</v>
       </c>
       <c r="G120" t="n">
-        <v>-364.2126393422404</v>
+        <v>-381.1098143708587</v>
       </c>
       <c r="H120" t="n">
-        <v>23668.76</v>
+        <v>22993.04679280318</v>
       </c>
       <c r="I120" t="n">
-        <v>24562.41263934224</v>
+        <v>24579.30981437086</v>
       </c>
       <c r="J120" t="n">
-        <v>24401.41702674051</v>
+        <v>24290.23088990601</v>
       </c>
       <c r="K120" t="n">
-        <v>23829.75746012918</v>
+        <v>23282.12762560055</v>
       </c>
     </row>
     <row r="121">
@@ -24137,19 +24137,19 @@
         <v>131.18</v>
       </c>
       <c r="G121" t="n">
-        <v>-881.4174371632253</v>
+        <v>-846.6610922054715</v>
       </c>
       <c r="H121" t="n">
-        <v>23668.62</v>
+        <v>22992.43582725407</v>
       </c>
       <c r="I121" t="n">
-        <v>24494.81743716323</v>
+        <v>24460.06109220547</v>
       </c>
       <c r="J121" t="n">
-        <v>24341.62967852998</v>
+        <v>24184.84521204595</v>
       </c>
       <c r="K121" t="n">
-        <v>23821.80944195697</v>
+        <v>23267.65353000825</v>
       </c>
     </row>
     <row r="122">
@@ -24163,19 +24163,19 @@
         <v>131.08</v>
       </c>
       <c r="G122" t="n">
-        <v>-730.347755680621</v>
+        <v>-649.5028613425275</v>
       </c>
       <c r="H122" t="n">
-        <v>23668.62</v>
+        <v>22991.98907036496</v>
       </c>
       <c r="I122" t="n">
-        <v>24434.84775568062</v>
+        <v>24354.00286134253</v>
       </c>
       <c r="J122" t="n">
-        <v>24288.91515947069</v>
+        <v>24091.68059849458</v>
       </c>
       <c r="K122" t="n">
-        <v>23814.55413533885</v>
+        <v>23254.31307542318</v>
       </c>
     </row>
     <row r="123">
@@ -24189,19 +24189,19 @@
         <v>130.98</v>
       </c>
       <c r="G123" t="n">
-        <v>-696.8677677887645</v>
+        <v>-574.6909183196149</v>
       </c>
       <c r="H123" t="n">
-        <v>23668.6</v>
+        <v>22991.52039072555</v>
       </c>
       <c r="I123" t="n">
-        <v>24381.26776778877</v>
+        <v>24259.09091831962</v>
       </c>
       <c r="J123" t="n">
-        <v>24242.08844003467</v>
+        <v>24008.78078452384</v>
       </c>
       <c r="K123" t="n">
-        <v>23807.78073965832</v>
+        <v>23241.83219130692</v>
       </c>
     </row>
     <row r="124">
@@ -24215,19 +24215,19 @@
         <v>130.88</v>
       </c>
       <c r="G124" t="n">
-        <v>-631.9184671578005</v>
+        <v>-472.5160304864985</v>
       </c>
       <c r="H124" t="n">
-        <v>23668.59</v>
+        <v>22991.05220069463</v>
       </c>
       <c r="I124" t="n">
-        <v>24333.2184671578</v>
+        <v>24173.8160304865</v>
       </c>
       <c r="J124" t="n">
-        <v>24200.33562440823</v>
+        <v>23934.71476792562</v>
       </c>
       <c r="K124" t="n">
-        <v>23801.47414190594</v>
+        <v>23230.1550592093</v>
       </c>
     </row>
     <row r="125">
@@ -24241,19 +24241,19 @@
         <v>130.78</v>
       </c>
       <c r="G125" t="n">
-        <v>-622.5501075825414</v>
+        <v>-429.5071226502841</v>
       </c>
       <c r="H125" t="n">
-        <v>23668.58</v>
+        <v>22990.58932837403</v>
       </c>
       <c r="I125" t="n">
-        <v>24289.95010758254</v>
+        <v>24096.90712265029</v>
       </c>
       <c r="J125" t="n">
-        <v>24162.94713486715</v>
+        <v>23868.28124869919</v>
       </c>
       <c r="K125" t="n">
-        <v>23795.58417154107</v>
+        <v>23219.21673170063</v>
       </c>
     </row>
     <row r="126">
@@ -24267,19 +24267,19 @@
         <v>130.68</v>
       </c>
       <c r="G126" t="n">
-        <v>-1100.413152360925</v>
+        <v>-876.8697410394598</v>
       </c>
       <c r="H126" t="n">
-        <v>23668.74</v>
+        <v>22990.3082774641</v>
       </c>
       <c r="I126" t="n">
-        <v>24251.01315236092</v>
+        <v>24027.46974103946</v>
       </c>
       <c r="J126" t="n">
-        <v>24129.50929507937</v>
+        <v>23808.64816211477</v>
       </c>
       <c r="K126" t="n">
-        <v>23790.24496648138</v>
+        <v>23209.13132312654</v>
       </c>
     </row>
     <row r="127">
@@ -24293,19 +24293,19 @@
         <v>130.58</v>
       </c>
       <c r="G127" t="n">
-        <v>-495.9955921503388</v>
+        <v>-244.7018055464614</v>
       </c>
       <c r="H127" t="n">
-        <v>23668.88</v>
+        <v>22990.01152328476</v>
       </c>
       <c r="I127" t="n">
-        <v>24215.69559215034</v>
+        <v>23964.40180554646</v>
       </c>
       <c r="J127" t="n">
-        <v>24099.34218926882</v>
+        <v>23754.76934621436</v>
       </c>
       <c r="K127" t="n">
-        <v>23785.23443172827</v>
+        <v>23199.64539036939</v>
       </c>
     </row>
     <row r="128">
@@ -24319,19 +24319,19 @@
         <v>130.48</v>
       </c>
       <c r="G128" t="n">
-        <v>-484.4050888334823</v>
+        <v>-207.768994712671</v>
       </c>
       <c r="H128" t="n">
-        <v>23668.85</v>
+        <v>22989.53300666262</v>
       </c>
       <c r="I128" t="n">
-        <v>24183.40508883348</v>
+        <v>23906.76899471267</v>
       </c>
       <c r="J128" t="n">
-        <v>24071.88226987772</v>
+        <v>23705.76071290671</v>
       </c>
       <c r="K128" t="n">
-        <v>23780.37377551776</v>
+        <v>23190.54264062367</v>
       </c>
     </row>
     <row r="129">
@@ -24345,19 +24345,19 @@
         <v>130.38</v>
       </c>
       <c r="G129" t="n">
-        <v>-581.2848112169559</v>
+        <v>-281.4438478301345</v>
       </c>
       <c r="H129" t="n">
-        <v>23668.87</v>
+        <v>22989.10112895167</v>
       </c>
       <c r="I129" t="n">
-        <v>24153.98481121696</v>
+        <v>23854.14384783014</v>
       </c>
       <c r="J129" t="n">
-        <v>24046.99859194764</v>
+        <v>23661.24002736949</v>
       </c>
       <c r="K129" t="n">
-        <v>23775.85711059662</v>
+        <v>23182.00624911454</v>
       </c>
     </row>
     <row r="130">
@@ -24371,19 +24371,19 @@
         <v>130.28</v>
       </c>
       <c r="G130" t="n">
-        <v>-458.1721185537463</v>
+        <v>-735.8253514816352</v>
       </c>
       <c r="H130" t="n">
-        <v>23070.3</v>
+        <v>22988.87748552632</v>
       </c>
       <c r="I130" t="n">
-        <v>23528.47211855375</v>
+        <v>23806.12535148163</v>
       </c>
       <c r="J130" t="n">
-        <v>23425.75184042621</v>
+        <v>23620.84707989843</v>
       </c>
       <c r="K130" t="n">
-        <v>23173.02111040492</v>
+        <v>23174.15700728007</v>
       </c>
     </row>
     <row r="131">
@@ -24397,19 +24397,19 @@
         <v>130.18</v>
       </c>
       <c r="G131" t="n">
-        <v>-433.4494579478851</v>
+        <v>-500.3249940129244</v>
       </c>
       <c r="H131" t="n">
-        <v>23261.8</v>
+        <v>22988.75837712768</v>
       </c>
       <c r="I131" t="n">
-        <v>23695.24945794788</v>
+        <v>23762.12499401292</v>
       </c>
       <c r="J131" t="n">
-        <v>23596.54552490981</v>
+        <v>23584.03024765663</v>
       </c>
       <c r="K131" t="n">
-        <v>23360.50471171166</v>
+        <v>23166.85432683882</v>
       </c>
     </row>
     <row r="132">
@@ -24423,19 +24423,19 @@
         <v>130.08</v>
       </c>
       <c r="G132" t="n">
-        <v>-410.7069954932485</v>
+        <v>-41.51766844487793</v>
       </c>
       <c r="H132" t="n">
-        <v>23679.9</v>
+        <v>22988.43826975755</v>
       </c>
       <c r="I132" t="n">
-        <v>24090.60699549325</v>
+        <v>23721.41766844488</v>
       </c>
       <c r="J132" t="n">
-        <v>23995.68886869326</v>
+        <v>23550.09783846042</v>
       </c>
       <c r="K132" t="n">
-        <v>23774.81885668251</v>
+        <v>23159.75925880864</v>
       </c>
     </row>
     <row r="133">
@@ -24449,19 +24449,19 @@
         <v>129.98</v>
       </c>
       <c r="G133" t="n">
-        <v>-389.736614620404</v>
+        <v>53.91969539556521</v>
       </c>
       <c r="H133" t="n">
-        <v>23737.6</v>
+        <v>22987.9586872592</v>
       </c>
       <c r="I133" t="n">
-        <v>24127.3366146204</v>
+        <v>23683.68030460443</v>
       </c>
       <c r="J133" t="n">
-        <v>24035.99103145105</v>
+        <v>23518.75710710166</v>
       </c>
       <c r="K133" t="n">
-        <v>23828.94626852811</v>
+        <v>23152.88300189459</v>
       </c>
     </row>
     <row r="134">
@@ -24475,19 +24475,19 @@
         <v>129.88</v>
       </c>
       <c r="G134" t="n">
-        <v>-370.3569997685227</v>
+        <v>-727.7040544929914</v>
       </c>
       <c r="H134" t="n">
-        <v>22921.3</v>
+        <v>22987.72882652525</v>
       </c>
       <c r="I134" t="n">
-        <v>23291.65699976852</v>
+        <v>23649.00405449299</v>
       </c>
       <c r="J134" t="n">
-        <v>23203.68638856105</v>
+        <v>23490.12677637875</v>
       </c>
       <c r="K134" t="n">
-        <v>23009.27125583825</v>
+        <v>23146.6071820329</v>
       </c>
     </row>
     <row r="135">
@@ -24501,19 +24501,19 @@
         <v>129.78</v>
       </c>
       <c r="G135" t="n">
-        <v>-352.4095870526144</v>
+        <v>-400.7351967131908</v>
       </c>
       <c r="H135" t="n">
-        <v>23216.3</v>
+        <v>22987.67342379733</v>
       </c>
       <c r="I135" t="n">
-        <v>23568.70958705261</v>
+        <v>23617.03519671319</v>
       </c>
       <c r="J135" t="n">
-        <v>23483.93065284831</v>
+        <v>23463.87823551875</v>
       </c>
       <c r="K135" t="n">
-        <v>23301.07954149365</v>
+        <v>23140.83142469412</v>
       </c>
     </row>
     <row r="136">
@@ -24527,19 +24527,19 @@
         <v>129.68</v>
       </c>
       <c r="G136" t="n">
-        <v>-335.7552116738916</v>
+        <v>-480.894578359319</v>
       </c>
       <c r="H136" t="n">
-        <v>23106.4</v>
+        <v>22987.55797460081</v>
       </c>
       <c r="I136" t="n">
-        <v>23442.15521167389</v>
+        <v>23587.29457835932</v>
       </c>
       <c r="J136" t="n">
-        <v>23360.39767195547</v>
+        <v>23439.55524018787</v>
       </c>
       <c r="K136" t="n">
-        <v>23188.15811269652</v>
+        <v>23135.29831669661</v>
       </c>
     </row>
     <row r="137">
@@ -24553,19 +24553,19 @@
         <v>129.58</v>
       </c>
       <c r="G137" t="n">
-        <v>-320.2713184531422</v>
+        <v>-339.4247604492775</v>
       </c>
       <c r="H137" t="n">
-        <v>23220.2</v>
+        <v>22987.44069738006</v>
       </c>
       <c r="I137" t="n">
-        <v>23540.47131845314</v>
+        <v>23559.62476044928</v>
       </c>
       <c r="J137" t="n">
-        <v>23461.57677064121</v>
+        <v>23417.02128507237</v>
       </c>
       <c r="K137" t="n">
-        <v>23299.09508919746</v>
+        <v>23130.04514269186</v>
       </c>
     </row>
     <row r="138">
@@ -24579,19 +24579,19 @@
         <v>129.48</v>
       </c>
       <c r="G138" t="n">
-        <v>-305.8496299700018</v>
+        <v>560.0903615948373</v>
       </c>
       <c r="H138" t="n">
-        <v>24093.6</v>
+        <v>22986.99618993334</v>
       </c>
       <c r="I138" t="n">
-        <v>24399.44962997</v>
+        <v>23533.50963840516</v>
       </c>
       <c r="J138" t="n">
-        <v>24323.27053496516</v>
+        <v>23395.77942470178</v>
       </c>
       <c r="K138" t="n">
-        <v>24169.77960724342</v>
+        <v>23124.72734125584</v>
       </c>
     </row>
     <row r="139">
@@ -24605,19 +24605,19 @@
         <v>129.38</v>
       </c>
       <c r="G139" t="n">
-        <v>-292.3941884929918</v>
+        <v>-1129.78328159895</v>
       </c>
       <c r="H139" t="n">
-        <v>22379.6</v>
+        <v>22986.82766424902</v>
       </c>
       <c r="I139" t="n">
-        <v>22671.99418849299</v>
+        <v>23509.38328159895</v>
       </c>
       <c r="J139" t="n">
-        <v>22598.39295664753</v>
+        <v>23376.28129007724</v>
       </c>
       <c r="K139" t="n">
-        <v>22453.20171714251</v>
+        <v>23119.93056264172</v>
       </c>
     </row>
     <row r="140">
@@ -24631,19 +24631,19 @@
         <v>129.28</v>
       </c>
       <c r="G140" t="n">
-        <v>-279.8197047488502</v>
+        <v>185.7394105517124</v>
       </c>
       <c r="H140" t="n">
-        <v>23672.7</v>
+        <v>22986.80047070657</v>
       </c>
       <c r="I140" t="n">
-        <v>23952.51970474885</v>
+        <v>23486.96058944829</v>
       </c>
       <c r="J140" t="n">
-        <v>23881.36787244484</v>
+        <v>23358.25790161884</v>
       </c>
       <c r="K140" t="n">
-        <v>23743.85229265312</v>
+        <v>23115.50403612852</v>
       </c>
     </row>
     <row r="141">
@@ -24657,19 +24657,19 @@
         <v>129.18</v>
       </c>
       <c r="G141" t="n">
-        <v>-268.0501597632719</v>
+        <v>-787.5679703466012</v>
       </c>
       <c r="H141" t="n">
-        <v>22678.3</v>
+        <v>22986.67520933949</v>
       </c>
       <c r="I141" t="n">
-        <v>22946.35015976327</v>
+        <v>23465.8679703466</v>
       </c>
       <c r="J141" t="n">
-        <v>22877.52764630539</v>
+        <v>23341.35048730907</v>
       </c>
       <c r="K141" t="n">
-        <v>22747.12295066518</v>
+        <v>23111.19354206998</v>
       </c>
     </row>
     <row r="142">
@@ -24683,19 +24683,19 @@
         <v>129.08</v>
       </c>
       <c r="G142" t="n">
-        <v>-257.017616370249</v>
+        <v>-520.6303155381283</v>
       </c>
       <c r="H142" t="n">
-        <v>22925.7</v>
+        <v>22986.79677427003</v>
       </c>
       <c r="I142" t="n">
-        <v>23182.71761637025</v>
+        <v>23446.33031553813</v>
       </c>
       <c r="J142" t="n">
-        <v>23116.11205221466</v>
+        <v>23325.79758036919</v>
       </c>
       <c r="K142" t="n">
-        <v>22992.30597986099</v>
+        <v>23107.33033252744</v>
       </c>
     </row>
     <row r="143">
@@ -24709,19 +24709,19 @@
         <v>128.98</v>
       </c>
       <c r="G143" t="n">
-        <v>-246.6612051822667</v>
+        <v>-193.3106387921434</v>
       </c>
       <c r="H143" t="n">
-        <v>23234.5</v>
+        <v>22986.73576235272</v>
       </c>
       <c r="I143" t="n">
-        <v>23481.16120518227</v>
+        <v>23427.81063879214</v>
       </c>
       <c r="J143" t="n">
-        <v>23416.66732364976</v>
+        <v>23311.07476923789</v>
       </c>
       <c r="K143" t="n">
-        <v>23298.99427722804</v>
+        <v>23103.47242960823</v>
       </c>
     </row>
     <row r="144">
@@ -24735,19 +24735,19 @@
         <v>128.88</v>
       </c>
       <c r="G144" t="n">
-        <v>-236.9262563262346</v>
+        <v>-200.3993364111629</v>
       </c>
       <c r="H144" t="n">
-        <v>23209.9</v>
+        <v>22986.57924972876</v>
       </c>
       <c r="I144" t="n">
-        <v>23446.82625632624</v>
+        <v>23410.29933641116</v>
       </c>
       <c r="J144" t="n">
-        <v>23384.34534191922</v>
+        <v>23297.18405603977</v>
       </c>
       <c r="K144" t="n">
-        <v>23272.38129145296</v>
+        <v>23099.69530355934</v>
       </c>
     </row>
     <row r="145">
@@ -24761,19 +24761,19 @@
         <v>128.78</v>
       </c>
       <c r="G145" t="n">
-        <v>-227.7635534527981</v>
+        <v>-434.7953872003454</v>
       </c>
       <c r="H145" t="n">
-        <v>22959.1</v>
+        <v>22986.51329626028</v>
       </c>
       <c r="I145" t="n">
-        <v>23186.8635534528</v>
+        <v>23393.89538720034</v>
       </c>
       <c r="J145" t="n">
-        <v>23126.30294073331</v>
+        <v>23284.2351445992</v>
       </c>
       <c r="K145" t="n">
-        <v>23019.66097235827</v>
+        <v>23096.17428915668</v>
       </c>
     </row>
     <row r="146">
@@ -24787,19 +24787,19 @@
         <v>128.68</v>
       </c>
       <c r="G146" t="n">
-        <v>-219.128690702415</v>
+        <v>-173.5318433071443</v>
       </c>
       <c r="H146" t="n">
-        <v>23204.9</v>
+        <v>22986.44956199191</v>
       </c>
       <c r="I146" t="n">
-        <v>23424.02869070242</v>
+        <v>23378.43184330715</v>
       </c>
       <c r="J146" t="n">
-        <v>23365.30130841396</v>
+        <v>23272.07101014698</v>
       </c>
       <c r="K146" t="n">
-        <v>23263.62772565703</v>
+        <v>23092.81112329936</v>
       </c>
     </row>
     <row r="147">
@@ -24813,19 +24813,19 @@
         <v>128.58</v>
       </c>
       <c r="G147" t="n">
-        <v>-210.9815166793887</v>
+        <v>-604.901680045572</v>
       </c>
       <c r="H147" t="n">
-        <v>22759</v>
+        <v>22986.45213124931</v>
       </c>
       <c r="I147" t="n">
-        <v>22969.98151667939</v>
+        <v>23363.90168004557</v>
       </c>
       <c r="J147" t="n">
-        <v>22913.00547242375</v>
+        <v>23260.69381990903</v>
       </c>
       <c r="K147" t="n">
-        <v>22815.97637239624</v>
+        <v>23089.66069834322</v>
       </c>
     </row>
     <row r="148">
@@ -24839,19 +24839,19 @@
         <v>128.48</v>
       </c>
       <c r="G148" t="n">
-        <v>-203.2856522128641</v>
+        <v>-131.4699984966282</v>
       </c>
       <c r="H148" t="n">
-        <v>23218.7</v>
+        <v>22986.45056099897</v>
       </c>
       <c r="I148" t="n">
-        <v>23421.98565221286</v>
+        <v>23350.16999849663</v>
       </c>
       <c r="J148" t="n">
-        <v>23366.68385353976</v>
+        <v>23249.97719930482</v>
       </c>
       <c r="K148" t="n">
-        <v>23274.00211254274</v>
+        <v>23086.64404686243</v>
       </c>
     </row>
     <row r="149">
@@ -24865,19 +24865,19 @@
         <v>128.38</v>
       </c>
       <c r="G149" t="n">
-        <v>-196.0080709032081</v>
+        <v>49.52567839968469</v>
       </c>
       <c r="H149" t="n">
-        <v>23386.5</v>
+        <v>22986.24091321528</v>
       </c>
       <c r="I149" t="n">
-        <v>23582.50807090321</v>
+        <v>23336.97432160032</v>
       </c>
       <c r="J149" t="n">
-        <v>23528.80787914663</v>
+        <v>23239.66658528695</v>
       </c>
       <c r="K149" t="n">
-        <v>23440.2004922355</v>
+        <v>23083.54931676858</v>
       </c>
     </row>
     <row r="150">
@@ -24891,19 +24891,19 @@
         <v>128.28</v>
       </c>
       <c r="G150" t="n">
-        <v>-189.1187332650989</v>
+        <v>-139.7792387745794</v>
       </c>
       <c r="H150" t="n">
-        <v>23184.7</v>
+        <v>22986.04104220896</v>
       </c>
       <c r="I150" t="n">
-        <v>23373.8187332651</v>
+        <v>23324.47923877458</v>
       </c>
       <c r="J150" t="n">
-        <v>23321.65164687535</v>
+        <v>23229.93392257056</v>
       </c>
       <c r="K150" t="n">
-        <v>23236.86737428882</v>
+        <v>23080.58700702839</v>
       </c>
     </row>
     <row r="151">
@@ -24917,19 +24917,19 @@
         <v>128.18</v>
       </c>
       <c r="G151" t="n">
-        <v>-182.5902667657319</v>
+        <v>-326.7852487828604</v>
       </c>
       <c r="H151" t="n">
         <v>22687</v>
       </c>
       <c r="I151" t="n">
-        <v>22869.59026676573</v>
+        <v>23013.78524878286</v>
       </c>
       <c r="J151" t="n">
-        <v>22818.89163124964</v>
+        <v>22921.88655309871</v>
       </c>
       <c r="K151" t="n">
-        <v>22737.69891158341</v>
+        <v>22778.89932643854</v>
       </c>
     </row>
     <row r="152">
@@ -24943,19 +24943,19 @@
         <v>128.08</v>
       </c>
       <c r="G152" t="n">
-        <v>-176.3976852807864</v>
+        <v>-315.7302298626892</v>
       </c>
       <c r="H152" t="n">
         <v>22924.4</v>
       </c>
       <c r="I152" t="n">
-        <v>23100.79768528079</v>
+        <v>23240.13022986269</v>
       </c>
       <c r="J152" t="n">
-        <v>23051.50642718066</v>
+        <v>23150.76872830416</v>
       </c>
       <c r="K152" t="n">
-        <v>22973.69152302691</v>
+        <v>23013.76211517463</v>
       </c>
     </row>
     <row r="153">
@@ -24969,19 +24969,19 @@
         <v>127.98</v>
       </c>
       <c r="G153" t="n">
-        <v>-170.5181425025949</v>
+        <v>-305.2325886052313</v>
       </c>
       <c r="H153" t="n">
         <v>22643.1</v>
       </c>
       <c r="I153" t="n">
-        <v>22813.61814250259</v>
+        <v>22948.33258860523</v>
       </c>
       <c r="J153" t="n">
-        <v>22765.67652512387</v>
+        <v>22861.40479613878</v>
       </c>
       <c r="K153" t="n">
-        <v>22691.04187180448</v>
+        <v>22730.02838962882</v>
       </c>
     </row>
     <row r="154">
@@ -24995,19 +24995,19 @@
         <v>127.88</v>
       </c>
       <c r="G154" t="n">
-        <v>-164.9307146739375</v>
+        <v>-295.2551750653183</v>
       </c>
       <c r="H154" t="n">
         <v>22647.9</v>
       </c>
       <c r="I154" t="n">
-        <v>22812.83071467394</v>
+        <v>22943.15517506532</v>
       </c>
       <c r="J154" t="n">
-        <v>22766.1841135174</v>
+        <v>22858.5631507744</v>
       </c>
       <c r="K154" t="n">
-        <v>22694.54684567382</v>
+        <v>22732.49260564844</v>
       </c>
     </row>
     <row r="155">
@@ -25021,19 +25021,19 @@
         <v>127.78</v>
       </c>
       <c r="G155" t="n">
-        <v>-159.6162087193225</v>
+        <v>-285.7639023741394</v>
       </c>
       <c r="H155" t="n">
         <v>23050.9</v>
       </c>
       <c r="I155" t="n">
-        <v>23210.51620871932</v>
+        <v>23336.66390237414</v>
       </c>
       <c r="J155" t="n">
-        <v>23165.11290478979</v>
+        <v>23254.31488362092</v>
       </c>
       <c r="K155" t="n">
-        <v>23096.30353908803</v>
+        <v>23133.24958492138</v>
       </c>
     </row>
     <row r="156">
@@ -25047,19 +25047,19 @@
         <v>127.68</v>
       </c>
       <c r="G156" t="n">
-        <v>-154.5569924284682</v>
+        <v>-276.7274472645986</v>
       </c>
       <c r="H156" t="n">
         <v>22933.5</v>
       </c>
       <c r="I156" t="n">
-        <v>23088.05699242847</v>
+        <v>23210.2274472646</v>
       </c>
       <c r="J156" t="n">
-        <v>23043.84798178339</v>
+        <v>23130.0335124022</v>
       </c>
       <c r="K156" t="n">
-        <v>22977.70923695542</v>
+        <v>23013.69448642534</v>
       </c>
     </row>
     <row r="157">
@@ -25073,19 +25073,19 @@
         <v>127.58</v>
       </c>
       <c r="G157" t="n">
-        <v>-149.7368438352532</v>
+        <v>-268.1169843104071</v>
       </c>
       <c r="H157" t="n">
         <v>23251.9</v>
       </c>
       <c r="I157" t="n">
-        <v>23401.63684383525</v>
+        <v>23520.01698431041</v>
       </c>
       <c r="J157" t="n">
-        <v>23358.57566190515</v>
+        <v>23441.89474138325</v>
       </c>
       <c r="K157" t="n">
-        <v>23294.96139986718</v>
+        <v>23330.02278043968</v>
       </c>
     </row>
     <row r="158">
@@ -25099,19 +25099,19 @@
         <v>127.48</v>
       </c>
       <c r="G158" t="n">
-        <v>-145.1408173456148</v>
+        <v>-259.9059496018708</v>
       </c>
       <c r="H158" t="n">
         <v>22359.8</v>
       </c>
       <c r="I158" t="n">
-        <v>22504.94081734561</v>
+        <v>22619.70594960187</v>
       </c>
       <c r="J158" t="n">
-        <v>22462.98337670813</v>
+        <v>22543.57624873069</v>
       </c>
       <c r="K158" t="n">
-        <v>22401.75765064353</v>
+        <v>22435.93022486052</v>
       </c>
     </row>
     <row r="159">
@@ -25125,19 +25125,19 @@
         <v>127.38</v>
       </c>
       <c r="G159" t="n">
-        <v>-140.7551245138893</v>
+        <v>-252.0698301828779</v>
       </c>
       <c r="H159" t="n">
         <v>23047.9</v>
       </c>
       <c r="I159" t="n">
-        <v>23188.65512451389</v>
+        <v>23299.96983018288</v>
       </c>
       <c r="J159" t="n">
-        <v>23147.75956493561</v>
+        <v>23225.75749756118</v>
       </c>
       <c r="K159" t="n">
-        <v>23088.79576206551</v>
+        <v>23122.11284358922</v>
       </c>
     </row>
     <row r="160">
@@ -25151,19 +25151,19 @@
         <v>127.28</v>
       </c>
       <c r="G160" t="n">
-        <v>-136.567027659119</v>
+        <v>-244.5859760824023</v>
       </c>
       <c r="H160" t="n">
         <v>22819.4</v>
       </c>
       <c r="I160" t="n">
-        <v>22955.96702765912</v>
+        <v>23063.9859760824</v>
       </c>
       <c r="J160" t="n">
-        <v>22916.09357733751</v>
+        <v>22991.61956771569</v>
       </c>
       <c r="K160" t="n">
-        <v>22859.27364567478</v>
+        <v>22891.76690678944</v>
       </c>
     </row>
     <row r="161">
@@ -25177,19 +25177,19 @@
         <v>127.18</v>
       </c>
       <c r="G161" t="n">
-        <v>-132.5647447610099</v>
+        <v>-237.4334322057475</v>
       </c>
       <c r="H161" t="n">
         <v>22415.3</v>
       </c>
       <c r="I161" t="n">
-        <v>22547.86474476101</v>
+        <v>22652.73343220575</v>
       </c>
       <c r="J161" t="n">
-        <v>22508.97559180316</v>
+        <v>22582.14500570696</v>
       </c>
       <c r="K161" t="n">
-        <v>22454.18934153639</v>
+        <v>22485.88891283087</v>
       </c>
     </row>
     <row r="162">
@@ -25203,19 +25203,19 @@
         <v>127.08</v>
       </c>
       <c r="G162" t="n">
-        <v>-128.7373642853127</v>
+        <v>-230.5927877180111</v>
       </c>
       <c r="H162" t="n">
         <v>23032.4</v>
       </c>
       <c r="I162" t="n">
-        <v>23161.13736428531</v>
+        <v>23262.99278771801</v>
       </c>
       <c r="J162" t="n">
-        <v>23123.19653755408</v>
+        <v>23194.11769063524</v>
       </c>
       <c r="K162" t="n">
-        <v>23070.34100887133</v>
+        <v>23101.27557175683</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mac: Add preference input for residuals, Yaxis...
</commit_message>
<xml_diff>
--- a/DATA/UKSAF/STO.xlsx
+++ b/DATA/UKSAF/STO.xlsx
@@ -20647,7 +20647,7 @@
       </c>
       <c r="K1" s="28" t="inlineStr">
         <is>
-          <t>Sr3d3/2 p2</t>
+          <t>Sr3d3/2_p2</t>
         </is>
       </c>
       <c r="L1" s="28" t="inlineStr"/>
@@ -20878,12 +20878,12 @@
       </c>
       <c r="AO2" s="33" t="inlineStr">
         <is>
-          <t>-285.30</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="AP2" t="inlineStr">
         <is>
-          <t>-715.80</t>
+          <t>0.00</t>
         </is>
       </c>
     </row>
@@ -20987,7 +20987,7 @@
       </c>
       <c r="Y4" s="33" t="inlineStr">
         <is>
-          <t>Sr3d3/2 p2</t>
+          <t>Sr3d3/2_p2</t>
         </is>
       </c>
       <c r="Z4" s="33" t="inlineStr">
@@ -21059,12 +21059,12 @@
       </c>
       <c r="AO4" s="33" t="inlineStr">
         <is>
-          <t>-285.30</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="AP4" t="inlineStr">
         <is>
-          <t>-715.80</t>
+          <t>0.00</t>
         </is>
       </c>
     </row>
@@ -22187,19 +22187,19 @@
         <v>138.68</v>
       </c>
       <c r="G46" t="n">
-        <v>75.78190308710691</v>
+        <v>75.7785697537729</v>
       </c>
       <c r="H46" t="n">
-        <v>24279.26666666667</v>
+        <v>24279.27</v>
       </c>
       <c r="I46" t="n">
-        <v>24908.11809691289</v>
+        <v>24908.12143024623</v>
       </c>
       <c r="J46" t="n">
-        <v>24526.90724074811</v>
+        <v>24526.91057408145</v>
       </c>
       <c r="K46" t="n">
-        <v>24660.48023794563</v>
+        <v>24660.48357127897</v>
       </c>
     </row>
     <row r="47">
@@ -22213,19 +22213,19 @@
         <v>138.58</v>
       </c>
       <c r="G47" t="n">
-        <v>76.1164334356472</v>
+        <v>76.11316950341643</v>
       </c>
       <c r="H47" t="n">
-        <v>24270.59673606777</v>
+        <v>24270.6</v>
       </c>
       <c r="I47" t="n">
-        <v>24931.88356656435</v>
+        <v>24931.88683049658</v>
       </c>
       <c r="J47" t="n">
-        <v>24527.9921420463</v>
+        <v>24527.99540597853</v>
       </c>
       <c r="K47" t="n">
-        <v>24674.49103791459</v>
+        <v>24674.49430184682</v>
       </c>
     </row>
     <row r="48">
@@ -22239,19 +22239,19 @@
         <v>138.48</v>
       </c>
       <c r="G48" t="n">
-        <v>26.80657731125029</v>
+        <v>26.80210008125505</v>
       </c>
       <c r="H48" t="n">
-        <v>24270.11552277</v>
+        <v>24270.12</v>
       </c>
       <c r="I48" t="n">
-        <v>24966.49342268875</v>
+        <v>24966.49789991874</v>
       </c>
       <c r="J48" t="n">
-        <v>24537.85176772598</v>
+        <v>24537.85624495597</v>
       </c>
       <c r="K48" t="n">
-        <v>24698.76023211993</v>
+        <v>24698.76470934992</v>
       </c>
     </row>
     <row r="49">
@@ -22265,19 +22265,19 @@
         <v>138.38</v>
       </c>
       <c r="G49" t="n">
-        <v>34.74206662172219</v>
+        <v>34.74014875895955</v>
       </c>
       <c r="H49" t="n">
-        <v>24269.62808213724</v>
+        <v>24269.63</v>
       </c>
       <c r="I49" t="n">
-        <v>25004.05793337828</v>
+        <v>25004.05985124104</v>
       </c>
       <c r="J49" t="n">
-        <v>24548.33890305723</v>
+        <v>24548.34082092</v>
       </c>
       <c r="K49" t="n">
-        <v>24725.35036059772</v>
+        <v>24725.35227846048</v>
       </c>
     </row>
     <row r="50">
@@ -22291,19 +22291,19 @@
         <v>138.28</v>
       </c>
       <c r="G50" t="n">
-        <v>-336.1246273528195</v>
+        <v>-336.1237749236643</v>
       </c>
       <c r="H50" t="n">
-        <v>24269.13085242916</v>
+        <v>24269.13</v>
       </c>
       <c r="I50" t="n">
-        <v>25044.92462735282</v>
+        <v>25044.92377492366</v>
       </c>
       <c r="J50" t="n">
-        <v>24559.50265838537</v>
+        <v>24559.50180595621</v>
       </c>
       <c r="K50" t="n">
-        <v>24754.55628212683</v>
+        <v>24754.55542969767</v>
       </c>
     </row>
     <row r="51">
@@ -22317,19 +22317,19 @@
         <v>138.18</v>
       </c>
       <c r="G51" t="n">
-        <v>-392.7036844257163</v>
+        <v>-392.7052450078518</v>
       </c>
       <c r="H51" t="n">
-        <v>24268.72843941786</v>
+        <v>24268.73</v>
       </c>
       <c r="I51" t="n">
-        <v>25089.60368442572</v>
+        <v>25089.60524500785</v>
       </c>
       <c r="J51" t="n">
-        <v>24571.50587836198</v>
+        <v>24571.50743894411</v>
       </c>
       <c r="K51" t="n">
-        <v>24786.82994013768</v>
+        <v>24786.83150071981</v>
       </c>
     </row>
     <row r="52">
@@ -22343,19 +22343,19 @@
         <v>138.08</v>
       </c>
       <c r="G52" t="n">
-        <v>-475.0839037351798</v>
+        <v>-475.0848735214386</v>
       </c>
       <c r="H52" t="n">
-        <v>24268.43903021374</v>
+        <v>24268.44</v>
       </c>
       <c r="I52" t="n">
-        <v>25138.58390373518</v>
+        <v>25138.58487352144</v>
       </c>
       <c r="J52" t="n">
-        <v>24584.43127407206</v>
+        <v>24584.43224385831</v>
       </c>
       <c r="K52" t="n">
-        <v>24822.5956127132</v>
+        <v>24822.59658249946</v>
       </c>
     </row>
     <row r="53">
@@ -22369,19 +22369,19 @@
         <v>137.98</v>
       </c>
       <c r="G53" t="n">
-        <v>-536.3158329654871</v>
+        <v>-536.3113354496127</v>
       </c>
       <c r="H53" t="n">
-        <v>24268.16449751587</v>
+        <v>24268.16</v>
       </c>
       <c r="I53" t="n">
-        <v>25192.31583296549</v>
+        <v>25192.31133544961</v>
       </c>
       <c r="J53" t="n">
-        <v>24598.25235560997</v>
+        <v>24598.24785809409</v>
       </c>
       <c r="K53" t="n">
-        <v>24862.23221357238</v>
+        <v>24862.2277160565</v>
       </c>
     </row>
     <row r="54">
@@ -22395,19 +22395,19 @@
         <v>137.88</v>
       </c>
       <c r="G54" t="n">
-        <v>-668.4410996875631</v>
+        <v>-668.4375570741722</v>
       </c>
       <c r="H54" t="n">
-        <v>24267.90354261339</v>
+        <v>24267.9</v>
       </c>
       <c r="I54" t="n">
-        <v>25251.44109968756</v>
+        <v>25251.43755707417</v>
       </c>
       <c r="J54" t="n">
-        <v>24613.04753302859</v>
+        <v>24613.0439904152</v>
       </c>
       <c r="K54" t="n">
-        <v>24906.30166557264</v>
+        <v>24906.29812295924</v>
       </c>
     </row>
     <row r="55">
@@ -22421,19 +22421,19 @@
         <v>137.78</v>
       </c>
       <c r="G55" t="n">
-        <v>-1040.131183722209</v>
+        <v>-1040.13102011037</v>
       </c>
       <c r="H55" t="n">
-        <v>24267.67016361184</v>
+        <v>24267.67</v>
       </c>
       <c r="I55" t="n">
-        <v>25316.73118372221</v>
+        <v>25316.73102011037</v>
       </c>
       <c r="J55" t="n">
-        <v>24628.91969573027</v>
+        <v>24628.91953211843</v>
       </c>
       <c r="K55" t="n">
-        <v>24955.4865620468</v>
+        <v>24955.48639843496</v>
       </c>
     </row>
     <row r="56">
@@ -22447,19 +22447,19 @@
         <v>137.68</v>
       </c>
       <c r="G56" t="n">
-        <v>-582.7809912688608</v>
+        <v>-582.7795871076596</v>
       </c>
       <c r="H56" t="n">
-        <v>24267.5614041612</v>
+        <v>24267.56</v>
       </c>
       <c r="I56" t="n">
-        <v>25389.18099126886</v>
+        <v>25389.17958710766</v>
       </c>
       <c r="J56" t="n">
-        <v>24646.06525408752</v>
+        <v>24646.06384992632</v>
       </c>
       <c r="K56" t="n">
-        <v>25010.68244821588</v>
+        <v>25010.68104405468</v>
       </c>
     </row>
     <row r="57">
@@ -22473,19 +22473,19 @@
         <v>137.58</v>
       </c>
       <c r="G57" t="n">
-        <v>-230.6609243262574</v>
+        <v>-230.6651888903289</v>
       </c>
       <c r="H57" t="n">
-        <v>24267.37573543593</v>
+        <v>24267.38</v>
       </c>
       <c r="I57" t="n">
-        <v>25469.66092432626</v>
+        <v>25469.66518889033</v>
       </c>
       <c r="J57" t="n">
-        <v>24664.3940306315</v>
+        <v>24664.39829519557</v>
       </c>
       <c r="K57" t="n">
-        <v>25072.64838163305</v>
+        <v>25072.65264619712</v>
       </c>
     </row>
     <row r="58">
@@ -22499,19 +22499,19 @@
         <v>137.48</v>
       </c>
       <c r="G58" t="n">
-        <v>-902.9221103615855</v>
+        <v>-902.91991071542</v>
       </c>
       <c r="H58" t="n">
-        <v>24266.87219964616</v>
+        <v>24266.87</v>
       </c>
       <c r="I58" t="n">
-        <v>25559.22211036158</v>
+        <v>25559.21991071542</v>
       </c>
       <c r="J58" t="n">
-        <v>24683.79017121546</v>
+        <v>24683.78797156929</v>
       </c>
       <c r="K58" t="n">
-        <v>25142.31039451995</v>
+        <v>25142.30819487379</v>
       </c>
     </row>
     <row r="59">
@@ -22525,19 +22525,19 @@
         <v>137.38</v>
       </c>
       <c r="G59" t="n">
-        <v>-1175.314975035089</v>
+        <v>-1175.314431162558</v>
       </c>
       <c r="H59" t="n">
-        <v>24266.42054387253</v>
+        <v>24266.42</v>
       </c>
       <c r="I59" t="n">
-        <v>25659.81497503509</v>
+        <v>25659.81443116256</v>
       </c>
       <c r="J59" t="n">
-        <v>24704.76435647314</v>
+        <v>24704.76381260061</v>
       </c>
       <c r="K59" t="n">
-        <v>25221.47798934589</v>
+        <v>25221.47744547336</v>
       </c>
     </row>
     <row r="60">
@@ -22551,19 +22551,19 @@
         <v>137.28</v>
       </c>
       <c r="G60" t="n">
-        <v>-665.4182678102625</v>
+        <v>-665.4219039000855</v>
       </c>
       <c r="H60" t="n">
-        <v>24266.21636391018</v>
+        <v>24266.22</v>
       </c>
       <c r="I60" t="n">
-        <v>25773.61826781026</v>
+        <v>25773.62190390009</v>
       </c>
       <c r="J60" t="n">
-        <v>24727.67139655773</v>
+        <v>24727.67503264756</v>
       </c>
       <c r="K60" t="n">
-        <v>25312.17071434627</v>
+        <v>25312.17435043609</v>
       </c>
     </row>
     <row r="61">
@@ -22577,19 +22577,19 @@
         <v>137.18</v>
       </c>
       <c r="G61" t="n">
-        <v>-946.6314490976656</v>
+        <v>-946.6303890096315</v>
       </c>
       <c r="H61" t="n">
-        <v>24265.86106008803</v>
+        <v>24265.86</v>
       </c>
       <c r="I61" t="n">
-        <v>25902.83144909767</v>
+        <v>25902.83038900963</v>
       </c>
       <c r="J61" t="n">
-        <v>24752.2930892424</v>
+        <v>24752.29202915436</v>
       </c>
       <c r="K61" t="n">
-        <v>25416.40764989552</v>
+        <v>25416.40658980749</v>
       </c>
     </row>
     <row r="62">
@@ -22603,19 +22603,19 @@
         <v>137.08</v>
       </c>
       <c r="G62" t="n">
-        <v>-945.5895853061265</v>
+        <v>-945.5898263408781</v>
       </c>
       <c r="H62" t="n">
-        <v>24265.34975896525</v>
+        <v>24265.35</v>
       </c>
       <c r="I62" t="n">
-        <v>26051.08958530613</v>
+        <v>26051.08982634088</v>
       </c>
       <c r="J62" t="n">
-        <v>24778.829592138</v>
+        <v>24778.82983317275</v>
       </c>
       <c r="K62" t="n">
-        <v>25537.6188560904</v>
+        <v>25537.61909712516</v>
       </c>
     </row>
     <row r="63">
@@ -22629,19 +22629,19 @@
         <v>136.98</v>
       </c>
       <c r="G63" t="n">
-        <v>-298.002893539433</v>
+        <v>-298.0074232020961</v>
       </c>
       <c r="H63" t="n">
-        <v>24264.83547033734</v>
+        <v>24264.84</v>
       </c>
       <c r="I63" t="n">
-        <v>26224.10289353943</v>
+        <v>26224.10742320209</v>
       </c>
       <c r="J63" t="n">
-        <v>24807.66769913946</v>
+        <v>24807.67222880212</v>
       </c>
       <c r="K63" t="n">
-        <v>25681.28080428822</v>
+        <v>25681.28533395089</v>
       </c>
     </row>
     <row r="64">
@@ -22655,19 +22655,19 @@
         <v>136.88</v>
       </c>
       <c r="G64" t="n">
-        <v>-596.3742627470929</v>
+        <v>-596.3765355939904</v>
       </c>
       <c r="H64" t="n">
-        <v>24263.99772715311</v>
+        <v>24264</v>
       </c>
       <c r="I64" t="n">
-        <v>26430.77426274709</v>
+        <v>26430.77653559399</v>
       </c>
       <c r="J64" t="n">
-        <v>24838.75441983809</v>
+        <v>24838.75669268498</v>
       </c>
       <c r="K64" t="n">
-        <v>25856.02897133622</v>
+        <v>25856.03124418311</v>
       </c>
     </row>
     <row r="65">
@@ -22681,19 +22681,19 @@
         <v>136.78</v>
       </c>
       <c r="G65" t="n">
-        <v>-358.87218837818</v>
+        <v>-358.8749745205314</v>
       </c>
       <c r="H65" t="n">
-        <v>24262.91721385765</v>
+        <v>24262.92</v>
       </c>
       <c r="I65" t="n">
-        <v>26687.37218837818</v>
+        <v>26687.37497452053</v>
       </c>
       <c r="J65" t="n">
-        <v>24872.47755770869</v>
+        <v>24872.48034385104</v>
       </c>
       <c r="K65" t="n">
-        <v>26077.82484812009</v>
+        <v>26077.82763426244</v>
       </c>
     </row>
     <row r="66">
@@ -22707,19 +22707,19 @@
         <v>136.68</v>
       </c>
       <c r="G66" t="n">
-        <v>-262.1912957378263</v>
+        <v>-262.1921830140782</v>
       </c>
       <c r="H66" t="n">
-        <v>24261.69911272375</v>
+        <v>24261.7</v>
       </c>
       <c r="I66" t="n">
-        <v>27022.89129573783</v>
+        <v>27022.89218301408</v>
       </c>
       <c r="J66" t="n">
-        <v>24909.2962575657</v>
+        <v>24909.29714484195</v>
       </c>
       <c r="K66" t="n">
-        <v>26375.30930311094</v>
+        <v>26375.31019038719</v>
       </c>
     </row>
     <row r="67">
@@ -22733,19 +22733,19 @@
         <v>136.58</v>
       </c>
       <c r="G67" t="n">
-        <v>-432.1530169218822</v>
+        <v>-432.1517830182638</v>
       </c>
       <c r="H67" t="n">
-        <v>24260.17123390361</v>
+        <v>24260.17</v>
       </c>
       <c r="I67" t="n">
-        <v>27487.75301692188</v>
+        <v>27487.75178301826</v>
       </c>
       <c r="J67" t="n">
-        <v>24949.44789485205</v>
+        <v>24949.44666094844</v>
       </c>
       <c r="K67" t="n">
-        <v>26798.49456491139</v>
+        <v>26798.49333100778</v>
       </c>
     </row>
     <row r="68">
@@ -22759,19 +22759,19 @@
         <v>136.48</v>
       </c>
       <c r="G68" t="n">
-        <v>-217.5803986307801</v>
+        <v>-217.5839076015764</v>
       </c>
       <c r="H68" t="n">
-        <v>24258.39649102921</v>
+        <v>24258.4</v>
       </c>
       <c r="I68" t="n">
-        <v>28166.68039863078</v>
+        <v>28166.68390760157</v>
       </c>
       <c r="J68" t="n">
-        <v>24993.4712617816</v>
+        <v>24993.47477075239</v>
       </c>
       <c r="K68" t="n">
-        <v>27431.62840858764</v>
+        <v>27431.63191755843</v>
       </c>
     </row>
     <row r="69">
@@ -22785,19 +22785,19 @@
         <v>136.38</v>
       </c>
       <c r="G69" t="n">
-        <v>-474.3437010405396</v>
+        <v>-474.3441249793614</v>
       </c>
       <c r="H69" t="n">
-        <v>24256.21957606118</v>
+        <v>24256.22</v>
       </c>
       <c r="I69" t="n">
-        <v>29192.24370104054</v>
+        <v>29192.24412497936</v>
       </c>
       <c r="J69" t="n">
-        <v>25041.76641141674</v>
+        <v>25041.76683535556</v>
       </c>
       <c r="K69" t="n">
-        <v>28406.7266861544</v>
+        <v>28406.72711009323</v>
       </c>
     </row>
     <row r="70">
@@ -22811,19 +22811,19 @@
         <v>136.28</v>
       </c>
       <c r="G70" t="n">
-        <v>-38.38701688474976</v>
+        <v>-38.39073899564028</v>
       </c>
       <c r="H70" t="n">
-        <v>24253.47627788911</v>
+        <v>24253.48</v>
       </c>
       <c r="I70" t="n">
-        <v>30755.98701688475</v>
+        <v>30755.99073899564</v>
       </c>
       <c r="J70" t="n">
-        <v>25094.82026473033</v>
+        <v>25094.82398684122</v>
       </c>
       <c r="K70" t="n">
-        <v>29914.6837357951</v>
+        <v>29914.68745790599</v>
       </c>
     </row>
     <row r="71">
@@ -22837,19 +22837,19 @@
         <v>136.18</v>
       </c>
       <c r="G71" t="n">
-        <v>-328.106517867127</v>
+        <v>-328.1056057343521</v>
       </c>
       <c r="H71" t="n">
-        <v>24249.79091213277</v>
+        <v>24249.79</v>
       </c>
       <c r="I71" t="n">
-        <v>33107.90651786713</v>
+        <v>33107.90560573436</v>
       </c>
       <c r="J71" t="n">
-        <v>25153.02432006955</v>
+        <v>25153.02340793678</v>
       </c>
       <c r="K71" t="n">
-        <v>32204.7303461613</v>
+        <v>32204.72943402853</v>
       </c>
     </row>
     <row r="72">
@@ -22863,19 +22863,19 @@
         <v>136.08</v>
       </c>
       <c r="G72" t="n">
-        <v>15.2054471838419</v>
+        <v>15.20383599681372</v>
       </c>
       <c r="H72" t="n">
-        <v>24244.71838881297</v>
+        <v>24244.72</v>
       </c>
       <c r="I72" t="n">
-        <v>36534.89455281616</v>
+        <v>36534.89616400318</v>
       </c>
       <c r="J72" t="n">
-        <v>25216.84217392903</v>
+        <v>25216.84378511606</v>
       </c>
       <c r="K72" t="n">
-        <v>35562.85224478443</v>
+        <v>35562.85385597146</v>
       </c>
     </row>
     <row r="73">
@@ -22889,19 +22889,19 @@
         <v>135.98</v>
       </c>
       <c r="G73" t="n">
-        <v>10.98983901194879</v>
+        <v>10.9895091986109</v>
       </c>
       <c r="H73" t="n">
-        <v>24237.63967018666</v>
+        <v>24237.64</v>
       </c>
       <c r="I73" t="n">
-        <v>41309.51016098805</v>
+        <v>41309.51049080139</v>
       </c>
       <c r="J73" t="n">
-        <v>25286.73729875178</v>
+        <v>25286.73762856512</v>
       </c>
       <c r="K73" t="n">
-        <v>40260.5279225381</v>
+        <v>40260.52825235144</v>
       </c>
     </row>
     <row r="74">
@@ -22915,19 +22915,19 @@
         <v>135.88</v>
       </c>
       <c r="G74" t="n">
-        <v>-240.486087600977</v>
+        <v>-240.4878219926904</v>
       </c>
       <c r="H74" t="n">
-        <v>24227.61826560828</v>
+        <v>24227.62</v>
       </c>
       <c r="I74" t="n">
-        <v>47609.18608760097</v>
+        <v>47609.18782199269</v>
       </c>
       <c r="J74" t="n">
-        <v>25363.07140998605</v>
+        <v>25363.07314437777</v>
       </c>
       <c r="K74" t="n">
-        <v>46473.89319514461</v>
+        <v>46473.89492953633</v>
       </c>
     </row>
     <row r="75">
@@ -22941,19 +22941,19 @@
         <v>135.78</v>
       </c>
       <c r="G75" t="n">
-        <v>125.6691488157085</v>
+        <v>125.6694235899777</v>
       </c>
       <c r="H75" t="n">
-        <v>24213.82027477426</v>
+        <v>24213.82</v>
       </c>
       <c r="I75" t="n">
-        <v>55418.63085118429</v>
+        <v>55418.63057641003</v>
       </c>
       <c r="J75" t="n">
-        <v>25446.58085880724</v>
+        <v>25446.58058403298</v>
       </c>
       <c r="K75" t="n">
-        <v>54186.08621387219</v>
+        <v>54186.08593909792</v>
       </c>
     </row>
     <row r="76">
@@ -22967,19 +22967,19 @@
         <v>135.68</v>
       </c>
       <c r="G76" t="n">
-        <v>-1044.273110955946</v>
+        <v>-1044.270662655741</v>
       </c>
       <c r="H76" t="n">
-        <v>24195.0424483002</v>
+        <v>24195.04</v>
       </c>
       <c r="I76" t="n">
-        <v>64436.17311095595</v>
+        <v>64436.17066265574</v>
       </c>
       <c r="J76" t="n">
-        <v>25537.98592480601</v>
+        <v>25537.98347650581</v>
       </c>
       <c r="K76" t="n">
-        <v>63093.50992830192</v>
+        <v>63093.50748000172</v>
       </c>
     </row>
     <row r="77">
@@ -22993,19 +22993,19 @@
         <v>135.58</v>
       </c>
       <c r="G77" t="n">
-        <v>-333.9010530837113</v>
+        <v>-333.9017906085646</v>
       </c>
       <c r="H77" t="n">
-        <v>24170.56926247515</v>
+        <v>24170.57</v>
       </c>
       <c r="I77" t="n">
-        <v>74007.80105308371</v>
+        <v>74007.80179060856</v>
       </c>
       <c r="J77" t="n">
-        <v>25638.97789138934</v>
+        <v>25638.97862891418</v>
       </c>
       <c r="K77" t="n">
-        <v>72539.74098919696</v>
+        <v>72539.74172672181</v>
       </c>
     </row>
     <row r="78">
@@ -23019,19 +23019,19 @@
         <v>135.48</v>
       </c>
       <c r="G78" t="n">
-        <v>419.6849089021271</v>
+        <v>419.680262072914</v>
       </c>
       <c r="H78" t="n">
-        <v>24139.55535317079</v>
+        <v>24139.56</v>
       </c>
       <c r="I78" t="n">
-        <v>83099.51509109787</v>
+        <v>83099.51973792708</v>
       </c>
       <c r="J78" t="n">
-        <v>25751.83581697066</v>
+        <v>25751.84046379987</v>
       </c>
       <c r="K78" t="n">
-        <v>81487.64791501428</v>
+        <v>81487.6525618435</v>
       </c>
     </row>
     <row r="79">
@@ -23045,19 +23045,19 @@
         <v>135.38</v>
       </c>
       <c r="G79" t="n">
-        <v>954.9103250145999</v>
+        <v>954.9148157017626</v>
       </c>
       <c r="H79" t="n">
-        <v>24101.36449068717</v>
+        <v>24101.36</v>
       </c>
       <c r="I79" t="n">
-        <v>90346.7896749854</v>
+        <v>90346.78518429823</v>
       </c>
       <c r="J79" t="n">
-        <v>25880.22868716476</v>
+        <v>25880.2241964776</v>
       </c>
       <c r="K79" t="n">
-        <v>88568.3900744483</v>
+        <v>88568.38558376112</v>
       </c>
     </row>
     <row r="80">
@@ -23071,19 +23071,19 @@
         <v>135.28</v>
       </c>
       <c r="G80" t="n">
-        <v>-448.2646820274531</v>
+        <v>-448.26045276472</v>
       </c>
       <c r="H80" t="n">
-        <v>24057.11422926274</v>
+        <v>24057.11</v>
       </c>
       <c r="I80" t="n">
-        <v>94311.36468202746</v>
+        <v>94311.36045276473</v>
       </c>
       <c r="J80" t="n">
-        <v>26031.71213236988</v>
+        <v>26031.70790310714</v>
       </c>
       <c r="K80" t="n">
-        <v>92337.25884266369</v>
+        <v>92337.25461340095</v>
       </c>
     </row>
     <row r="81">
@@ -23097,19 +23097,19 @@
         <v>135.18</v>
       </c>
       <c r="G81" t="n">
-        <v>809.115553890384</v>
+        <v>809.115783113215</v>
       </c>
       <c r="H81" t="n">
-        <v>24009.49022922284</v>
+        <v>24009.49</v>
       </c>
       <c r="I81" t="n">
-        <v>94059.38444610962</v>
+        <v>94059.38421688678</v>
       </c>
       <c r="J81" t="n">
-        <v>26219.47797009807</v>
+        <v>26219.47774087522</v>
       </c>
       <c r="K81" t="n">
-        <v>91849.88556622883</v>
+        <v>91849.885337006</v>
       </c>
     </row>
     <row r="82">
@@ -23123,19 +23123,19 @@
         <v>135.08</v>
       </c>
       <c r="G82" t="n">
-        <v>-239.2863041538221</v>
+        <v>-239.2880676349014</v>
       </c>
       <c r="H82" t="n">
-        <v>23961.17823651893</v>
+        <v>23961.18</v>
       </c>
       <c r="I82" t="n">
-        <v>89728.18630415382</v>
+        <v>89728.1880676349</v>
       </c>
       <c r="J82" t="n">
-        <v>26464.53754670743</v>
+        <v>26464.5393101885</v>
       </c>
       <c r="K82" t="n">
-        <v>87225.28281794238</v>
+        <v>87225.28458142345</v>
       </c>
     </row>
     <row r="83">
@@ -23149,19 +23149,19 @@
         <v>134.98</v>
       </c>
       <c r="G83" t="n">
-        <v>-800.4941224317445</v>
+        <v>-800.4975198189641</v>
       </c>
       <c r="H83" t="n">
-        <v>23915.3066026128</v>
+        <v>23915.31</v>
       </c>
       <c r="I83" t="n">
-        <v>82456.19412243174</v>
+        <v>82456.19751981896</v>
       </c>
       <c r="J83" t="n">
-        <v>26802.92599587788</v>
+        <v>26802.92939326509</v>
       </c>
       <c r="K83" t="n">
-        <v>79568.97562618672</v>
+        <v>79568.97902357392</v>
       </c>
     </row>
     <row r="84">
@@ -23175,19 +23175,19 @@
         <v>134.88</v>
       </c>
       <c r="G84" t="n">
-        <v>-910.3065523035766</v>
+        <v>-910.3059477110364</v>
       </c>
       <c r="H84" t="n">
-        <v>23874.62060459255</v>
+        <v>23874.62</v>
       </c>
       <c r="I84" t="n">
-        <v>73771.40655230358</v>
+        <v>73771.40594771104</v>
       </c>
       <c r="J84" t="n">
-        <v>27295.96963063289</v>
+        <v>27295.96902604034</v>
       </c>
       <c r="K84" t="n">
-        <v>70350.39217390463</v>
+        <v>70350.39156931208</v>
       </c>
     </row>
     <row r="85">
@@ -23201,19 +23201,19 @@
         <v>134.78</v>
       </c>
       <c r="G85" t="n">
-        <v>140.1619977827868</v>
+        <v>140.1659041687672</v>
       </c>
       <c r="H85" t="n">
-        <v>23839.91390638598</v>
+        <v>23839.91</v>
       </c>
       <c r="I85" t="n">
-        <v>65087.83800221721</v>
+        <v>65087.83409583123</v>
       </c>
       <c r="J85" t="n">
-        <v>28044.86469063379</v>
+        <v>28044.86078424781</v>
       </c>
       <c r="K85" t="n">
-        <v>60883.1537462831</v>
+        <v>60883.14983989713</v>
       </c>
     </row>
     <row r="86">
@@ -23227,19 +23227,19 @@
         <v>134.68</v>
       </c>
       <c r="G86" t="n">
-        <v>297.0852744690856</v>
+        <v>297.0899954391862</v>
       </c>
       <c r="H86" t="n">
-        <v>23810.8947209701</v>
+        <v>23810.89</v>
       </c>
       <c r="I86" t="n">
-        <v>57527.91472553091</v>
+        <v>57527.91000456081</v>
       </c>
       <c r="J86" t="n">
-        <v>29211.51040907225</v>
+        <v>29211.50568810214</v>
       </c>
       <c r="K86" t="n">
-        <v>52127.50248034927</v>
+        <v>52127.49775937917</v>
       </c>
     </row>
     <row r="87">
@@ -23253,19 +23253,19 @@
         <v>134.58</v>
       </c>
       <c r="G87" t="n">
-        <v>790.0524703199771</v>
+        <v>790.0560174259008</v>
       </c>
       <c r="H87" t="n">
-        <v>23786.85354710593</v>
+        <v>23786.85</v>
       </c>
       <c r="I87" t="n">
-        <v>51915.14752968002</v>
+        <v>51915.1439825741</v>
       </c>
       <c r="J87" t="n">
-        <v>31038.00755892611</v>
+        <v>31038.00401182018</v>
       </c>
       <c r="K87" t="n">
-        <v>44664.1430686315</v>
+        <v>44664.13952152558</v>
       </c>
     </row>
     <row r="88">
@@ -23279,19 +23279,19 @@
         <v>134.48</v>
       </c>
       <c r="G88" t="n">
-        <v>694.1590207966437</v>
+        <v>694.161567210067</v>
       </c>
       <c r="H88" t="n">
-        <v>23766.62254641343</v>
+        <v>23766.62</v>
       </c>
       <c r="I88" t="n">
-        <v>48818.24097920336</v>
+        <v>48818.23843278993</v>
       </c>
       <c r="J88" t="n">
-        <v>33854.37404891378</v>
+        <v>33854.37150250035</v>
       </c>
       <c r="K88" t="n">
-        <v>38730.59600467066</v>
+        <v>38730.59345825723</v>
       </c>
     </row>
     <row r="89">
@@ -23305,19 +23305,19 @@
         <v>134.38</v>
       </c>
       <c r="G89" t="n">
-        <v>712.4446502949941</v>
+        <v>712.4466391738824</v>
       </c>
       <c r="H89" t="n">
-        <v>23748.59198887889</v>
+        <v>23748.59</v>
       </c>
       <c r="I89" t="n">
-        <v>48607.155349705</v>
+        <v>48607.15336082612</v>
       </c>
       <c r="J89" t="n">
-        <v>38061.13300739953</v>
+        <v>38061.13101852063</v>
       </c>
       <c r="K89" t="n">
-        <v>34294.6884307342</v>
+        <v>34294.68644185532</v>
       </c>
     </row>
     <row r="90">
@@ -23331,19 +23331,19 @@
         <v>134.28</v>
       </c>
       <c r="G90" t="n">
-        <v>1217.652575671607</v>
+        <v>1217.648954863987</v>
       </c>
       <c r="H90" t="n">
-        <v>23730.78637919238</v>
+        <v>23730.79</v>
       </c>
       <c r="I90" t="n">
-        <v>51492.84742432839</v>
+        <v>51492.85104513601</v>
       </c>
       <c r="J90" t="n">
-        <v>44072.88424501078</v>
+        <v>44072.8878658184</v>
       </c>
       <c r="K90" t="n">
-        <v>31150.80029911123</v>
+        <v>31150.80391991885</v>
       </c>
     </row>
     <row r="91">
@@ -23357,19 +23357,19 @@
         <v>134.18</v>
       </c>
       <c r="G91" t="n">
-        <v>-1018.542652055869</v>
+        <v>-1018.546056889958</v>
       </c>
       <c r="H91" t="n">
-        <v>23711.26659516591</v>
+        <v>23711.27</v>
       </c>
       <c r="I91" t="n">
-        <v>57522.44265205587</v>
+        <v>57522.44605688996</v>
       </c>
       <c r="J91" t="n">
-        <v>52217.31744920356</v>
+        <v>52217.32085403765</v>
       </c>
       <c r="K91" t="n">
-        <v>29016.4261813831</v>
+        <v>29016.42958621719</v>
       </c>
     </row>
     <row r="92">
@@ -23383,19 +23383,19 @@
         <v>134.08</v>
       </c>
       <c r="G92" t="n">
-        <v>-298.4727983798948</v>
+        <v>-298.4680209723156</v>
       </c>
       <c r="H92" t="n">
-        <v>23688.24477740759</v>
+        <v>23688.24</v>
       </c>
       <c r="I92" t="n">
-        <v>66518.67279837989</v>
+        <v>66518.66802097231</v>
       </c>
       <c r="J92" t="n">
-        <v>62599.3093526244</v>
+        <v>62599.30457521681</v>
       </c>
       <c r="K92" t="n">
-        <v>27607.63120211365</v>
+        <v>27607.62642470606</v>
       </c>
     </row>
     <row r="93">
@@ -23409,19 +23409,19 @@
         <v>133.98</v>
       </c>
       <c r="G93" t="n">
-        <v>-1230.028411335763</v>
+        <v>-1230.031974175174</v>
       </c>
       <c r="H93" t="n">
-        <v>23659.33643716058</v>
+        <v>23659.34</v>
       </c>
       <c r="I93" t="n">
-        <v>77981.12841133577</v>
+        <v>77981.13197417518</v>
       </c>
       <c r="J93" t="n">
-        <v>74957.25385282602</v>
+        <v>74957.25741566544</v>
       </c>
       <c r="K93" t="n">
-        <v>26683.22583631853</v>
+        <v>26683.22939915795</v>
       </c>
     </row>
     <row r="94">
@@ -23435,19 +23435,19 @@
         <v>133.88</v>
       </c>
       <c r="G94" t="n">
-        <v>-273.3017879428517</v>
+        <v>-273.3013149968028</v>
       </c>
       <c r="H94" t="n">
-        <v>23622.40047294605</v>
+        <v>23622.4</v>
       </c>
       <c r="I94" t="n">
-        <v>90988.00178794285</v>
+        <v>90988.0013149968</v>
       </c>
       <c r="J94" t="n">
-        <v>88548.14871889887</v>
+        <v>88548.14824595282</v>
       </c>
       <c r="K94" t="n">
-        <v>26062.26232173021</v>
+        <v>26062.26184878415</v>
       </c>
     </row>
     <row r="95">
@@ -23461,19 +23461,19 @@
         <v>133.78</v>
       </c>
       <c r="G95" t="n">
-        <v>-2234.005892268789</v>
+        <v>-2234.006854566775</v>
       </c>
       <c r="H95" t="n">
-        <v>23576.349037702</v>
+        <v>23576.35</v>
       </c>
       <c r="I95" t="n">
-        <v>104129.0058922688</v>
+        <v>104129.0068545668</v>
       </c>
       <c r="J95" t="n">
-        <v>102083.2126717261</v>
+        <v>102083.2136340241</v>
       </c>
       <c r="K95" t="n">
-        <v>25622.14635314</v>
+        <v>25622.147315438</v>
       </c>
     </row>
     <row r="96">
@@ -23487,19 +23487,19 @@
         <v>133.68</v>
       </c>
       <c r="G96" t="n">
-        <v>292.4749688581651</v>
+        <v>292.4787967202137</v>
       </c>
       <c r="H96" t="n">
-        <v>23520.88382786206</v>
+        <v>23520.88</v>
       </c>
       <c r="I96" t="n">
-        <v>115506.5250311418</v>
+        <v>115506.5212032798</v>
       </c>
       <c r="J96" t="n">
-        <v>113741.1019453441</v>
+        <v>113741.0981174821</v>
       </c>
       <c r="K96" t="n">
-        <v>25286.30739699761</v>
+        <v>25286.30356913555</v>
       </c>
     </row>
     <row r="97">
@@ -23513,19 +23513,19 @@
         <v>133.58</v>
       </c>
       <c r="G97" t="n">
-        <v>-520.6218537333916</v>
+        <v>-520.6238713186176</v>
       </c>
       <c r="H97" t="n">
-        <v>23456.82798241478</v>
+        <v>23456.83</v>
       </c>
       <c r="I97" t="n">
-        <v>122940.6218537334</v>
+        <v>122940.6238713186</v>
       </c>
       <c r="J97" t="n">
-        <v>121386.8435674175</v>
+        <v>121386.8455850027</v>
       </c>
       <c r="K97" t="n">
-        <v>25010.60417948982</v>
+        <v>25010.60619707504</v>
       </c>
     </row>
     <row r="98">
@@ -23539,19 +23539,19 @@
         <v>133.48</v>
       </c>
       <c r="G98" t="n">
-        <v>-710.6360194476147</v>
+        <v>-710.6350694845314</v>
       </c>
       <c r="H98" t="n">
-        <v>23387.77094996308</v>
+        <v>23387.77</v>
       </c>
       <c r="I98" t="n">
-        <v>124617.6360194476</v>
+        <v>124617.6350694845</v>
       </c>
       <c r="J98" t="n">
-        <v>123232.1756122969</v>
+        <v>123232.1746623338</v>
       </c>
       <c r="K98" t="n">
-        <v>24773.22779435893</v>
+        <v>24773.22684439585</v>
       </c>
     </row>
     <row r="99">
@@ -23565,19 +23565,19 @@
         <v>133.38</v>
       </c>
       <c r="G99" t="n">
-        <v>1485.597162367121</v>
+        <v>1485.59533276521</v>
       </c>
       <c r="H99" t="n">
-        <v>23317.84817039809</v>
+        <v>23317.85</v>
       </c>
       <c r="I99" t="n">
-        <v>120024.4028376329</v>
+        <v>120024.4046672348</v>
       </c>
       <c r="J99" t="n">
-        <v>118778.0624544752</v>
+        <v>118778.0642840771</v>
       </c>
       <c r="K99" t="n">
-        <v>24564.18458277292</v>
+        <v>24564.18641237482</v>
       </c>
     </row>
     <row r="100">
@@ -23591,19 +23591,19 @@
         <v>133.28</v>
       </c>
       <c r="G100" t="n">
-        <v>1732.538203689779</v>
+        <v>1732.53526796661</v>
       </c>
       <c r="H100" t="n">
-        <v>23251.27706427683</v>
+        <v>23251.28</v>
       </c>
       <c r="I100" t="n">
-        <v>110273.4617963102</v>
+        <v>110273.4647320334</v>
       </c>
       <c r="J100" t="n">
-        <v>109145.0708173719</v>
+        <v>109145.0737530951</v>
       </c>
       <c r="K100" t="n">
-        <v>24379.66452047916</v>
+        <v>24379.66745620233</v>
       </c>
     </row>
     <row r="101">
@@ -23617,19 +23617,19 @@
         <v>133.18</v>
       </c>
       <c r="G101" t="n">
-        <v>299.0577066347614</v>
+        <v>299.0574430260895</v>
       </c>
       <c r="H101" t="n">
-        <v>23192.70973639133</v>
+        <v>23192.71</v>
       </c>
       <c r="I101" t="n">
-        <v>97405.14229336524</v>
+        <v>97405.14255697391</v>
       </c>
       <c r="J101" t="n">
-        <v>96378.37199812694</v>
+        <v>96378.37226173561</v>
       </c>
       <c r="K101" t="n">
-        <v>24219.47750112756</v>
+        <v>24219.47776473624</v>
       </c>
     </row>
     <row r="102">
@@ -23643,19 +23643,19 @@
         <v>133.08</v>
       </c>
       <c r="G102" t="n">
-        <v>-619.4066308412148</v>
+        <v>-619.4084844890749</v>
       </c>
       <c r="H102" t="n">
-        <v>23144.68814635215</v>
+        <v>23144.69</v>
       </c>
       <c r="I102" t="n">
-        <v>83478.50663084122</v>
+        <v>83478.50848448908</v>
       </c>
       <c r="J102" t="n">
-        <v>82540.2087830291</v>
+        <v>82540.21063667694</v>
       </c>
       <c r="K102" t="n">
-        <v>24082.98469757122</v>
+        <v>24082.98655121908</v>
       </c>
     </row>
     <row r="103">
@@ -23669,19 +23669,19 @@
         <v>132.98</v>
       </c>
       <c r="G103" t="n">
-        <v>741.5928337207733</v>
+        <v>741.5970937690581</v>
       </c>
       <c r="H103" t="n">
-        <v>23106.65426004829</v>
+        <v>23106.65</v>
       </c>
       <c r="I103" t="n">
-        <v>70108.30716627922</v>
+        <v>70108.30290623094</v>
       </c>
       <c r="J103" t="n">
-        <v>69247.60761248809</v>
+        <v>69247.60335243981</v>
       </c>
       <c r="K103" t="n">
-        <v>23967.35375686607</v>
+        <v>23967.34949681778</v>
       </c>
     </row>
     <row r="104">
@@ -23695,19 +23695,19 @@
         <v>132.88</v>
       </c>
       <c r="G104" t="n">
-        <v>490.599166789485</v>
+        <v>490.6013548043265</v>
       </c>
       <c r="H104" t="n">
-        <v>23077.38218801484</v>
+        <v>23077.38</v>
       </c>
       <c r="I104" t="n">
-        <v>58356.60083321051</v>
+        <v>58356.59864519567</v>
       </c>
       <c r="J104" t="n">
-        <v>57564.35989312951</v>
+        <v>57564.35770511467</v>
       </c>
       <c r="K104" t="n">
-        <v>23869.62415938352</v>
+        <v>23869.62197136868</v>
       </c>
     </row>
     <row r="105">
@@ -23721,19 +23721,19 @@
         <v>132.78</v>
       </c>
       <c r="G105" t="n">
-        <v>-535.5975089164567</v>
+        <v>-535.5975022240746</v>
       </c>
       <c r="H105" t="n">
-        <v>23056.15000669238</v>
+        <v>23056.15</v>
       </c>
       <c r="I105" t="n">
-        <v>48758.49750891646</v>
+        <v>48758.49750222408</v>
       </c>
       <c r="J105" t="n">
-        <v>48026.95365226395</v>
+        <v>48026.95364557157</v>
       </c>
       <c r="K105" t="n">
-        <v>23787.69574867812</v>
+        <v>23787.69574198574</v>
       </c>
     </row>
     <row r="106">
@@ -23747,19 +23747,19 @@
         <v>132.68</v>
       </c>
       <c r="G106" t="n">
-        <v>-195.3476995438614</v>
+        <v>-195.3520048458595</v>
       </c>
       <c r="H106" t="n">
-        <v>23041.17569469801</v>
+        <v>23041.18</v>
       </c>
       <c r="I106" t="n">
-        <v>41407.84769954386</v>
+        <v>41407.85200484586</v>
       </c>
       <c r="J106" t="n">
-        <v>40730.36069530147</v>
+        <v>40730.36500060346</v>
       </c>
       <c r="K106" t="n">
-        <v>23718.6651828854</v>
+        <v>23718.6694881874</v>
       </c>
     </row>
     <row r="107">
@@ -23773,19 +23773,19 @@
         <v>132.58</v>
       </c>
       <c r="G107" t="n">
-        <v>1014.376741196109</v>
+        <v>1014.37679110287</v>
       </c>
       <c r="H107" t="n">
-        <v>23030.15004990677</v>
+        <v>23030.15</v>
       </c>
       <c r="I107" t="n">
-        <v>36088.02325880389</v>
+        <v>36088.02320889713</v>
       </c>
       <c r="J107" t="n">
-        <v>35458.87800450102</v>
+        <v>35458.87795459425</v>
       </c>
       <c r="K107" t="n">
-        <v>23659.29815362755</v>
+        <v>23659.29810372079</v>
       </c>
     </row>
     <row r="108">
@@ -23799,19 +23799,19 @@
         <v>132.48</v>
       </c>
       <c r="G108" t="n">
-        <v>1375.151857357534</v>
+        <v>1375.152737239256</v>
       </c>
       <c r="H108" t="n">
-        <v>23021.71087988172</v>
+        <v>23021.71</v>
       </c>
       <c r="I108" t="n">
-        <v>32417.64814264247</v>
+        <v>32417.64726276075</v>
       </c>
       <c r="J108" t="n">
-        <v>31831.89981751545</v>
+        <v>31831.89893763373</v>
       </c>
       <c r="K108" t="n">
-        <v>23607.46223268421</v>
+        <v>23607.46135280249</v>
       </c>
     </row>
     <row r="109">
@@ -23825,19 +23825,19 @@
         <v>132.38</v>
       </c>
       <c r="G109" t="n">
-        <v>717.9045956399677</v>
+        <v>717.900666969821</v>
       </c>
       <c r="H109" t="n">
-        <v>23015.45607132985</v>
+        <v>23015.46</v>
       </c>
       <c r="I109" t="n">
-        <v>29975.19540436003</v>
+        <v>29975.19933303018</v>
       </c>
       <c r="J109" t="n">
-        <v>29428.54499393664</v>
+        <v>29428.54892260678</v>
       </c>
       <c r="K109" t="n">
-        <v>23562.10955288914</v>
+        <v>23562.11348155929</v>
       </c>
     </row>
     <row r="110">
@@ -23851,19 +23851,19 @@
         <v>132.28</v>
       </c>
       <c r="G110" t="n">
-        <v>918.1144763769626</v>
+        <v>918.1121199581576</v>
       </c>
       <c r="H110" t="n">
-        <v>23010.7376435812</v>
+        <v>23010.74</v>
       </c>
       <c r="I110" t="n">
-        <v>28381.38552362304</v>
+        <v>28381.38788004184</v>
       </c>
       <c r="J110" t="n">
-        <v>27870.07865377862</v>
+        <v>27870.08101019742</v>
       </c>
       <c r="K110" t="n">
-        <v>23522.0475406183</v>
+        <v>23522.0498970371</v>
       </c>
     </row>
     <row r="111">
@@ -23877,19 +23877,19 @@
         <v>132.18</v>
       </c>
       <c r="G111" t="n">
-        <v>364.5336519851335</v>
+        <v>364.5317023649623</v>
       </c>
       <c r="H111" t="n">
-        <v>23007.03805037983</v>
+        <v>23007.04</v>
       </c>
       <c r="I111" t="n">
-        <v>27339.06634801487</v>
+        <v>27339.06829763504</v>
       </c>
       <c r="J111" t="n">
-        <v>26859.81042254122</v>
+        <v>26859.8123721614</v>
       </c>
       <c r="K111" t="n">
-        <v>23486.29690857145</v>
+        <v>23486.29885819162</v>
       </c>
     </row>
     <row r="112">
@@ -23903,19 +23903,19 @@
         <v>132.08</v>
       </c>
       <c r="G112" t="n">
-        <v>-28.30056289857748</v>
+        <v>-28.2979028168993</v>
       </c>
       <c r="H112" t="n">
-        <v>23004.24266008168</v>
+        <v>23004.24</v>
       </c>
       <c r="I112" t="n">
-        <v>26639.00056289858</v>
+        <v>26638.9979028169</v>
       </c>
       <c r="J112" t="n">
-        <v>26188.89645963996</v>
+        <v>26188.89379955828</v>
       </c>
       <c r="K112" t="n">
-        <v>23454.34957654734</v>
+        <v>23454.34691646566</v>
       </c>
     </row>
     <row r="113">
@@ -23929,19 +23929,19 @@
         <v>131.98</v>
       </c>
       <c r="G113" t="n">
-        <v>-364.0100308202018</v>
+        <v>-364.0138200035581</v>
       </c>
       <c r="H113" t="n">
-        <v>23002.09621081664</v>
+        <v>23002.1</v>
       </c>
       <c r="I113" t="n">
-        <v>26145.6100308202</v>
+        <v>26145.61382000356</v>
       </c>
       <c r="J113" t="n">
-        <v>25722.09547662278</v>
+        <v>25722.09926580614</v>
       </c>
       <c r="K113" t="n">
-        <v>23425.61344956775</v>
+        <v>23425.61723875111</v>
       </c>
     </row>
     <row r="114">
@@ -23955,19 +23955,19 @@
         <v>131.88</v>
       </c>
       <c r="G114" t="n">
-        <v>-117.9511374985887</v>
+        <v>-117.9472118471494</v>
       </c>
       <c r="H114" t="n">
-        <v>23000.27392565144</v>
+        <v>23000.27</v>
       </c>
       <c r="I114" t="n">
-        <v>25776.85113749859</v>
+        <v>25776.84721184715</v>
       </c>
       <c r="J114" t="n">
-        <v>25377.65351493757</v>
+        <v>25377.64958928613</v>
       </c>
       <c r="K114" t="n">
-        <v>23399.47410393483</v>
+        <v>23399.47017828339</v>
       </c>
     </row>
     <row r="115">
@@ -23981,19 +23981,19 @@
         <v>131.78</v>
       </c>
       <c r="G115" t="n">
-        <v>-152.8439196473228</v>
+        <v>-152.8400318774911</v>
       </c>
       <c r="H115" t="n">
-        <v>22998.60388776983</v>
+        <v>22998.6</v>
       </c>
       <c r="I115" t="n">
-        <v>25485.64391964732</v>
+        <v>25485.64003187749</v>
       </c>
       <c r="J115" t="n">
-        <v>25108.74073614763</v>
+        <v>25108.7368483778</v>
       </c>
       <c r="K115" t="n">
-        <v>23375.5095025123</v>
+        <v>23375.50561474247</v>
       </c>
     </row>
     <row r="116">
@@ -24007,19 +24007,19 @@
         <v>131.68</v>
       </c>
       <c r="G116" t="n">
-        <v>-137.9889494714953</v>
+        <v>-137.9922415451656</v>
       </c>
       <c r="H116" t="n">
-        <v>22997.11670792633</v>
+        <v>22997.12</v>
       </c>
       <c r="I116" t="n">
-        <v>25245.78894947149</v>
+        <v>25245.79224154516</v>
       </c>
       <c r="J116" t="n">
-        <v>24889.37456590213</v>
+        <v>24889.3778579758</v>
       </c>
       <c r="K116" t="n">
-        <v>23353.53340457795</v>
+        <v>23353.53669665162</v>
       </c>
     </row>
     <row r="117">
@@ -24033,19 +24033,19 @@
         <v>131.58</v>
       </c>
       <c r="G117" t="n">
-        <v>96.40476015530294</v>
+        <v>96.40012903301249</v>
       </c>
       <c r="H117" t="n">
-        <v>22995.69536887771</v>
+        <v>22995.7</v>
       </c>
       <c r="I117" t="n">
-        <v>25042.3952398447</v>
+        <v>25042.39987096699</v>
       </c>
       <c r="J117" t="n">
-        <v>24704.852739522</v>
+        <v>24704.85737064429</v>
       </c>
       <c r="K117" t="n">
-        <v>23333.24007106022</v>
+        <v>23333.24470218251</v>
       </c>
     </row>
     <row r="118">
@@ -24059,19 +24059,19 @@
         <v>131.48</v>
       </c>
       <c r="G118" t="n">
-        <v>-622.1630938380913</v>
+        <v>-622.1644686288491</v>
       </c>
       <c r="H118" t="n">
-        <v>22994.55862520924</v>
+        <v>22994.56</v>
       </c>
       <c r="I118" t="n">
-        <v>24866.96309383809</v>
+        <v>24866.96446862885</v>
       </c>
       <c r="J118" t="n">
-        <v>24546.84039426616</v>
+        <v>24546.84176905692</v>
       </c>
       <c r="K118" t="n">
-        <v>23314.68342232909</v>
+        <v>23314.68479711984</v>
       </c>
     </row>
     <row r="119">
@@ -24085,19 +24085,19 @@
         <v>131.38</v>
       </c>
       <c r="G119" t="n">
-        <v>-690.3121216840518</v>
+        <v>-690.3092134957369</v>
       </c>
       <c r="H119" t="n">
-        <v>22993.79290818832</v>
+        <v>22993.79</v>
       </c>
       <c r="I119" t="n">
-        <v>24714.01212168405</v>
+        <v>24714.00921349574</v>
       </c>
       <c r="J119" t="n">
-        <v>24410.00160505836</v>
+        <v>24409.99869687004</v>
       </c>
       <c r="K119" t="n">
-        <v>23297.80542465495</v>
+        <v>23297.80251646664</v>
       </c>
     </row>
     <row r="120">
@@ -24111,19 +24111,19 @@
         <v>131.28</v>
       </c>
       <c r="G120" t="n">
-        <v>-381.1098143708587</v>
+        <v>-381.1130215676822</v>
       </c>
       <c r="H120" t="n">
-        <v>22993.04679280318</v>
+        <v>22993.05</v>
       </c>
       <c r="I120" t="n">
-        <v>24579.30981437086</v>
+        <v>24579.31302156768</v>
       </c>
       <c r="J120" t="n">
-        <v>24290.23088990601</v>
+        <v>24290.23409710284</v>
       </c>
       <c r="K120" t="n">
-        <v>23282.12762560055</v>
+        <v>23282.13083279737</v>
       </c>
     </row>
     <row r="121">
@@ -24137,19 +24137,19 @@
         <v>131.18</v>
       </c>
       <c r="G121" t="n">
-        <v>-846.6610922054715</v>
+        <v>-846.6652649513962</v>
       </c>
       <c r="H121" t="n">
-        <v>22992.43582725407</v>
+        <v>22992.44</v>
       </c>
       <c r="I121" t="n">
-        <v>24460.06109220547</v>
+        <v>24460.0652649514</v>
       </c>
       <c r="J121" t="n">
-        <v>24184.84521204595</v>
+        <v>24184.84938479187</v>
       </c>
       <c r="K121" t="n">
-        <v>23267.65353000825</v>
+        <v>23267.65770275418</v>
       </c>
     </row>
     <row r="122">
@@ -24163,19 +24163,19 @@
         <v>131.08</v>
       </c>
       <c r="G122" t="n">
-        <v>-649.5028613425275</v>
+        <v>-649.503790977571</v>
       </c>
       <c r="H122" t="n">
-        <v>22991.98907036496</v>
+        <v>22991.99</v>
       </c>
       <c r="I122" t="n">
-        <v>24354.00286134253</v>
+        <v>24354.00379097757</v>
       </c>
       <c r="J122" t="n">
-        <v>24091.68059849458</v>
+        <v>24091.68152812962</v>
       </c>
       <c r="K122" t="n">
-        <v>23254.31307542318</v>
+        <v>23254.31400505822</v>
       </c>
     </row>
     <row r="123">
@@ -24189,19 +24189,19 @@
         <v>130.98</v>
       </c>
       <c r="G123" t="n">
-        <v>-574.6909183196149</v>
+        <v>-574.6905275940626</v>
       </c>
       <c r="H123" t="n">
-        <v>22991.52039072555</v>
+        <v>22991.52</v>
       </c>
       <c r="I123" t="n">
-        <v>24259.09091831962</v>
+        <v>24259.09052759406</v>
       </c>
       <c r="J123" t="n">
-        <v>24008.78078452384</v>
+        <v>24008.78039379829</v>
       </c>
       <c r="K123" t="n">
-        <v>23241.83219130692</v>
+        <v>23241.83180058136</v>
       </c>
     </row>
     <row r="124">
@@ -24215,19 +24215,19 @@
         <v>130.88</v>
       </c>
       <c r="G124" t="n">
-        <v>-472.5160304864985</v>
+        <v>-472.5138297918711</v>
       </c>
       <c r="H124" t="n">
-        <v>22991.05220069463</v>
+        <v>22991.05</v>
       </c>
       <c r="I124" t="n">
-        <v>24173.8160304865</v>
+        <v>24173.81382979187</v>
       </c>
       <c r="J124" t="n">
-        <v>23934.71476792562</v>
+        <v>23934.71256723099</v>
       </c>
       <c r="K124" t="n">
-        <v>23230.1550592093</v>
+        <v>23230.15285851468</v>
       </c>
     </row>
     <row r="125">
@@ -24241,19 +24241,19 @@
         <v>130.78</v>
       </c>
       <c r="G125" t="n">
-        <v>-429.5071226502841</v>
+        <v>-429.5077942762509</v>
       </c>
       <c r="H125" t="n">
-        <v>22990.58932837403</v>
+        <v>22990.59</v>
       </c>
       <c r="I125" t="n">
-        <v>24096.90712265029</v>
+        <v>24096.90779427625</v>
       </c>
       <c r="J125" t="n">
-        <v>23868.28124869919</v>
+        <v>23868.28192032516</v>
       </c>
       <c r="K125" t="n">
-        <v>23219.21673170063</v>
+        <v>23219.21740332659</v>
       </c>
     </row>
     <row r="126">
@@ -24267,19 +24267,19 @@
         <v>130.68</v>
       </c>
       <c r="G126" t="n">
-        <v>-876.8697410394598</v>
+        <v>-876.8714635753604</v>
       </c>
       <c r="H126" t="n">
-        <v>22990.3082774641</v>
+        <v>22990.31</v>
       </c>
       <c r="I126" t="n">
-        <v>24027.46974103946</v>
+        <v>24027.47146357536</v>
       </c>
       <c r="J126" t="n">
-        <v>23808.64816211477</v>
+        <v>23808.64988465067</v>
       </c>
       <c r="K126" t="n">
-        <v>23209.13132312654</v>
+        <v>23209.13304566244</v>
       </c>
     </row>
     <row r="127">
@@ -24293,19 +24293,19 @@
         <v>130.58</v>
       </c>
       <c r="G127" t="n">
-        <v>-244.7018055464614</v>
+        <v>-244.7002822617033</v>
       </c>
       <c r="H127" t="n">
-        <v>22990.01152328476</v>
+        <v>22990.01</v>
       </c>
       <c r="I127" t="n">
-        <v>23964.40180554646</v>
+        <v>23964.4002822617</v>
       </c>
       <c r="J127" t="n">
-        <v>23754.76934621436</v>
+        <v>23754.7678229296</v>
       </c>
       <c r="K127" t="n">
-        <v>23199.64539036939</v>
+        <v>23199.64386708463</v>
       </c>
     </row>
     <row r="128">
@@ -24319,19 +24319,19 @@
         <v>130.48</v>
       </c>
       <c r="G128" t="n">
-        <v>-207.768994712671</v>
+        <v>-207.7659880500469</v>
       </c>
       <c r="H128" t="n">
-        <v>22989.53300666262</v>
+        <v>22989.53</v>
       </c>
       <c r="I128" t="n">
-        <v>23906.76899471267</v>
+        <v>23906.76598805005</v>
       </c>
       <c r="J128" t="n">
-        <v>23705.76071290671</v>
+        <v>23705.75770624408</v>
       </c>
       <c r="K128" t="n">
-        <v>23190.54264062367</v>
+        <v>23190.53963396105</v>
       </c>
     </row>
     <row r="129">
@@ -24345,19 +24345,19 @@
         <v>130.38</v>
       </c>
       <c r="G129" t="n">
-        <v>-281.4438478301345</v>
+        <v>-281.4427188784648</v>
       </c>
       <c r="H129" t="n">
-        <v>22989.10112895167</v>
+        <v>22989.1</v>
       </c>
       <c r="I129" t="n">
-        <v>23854.14384783014</v>
+        <v>23854.14271887847</v>
       </c>
       <c r="J129" t="n">
-        <v>23661.24002736949</v>
+        <v>23661.23889841782</v>
       </c>
       <c r="K129" t="n">
-        <v>23182.00624911454</v>
+        <v>23182.00512016287</v>
       </c>
     </row>
     <row r="130">
@@ -24371,19 +24371,19 @@
         <v>130.28</v>
       </c>
       <c r="G130" t="n">
-        <v>-735.8253514816352</v>
+        <v>-735.8278659553143</v>
       </c>
       <c r="H130" t="n">
-        <v>22988.87748552632</v>
+        <v>22988.88</v>
       </c>
       <c r="I130" t="n">
-        <v>23806.12535148163</v>
+        <v>23806.12786595531</v>
       </c>
       <c r="J130" t="n">
-        <v>23620.84707989843</v>
+        <v>23620.84959437211</v>
       </c>
       <c r="K130" t="n">
-        <v>23174.15700728007</v>
+        <v>23174.15952175375</v>
       </c>
     </row>
     <row r="131">
@@ -24397,19 +24397,19 @@
         <v>130.18</v>
       </c>
       <c r="G131" t="n">
-        <v>-500.3249940129244</v>
+        <v>-500.326616885246</v>
       </c>
       <c r="H131" t="n">
-        <v>22988.75837712768</v>
+        <v>22988.76</v>
       </c>
       <c r="I131" t="n">
-        <v>23762.12499401292</v>
+        <v>23762.12661688525</v>
       </c>
       <c r="J131" t="n">
-        <v>23584.03024765663</v>
+        <v>23584.03187052895</v>
       </c>
       <c r="K131" t="n">
-        <v>23166.85432683882</v>
+        <v>23166.85594971115</v>
       </c>
     </row>
     <row r="132">
@@ -24423,19 +24423,19 @@
         <v>130.08</v>
       </c>
       <c r="G132" t="n">
-        <v>-41.51766844487793</v>
+        <v>-41.51939868733098</v>
       </c>
       <c r="H132" t="n">
-        <v>22988.43826975755</v>
+        <v>22988.44</v>
       </c>
       <c r="I132" t="n">
-        <v>23721.41766844488</v>
+        <v>23721.41939868733</v>
       </c>
       <c r="J132" t="n">
-        <v>23550.09783846042</v>
+        <v>23550.09956870288</v>
       </c>
       <c r="K132" t="n">
-        <v>23159.75925880864</v>
+        <v>23159.76098905109</v>
       </c>
     </row>
     <row r="133">
@@ -24449,19 +24449,19 @@
         <v>129.98</v>
       </c>
       <c r="G133" t="n">
-        <v>53.91969539556521</v>
+        <v>53.9183826547669</v>
       </c>
       <c r="H133" t="n">
-        <v>22987.9586872592</v>
+        <v>22987.96</v>
       </c>
       <c r="I133" t="n">
-        <v>23683.68030460443</v>
+        <v>23683.68161734523</v>
       </c>
       <c r="J133" t="n">
-        <v>23518.75710710166</v>
+        <v>23518.75841984246</v>
       </c>
       <c r="K133" t="n">
-        <v>23152.88300189459</v>
+        <v>23152.88431463539</v>
       </c>
     </row>
     <row r="134">
@@ -24475,19 +24475,19 @@
         <v>129.88</v>
       </c>
       <c r="G134" t="n">
-        <v>-727.7040544929914</v>
+        <v>-727.7052279677409</v>
       </c>
       <c r="H134" t="n">
-        <v>22987.72882652525</v>
+        <v>22987.73</v>
       </c>
       <c r="I134" t="n">
-        <v>23649.00405449299</v>
+        <v>23649.00522796774</v>
       </c>
       <c r="J134" t="n">
-        <v>23490.12677637875</v>
+        <v>23490.1279498535</v>
       </c>
       <c r="K134" t="n">
-        <v>23146.6071820329</v>
+        <v>23146.60835550765</v>
       </c>
     </row>
     <row r="135">
@@ -24501,19 +24501,19 @@
         <v>129.78</v>
       </c>
       <c r="G135" t="n">
-        <v>-400.7351967131908</v>
+        <v>-400.7317729158603</v>
       </c>
       <c r="H135" t="n">
-        <v>22987.67342379733</v>
+        <v>22987.67</v>
       </c>
       <c r="I135" t="n">
-        <v>23617.03519671319</v>
+        <v>23617.03177291586</v>
       </c>
       <c r="J135" t="n">
-        <v>23463.87823551875</v>
+        <v>23463.87481172142</v>
       </c>
       <c r="K135" t="n">
-        <v>23140.83142469412</v>
+        <v>23140.82800089678</v>
       </c>
     </row>
     <row r="136">
@@ -24527,19 +24527,19 @@
         <v>129.68</v>
       </c>
       <c r="G136" t="n">
-        <v>-480.894578359319</v>
+        <v>-480.8966037585124</v>
       </c>
       <c r="H136" t="n">
-        <v>22987.55797460081</v>
+        <v>22987.56</v>
       </c>
       <c r="I136" t="n">
-        <v>23587.29457835932</v>
+        <v>23587.29660375851</v>
       </c>
       <c r="J136" t="n">
-        <v>23439.55524018787</v>
+        <v>23439.55726558706</v>
       </c>
       <c r="K136" t="n">
-        <v>23135.29831669661</v>
+        <v>23135.3003420958</v>
       </c>
     </row>
     <row r="137">
@@ -24553,19 +24553,19 @@
         <v>129.58</v>
       </c>
       <c r="G137" t="n">
-        <v>-339.4247604492775</v>
+        <v>-339.4240630692148</v>
       </c>
       <c r="H137" t="n">
-        <v>22987.44069738006</v>
+        <v>22987.44</v>
       </c>
       <c r="I137" t="n">
-        <v>23559.62476044928</v>
+        <v>23559.62406306922</v>
       </c>
       <c r="J137" t="n">
-        <v>23417.02128507237</v>
+        <v>23417.02058769231</v>
       </c>
       <c r="K137" t="n">
-        <v>23130.04514269186</v>
+        <v>23130.0444453118</v>
       </c>
     </row>
     <row r="138">
@@ -24579,19 +24579,19 @@
         <v>129.48</v>
       </c>
       <c r="G138" t="n">
-        <v>560.0903615948373</v>
+        <v>560.086551528173</v>
       </c>
       <c r="H138" t="n">
-        <v>22986.99618993334</v>
+        <v>22987</v>
       </c>
       <c r="I138" t="n">
-        <v>23533.50963840516</v>
+        <v>23533.51344847183</v>
       </c>
       <c r="J138" t="n">
-        <v>23395.77942470178</v>
+        <v>23395.78323476845</v>
       </c>
       <c r="K138" t="n">
-        <v>23124.72734125584</v>
+        <v>23124.7311513225</v>
       </c>
     </row>
     <row r="139">
@@ -24605,19 +24605,19 @@
         <v>129.38</v>
       </c>
       <c r="G139" t="n">
-        <v>-1129.78328159895</v>
+        <v>-1129.785617349931</v>
       </c>
       <c r="H139" t="n">
-        <v>22986.82766424902</v>
+        <v>22986.83</v>
       </c>
       <c r="I139" t="n">
-        <v>23509.38328159895</v>
+        <v>23509.38561734993</v>
       </c>
       <c r="J139" t="n">
-        <v>23376.28129007724</v>
+        <v>23376.28362582823</v>
       </c>
       <c r="K139" t="n">
-        <v>23119.93056264172</v>
+        <v>23119.9328983927</v>
       </c>
     </row>
     <row r="140">
@@ -24631,19 +24631,19 @@
         <v>129.28</v>
       </c>
       <c r="G140" t="n">
-        <v>185.7394105517124</v>
+        <v>185.7398812582833</v>
       </c>
       <c r="H140" t="n">
-        <v>22986.80047070657</v>
+        <v>22986.8</v>
       </c>
       <c r="I140" t="n">
-        <v>23486.96058944829</v>
+        <v>23486.96011874172</v>
       </c>
       <c r="J140" t="n">
-        <v>23358.25790161884</v>
+        <v>23358.25743091226</v>
       </c>
       <c r="K140" t="n">
-        <v>23115.50403612852</v>
+        <v>23115.50356542195</v>
       </c>
     </row>
     <row r="141">
@@ -24657,19 +24657,19 @@
         <v>129.18</v>
       </c>
       <c r="G141" t="n">
-        <v>-787.5679703466012</v>
+        <v>-787.5727610071117</v>
       </c>
       <c r="H141" t="n">
-        <v>22986.67520933949</v>
+        <v>22986.68</v>
       </c>
       <c r="I141" t="n">
-        <v>23465.8679703466</v>
+        <v>23465.87276100711</v>
       </c>
       <c r="J141" t="n">
-        <v>23341.35048730907</v>
+        <v>23341.35527796958</v>
       </c>
       <c r="K141" t="n">
-        <v>23111.19354206998</v>
+        <v>23111.19833273049</v>
       </c>
     </row>
     <row r="142">
@@ -24683,19 +24683,19 @@
         <v>129.08</v>
       </c>
       <c r="G142" t="n">
-        <v>-520.6303155381283</v>
+        <v>-520.6335412680965</v>
       </c>
       <c r="H142" t="n">
-        <v>22986.79677427003</v>
+        <v>22986.8</v>
       </c>
       <c r="I142" t="n">
-        <v>23446.33031553813</v>
+        <v>23446.3335412681</v>
       </c>
       <c r="J142" t="n">
-        <v>23325.79758036919</v>
+        <v>23325.80080609916</v>
       </c>
       <c r="K142" t="n">
-        <v>23107.33033252744</v>
+        <v>23107.33355825741</v>
       </c>
     </row>
     <row r="143">
@@ -24709,19 +24709,19 @@
         <v>128.98</v>
       </c>
       <c r="G143" t="n">
-        <v>-193.3106387921434</v>
+        <v>-193.3148764394246</v>
       </c>
       <c r="H143" t="n">
-        <v>22986.73576235272</v>
+        <v>22986.74</v>
       </c>
       <c r="I143" t="n">
-        <v>23427.81063879214</v>
+        <v>23427.81487643942</v>
       </c>
       <c r="J143" t="n">
-        <v>23311.07476923789</v>
+        <v>23311.07900688517</v>
       </c>
       <c r="K143" t="n">
-        <v>23103.47242960823</v>
+        <v>23103.47666725551</v>
       </c>
     </row>
     <row r="144">
@@ -24735,19 +24735,19 @@
         <v>128.88</v>
       </c>
       <c r="G144" t="n">
-        <v>-200.3993364111629</v>
+        <v>-200.4000866824063</v>
       </c>
       <c r="H144" t="n">
-        <v>22986.57924972876</v>
+        <v>22986.58</v>
       </c>
       <c r="I144" t="n">
-        <v>23410.29933641116</v>
+        <v>23410.30008668241</v>
       </c>
       <c r="J144" t="n">
-        <v>23297.18405603977</v>
+        <v>23297.18480631101</v>
       </c>
       <c r="K144" t="n">
-        <v>23099.69530355934</v>
+        <v>23099.69605383058</v>
       </c>
     </row>
     <row r="145">
@@ -24761,19 +24761,19 @@
         <v>128.78</v>
       </c>
       <c r="G145" t="n">
-        <v>-434.7953872003454</v>
+        <v>-434.7920909400636</v>
       </c>
       <c r="H145" t="n">
-        <v>22986.51329626028</v>
+        <v>22986.51</v>
       </c>
       <c r="I145" t="n">
-        <v>23393.89538720034</v>
+        <v>23393.89209094006</v>
       </c>
       <c r="J145" t="n">
-        <v>23284.2351445992</v>
+        <v>23284.23184833892</v>
       </c>
       <c r="K145" t="n">
-        <v>23096.17428915668</v>
+        <v>23096.1709928964</v>
       </c>
     </row>
     <row r="146">
@@ -24787,19 +24787,19 @@
         <v>128.68</v>
       </c>
       <c r="G146" t="n">
-        <v>-173.5318433071443</v>
+        <v>-173.5322813152343</v>
       </c>
       <c r="H146" t="n">
-        <v>22986.44956199191</v>
+        <v>22986.45</v>
       </c>
       <c r="I146" t="n">
-        <v>23378.43184330715</v>
+        <v>23378.43228131524</v>
       </c>
       <c r="J146" t="n">
-        <v>23272.07101014698</v>
+        <v>23272.07144815507</v>
       </c>
       <c r="K146" t="n">
-        <v>23092.81112329936</v>
+        <v>23092.81156130745</v>
       </c>
     </row>
     <row r="147">
@@ -24813,19 +24813,19 @@
         <v>128.58</v>
       </c>
       <c r="G147" t="n">
-        <v>-604.901680045572</v>
+        <v>-604.8995487962675</v>
       </c>
       <c r="H147" t="n">
-        <v>22986.45213124931</v>
+        <v>22986.45</v>
       </c>
       <c r="I147" t="n">
-        <v>23363.90168004557</v>
+        <v>23363.89954879627</v>
       </c>
       <c r="J147" t="n">
-        <v>23260.69381990903</v>
+        <v>23260.69168865973</v>
       </c>
       <c r="K147" t="n">
-        <v>23089.66069834322</v>
+        <v>23089.65856709391</v>
       </c>
     </row>
     <row r="148">
@@ -24839,19 +24839,19 @@
         <v>128.48</v>
       </c>
       <c r="G148" t="n">
-        <v>-131.4699984966282</v>
+        <v>-131.4694374976607</v>
       </c>
       <c r="H148" t="n">
-        <v>22986.45056099897</v>
+        <v>22986.45</v>
       </c>
       <c r="I148" t="n">
-        <v>23350.16999849663</v>
+        <v>23350.16943749766</v>
       </c>
       <c r="J148" t="n">
-        <v>23249.97719930482</v>
+        <v>23249.97663830585</v>
       </c>
       <c r="K148" t="n">
-        <v>23086.64404686243</v>
+        <v>23086.64348586346</v>
       </c>
     </row>
     <row r="149">
@@ -24865,19 +24865,19 @@
         <v>128.38</v>
       </c>
       <c r="G149" t="n">
-        <v>49.52567839968469</v>
+        <v>49.52659161496194</v>
       </c>
       <c r="H149" t="n">
-        <v>22986.24091321528</v>
+        <v>22986.24</v>
       </c>
       <c r="I149" t="n">
-        <v>23336.97432160032</v>
+        <v>23336.97340838504</v>
       </c>
       <c r="J149" t="n">
-        <v>23239.66658528695</v>
+        <v>23239.66567207167</v>
       </c>
       <c r="K149" t="n">
-        <v>23083.54931676858</v>
+        <v>23083.5484035533</v>
       </c>
     </row>
     <row r="150">
@@ -24891,19 +24891,19 @@
         <v>128.28</v>
       </c>
       <c r="G150" t="n">
-        <v>-139.7792387745794</v>
+        <v>-139.778196565625</v>
       </c>
       <c r="H150" t="n">
-        <v>22986.04104220896</v>
+        <v>22986.04</v>
       </c>
       <c r="I150" t="n">
-        <v>23324.47923877458</v>
+        <v>23324.47819656563</v>
       </c>
       <c r="J150" t="n">
-        <v>23229.93392257056</v>
+        <v>23229.93288036161</v>
       </c>
       <c r="K150" t="n">
-        <v>23080.58700702839</v>
+        <v>23080.58596481943</v>
       </c>
     </row>
     <row r="151">

</xml_diff>

<commit_message>
Mac: Improve help menu
</commit_message>
<xml_diff>
--- a/DATA/UKSAF/STO.xlsx
+++ b/DATA/UKSAF/STO.xlsx
@@ -25893,6 +25893,11 @@
       <c r="K6" t="n">
         <v>26730.93264749989</v>
       </c>
+      <c r="X6" s="50" t="inlineStr">
+        <is>
+          <t>Please cite KherveFitting software: Kerherve G. et al. Surface and Interface Analysis (2025) TBD</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -25919,11 +25924,6 @@
       <c r="K7" t="n">
         <v>26261.66297523991</v>
       </c>
-      <c r="X7" s="50" t="inlineStr">
-        <is>
-          <t>Please cite KherveFitting software: G. Kerherve et al. Surface and Interface Analysis, xxx, 2025</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -29957,7 +29957,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="X7:AP7"/>
+    <mergeCell ref="X6:AP6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Mac: Improve doublet for Ti2p and V2p
</commit_message>
<xml_diff>
--- a/DATA/UKSAF/STO.xlsx
+++ b/DATA/UKSAF/STO.xlsx
@@ -25485,19 +25485,19 @@
         <v>142.34</v>
       </c>
       <c r="G2" t="n">
-        <v>-242.0628158015861</v>
+        <v>-176.8845501467986</v>
       </c>
       <c r="H2" t="n">
         <v>26049.5</v>
       </c>
       <c r="I2" t="n">
-        <v>26291.56281580159</v>
+        <v>26226.3845501468</v>
       </c>
       <c r="J2" t="n">
-        <v>26178.18175783558</v>
+        <v>26177.64929272504</v>
       </c>
       <c r="K2" t="n">
-        <v>26162.88105796601</v>
+        <v>26098.23525742176</v>
       </c>
       <c r="X2" s="32" t="inlineStr">
         <is>
@@ -25516,7 +25516,7 @@
       </c>
       <c r="AA2" s="33" t="inlineStr">
         <is>
-          <t>99789</t>
+          <t>99212</t>
         </is>
       </c>
       <c r="AB2" s="33" t="inlineStr">
@@ -25526,22 +25526,22 @@
       </c>
       <c r="AC2" s="33" t="inlineStr">
         <is>
-          <t>14.74</t>
+          <t>14.54</t>
         </is>
       </c>
       <c r="AD2" s="33" t="inlineStr">
         <is>
-          <t>118328</t>
+          <t>118158</t>
         </is>
       </c>
       <c r="AE2" s="33" t="inlineStr">
         <is>
-          <t>0.810</t>
+          <t>0.817</t>
         </is>
       </c>
       <c r="AF2" s="33" t="inlineStr">
         <is>
-          <t>0.140</t>
+          <t>0.139</t>
         </is>
       </c>
       <c r="AG2" s="33" t="inlineStr">
@@ -25551,7 +25551,7 @@
       </c>
       <c r="AH2" s="33" t="inlineStr">
         <is>
-          <t>59.8</t>
+          <t>59.7</t>
         </is>
       </c>
       <c r="AI2" s="33" t="inlineStr">
@@ -25566,32 +25566,32 @@
       </c>
       <c r="AK2" s="33" t="inlineStr">
         <is>
-          <t>DS*G (A, σ, γ)</t>
+          <t>DS*G (A, σ, γ, S)</t>
         </is>
       </c>
       <c r="AL2" s="33" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Multi-Regions Smart</t>
         </is>
       </c>
       <c r="AM2" s="33" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>126.07</t>
         </is>
       </c>
       <c r="AN2" s="33" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>142.07</t>
         </is>
       </c>
       <c r="AO2" s="33" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="AP2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.00</t>
         </is>
       </c>
     </row>
@@ -25606,19 +25606,19 @@
         <v>142.24</v>
       </c>
       <c r="G3" t="n">
-        <v>-259.07977677093</v>
+        <v>-184.3757833721611</v>
       </c>
       <c r="H3" t="n">
         <v>26437.6</v>
       </c>
       <c r="I3" t="n">
-        <v>26696.67977677093</v>
+        <v>26621.97578337216</v>
       </c>
       <c r="J3" t="n">
-        <v>26566.28175783558</v>
+        <v>26565.74929272504</v>
       </c>
       <c r="K3" t="n">
-        <v>26567.99801893535</v>
+        <v>26493.82649064712</v>
       </c>
       <c r="X3" s="35" t="inlineStr"/>
       <c r="Y3" s="36" t="inlineStr"/>
@@ -25682,19 +25682,19 @@
         <v>142.14</v>
       </c>
       <c r="G4" t="n">
-        <v>-273.4423578925416</v>
+        <v>-190.8303463883931</v>
       </c>
       <c r="H4" t="n">
         <v>26696.9</v>
       </c>
       <c r="I4" t="n">
-        <v>26970.34235789254</v>
+        <v>26887.73034638839</v>
       </c>
       <c r="J4" t="n">
-        <v>26825.58175783558</v>
+        <v>26825.04929272504</v>
       </c>
       <c r="K4" t="n">
-        <v>26841.66060005697</v>
+        <v>26759.58105366336</v>
       </c>
       <c r="X4" s="32" t="inlineStr">
         <is>
@@ -25713,7 +25713,7 @@
       </c>
       <c r="AA4" s="33" t="inlineStr">
         <is>
-          <t>67195</t>
+          <t>68864</t>
         </is>
       </c>
       <c r="AB4" s="33" t="inlineStr">
@@ -25723,37 +25723,37 @@
       </c>
       <c r="AC4" s="33" t="inlineStr">
         <is>
-          <t>14.74</t>
+          <t>14.54</t>
         </is>
       </c>
       <c r="AD4" s="33" t="inlineStr">
         <is>
-          <t>79679</t>
+          <t>79796</t>
         </is>
       </c>
       <c r="AE4" s="33" t="inlineStr">
         <is>
-          <t>0.810</t>
+          <t>0.817</t>
         </is>
       </c>
       <c r="AF4" s="33" t="inlineStr">
         <is>
-          <t>0.140</t>
+          <t>0.139</t>
         </is>
       </c>
       <c r="AG4" s="33" t="inlineStr">
         <is>
-          <t>0.010</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="AH4" s="33" t="inlineStr">
         <is>
-          <t>40.2</t>
+          <t>40.3</t>
         </is>
       </c>
       <c r="AI4" s="33" t="inlineStr">
         <is>
-          <t>67.3</t>
+          <t>67.5</t>
         </is>
       </c>
       <c r="AJ4" s="33" t="inlineStr">
@@ -25763,32 +25763,32 @@
       </c>
       <c r="AK4" s="33" t="inlineStr">
         <is>
-          <t>DS*G (A, σ, γ)</t>
+          <t>DS*G (A, σ, γ, S)</t>
         </is>
       </c>
       <c r="AL4" s="33" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Multi-Regions Smart</t>
         </is>
       </c>
       <c r="AM4" s="33" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>126.07</t>
         </is>
       </c>
       <c r="AN4" s="33" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>142.07</t>
         </is>
       </c>
       <c r="AO4" s="33" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="AP4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.00</t>
         </is>
       </c>
     </row>
@@ -25803,19 +25803,19 @@
         <v>142.04</v>
       </c>
       <c r="G5" t="n">
-        <v>-284.9319185278218</v>
+        <v>-196.1473008951689</v>
       </c>
       <c r="H5" t="n">
         <v>25942.6</v>
       </c>
       <c r="I5" t="n">
-        <v>26227.53191852782</v>
+        <v>26138.74730089517</v>
       </c>
       <c r="J5" t="n">
-        <v>26071.28175783558</v>
+        <v>26070.74929272504</v>
       </c>
       <c r="K5" t="n">
-        <v>26098.85016069224</v>
+        <v>26010.59800817013</v>
       </c>
       <c r="X5" s="35" t="inlineStr"/>
       <c r="Y5" s="36" t="inlineStr"/>
@@ -25879,19 +25879,19 @@
         <v>141.94</v>
       </c>
       <c r="G6" t="n">
-        <v>-293.8144053354699</v>
+        <v>-200.4247490158414</v>
       </c>
       <c r="H6" t="n">
         <v>26565.8</v>
       </c>
       <c r="I6" t="n">
-        <v>26859.61440533547</v>
+        <v>26766.22474901584</v>
       </c>
       <c r="J6" t="n">
-        <v>26694.48175783558</v>
+        <v>26693.94929272504</v>
       </c>
       <c r="K6" t="n">
-        <v>26730.93264749989</v>
+        <v>26638.0754562908</v>
       </c>
       <c r="X6" s="50" t="inlineStr">
         <is>
@@ -25910,19 +25910,19 @@
         <v>141.84</v>
       </c>
       <c r="G7" t="n">
-        <v>-300.6447330754854</v>
+        <v>-203.882798631279</v>
       </c>
       <c r="H7" t="n">
         <v>26089.7</v>
       </c>
       <c r="I7" t="n">
-        <v>26390.34473307549</v>
+        <v>26293.58279863128</v>
       </c>
       <c r="J7" t="n">
-        <v>26218.38175783558</v>
+        <v>26217.84929272504</v>
       </c>
       <c r="K7" t="n">
-        <v>26261.66297523991</v>
+        <v>26165.43350590624</v>
       </c>
     </row>
     <row r="8">
@@ -25936,19 +25936,19 @@
         <v>141.74</v>
       </c>
       <c r="G8" t="n">
-        <v>-306.0574478725102</v>
+        <v>-206.7791303205959</v>
       </c>
       <c r="H8" t="n">
         <v>26784.6</v>
       </c>
       <c r="I8" t="n">
-        <v>27090.65744787251</v>
+        <v>26991.37913032059</v>
       </c>
       <c r="J8" t="n">
-        <v>26913.28175783558</v>
+        <v>26912.74929272504</v>
       </c>
       <c r="K8" t="n">
-        <v>26961.97569003693</v>
+        <v>26863.22983759556</v>
       </c>
     </row>
     <row r="9">
@@ -25962,19 +25962,19 @@
         <v>141.64</v>
       </c>
       <c r="G9" t="n">
-        <v>-310.6151463741953</v>
+        <v>-209.3462996737653</v>
       </c>
       <c r="H9" t="n">
         <v>26357.7</v>
       </c>
       <c r="I9" t="n">
-        <v>26668.3151463742</v>
+        <v>26567.04629967377</v>
       </c>
       <c r="J9" t="n">
-        <v>26486.38175783558</v>
+        <v>26485.84929272504</v>
       </c>
       <c r="K9" t="n">
-        <v>26539.63338853862</v>
+        <v>26438.89700694873</v>
       </c>
     </row>
     <row r="10">
@@ -25988,19 +25988,19 @@
         <v>141.54</v>
       </c>
       <c r="G10" t="n">
-        <v>-314.7384846829336</v>
+        <v>-211.7613684180506</v>
       </c>
       <c r="H10" t="n">
         <v>26256</v>
       </c>
       <c r="I10" t="n">
-        <v>26570.73848468293</v>
+        <v>26467.76136841805</v>
       </c>
       <c r="J10" t="n">
-        <v>26384.68175783558</v>
+        <v>26384.14929272504</v>
       </c>
       <c r="K10" t="n">
-        <v>26442.05672684736</v>
+        <v>26339.61207569301</v>
       </c>
     </row>
     <row r="11">
@@ -26014,19 +26014,19 @@
         <v>141.44</v>
       </c>
       <c r="G11" t="n">
-        <v>-318.7025228873354</v>
+        <v>-214.1426635644675</v>
       </c>
       <c r="H11" t="n">
         <v>26519.3</v>
       </c>
       <c r="I11" t="n">
-        <v>26838.00252288733</v>
+        <v>26733.44266356447</v>
       </c>
       <c r="J11" t="n">
-        <v>26647.98175783558</v>
+        <v>26647.44929272504</v>
       </c>
       <c r="K11" t="n">
-        <v>26709.32076505176</v>
+        <v>26605.29337083943</v>
       </c>
     </row>
     <row r="12">
@@ -26040,19 +26040,19 @@
         <v>141.34</v>
       </c>
       <c r="G12" t="n">
-        <v>-322.668293015955</v>
+        <v>-216.5615702263894</v>
       </c>
       <c r="H12" t="n">
         <v>25948.6</v>
       </c>
       <c r="I12" t="n">
-        <v>26271.26829301595</v>
+        <v>26165.16157022639</v>
       </c>
       <c r="J12" t="n">
-        <v>26077.28175783558</v>
+        <v>26076.74929272504</v>
       </c>
       <c r="K12" t="n">
-        <v>26142.58653518038</v>
+        <v>26037.01227750135</v>
       </c>
     </row>
     <row r="13">
@@ -26066,19 +26066,19 @@
         <v>141.24</v>
       </c>
       <c r="G13" t="n">
-        <v>-326.7223837418642</v>
+        <v>-219.0583211691119</v>
       </c>
       <c r="H13" t="n">
         <v>26945.3</v>
       </c>
       <c r="I13" t="n">
-        <v>27272.02238374186</v>
+        <v>27164.35832116911</v>
       </c>
       <c r="J13" t="n">
-        <v>27073.98175783558</v>
+        <v>27073.44929272504</v>
       </c>
       <c r="K13" t="n">
-        <v>27143.34062590629</v>
+        <v>27036.20902844407</v>
       </c>
     </row>
     <row r="14">
@@ -26092,19 +26092,19 @@
         <v>141.14</v>
       </c>
       <c r="G14" t="n">
-        <v>-330.9094793346485</v>
+        <v>-221.6553862449655</v>
       </c>
       <c r="H14" t="n">
         <v>26444</v>
       </c>
       <c r="I14" t="n">
-        <v>26774.90947933465</v>
+        <v>26665.65538624497</v>
       </c>
       <c r="J14" t="n">
-        <v>26572.68175783558</v>
+        <v>26572.14929272504</v>
       </c>
       <c r="K14" t="n">
-        <v>26646.22772149907</v>
+        <v>26537.50609351993</v>
       </c>
     </row>
     <row r="15">
@@ -26118,19 +26118,19 @@
         <v>141.04</v>
       </c>
       <c r="G15" t="n">
-        <v>-335.2536690427951</v>
+        <v>-224.366460332727</v>
       </c>
       <c r="H15" t="n">
         <v>26729.6</v>
       </c>
       <c r="I15" t="n">
-        <v>27064.85366904279</v>
+        <v>26953.96646033273</v>
       </c>
       <c r="J15" t="n">
-        <v>26858.28175783558</v>
+        <v>26857.74929272504</v>
       </c>
       <c r="K15" t="n">
-        <v>26936.17191120722</v>
+        <v>26825.81716760769</v>
       </c>
     </row>
     <row r="16">
@@ -26144,19 +26144,19 @@
         <v>140.94</v>
       </c>
       <c r="G16" t="n">
-        <v>-339.7702716211097</v>
+        <v>-227.2015721649477</v>
       </c>
       <c r="H16" t="n">
         <v>27045.9</v>
       </c>
       <c r="I16" t="n">
-        <v>27385.67027162111</v>
+        <v>27273.10157216495</v>
       </c>
       <c r="J16" t="n">
-        <v>27174.58175783558</v>
+        <v>27174.04929272504</v>
       </c>
       <c r="K16" t="n">
-        <v>27256.98851378553</v>
+        <v>27144.95227943991</v>
       </c>
     </row>
     <row r="17">
@@ -26170,19 +26170,19 @@
         <v>140.84</v>
       </c>
       <c r="G17" t="n">
-        <v>-344.4715650429571</v>
+        <v>-230.1696276668117</v>
       </c>
       <c r="H17" t="n">
         <v>26274.3</v>
       </c>
       <c r="I17" t="n">
-        <v>26618.77156504296</v>
+        <v>26504.46962766681</v>
       </c>
       <c r="J17" t="n">
-        <v>26402.98175783558</v>
+        <v>26402.44929272504</v>
       </c>
       <c r="K17" t="n">
-        <v>26490.08980720738</v>
+        <v>26376.32033494177</v>
       </c>
     </row>
     <row r="18">
@@ -26196,19 +26196,19 @@
         <v>140.74</v>
       </c>
       <c r="G18" t="n">
-        <v>-349.3692666630013</v>
+        <v>-233.2795516295082</v>
       </c>
       <c r="H18" t="n">
         <v>25721.7</v>
       </c>
       <c r="I18" t="n">
-        <v>26071.069266663</v>
+        <v>25954.97955162951</v>
       </c>
       <c r="J18" t="n">
-        <v>25850.38175783558</v>
+        <v>25849.84929272504</v>
       </c>
       <c r="K18" t="n">
-        <v>25942.38750882743</v>
+        <v>25826.83025890447</v>
       </c>
     </row>
     <row r="19">
@@ -26222,19 +26222,19 @@
         <v>140.64</v>
       </c>
       <c r="G19" t="n">
-        <v>-383.1279598107212</v>
+        <v>-264.8617865569431</v>
       </c>
       <c r="H19" t="n">
         <v>26199.6</v>
       </c>
       <c r="I19" t="n">
-        <v>26582.72795981072</v>
+        <v>26464.46178655694</v>
       </c>
       <c r="J19" t="n">
-        <v>26356.93419282816</v>
+        <v>26356.07030598944</v>
       </c>
       <c r="K19" t="n">
-        <v>26425.39376698256</v>
+        <v>26307.9914805675</v>
       </c>
     </row>
     <row r="20">
@@ -26248,19 +26248,19 @@
         <v>140.54</v>
       </c>
       <c r="G20" t="n">
-        <v>-415.015673715232</v>
+        <v>-294.5800365026771</v>
       </c>
       <c r="H20" t="n">
         <v>27175.7</v>
       </c>
       <c r="I20" t="n">
-        <v>27590.71567371523</v>
+        <v>27470.28003650268</v>
       </c>
       <c r="J20" t="n">
-        <v>27359.59411556653</v>
+        <v>27358.46588348502</v>
       </c>
       <c r="K20" t="n">
-        <v>27406.8215581487</v>
+        <v>27287.51415301766</v>
       </c>
     </row>
     <row r="21">
@@ -26274,19 +26274,19 @@
         <v>140.44</v>
       </c>
       <c r="G21" t="n">
-        <v>-443.5605672934907</v>
+        <v>-320.9917234665409</v>
       </c>
       <c r="H21" t="n">
         <v>26142</v>
       </c>
       <c r="I21" t="n">
-        <v>26585.56056729349</v>
+        <v>26462.99172346654</v>
       </c>
       <c r="J21" t="n">
-        <v>26348.87568899338</v>
+        <v>26347.58244257609</v>
       </c>
       <c r="K21" t="n">
-        <v>26378.68487830011</v>
+        <v>26257.40928089045</v>
       </c>
     </row>
     <row r="22">
@@ -26300,19 +26300,19 @@
         <v>140.34</v>
       </c>
       <c r="G22" t="n">
-        <v>-468.1182867532261</v>
+        <v>-343.4489126978042</v>
       </c>
       <c r="H22" t="n">
         <v>26419.9</v>
       </c>
       <c r="I22" t="n">
-        <v>26888.01828675323</v>
+        <v>26763.34891269781</v>
       </c>
       <c r="J22" t="n">
-        <v>26645.51938940299</v>
+        <v>26644.16007229259</v>
       </c>
       <c r="K22" t="n">
-        <v>26662.39889735023</v>
+        <v>26539.08884040522</v>
       </c>
     </row>
     <row r="23">
@@ -26326,19 +26326,19 @@
         <v>140.24</v>
       </c>
       <c r="G23" t="n">
-        <v>-488.844095629498</v>
+        <v>-362.0775391341085</v>
       </c>
       <c r="H23" t="n">
         <v>27293.7</v>
       </c>
       <c r="I23" t="n">
-        <v>27782.5440956295</v>
+        <v>27655.77753913411</v>
       </c>
       <c r="J23" t="n">
-        <v>27533.9637601367</v>
+        <v>27532.61146771656</v>
       </c>
       <c r="K23" t="n">
-        <v>27542.2803354928</v>
+        <v>27416.86607141755</v>
       </c>
     </row>
     <row r="24">
@@ -26352,19 +26352,19 @@
         <v>140.14</v>
       </c>
       <c r="G24" t="n">
-        <v>-506.4490694145497</v>
+        <v>-377.5492486675903</v>
       </c>
       <c r="H24" t="n">
         <v>26191.1</v>
       </c>
       <c r="I24" t="n">
-        <v>26697.54906941455</v>
+        <v>26568.64924866759</v>
       </c>
       <c r="J24" t="n">
-        <v>26442.60229632735</v>
+        <v>26441.29426641887</v>
       </c>
       <c r="K24" t="n">
-        <v>26446.0467730872</v>
+        <v>26318.45498224872</v>
       </c>
     </row>
     <row r="25">
@@ -26378,19 +26378,19 @@
         <v>140.04</v>
       </c>
       <c r="G25" t="n">
-        <v>-521.8817835976297</v>
+        <v>-390.7774030082255</v>
       </c>
       <c r="H25" t="n">
         <v>26444.7</v>
       </c>
       <c r="I25" t="n">
-        <v>26966.58178359763</v>
+        <v>26835.47740300823</v>
       </c>
       <c r="J25" t="n">
-        <v>26704.96415064831</v>
+        <v>26703.70630962114</v>
       </c>
       <c r="K25" t="n">
-        <v>26706.31763294932</v>
+        <v>26576.47109338709</v>
       </c>
     </row>
     <row r="26">
@@ -26404,19 +26404,19 @@
         <v>139.94</v>
       </c>
       <c r="G26" t="n">
-        <v>-536.0606434446127</v>
+        <v>-402.6571021098644</v>
       </c>
       <c r="H26" t="n">
         <v>26393.8</v>
       </c>
       <c r="I26" t="n">
-        <v>26929.86064344461</v>
+        <v>26796.45710210986</v>
       </c>
       <c r="J26" t="n">
-        <v>26661.24656215397</v>
+        <v>26660.02571522601</v>
       </c>
       <c r="K26" t="n">
-        <v>26662.41408129064</v>
+        <v>26530.23138688386</v>
       </c>
     </row>
     <row r="27">
@@ -26430,19 +26430,19 @@
         <v>139.84</v>
       </c>
       <c r="G27" t="n">
-        <v>-549.7223022487124</v>
+        <v>-413.9137388872659</v>
       </c>
       <c r="H27" t="n">
         <v>26023.2</v>
       </c>
       <c r="I27" t="n">
-        <v>26572.92230224871</v>
+        <v>26437.11373888727</v>
       </c>
       <c r="J27" t="n">
-        <v>26296.96307917663</v>
+        <v>26295.75926306888</v>
       </c>
       <c r="K27" t="n">
-        <v>26299.15922307208</v>
+        <v>26164.55447581839</v>
       </c>
     </row>
     <row r="28">
@@ -26456,19 +26456,19 @@
         <v>139.74</v>
       </c>
       <c r="G28" t="n">
-        <v>-563.382511324362</v>
+        <v>-425.059649392475</v>
       </c>
       <c r="H28" t="n">
         <v>27069.8</v>
       </c>
       <c r="I28" t="n">
-        <v>27633.18251132436</v>
+        <v>27494.85964939247</v>
       </c>
       <c r="J28" t="n">
-        <v>27349.50418756175</v>
+        <v>27348.29885212067</v>
       </c>
       <c r="K28" t="n">
-        <v>27353.47832376261</v>
+        <v>27216.3607972718</v>
       </c>
     </row>
     <row r="29">
@@ -26482,19 +26482,19 @@
         <v>139.64</v>
       </c>
       <c r="G29" t="n">
-        <v>-577.3681929805389</v>
+        <v>-436.4213419275948</v>
       </c>
       <c r="H29" t="n">
         <v>26161.8</v>
       </c>
       <c r="I29" t="n">
-        <v>26739.16819298054</v>
+        <v>26598.22134192759</v>
       </c>
       <c r="J29" t="n">
-        <v>26447.36913125971</v>
+        <v>26446.14850928855</v>
       </c>
       <c r="K29" t="n">
-        <v>26453.59906172083</v>
+        <v>26313.87283263904</v>
       </c>
     </row>
     <row r="30">
@@ -26508,19 +26508,19 @@
         <v>139.54</v>
       </c>
       <c r="G30" t="n">
-        <v>-591.8755536596618</v>
+        <v>-448.1942808730673</v>
       </c>
       <c r="H30" t="n">
         <v>26300.2</v>
       </c>
       <c r="I30" t="n">
-        <v>26892.07555365966</v>
+        <v>26748.39428087307</v>
       </c>
       <c r="J30" t="n">
-        <v>26591.72373746971</v>
+        <v>26590.47892104822</v>
       </c>
       <c r="K30" t="n">
-        <v>26600.55181618995</v>
+        <v>26458.11535982485</v>
       </c>
     </row>
     <row r="31">
@@ -26534,19 +26534,19 @@
         <v>139.44</v>
       </c>
       <c r="G31" t="n">
-        <v>-607.0243687821749</v>
+        <v>-460.4957276063869</v>
       </c>
       <c r="H31" t="n">
         <v>26179.2</v>
       </c>
       <c r="I31" t="n">
-        <v>26786.22436878218</v>
+        <v>26639.69572760639</v>
       </c>
       <c r="J31" t="n">
-        <v>26476.8543719439</v>
+        <v>26475.57998486442</v>
       </c>
       <c r="K31" t="n">
-        <v>26488.56999683828</v>
+        <v>26343.31574274197</v>
       </c>
     </row>
     <row r="32">
@@ -26560,19 +26560,19 @@
         <v>139.34</v>
       </c>
       <c r="G32" t="n">
-        <v>-622.8966155273447</v>
+        <v>-473.4032007604437</v>
       </c>
       <c r="H32" t="n">
         <v>25952.4</v>
       </c>
       <c r="I32" t="n">
-        <v>26575.29661552735</v>
+        <v>26425.80320076045</v>
       </c>
       <c r="J32" t="n">
-        <v>26256.40619360327</v>
+        <v>26255.09893616584</v>
       </c>
       <c r="K32" t="n">
-        <v>26271.29042192407</v>
+        <v>26123.1042645946</v>
       </c>
     </row>
     <row r="33">
@@ -26586,19 +26586,19 @@
         <v>139.24</v>
       </c>
       <c r="G33" t="n">
-        <v>-639.5594770815187</v>
+        <v>-486.9778271004107</v>
       </c>
       <c r="H33" t="n">
         <v>25823.1</v>
       </c>
       <c r="I33" t="n">
-        <v>26462.65947708152</v>
+        <v>26310.07782710041</v>
       </c>
       <c r="J33" t="n">
-        <v>26133.70572351687</v>
+        <v>26132.36331436634</v>
       </c>
       <c r="K33" t="n">
-        <v>26152.05375356464</v>
+        <v>26000.81451273406</v>
       </c>
     </row>
     <row r="34">
@@ -26612,19 +26612,19 @@
         <v>139.14</v>
       </c>
       <c r="G34" t="n">
-        <v>-657.0773576439933</v>
+        <v>-501.2767431146931</v>
       </c>
       <c r="H34" t="n">
         <v>25796.2</v>
       </c>
       <c r="I34" t="n">
-        <v>26453.27735764399</v>
+        <v>26297.47674311469</v>
       </c>
       <c r="J34" t="n">
-        <v>26113.67235733539</v>
+        <v>26112.29291863642</v>
       </c>
       <c r="K34" t="n">
-        <v>26135.80500030861</v>
+        <v>25981.38382447827</v>
       </c>
     </row>
     <row r="35">
@@ -26638,19 +26638,19 @@
         <v>139.04</v>
       </c>
       <c r="G35" t="n">
-        <v>-675.5176641985199</v>
+        <v>-516.3591232754115</v>
       </c>
       <c r="H35" t="n">
         <v>25706.9</v>
       </c>
       <c r="I35" t="n">
-        <v>26382.41766419852</v>
+        <v>26223.25912327541</v>
       </c>
       <c r="J35" t="n">
-        <v>26031.52356486925</v>
+        <v>26030.10531800633</v>
       </c>
       <c r="K35" t="n">
-        <v>26057.79409932927</v>
+        <v>25900.05380526908</v>
       </c>
     </row>
     <row r="36">
@@ -26664,19 +26664,19 @@
         <v>138.94</v>
       </c>
       <c r="G36" t="n">
-        <v>-694.9536179632341</v>
+        <v>-532.2890895551427</v>
       </c>
       <c r="H36" t="n">
         <v>25865.6</v>
       </c>
       <c r="I36" t="n">
-        <v>26560.55361796323</v>
+        <v>26397.88908955514</v>
       </c>
       <c r="J36" t="n">
-        <v>26197.67702478099</v>
+        <v>26196.21815655055</v>
       </c>
       <c r="K36" t="n">
-        <v>26228.47659318224</v>
+        <v>26067.27093300459</v>
       </c>
     </row>
     <row r="37">
@@ -26690,19 +26690,19 @@
         <v>138.84</v>
       </c>
       <c r="G37" t="n">
-        <v>-715.4658860195304</v>
+        <v>-549.137339220717</v>
       </c>
       <c r="H37" t="n">
         <v>26150.6</v>
       </c>
       <c r="I37" t="n">
-        <v>26866.06588601953</v>
+        <v>26699.73733922072</v>
       </c>
       <c r="J37" t="n">
-        <v>26490.45146668083</v>
+        <v>26488.95007376299</v>
       </c>
       <c r="K37" t="n">
-        <v>26526.2144193387</v>
+        <v>26361.38726545772</v>
       </c>
     </row>
     <row r="38">
@@ -26716,19 +26716,19 @@
         <v>138.74</v>
       </c>
       <c r="G38" t="n">
-        <v>-737.143872546545</v>
+        <v>-566.982373475319</v>
       </c>
       <c r="H38" t="n">
         <v>25610.5</v>
       </c>
       <c r="I38" t="n">
-        <v>26347.64387254655</v>
+        <v>26177.48237347532</v>
       </c>
       <c r="J38" t="n">
-        <v>25958.46703774948</v>
+        <v>25956.92110192361</v>
       </c>
       <c r="K38" t="n">
-        <v>25999.67683479706</v>
+        <v>25831.06127155171</v>
       </c>
     </row>
     <row r="39">
@@ -26742,19 +26742,19 @@
         <v>138.64</v>
       </c>
       <c r="G39" t="n">
-        <v>-760.0870248569154</v>
+        <v>-585.9117073193447</v>
       </c>
       <c r="H39" t="n">
         <v>25614.3</v>
       </c>
       <c r="I39" t="n">
-        <v>26374.38702485691</v>
+        <v>26200.21170731934</v>
       </c>
       <c r="J39" t="n">
-        <v>25970.74552162999</v>
+        <v>25969.15289518415</v>
       </c>
       <c r="K39" t="n">
-        <v>26017.94150322692</v>
+        <v>25845.35881213519</v>
       </c>
     </row>
     <row r="40">
@@ -26768,19 +26768,19 @@
         <v>138.54</v>
       </c>
       <c r="G40" t="n">
-        <v>-784.4063051644698</v>
+        <v>-606.0232222493032</v>
       </c>
       <c r="H40" t="n">
         <v>25482.4</v>
       </c>
       <c r="I40" t="n">
-        <v>26266.80630516447</v>
+        <v>26088.4232222493</v>
       </c>
       <c r="J40" t="n">
-        <v>25847.71052654233</v>
+        <v>25846.06892016208</v>
       </c>
       <c r="K40" t="n">
-        <v>25901.49577862214</v>
+        <v>25724.75430208723</v>
       </c>
     </row>
     <row r="41">
@@ -26794,19 +26794,19 @@
         <v>138.44</v>
       </c>
       <c r="G41" t="n">
-        <v>-810.2259089348299</v>
+        <v>-627.4267452078966</v>
       </c>
       <c r="H41" t="n">
         <v>25820.7</v>
       </c>
       <c r="I41" t="n">
-        <v>26630.92590893483</v>
+        <v>26448.1267452079</v>
       </c>
       <c r="J41" t="n">
-        <v>26195.28768117997</v>
+        <v>26193.59465171572</v>
       </c>
       <c r="K41" t="n">
-        <v>26256.33822775486</v>
+        <v>26075.23209349218</v>
       </c>
     </row>
     <row r="42">
@@ -26820,19 +26820,19 @@
         <v>138.34</v>
       </c>
       <c r="G42" t="n">
-        <v>-837.6852959324424</v>
+        <v>-650.2459186094529</v>
       </c>
       <c r="H42" t="n">
         <v>25337.9</v>
       </c>
       <c r="I42" t="n">
-        <v>26175.58529593244</v>
+        <v>25988.14591860945</v>
       </c>
       <c r="J42" t="n">
-        <v>25722.20485154207</v>
+        <v>25720.45778880652</v>
       </c>
       <c r="K42" t="n">
-        <v>25791.28044439038</v>
+        <v>25605.58812980293</v>
       </c>
     </row>
     <row r="43">
@@ -26846,19 +26846,19 @@
         <v>138.24</v>
       </c>
       <c r="G43" t="n">
-        <v>-866.941606851673</v>
+        <v>-674.620431211406</v>
       </c>
       <c r="H43" t="n">
         <v>25660.4</v>
       </c>
       <c r="I43" t="n">
-        <v>26527.34160685167</v>
+        <v>26335.02043121141</v>
       </c>
       <c r="J43" t="n">
-        <v>26054.89238484179</v>
+        <v>26053.08849710634</v>
       </c>
       <c r="K43" t="n">
-        <v>26132.84922200989</v>
+        <v>25942.33193410507</v>
       </c>
     </row>
     <row r="44">
@@ -26872,19 +26872,19 @@
         <v>138.14</v>
       </c>
       <c r="G44" t="n">
-        <v>-898.1725550270712</v>
+        <v>-700.7086950976773</v>
       </c>
       <c r="H44" t="n">
         <v>25130.5</v>
       </c>
       <c r="I44" t="n">
-        <v>26028.67255502707</v>
+        <v>25831.20869509768</v>
       </c>
       <c r="J44" t="n">
-        <v>25535.68338528609</v>
+        <v>25533.81968326939</v>
       </c>
       <c r="K44" t="n">
-        <v>25623.48916974098</v>
+        <v>25427.88901182829</v>
       </c>
     </row>
     <row r="45">
@@ -26898,19 +26898,19 @@
         <v>138.04</v>
       </c>
       <c r="G45" t="n">
-        <v>-931.5799065655519</v>
+        <v>-728.6910769038477</v>
       </c>
       <c r="H45" t="n">
         <v>25320.6</v>
       </c>
       <c r="I45" t="n">
-        <v>26252.17990656555</v>
+        <v>26049.29107690385</v>
       </c>
       <c r="J45" t="n">
-        <v>25737.0140268023</v>
+        <v>25735.08730595594</v>
       </c>
       <c r="K45" t="n">
-        <v>25835.76587976325</v>
+        <v>25634.8037709479</v>
       </c>
     </row>
     <row r="46">
@@ -26924,19 +26924,19 @@
         <v>137.94</v>
       </c>
       <c r="G46" t="n">
-        <v>-262.7636942426216</v>
+        <v>-54.1438223283476</v>
       </c>
       <c r="H46" t="n">
         <v>24279.27</v>
       </c>
       <c r="I46" t="n">
-        <v>25246.66369424262</v>
+        <v>25038.04382232835</v>
       </c>
       <c r="J46" t="n">
-        <v>24707.49390857762</v>
+        <v>24705.50072945604</v>
       </c>
       <c r="K46" t="n">
-        <v>24818.439785665</v>
+        <v>24611.81309287231</v>
       </c>
     </row>
     <row r="47">
@@ -26950,19 +26950,19 @@
         <v>137.84</v>
       </c>
       <c r="G47" t="n">
-        <v>-268.477353269438</v>
+        <v>-53.79385445666412</v>
       </c>
       <c r="H47" t="n">
         <v>24270.6</v>
       </c>
       <c r="I47" t="n">
-        <v>25276.47735326944</v>
+        <v>25061.79385445666</v>
       </c>
       <c r="J47" t="n">
-        <v>24711.25646032982</v>
+        <v>24709.19312680302</v>
       </c>
       <c r="K47" t="n">
-        <v>24835.82089293962</v>
+        <v>24623.20072765364</v>
       </c>
     </row>
     <row r="48">
@@ -26976,19 +26976,19 @@
         <v>137.74</v>
       </c>
       <c r="G48" t="n">
-        <v>-324.1540246468721</v>
+        <v>-103.044682504973</v>
       </c>
       <c r="H48" t="n">
         <v>24270.12</v>
       </c>
       <c r="I48" t="n">
-        <v>25317.45402464687</v>
+        <v>25096.34468250497</v>
       </c>
       <c r="J48" t="n">
-        <v>24723.87940551864</v>
+        <v>24721.741940553</v>
       </c>
       <c r="K48" t="n">
-        <v>24863.69461912823</v>
+        <v>24644.72274195197</v>
       </c>
     </row>
     <row r="49">
@@ -27002,19 +27002,19 @@
         <v>137.64</v>
       </c>
       <c r="G49" t="n">
-        <v>-322.9443502613176</v>
+        <v>-95.01373422054894</v>
       </c>
       <c r="H49" t="n">
         <v>24269.63</v>
       </c>
       <c r="I49" t="n">
-        <v>25361.74435026132</v>
+        <v>25133.81373422055</v>
       </c>
       <c r="J49" t="n">
-        <v>24737.21529227953</v>
+        <v>24734.99941097262</v>
       </c>
       <c r="K49" t="n">
-        <v>24894.15905798179</v>
+        <v>24668.44432324793</v>
       </c>
     </row>
     <row r="50">
@@ -27028,19 +27028,19 @@
         <v>137.54</v>
       </c>
       <c r="G50" t="n">
-        <v>-700.9561919601401</v>
+        <v>-465.7715311666288</v>
       </c>
       <c r="H50" t="n">
         <v>24269.13</v>
       </c>
       <c r="I50" t="n">
-        <v>25409.75619196014</v>
+        <v>25174.57153116663</v>
       </c>
       <c r="J50" t="n">
-        <v>24751.32210377855</v>
+        <v>24749.02318328911</v>
       </c>
       <c r="K50" t="n">
-        <v>24927.56408818159</v>
+        <v>24694.67834787751</v>
       </c>
     </row>
     <row r="51">
@@ -27054,19 +27054,19 @@
         <v>137.44</v>
       </c>
       <c r="G51" t="n">
-        <v>-765.1768577378607</v>
+        <v>-522.263274685738</v>
       </c>
       <c r="H51" t="n">
         <v>24268.73</v>
       </c>
       <c r="I51" t="n">
-        <v>25462.07685773786</v>
+        <v>25219.16327468574</v>
       </c>
       <c r="J51" t="n">
-        <v>24766.37396203597</v>
+        <v>24763.98700799827</v>
       </c>
       <c r="K51" t="n">
-        <v>24964.43289570189</v>
+        <v>24723.90626668747</v>
       </c>
     </row>
     <row r="52">
@@ -27080,19 +27080,19 @@
         <v>137.34</v>
       </c>
       <c r="G52" t="n">
-        <v>-855.7786318839389</v>
+        <v>-604.6136216644918</v>
       </c>
       <c r="H52" t="n">
         <v>24268.44</v>
       </c>
       <c r="I52" t="n">
-        <v>25519.27863188394</v>
+        <v>25268.11362166449</v>
       </c>
       <c r="J52" t="n">
-        <v>24782.45194215534</v>
+        <v>24779.97155110757</v>
       </c>
       <c r="K52" t="n">
-        <v>25005.2666897286</v>
+        <v>24756.58207055692</v>
       </c>
     </row>
     <row r="53">
@@ -27106,19 +27106,19 @@
         <v>137.24</v>
       </c>
       <c r="G53" t="n">
-        <v>-925.9287135344384</v>
+        <v>-665.9357347895711</v>
       </c>
       <c r="H53" t="n">
         <v>24268.16</v>
       </c>
       <c r="I53" t="n">
-        <v>25581.92871353444</v>
+        <v>25321.93573478957</v>
       </c>
       <c r="J53" t="n">
-        <v>24799.53501746685</v>
+        <v>24796.95533475555</v>
       </c>
       <c r="K53" t="n">
-        <v>25050.55369606759</v>
+        <v>24793.14040003402</v>
       </c>
     </row>
     <row r="54">
@@ -27132,19 +27132,19 @@
         <v>137.14</v>
       </c>
       <c r="G54" t="n">
-        <v>-1067.835118780895</v>
+        <v>-798.3761420153569</v>
       </c>
       <c r="H54" t="n">
         <v>24267.9</v>
       </c>
       <c r="I54" t="n">
-        <v>25650.83511878089</v>
+        <v>25381.37614201536</v>
       </c>
       <c r="J54" t="n">
-        <v>24817.72116053248</v>
+        <v>24815.03583307644</v>
       </c>
       <c r="K54" t="n">
-        <v>25101.01395824841</v>
+        <v>24834.24030893892</v>
       </c>
     </row>
     <row r="55">
@@ -27158,19 +27158,19 @@
         <v>137.04</v>
       </c>
       <c r="G55" t="n">
-        <v>-1450.370775515752</v>
+        <v>-1170.737616810071</v>
       </c>
       <c r="H55" t="n">
         <v>24267.67</v>
       </c>
       <c r="I55" t="n">
-        <v>25726.97077551575</v>
+        <v>25447.33761681007</v>
       </c>
       <c r="J55" t="n">
-        <v>24837.11863050317</v>
+        <v>24834.32075371268</v>
       </c>
       <c r="K55" t="n">
-        <v>25157.52214501258</v>
+        <v>24880.68686309739</v>
       </c>
     </row>
     <row r="56">
@@ -27184,19 +27184,19 @@
         <v>136.94</v>
       </c>
       <c r="G56" t="n">
-        <v>-1005.199072182961</v>
+        <v>-714.6033337986883</v>
       </c>
       <c r="H56" t="n">
         <v>24267.56</v>
       </c>
       <c r="I56" t="n">
-        <v>25811.59907218296</v>
+        <v>25521.00333379869</v>
       </c>
       <c r="J56" t="n">
-        <v>24857.92748428142</v>
+        <v>24855.00954232862</v>
       </c>
       <c r="K56" t="n">
-        <v>25221.23158790154</v>
+        <v>24933.55379147007</v>
       </c>
     </row>
     <row r="57">
@@ -27210,19 +27210,19 @@
         <v>136.84</v>
       </c>
       <c r="G57" t="n">
-        <v>-666.9757459368593</v>
+        <v>-364.537208665377</v>
       </c>
       <c r="H57" t="n">
         <v>24267.38</v>
       </c>
       <c r="I57" t="n">
-        <v>25905.97574593686</v>
+        <v>25603.53720866538</v>
       </c>
       <c r="J57" t="n">
-        <v>24880.08135773825</v>
+        <v>24877.03515626397</v>
       </c>
       <c r="K57" t="n">
-        <v>25293.27438819861</v>
+        <v>24993.88205240141</v>
       </c>
     </row>
     <row r="58">
@@ -27236,19 +27236,19 @@
         <v>136.74</v>
       </c>
       <c r="G58" t="n">
-        <v>-1355.344637910257</v>
+        <v>-1040.078046370843</v>
       </c>
       <c r="H58" t="n">
         <v>24266.87</v>
       </c>
       <c r="I58" t="n">
-        <v>26011.64463791026</v>
+        <v>25696.37804637084</v>
       </c>
       <c r="J58" t="n">
-        <v>24903.45957441537</v>
+        <v>24900.2761646365</v>
       </c>
       <c r="K58" t="n">
-        <v>25375.05506349488</v>
+        <v>25062.97188173434</v>
       </c>
     </row>
     <row r="59">
@@ -27262,19 +27262,19 @@
         <v>136.64</v>
       </c>
       <c r="G59" t="n">
-        <v>-1646.77931195038</v>
+        <v>-1317.579762733909</v>
       </c>
       <c r="H59" t="n">
         <v>24266.42</v>
       </c>
       <c r="I59" t="n">
-        <v>26131.27931195038</v>
+        <v>25802.07976273391</v>
       </c>
       <c r="J59" t="n">
-        <v>24928.60965345078</v>
+        <v>24925.27924650339</v>
       </c>
       <c r="K59" t="n">
-        <v>25469.0896584996</v>
+        <v>25143.22051623051</v>
       </c>
     </row>
     <row r="60">
@@ -27288,19 +27288,19 @@
         <v>136.54</v>
       </c>
       <c r="G60" t="n">
-        <v>-1159.810431676422</v>
+        <v>-815.4382444800358</v>
       </c>
       <c r="H60" t="n">
         <v>24266.22</v>
       </c>
       <c r="I60" t="n">
-        <v>26268.01043167642</v>
+        <v>25923.63824448004</v>
       </c>
       <c r="J60" t="n">
-        <v>24955.90030690072</v>
+        <v>24952.41217712323</v>
       </c>
       <c r="K60" t="n">
-        <v>25578.3301247757</v>
+        <v>25237.4460673568</v>
       </c>
     </row>
     <row r="61">
@@ -27314,19 +27314,19 @@
         <v>136.44</v>
       </c>
       <c r="G61" t="n">
-        <v>-1469.093387337478</v>
+        <v>-1108.160929297122</v>
       </c>
       <c r="H61" t="n">
         <v>24265.86</v>
       </c>
       <c r="I61" t="n">
-        <v>26425.29338733748</v>
+        <v>26064.36092929712</v>
       </c>
       <c r="J61" t="n">
-        <v>24985.12504056088</v>
+        <v>24981.46741629896</v>
       </c>
       <c r="K61" t="n">
-        <v>25706.0283467766</v>
+        <v>25348.75351299817</v>
       </c>
     </row>
     <row r="62">
@@ -27340,19 +27340,19 @@
         <v>136.34</v>
       </c>
       <c r="G62" t="n">
-        <v>-1502.848610211768</v>
+        <v>-1123.815166159759</v>
       </c>
       <c r="H62" t="n">
         <v>24265.35</v>
       </c>
       <c r="I62" t="n">
-        <v>26608.34861021177</v>
+        <v>26229.31516615976</v>
       </c>
       <c r="J62" t="n">
-        <v>25016.5265036968</v>
+        <v>25012.68644411642</v>
       </c>
       <c r="K62" t="n">
-        <v>25857.17210651496</v>
+        <v>25481.97872204334</v>
       </c>
     </row>
     <row r="63">
@@ -27366,19 +27366,19 @@
         <v>136.24</v>
       </c>
       <c r="G63" t="n">
-        <v>-898.4712496525062</v>
+        <v>-499.6598630684093</v>
       </c>
       <c r="H63" t="n">
         <v>24264.84</v>
       </c>
       <c r="I63" t="n">
-        <v>26824.5712496525</v>
+        <v>26425.75986306841</v>
       </c>
       <c r="J63" t="n">
-        <v>25050.52177440163</v>
+        <v>25046.48503076104</v>
       </c>
       <c r="K63" t="n">
-        <v>26038.88947525088</v>
+        <v>25644.11483230737</v>
       </c>
     </row>
     <row r="64">
@@ -27392,19 +27392,19 @@
         <v>136.14</v>
       </c>
       <c r="G64" t="n">
-        <v>-1249.690030861104</v>
+        <v>-829.3559375136356</v>
       </c>
       <c r="H64" t="n">
         <v>24264</v>
       </c>
       <c r="I64" t="n">
-        <v>27084.09003086111</v>
+        <v>26663.75593751364</v>
       </c>
       <c r="J64" t="n">
-        <v>25087.08882229625</v>
+        <v>25082.83968220674</v>
       </c>
       <c r="K64" t="n">
-        <v>26261.00120856486</v>
+        <v>25844.9162553069</v>
       </c>
     </row>
     <row r="65">
@@ -27418,19 +27418,19 @@
         <v>136.04</v>
       </c>
       <c r="G65" t="n">
-        <v>-1074.238791086322</v>
+        <v>-630.7472754132068</v>
       </c>
       <c r="H65" t="n">
         <v>24262.92</v>
       </c>
       <c r="I65" t="n">
-        <v>27402.73879108632</v>
+        <v>26959.24727541321</v>
       </c>
       <c r="J65" t="n">
-        <v>25126.67446422741</v>
+        <v>25122.19557771926</v>
       </c>
       <c r="K65" t="n">
-        <v>26538.98432685891</v>
+        <v>26099.97169769394</v>
       </c>
     </row>
     <row r="66">
@@ -27444,19 +27444,19 @@
         <v>135.94</v>
       </c>
       <c r="G66" t="n">
-        <v>-1044.601325362182</v>
+        <v>-576.8159764272496</v>
       </c>
       <c r="H66" t="n">
         <v>24261.7</v>
       </c>
       <c r="I66" t="n">
-        <v>27805.30132536218</v>
+        <v>27337.51597642725</v>
       </c>
       <c r="J66" t="n">
-        <v>25169.79422907996</v>
+        <v>25165.06641594002</v>
       </c>
       <c r="K66" t="n">
-        <v>26897.20709628222</v>
+        <v>26434.14956048723</v>
       </c>
     </row>
     <row r="67">
@@ -27470,19 +27470,19 @@
         <v>135.84</v>
       </c>
       <c r="G67" t="n">
-        <v>-1275.906081387304</v>
+        <v>-783.9386424035147</v>
       </c>
       <c r="H67" t="n">
         <v>24260.17</v>
       </c>
       <c r="I67" t="n">
-        <v>28331.5060813873</v>
+        <v>27839.53864240351</v>
       </c>
       <c r="J67" t="n">
-        <v>25216.76468588111</v>
+        <v>25211.7667250054</v>
       </c>
       <c r="K67" t="n">
-        <v>27374.91139550619</v>
+        <v>26887.94191739811</v>
       </c>
     </row>
     <row r="68">
@@ -27496,19 +27496,19 @@
         <v>135.74</v>
       </c>
       <c r="G68" t="n">
-        <v>-1097.53794441108</v>
+        <v>-584.0377543054237</v>
       </c>
       <c r="H68" t="n">
         <v>24258.4</v>
       </c>
       <c r="I68" t="n">
-        <v>29046.63794441108</v>
+        <v>28533.13775430542</v>
       </c>
       <c r="J68" t="n">
-        <v>25268.22898149524</v>
+        <v>25262.9373853531</v>
       </c>
       <c r="K68" t="n">
-        <v>28036.80896291584</v>
+        <v>27528.60036895232</v>
       </c>
     </row>
     <row r="69">
@@ -27522,19 +27522,19 @@
         <v>135.64</v>
       </c>
       <c r="G69" t="n">
-        <v>-1337.71297634851</v>
+        <v>-809.8168118380599</v>
       </c>
       <c r="H69" t="n">
         <v>24256.22</v>
       </c>
       <c r="I69" t="n">
-        <v>30055.61297634851</v>
+        <v>29527.71681183806</v>
       </c>
       <c r="J69" t="n">
-        <v>25324.69660524233</v>
+        <v>25319.08538675237</v>
       </c>
       <c r="K69" t="n">
-        <v>28987.13637110619</v>
+        <v>28464.8514250857</v>
       </c>
     </row>
     <row r="70">
@@ -27548,19 +27548,19 @@
         <v>135.54</v>
       </c>
       <c r="G70" t="n">
-        <v>-803.0014660123488</v>
+        <v>-274.8502644255241</v>
       </c>
       <c r="H70" t="n">
         <v>24253.48</v>
       </c>
       <c r="I70" t="n">
-        <v>31520.60146601235</v>
+        <v>30992.45026442552</v>
       </c>
       <c r="J70" t="n">
-        <v>25386.82878598349</v>
+        <v>25380.86923251464</v>
       </c>
       <c r="K70" t="n">
-        <v>30387.25268002886</v>
+        <v>29865.06103191088</v>
       </c>
     </row>
     <row r="71">
@@ -27574,19 +27574,19 @@
         <v>135.44</v>
       </c>
       <c r="G71" t="n">
-        <v>-894.6934425601576</v>
+        <v>-390.0266009412298</v>
       </c>
       <c r="H71" t="n">
         <v>24249.79</v>
       </c>
       <c r="I71" t="n">
-        <v>33674.49344256016</v>
+        <v>33169.82660094123</v>
       </c>
       <c r="J71" t="n">
-        <v>25455.2114927637</v>
+        <v>25448.87197503351</v>
       </c>
       <c r="K71" t="n">
-        <v>32469.07194979646</v>
+        <v>31970.74462590772</v>
       </c>
     </row>
     <row r="72">
@@ -27600,19 +27600,19 @@
         <v>135.34</v>
       </c>
       <c r="G72" t="n">
-        <v>-267.7868736636156</v>
+        <v>178.339114912982</v>
       </c>
       <c r="H72" t="n">
         <v>24244.72</v>
       </c>
       <c r="I72" t="n">
-        <v>36817.88687366361</v>
+        <v>36371.76088508702</v>
       </c>
       <c r="J72" t="n">
-        <v>25530.6064391092</v>
+        <v>25523.85227682254</v>
       </c>
       <c r="K72" t="n">
-        <v>35532.00043455441</v>
+        <v>35092.62860826448</v>
       </c>
     </row>
     <row r="73">
@@ -27626,19 +27626,19 @@
         <v>135.24</v>
       </c>
       <c r="G73" t="n">
-        <v>40.57320765502664</v>
+        <v>382.1410577654824</v>
       </c>
       <c r="H73" t="n">
         <v>24237.64</v>
       </c>
       <c r="I73" t="n">
-        <v>41279.92679234497</v>
+        <v>40938.35894223452</v>
       </c>
       <c r="J73" t="n">
-        <v>25613.83346343449</v>
+        <v>25606.62703746122</v>
       </c>
       <c r="K73" t="n">
-        <v>39903.73332891048</v>
+        <v>39569.37190477329</v>
       </c>
     </row>
     <row r="74">
@@ -27652,19 +27652,19 @@
         <v>135.14</v>
       </c>
       <c r="G74" t="n">
-        <v>41.42843151932175</v>
+        <v>224.7897065513971</v>
       </c>
       <c r="H74" t="n">
         <v>24227.62</v>
       </c>
       <c r="I74" t="n">
-        <v>47327.27156848068</v>
+        <v>47143.9102934486</v>
       </c>
       <c r="J74" t="n">
-        <v>25705.75558781564</v>
+        <v>25698.05676987315</v>
       </c>
       <c r="K74" t="n">
-        <v>45849.13598066504</v>
+        <v>45673.47352357545</v>
       </c>
     </row>
     <row r="75">
@@ -27678,19 +27678,19 @@
         <v>135.04</v>
       </c>
       <c r="G75" t="n">
-        <v>520.9855244375431</v>
+        <v>491.1367228421004</v>
       </c>
       <c r="H75" t="n">
         <v>24213.82</v>
       </c>
       <c r="I75" t="n">
-        <v>55023.31447556246</v>
+        <v>55053.1632771579</v>
       </c>
       <c r="J75" t="n">
-        <v>25807.78261957447</v>
+        <v>25799.54985438079</v>
       </c>
       <c r="K75" t="n">
-        <v>53429.35185598799</v>
+        <v>53467.43342277711</v>
       </c>
     </row>
     <row r="76">
@@ -27704,19 +27704,19 @@
         <v>134.94</v>
       </c>
       <c r="G76" t="n">
-        <v>-680.1327149336139</v>
+        <v>-971.5200292841182</v>
       </c>
       <c r="H76" t="n">
         <v>24195.04</v>
       </c>
       <c r="I76" t="n">
-        <v>64072.03271493362</v>
+        <v>64363.42002928412</v>
       </c>
       <c r="J76" t="n">
-        <v>25921.57099625635</v>
+        <v>25912.76368385668</v>
       </c>
       <c r="K76" t="n">
-        <v>62345.50171867727</v>
+        <v>62645.69634542744</v>
       </c>
     </row>
     <row r="77">
@@ -27730,19 +27730,19 @@
         <v>134.84</v>
       </c>
       <c r="G77" t="n">
-        <v>-40.31287357048132</v>
+        <v>-626.7339548244781</v>
       </c>
       <c r="H77" t="n">
         <v>24170.57</v>
       </c>
       <c r="I77" t="n">
-        <v>73714.21287357048</v>
+        <v>74300.63395482447</v>
       </c>
       <c r="J77" t="n">
-        <v>26050.09530349869</v>
+        <v>26040.67869339776</v>
       </c>
       <c r="K77" t="n">
-        <v>71834.68757007178</v>
+        <v>72430.52526142669</v>
       </c>
     </row>
     <row r="78">
@@ -27756,19 +27756,19 @@
         <v>134.74</v>
       </c>
       <c r="G78" t="n">
-        <v>751.9048075618193</v>
+        <v>-141.5954679548449</v>
       </c>
       <c r="H78" t="n">
         <v>24139.56</v>
       </c>
       <c r="I78" t="n">
-        <v>82767.29519243818</v>
+        <v>83660.79546795484</v>
       </c>
       <c r="J78" t="n">
-        <v>26197.34897598379</v>
+        <v>26187.30407673886</v>
       </c>
       <c r="K78" t="n">
-        <v>80709.50621645438</v>
+        <v>81613.05139121599</v>
       </c>
     </row>
     <row r="79">
@@ -27782,19 +27782,19 @@
         <v>134.64</v>
       </c>
       <c r="G79" t="n">
-        <v>1458.924126397353</v>
+        <v>272.3947884761292</v>
       </c>
       <c r="H79" t="n">
         <v>24101.36</v>
       </c>
       <c r="I79" t="n">
-        <v>89842.77587360264</v>
+        <v>91029.30521152387</v>
       </c>
       <c r="J79" t="n">
-        <v>26369.19683267976</v>
+        <v>26358.54051209449</v>
       </c>
       <c r="K79" t="n">
-        <v>87574.93904092288</v>
+        <v>88772.12469942938</v>
       </c>
     </row>
     <row r="80">
@@ -27808,19 +27808,19 @@
         <v>134.54</v>
       </c>
       <c r="G80" t="n">
-        <v>155.8292305408104</v>
+        <v>-1281.091234763444</v>
       </c>
       <c r="H80" t="n">
         <v>24057.11</v>
       </c>
       <c r="I80" t="n">
-        <v>93707.2707694592</v>
+        <v>95144.19123476345</v>
       </c>
       <c r="J80" t="n">
-        <v>26575.79393890357</v>
+        <v>26564.61974157633</v>
       </c>
       <c r="K80" t="n">
-        <v>91188.58683055562</v>
+        <v>92636.68149318712</v>
       </c>
     </row>
     <row r="81">
@@ -27834,19 +27834,19 @@
         <v>134.44</v>
       </c>
       <c r="G81" t="n">
-        <v>1208.325286108215</v>
+        <v>-408.3213899115508</v>
       </c>
       <c r="H81" t="n">
         <v>24009.49</v>
       </c>
       <c r="I81" t="n">
-        <v>93660.17471389179</v>
+        <v>95276.82138991155</v>
       </c>
       <c r="J81" t="n">
-        <v>26832.73448712341</v>
+        <v>26821.29448164431</v>
       </c>
       <c r="K81" t="n">
-        <v>90836.93022676838</v>
+        <v>92465.01690826725</v>
       </c>
     </row>
     <row r="82">
@@ -27860,19 +27860,19 @@
         <v>134.34</v>
       </c>
       <c r="G82" t="n">
-        <v>-280.851806400955</v>
+        <v>-1983.961619220339</v>
       </c>
       <c r="H82" t="n">
         <v>23961.18</v>
       </c>
       <c r="I82" t="n">
-        <v>89769.75180640095</v>
+        <v>91472.86161922033</v>
       </c>
       <c r="J82" t="n">
-        <v>27161.95373917238</v>
+        <v>27150.81683165713</v>
       </c>
       <c r="K82" t="n">
-        <v>86568.97806722857</v>
+        <v>88283.2247875632</v>
       </c>
     </row>
     <row r="83">
@@ -27886,19 +27886,19 @@
         <v>134.24</v>
       </c>
       <c r="G83" t="n">
-        <v>-1208.322879710176</v>
+        <v>-2893.71297290294</v>
       </c>
       <c r="H83" t="n">
         <v>23915.31</v>
       </c>
       <c r="I83" t="n">
-        <v>82864.02287971017</v>
+        <v>84549.41297290294</v>
       </c>
       <c r="J83" t="n">
-        <v>27596.50084059838</v>
+        <v>27586.83930918093</v>
       </c>
       <c r="K83" t="n">
-        <v>79182.8320391118</v>
+        <v>80877.88366372201</v>
       </c>
     </row>
     <row r="84">
@@ -27912,19 +27912,19 @@
         <v>134.14</v>
       </c>
       <c r="G84" t="n">
-        <v>-1419.526601079007</v>
+        <v>-2988.918362519864</v>
       </c>
       <c r="H84" t="n">
         <v>23874.62</v>
       </c>
       <c r="I84" t="n">
-        <v>74280.62660107901</v>
+        <v>75850.01836251987</v>
       </c>
       <c r="J84" t="n">
-        <v>28187.23986726766</v>
+        <v>28181.29584912876</v>
       </c>
       <c r="K84" t="n">
-        <v>69968.00673381136</v>
+        <v>71543.34251339111</v>
       </c>
     </row>
     <row r="85">
@@ -27938,19 +27938,19 @@
         <v>134.04</v>
       </c>
       <c r="G85" t="n">
-        <v>-266.467043394674</v>
+        <v>-1645.119460156755</v>
       </c>
       <c r="H85" t="n">
         <v>23839.91</v>
       </c>
       <c r="I85" t="n">
-        <v>65494.46704339467</v>
+        <v>66873.11946015675</v>
       </c>
       <c r="J85" t="n">
-        <v>29013.82157093985</v>
+        <v>29015.54873043458</v>
       </c>
       <c r="K85" t="n">
-        <v>60320.55547245483</v>
+        <v>61697.48072972217</v>
       </c>
     </row>
     <row r="86">
@@ -27964,19 +27964,19 @@
         <v>133.94</v>
       </c>
       <c r="G86" t="n">
-        <v>37.86489463433099</v>
+        <v>-1111.370550390682</v>
       </c>
       <c r="H86" t="n">
         <v>23810.89</v>
       </c>
       <c r="I86" t="n">
-        <v>57787.13510536567</v>
+        <v>58936.37055039068</v>
       </c>
       <c r="J86" t="n">
-        <v>30204.51621751941</v>
+        <v>30220.22025862023</v>
       </c>
       <c r="K86" t="n">
-        <v>51393.50888784626</v>
+        <v>52527.04029177046</v>
       </c>
     </row>
     <row r="87">
@@ -27990,19 +27990,19 @@
         <v>133.84</v>
       </c>
       <c r="G87" t="n">
-        <v>632.2609856423078</v>
+        <v>-287.8759434400417</v>
       </c>
       <c r="H87" t="n">
         <v>23786.85</v>
       </c>
       <c r="I87" t="n">
-        <v>52072.93901435769</v>
+        <v>52993.07594344004</v>
       </c>
       <c r="J87" t="n">
-        <v>31961.61010048373</v>
+        <v>32000.09158891131</v>
       </c>
       <c r="K87" t="n">
-        <v>43898.17891387396</v>
+        <v>44779.83435452873</v>
       </c>
     </row>
     <row r="88">
@@ -28016,19 +28016,19 @@
         <v>133.74</v>
       </c>
       <c r="G88" t="n">
-        <v>608.335047758439</v>
+        <v>-114.4385715020908</v>
       </c>
       <c r="H88" t="n">
         <v>23766.62</v>
       </c>
       <c r="I88" t="n">
-        <v>48904.06495224156</v>
+        <v>49626.83857150209</v>
       </c>
       <c r="J88" t="n">
-        <v>34585.5527831723</v>
+        <v>34656.87652739207</v>
       </c>
       <c r="K88" t="n">
-        <v>38085.13216906926</v>
+        <v>38736.58204411003</v>
       </c>
     </row>
     <row r="89">
@@ -28042,19 +28042,19 @@
         <v>133.64</v>
       </c>
       <c r="G89" t="n">
-        <v>729.4104806039468</v>
+        <v>156.3386801009692</v>
       </c>
       <c r="H89" t="n">
         <v>23748.59</v>
       </c>
       <c r="I89" t="n">
-        <v>48590.18951939605</v>
+        <v>49163.26131989903</v>
       </c>
       <c r="J89" t="n">
-        <v>38483.06017302025</v>
+        <v>38594.95533776908</v>
       </c>
       <c r="K89" t="n">
-        <v>33855.7193463758</v>
+        <v>34316.89598212994</v>
       </c>
     </row>
     <row r="90">
@@ -28068,19 +28068,19 @@
         <v>133.54</v>
       </c>
       <c r="G90" t="n">
-        <v>1385.939923422142</v>
+        <v>917.8053489239101</v>
       </c>
       <c r="H90" t="n">
         <v>23730.79</v>
       </c>
       <c r="I90" t="n">
-        <v>51324.56007657786</v>
+        <v>51792.69465107609</v>
       </c>
       <c r="J90" t="n">
-        <v>44133.70413969466</v>
+        <v>44285.24692696278</v>
       </c>
       <c r="K90" t="n">
-        <v>30921.6459368832</v>
+        <v>31238.23772411331</v>
       </c>
     </row>
     <row r="91">
@@ -28094,19 +28094,19 @@
         <v>133.44</v>
       </c>
       <c r="G91" t="n">
-        <v>-716.7645119162626</v>
+        <v>-1104.83572642276</v>
       </c>
       <c r="H91" t="n">
         <v>23711.27</v>
       </c>
       <c r="I91" t="n">
-        <v>57220.66451191626</v>
+        <v>57608.73572642276</v>
       </c>
       <c r="J91" t="n">
-        <v>51987.51422803442</v>
+        <v>52161.50076612829</v>
       </c>
       <c r="K91" t="n">
-        <v>28944.42028388185</v>
+        <v>29158.50496029447</v>
       </c>
     </row>
     <row r="92">
@@ -28120,19 +28120,19 @@
         <v>133.34</v>
       </c>
       <c r="G92" t="n">
-        <v>4.241346436785534</v>
+        <v>-298.7853238846001</v>
       </c>
       <c r="H92" t="n">
         <v>23688.24</v>
       </c>
       <c r="I92" t="n">
-        <v>66215.95865356321</v>
+        <v>66518.9853238846</v>
       </c>
       <c r="J92" t="n">
-        <v>62282.08673607494</v>
+        <v>62439.91164308523</v>
       </c>
       <c r="K92" t="n">
-        <v>27622.11191748828</v>
+        <v>27767.31368079937</v>
       </c>
     </row>
     <row r="93">
@@ -28146,19 +28146,19 @@
         <v>133.24</v>
       </c>
       <c r="G93" t="n">
-        <v>-1122.297645561965</v>
+        <v>-1307.106921328246</v>
       </c>
       <c r="H93" t="n">
         <v>23659.34</v>
       </c>
       <c r="I93" t="n">
-        <v>77873.39764556197</v>
+        <v>78058.20692132825</v>
       </c>
       <c r="J93" t="n">
-        <v>74809.21975723533</v>
+        <v>74893.5082711693</v>
       </c>
       <c r="K93" t="n">
-        <v>26723.51788832664</v>
+        <v>26824.03865015896</v>
       </c>
     </row>
     <row r="94">
@@ -28172,19 +28172,19 @@
         <v>133.14</v>
       </c>
       <c r="G94" t="n">
-        <v>-471.3720110031427</v>
+        <v>-491.8852945529798</v>
       </c>
       <c r="H94" t="n">
         <v>23622.4</v>
       </c>
       <c r="I94" t="n">
-        <v>91186.07201100314</v>
+        <v>91206.58529455298</v>
       </c>
       <c r="J94" t="n">
-        <v>88719.08095341083</v>
+        <v>88667.64286723742</v>
       </c>
       <c r="K94" t="n">
-        <v>26089.39105759232</v>
+        <v>26161.34242731555</v>
       </c>
     </row>
     <row r="95">
@@ -28198,19 +28198,19 @@
         <v>133.04</v>
       </c>
       <c r="G95" t="n">
-        <v>-2628.264402914778</v>
+        <v>-2450.907650958368</v>
       </c>
       <c r="H95" t="n">
         <v>23576.35</v>
       </c>
       <c r="I95" t="n">
-        <v>104523.2644029148</v>
+        <v>104345.9076509584</v>
       </c>
       <c r="J95" t="n">
-        <v>102481.3598826086</v>
+        <v>102250.4596721937</v>
       </c>
       <c r="K95" t="n">
-        <v>25618.25452030614</v>
+        <v>25671.79797876471</v>
       </c>
     </row>
     <row r="96">
@@ -28224,19 +28224,19 @@
         <v>132.94</v>
       </c>
       <c r="G96" t="n">
-        <v>-26.43723670317559</v>
+        <v>344.3810711253027</v>
       </c>
       <c r="H96" t="n">
         <v>23520.88</v>
       </c>
       <c r="I96" t="n">
-        <v>115825.4372367032</v>
+        <v>115454.6189288747</v>
       </c>
       <c r="J96" t="n">
-        <v>114098.0436539021</v>
+        <v>113685.8657394726</v>
       </c>
       <c r="K96" t="n">
-        <v>25248.27358280104</v>
+        <v>25289.63318940206</v>
       </c>
     </row>
     <row r="97">
@@ -28250,19 +28250,19 @@
         <v>132.84</v>
       </c>
       <c r="G97" t="n">
-        <v>-633.2162578422431</v>
+        <v>-123.7393424757174</v>
       </c>
       <c r="H97" t="n">
         <v>23456.83</v>
       </c>
       <c r="I97" t="n">
-        <v>123053.2162578422</v>
+        <v>122543.7393424757</v>
       </c>
       <c r="J97" t="n">
-        <v>121566.9058541559</v>
+        <v>121024.454696436</v>
       </c>
       <c r="K97" t="n">
-        <v>24943.14040368633</v>
+        <v>24976.11464603976</v>
       </c>
     </row>
     <row r="98">
@@ -28276,19 +28276,19 @@
         <v>132.74</v>
       </c>
       <c r="G98" t="n">
-        <v>-847.254033613237</v>
+        <v>-294.8900122033665</v>
       </c>
       <c r="H98" t="n">
         <v>23387.77</v>
       </c>
       <c r="I98" t="n">
-        <v>124754.2540336132</v>
+        <v>124201.8900122034</v>
       </c>
       <c r="J98" t="n">
-        <v>123458.2654125064</v>
+        <v>122878.9477387197</v>
       </c>
       <c r="K98" t="n">
-        <v>24683.75862110684</v>
+        <v>24710.71227348368</v>
       </c>
     </row>
     <row r="99">
@@ -28302,19 +28302,19 @@
         <v>132.64</v>
       </c>
       <c r="G99" t="n">
-        <v>996.3643019874289</v>
+        <v>1483.952632450411</v>
       </c>
       <c r="H99" t="n">
         <v>23317.85</v>
       </c>
       <c r="I99" t="n">
-        <v>120513.6356980126</v>
+        <v>120026.0473675496</v>
       </c>
       <c r="J99" t="n">
-        <v>119371.4583700546</v>
+        <v>118861.4095516902</v>
       </c>
       <c r="K99" t="n">
-        <v>24460.02732795796</v>
+        <v>24482.48781585934</v>
       </c>
     </row>
     <row r="100">
@@ -28328,19 +28328,19 @@
         <v>132.54</v>
       </c>
       <c r="G100" t="n">
-        <v>918.9035709083983</v>
+        <v>1257.582514594324</v>
       </c>
       <c r="H100" t="n">
         <v>23251.28</v>
       </c>
       <c r="I100" t="n">
-        <v>111087.0964290916</v>
+        <v>110748.4174854057</v>
       </c>
       <c r="J100" t="n">
-        <v>110071.5494876127</v>
+        <v>109713.872168858</v>
       </c>
       <c r="K100" t="n">
-        <v>24266.82694147893</v>
+        <v>24285.82531654771</v>
       </c>
     </row>
     <row r="101">
@@ -28354,19 +28354,19 @@
         <v>132.44</v>
       </c>
       <c r="G101" t="n">
-        <v>-446.5442851903354</v>
+        <v>-292.5782954667666</v>
       </c>
       <c r="H101" t="n">
         <v>23192.71</v>
       </c>
       <c r="I101" t="n">
-        <v>98150.74428519033</v>
+        <v>97996.77829546676</v>
       </c>
       <c r="J101" t="n">
-        <v>97241.01591973761</v>
+        <v>97070.78732660529</v>
       </c>
       <c r="K101" t="n">
-        <v>24102.43836545273</v>
+        <v>24118.70096886146</v>
       </c>
     </row>
     <row r="102">
@@ -28380,19 +28380,19 @@
         <v>132.34</v>
       </c>
       <c r="G102" t="n">
-        <v>-917.997290328567</v>
+        <v>-932.5439748746139</v>
       </c>
       <c r="H102" t="n">
         <v>23144.69</v>
       </c>
       <c r="I102" t="n">
-        <v>83777.09729032857</v>
+        <v>83791.64397487462</v>
       </c>
       <c r="J102" t="n">
-        <v>82956.89003043495</v>
+        <v>82957.37916173936</v>
       </c>
       <c r="K102" t="n">
-        <v>23964.89725989363</v>
+        <v>23978.95481313526</v>
       </c>
     </row>
     <row r="103">
@@ -28406,19 +28406,19 @@
         <v>132.24</v>
       </c>
       <c r="G103" t="n">
-        <v>982.3882959921757</v>
+        <v>851.5115147696924</v>
       </c>
       <c r="H103" t="n">
         <v>23106.65</v>
       </c>
       <c r="I103" t="n">
-        <v>69867.51170400782</v>
+        <v>69998.3884852303</v>
       </c>
       <c r="J103" t="n">
-        <v>69123.82908596065</v>
+        <v>69242.45399410227</v>
       </c>
       <c r="K103" t="n">
-        <v>23850.33261804718</v>
+        <v>23862.58449112804</v>
       </c>
     </row>
     <row r="104">
@@ -28432,19 +28432,19 @@
         <v>132.14</v>
       </c>
       <c r="G104" t="n">
-        <v>1091.85439281899</v>
+        <v>907.8998512304825</v>
       </c>
       <c r="H104" t="n">
         <v>23077.38</v>
       </c>
       <c r="I104" t="n">
-        <v>57755.34560718101</v>
+        <v>57939.30014876951</v>
       </c>
       <c r="J104" t="n">
-        <v>57077.6666168933</v>
+        <v>57250.86732540961</v>
       </c>
       <c r="K104" t="n">
-        <v>23755.05899028771</v>
+        <v>23765.81282335991</v>
       </c>
     </row>
     <row r="105">
@@ -28458,19 +28458,19 @@
         <v>132.04</v>
       </c>
       <c r="G105" t="n">
-        <v>148.4931845070896</v>
+        <v>-35.58232919350849</v>
       </c>
       <c r="H105" t="n">
         <v>23056.15</v>
       </c>
       <c r="I105" t="n">
-        <v>48074.40681549291</v>
+        <v>48258.48232919351</v>
       </c>
       <c r="J105" t="n">
-        <v>47454.10532813717</v>
+        <v>47628.68355898856</v>
       </c>
       <c r="K105" t="n">
-        <v>23676.45148735574</v>
+        <v>23685.94877020495</v>
       </c>
     </row>
     <row r="106">
@@ -28484,19 +28484,19 @@
         <v>131.94</v>
       </c>
       <c r="G106" t="n">
-        <v>354.0943578698716</v>
+        <v>201.9559118290344</v>
       </c>
       <c r="H106" t="n">
         <v>23041.18</v>
       </c>
       <c r="I106" t="n">
-        <v>40858.40564213013</v>
+        <v>41010.54408817097</v>
       </c>
       <c r="J106" t="n">
-        <v>40288.33099746525</v>
+        <v>40432.03617184926</v>
       </c>
       <c r="K106" t="n">
-        <v>23611.25464466488</v>
+        <v>23619.68791632171</v>
       </c>
     </row>
     <row r="107">
@@ -28510,19 +28510,19 @@
         <v>131.84</v>
       </c>
       <c r="G107" t="n">
-        <v>1338.601258373536</v>
+        <v>1229.766766956833</v>
       </c>
       <c r="H107" t="n">
         <v>23030.15</v>
       </c>
       <c r="I107" t="n">
-        <v>35763.79874162647</v>
+        <v>35872.63323304317</v>
       </c>
       <c r="J107" t="n">
-        <v>35237.96595238106</v>
+        <v>35339.27563531283</v>
       </c>
       <c r="K107" t="n">
-        <v>23555.98278924541</v>
+        <v>23563.50759773034</v>
       </c>
     </row>
     <row r="108">
@@ -28536,19 +28536,19 @@
         <v>131.74</v>
       </c>
       <c r="G108" t="n">
-        <v>1494.121696182017</v>
+        <v>1425.758475825816</v>
       </c>
       <c r="H108" t="n">
         <v>23021.71</v>
       </c>
       <c r="I108" t="n">
-        <v>32298.67830381799</v>
+        <v>32367.04152417419</v>
       </c>
       <c r="J108" t="n">
-        <v>31812.03496446081</v>
+        <v>31873.65473676208</v>
       </c>
       <c r="K108" t="n">
-        <v>23508.35333935718</v>
+        <v>23515.09678741211</v>
       </c>
     </row>
     <row r="109">
@@ -28562,19 +28562,19 @@
         <v>131.64</v>
       </c>
       <c r="G109" t="n">
-        <v>708.4086959169836</v>
+        <v>671.1322547328891</v>
       </c>
       <c r="H109" t="n">
         <v>23015.46</v>
       </c>
       <c r="I109" t="n">
-        <v>29984.69130408301</v>
+        <v>30021.96774526711</v>
       </c>
       <c r="J109" t="n">
-        <v>29532.93941224441</v>
+        <v>29564.14886411087</v>
       </c>
       <c r="K109" t="n">
-        <v>23467.21189183861</v>
+        <v>23473.27888115624</v>
       </c>
     </row>
     <row r="110">
@@ -28588,19 +28588,19 @@
         <v>131.54</v>
       </c>
       <c r="G110" t="n">
-        <v>863.3282781193448</v>
+        <v>846.8444032967345</v>
       </c>
       <c r="H110" t="n">
         <v>23010.74</v>
       </c>
       <c r="I110" t="n">
-        <v>28436.17172188066</v>
+        <v>28452.65559670327</v>
       </c>
       <c r="J110" t="n">
-        <v>28015.62958608614</v>
+        <v>28026.63558083956</v>
       </c>
       <c r="K110" t="n">
-        <v>23431.28213579452</v>
+        <v>23436.76001586371</v>
       </c>
     </row>
     <row r="111">
@@ -28614,19 +28614,19 @@
         <v>131.44</v>
       </c>
       <c r="G111" t="n">
-        <v>325.4429672257684</v>
+        <v>321.3915696968652</v>
       </c>
       <c r="H111" t="n">
         <v>23007.04</v>
       </c>
       <c r="I111" t="n">
-        <v>27378.15703277423</v>
+        <v>27382.20843030313</v>
       </c>
       <c r="J111" t="n">
-        <v>26985.65093724597</v>
+        <v>26984.74024957564</v>
       </c>
       <c r="K111" t="n">
-        <v>23399.54609552826</v>
+        <v>23404.50818072749</v>
       </c>
     </row>
     <row r="112">
@@ -28640,19 +28640,19 @@
         <v>131.34</v>
       </c>
       <c r="G112" t="n">
-        <v>-19.87882364663892</v>
+        <v>-17.21591087845809</v>
       </c>
       <c r="H112" t="n">
         <v>23004.24</v>
       </c>
       <c r="I112" t="n">
-        <v>26630.57882364664</v>
+        <v>26627.91591087846</v>
       </c>
       <c r="J112" t="n">
-        <v>26263.35710861612</v>
+        <v>26256.18592786009</v>
       </c>
       <c r="K112" t="n">
-        <v>23371.46171503052</v>
+        <v>23375.96998301837</v>
       </c>
     </row>
     <row r="113">
@@ -28666,19 +28666,19 @@
         <v>131.24</v>
       </c>
       <c r="G113" t="n">
-        <v>-299.7449076725425</v>
+        <v>-293.8346733342587</v>
       </c>
       <c r="H113" t="n">
         <v>23002.1</v>
       </c>
       <c r="I113" t="n">
-        <v>26081.34490767254</v>
+        <v>26075.43467333426</v>
       </c>
       <c r="J113" t="n">
-        <v>25737.00915593097</v>
+        <v>25726.99173381168</v>
       </c>
       <c r="K113" t="n">
-        <v>23346.43575174157</v>
+        <v>23350.54293952258</v>
       </c>
     </row>
     <row r="114">
@@ -28692,19 +28692,19 @@
         <v>131.14</v>
       </c>
       <c r="G114" t="n">
-        <v>-3.413885219048097</v>
+        <v>3.826305564813083</v>
       </c>
       <c r="H114" t="n">
         <v>23000.27</v>
       </c>
       <c r="I114" t="n">
-        <v>25662.31388521905</v>
+        <v>25655.07369443519</v>
       </c>
       <c r="J114" t="n">
-        <v>25338.76331629265</v>
+        <v>25327.77187526366</v>
       </c>
       <c r="K114" t="n">
-        <v>23323.8205689264</v>
+        <v>23327.57181917153</v>
       </c>
     </row>
     <row r="115">
@@ -28718,19 +28718,19 @@
         <v>131.04</v>
       </c>
       <c r="G115" t="n">
-        <v>0.6078190229200118</v>
+        <v>8.193345365089044</v>
       </c>
       <c r="H115" t="n">
         <v>22998.6</v>
       </c>
       <c r="I115" t="n">
-        <v>25332.19218097708</v>
+        <v>25324.60665463491</v>
       </c>
       <c r="J115" t="n">
-        <v>25027.57835094733</v>
+        <v>25016.55865750458</v>
       </c>
       <c r="K115" t="n">
-        <v>23303.21383002975</v>
+        <v>23306.64799713033</v>
       </c>
     </row>
     <row r="116">
@@ -28744,19 +28744,19 @@
         <v>130.94</v>
       </c>
       <c r="G116" t="n">
-        <v>42.35957054391838</v>
+        <v>49.81753819439109</v>
       </c>
       <c r="H116" t="n">
         <v>22997.12</v>
       </c>
       <c r="I116" t="n">
-        <v>25065.44042945608</v>
+        <v>25057.98246180561</v>
       </c>
       <c r="J116" t="n">
-        <v>24778.13004967465</v>
+        <v>24767.5213864003</v>
       </c>
       <c r="K116" t="n">
-        <v>23284.43037978143</v>
+        <v>23287.58107540531</v>
       </c>
     </row>
     <row r="117">
@@ -28770,19 +28770,19 @@
         <v>130.84</v>
       </c>
       <c r="G117" t="n">
-        <v>293.3763609144808</v>
+        <v>300.4972442259677</v>
       </c>
       <c r="H117" t="n">
         <v>22995.7</v>
       </c>
       <c r="I117" t="n">
-        <v>24845.42363908552</v>
+        <v>24838.30275577403</v>
       </c>
       <c r="J117" t="n">
-        <v>24573.96784756466</v>
+        <v>24563.95052717894</v>
       </c>
       <c r="K117" t="n">
-        <v>23267.15579152086</v>
+        <v>23270.05222859509</v>
       </c>
     </row>
     <row r="118">
@@ -28796,19 +28796,19 @@
         <v>130.74</v>
       </c>
       <c r="G118" t="n">
-        <v>-416.4437110543113</v>
+        <v>-409.7394686107946</v>
       </c>
       <c r="H118" t="n">
         <v>22994.56</v>
       </c>
       <c r="I118" t="n">
-        <v>24661.24371105431</v>
+        <v>24654.53946861079</v>
       </c>
       <c r="J118" t="n">
-        <v>24404.35251397893</v>
+        <v>24394.98059234702</v>
       </c>
       <c r="K118" t="n">
-        <v>23251.45119707538</v>
+        <v>23254.11887626378</v>
       </c>
     </row>
     <row r="119">
@@ -28822,19 +28822,19 @@
         <v>130.64</v>
       </c>
       <c r="G119" t="n">
-        <v>-481.4957000921822</v>
+        <v>-475.2253113631632</v>
       </c>
       <c r="H119" t="n">
         <v>22993.79</v>
       </c>
       <c r="I119" t="n">
-        <v>24505.19570009218</v>
+        <v>24498.92531136316</v>
       </c>
       <c r="J119" t="n">
-        <v>24261.71658697056</v>
+        <v>24252.98492623578</v>
       </c>
       <c r="K119" t="n">
-        <v>23237.26911312162</v>
+        <v>23239.73038512739</v>
       </c>
     </row>
     <row r="120">
@@ -28848,19 +28848,19 @@
         <v>130.54</v>
       </c>
       <c r="G120" t="n">
-        <v>-173.0859038588678</v>
+        <v>-167.2375346347326</v>
       </c>
       <c r="H120" t="n">
         <v>22993.05</v>
       </c>
       <c r="I120" t="n">
-        <v>24371.28590385887</v>
+        <v>24365.43753463473</v>
       </c>
       <c r="J120" t="n">
-        <v>24140.18585539834</v>
+        <v>24132.06295701196</v>
       </c>
       <c r="K120" t="n">
-        <v>23224.15004846052</v>
+        <v>23226.42457762277</v>
       </c>
     </row>
     <row r="121">
@@ -28874,19 +28874,19 @@
         <v>130.44</v>
       </c>
       <c r="G121" t="n">
-        <v>-641.9989472179514</v>
+        <v>-636.5479899689053</v>
       </c>
       <c r="H121" t="n">
         <v>22992.44</v>
       </c>
       <c r="I121" t="n">
-        <v>24255.39894721795</v>
+        <v>24249.94798996891</v>
       </c>
       <c r="J121" t="n">
-        <v>24035.74921904541</v>
+        <v>24028.19311296597</v>
       </c>
       <c r="K121" t="n">
-        <v>23212.08972817254</v>
+        <v>23214.19487700293</v>
       </c>
     </row>
     <row r="122">
@@ -28900,19 +28900,19 @@
         <v>130.34</v>
       </c>
       <c r="G122" t="n">
-        <v>-449.8508107799171</v>
+        <v>-444.7678738064133</v>
       </c>
       <c r="H122" t="n">
         <v>22991.99</v>
       </c>
       <c r="I122" t="n">
-        <v>24154.35081077992</v>
+        <v>24149.26787380641</v>
       </c>
       <c r="J122" t="n">
-        <v>23945.31400207506</v>
+        <v>23938.27991515477</v>
       </c>
       <c r="K122" t="n">
-        <v>23201.02680870486</v>
+        <v>23202.97795865165</v>
       </c>
     </row>
     <row r="123">
@@ -28926,19 +28926,19 @@
         <v>130.24</v>
       </c>
       <c r="G123" t="n">
-        <v>-381.0654064673145</v>
+        <v>-376.320247059979</v>
       </c>
       <c r="H123" t="n">
         <v>22991.52</v>
       </c>
       <c r="I123" t="n">
-        <v>24065.46540646732</v>
+        <v>24060.72024705998</v>
       </c>
       <c r="J123" t="n">
-        <v>23866.28442009511</v>
+        <v>23859.72844025632</v>
       </c>
       <c r="K123" t="n">
-        <v>23190.70098637221</v>
+        <v>23192.51180680366</v>
       </c>
     </row>
     <row r="124">
@@ -28952,19 +28952,19 @@
         <v>130.14</v>
       </c>
       <c r="G124" t="n">
-        <v>-285.49388666905</v>
+        <v>-281.057317646726</v>
       </c>
       <c r="H124" t="n">
         <v>22991.05</v>
       </c>
       <c r="I124" t="n">
-        <v>23986.79388666905</v>
+        <v>23982.35731764673</v>
       </c>
       <c r="J124" t="n">
-        <v>23796.78246349526</v>
+        <v>23790.66321958779</v>
       </c>
       <c r="K124" t="n">
-        <v>23181.06142317379</v>
+        <v>23182.74409805893</v>
       </c>
     </row>
     <row r="125">
@@ -28978,19 +28978,19 @@
         <v>130.04</v>
       </c>
       <c r="G125" t="n">
-        <v>-249.3750255586929</v>
+        <v>-245.2197719792603</v>
       </c>
       <c r="H125" t="n">
         <v>22990.59</v>
       </c>
       <c r="I125" t="n">
-        <v>23916.77502555869</v>
+        <v>23912.61977197926</v>
       </c>
       <c r="J125" t="n">
-        <v>23735.30959544911</v>
+        <v>23729.58892203936</v>
       </c>
       <c r="K125" t="n">
-        <v>23172.05543010958</v>
+        <v>23173.6208499399</v>
       </c>
     </row>
     <row r="126">
@@ -29004,19 +29004,19 @@
         <v>129.94</v>
       </c>
       <c r="G126" t="n">
-        <v>-703.7070462156153</v>
+        <v>-699.8080822426964</v>
       </c>
       <c r="H126" t="n">
         <v>22990.31</v>
       </c>
       <c r="I126" t="n">
-        <v>23854.30704621561</v>
+        <v>23850.40808224269</v>
       </c>
       <c r="J126" t="n">
-        <v>23680.81968556122</v>
+        <v>23675.46279659266</v>
       </c>
       <c r="K126" t="n">
-        <v>23163.79736065439</v>
+        <v>23165.25528565004</v>
       </c>
     </row>
     <row r="127">
@@ -29030,19 +29030,19 @@
         <v>129.84</v>
       </c>
       <c r="G127" t="n">
-        <v>-78.44423578176793</v>
+        <v>-74.77887397660015</v>
       </c>
       <c r="H127" t="n">
         <v>22990.01</v>
       </c>
       <c r="I127" t="n">
-        <v>23798.14423578177</v>
+        <v>23794.4788739766</v>
       </c>
       <c r="J127" t="n">
-        <v>23632.11655910227</v>
+        <v>23627.09199782472</v>
       </c>
       <c r="K127" t="n">
-        <v>23156.0376766795</v>
+        <v>23157.39687615188</v>
       </c>
     </row>
     <row r="128">
@@ -29056,19 +29056,19 @@
         <v>129.74</v>
       </c>
       <c r="G128" t="n">
-        <v>-48.26913610279371</v>
+        <v>-44.81690801983495</v>
       </c>
       <c r="H128" t="n">
         <v>22989.53</v>
       </c>
       <c r="I128" t="n">
-        <v>23747.26913610279</v>
+        <v>23743.81690801983</v>
       </c>
       <c r="J128" t="n">
-        <v>23588.22697950155</v>
+        <v>23583.50637959792</v>
       </c>
       <c r="K128" t="n">
-        <v>23148.57215660124</v>
+        <v>23149.84052842191</v>
       </c>
     </row>
     <row r="129">
@@ -29082,19 +29082,19 @@
         <v>129.64</v>
       </c>
       <c r="G129" t="n">
-        <v>-128.4987266504322</v>
+        <v>-125.2412294255191</v>
       </c>
       <c r="H129" t="n">
         <v>22989.1</v>
       </c>
       <c r="I129" t="n">
-        <v>23701.19872665043</v>
+        <v>23697.94122942552</v>
       </c>
       <c r="J129" t="n">
-        <v>23548.70732004178</v>
+        <v>23544.26514642833</v>
       </c>
       <c r="K129" t="n">
-        <v>23141.59140660865</v>
+        <v>23142.77608299718</v>
       </c>
     </row>
     <row r="130">
@@ -29108,19 +29108,19 @@
         <v>129.54</v>
       </c>
       <c r="G130" t="n">
-        <v>-589.195309573639</v>
+        <v>-586.1160212202012</v>
       </c>
       <c r="H130" t="n">
         <v>22988.88</v>
       </c>
       <c r="I130" t="n">
-        <v>23659.49530957364</v>
+        <v>23656.4160212202</v>
       </c>
       <c r="J130" t="n">
-        <v>23513.15535420827</v>
+        <v>23508.96863204107</v>
       </c>
       <c r="K130" t="n">
-        <v>23135.21995536537</v>
+        <v>23136.32738917913</v>
       </c>
     </row>
     <row r="131">
@@ -29134,19 +29134,19 @@
         <v>129.44</v>
       </c>
       <c r="G131" t="n">
-        <v>-359.7441428079183</v>
+        <v>-356.8282308573143</v>
       </c>
       <c r="H131" t="n">
         <v>22988.76</v>
       </c>
       <c r="I131" t="n">
-        <v>23621.54414280792</v>
+        <v>23618.62823085731</v>
       </c>
       <c r="J131" t="n">
-        <v>23480.98857058798</v>
+        <v>23477.03662224834</v>
       </c>
       <c r="K131" t="n">
-        <v>23129.31557221993</v>
+        <v>23130.35160860897</v>
       </c>
     </row>
     <row r="132">
@@ -29160,19 +29160,19 @@
         <v>129.34</v>
       </c>
       <c r="G132" t="n">
-        <v>93.28320507194076</v>
+        <v>96.04905721805699</v>
       </c>
       <c r="H132" t="n">
         <v>22988.44</v>
       </c>
       <c r="I132" t="n">
-        <v>23586.61679492806</v>
+        <v>23583.85094278194</v>
       </c>
       <c r="J132" t="n">
-        <v>23451.5073197057</v>
+        <v>23447.77151939903</v>
       </c>
       <c r="K132" t="n">
-        <v>23123.54947522236</v>
+        <v>23124.51942338291</v>
       </c>
     </row>
     <row r="133">
@@ -29186,19 +29186,19 @@
         <v>129.24</v>
       </c>
       <c r="G133" t="n">
-        <v>183.2127526567892</v>
+        <v>185.8405112731125</v>
       </c>
       <c r="H133" t="n">
         <v>22987.96</v>
       </c>
       <c r="I133" t="n">
-        <v>23554.38724734321</v>
+        <v>23551.75948872689</v>
       </c>
       <c r="J133" t="n">
-        <v>23424.41158516595</v>
+        <v>23420.87513514446</v>
       </c>
       <c r="K133" t="n">
-        <v>23117.93566217726</v>
+        <v>23118.84435358243</v>
       </c>
     </row>
     <row r="134">
@@ -29212,19 +29212,19 @@
         <v>129.14</v>
       </c>
       <c r="G134" t="n">
-        <v>-603.6510980005914</v>
+        <v>-601.1506666500973</v>
       </c>
       <c r="H134" t="n">
         <v>22987.73</v>
       </c>
       <c r="I134" t="n">
-        <v>23524.95109800059</v>
+        <v>23522.4506666501</v>
       </c>
       <c r="J134" t="n">
-        <v>23399.82050481339</v>
+        <v>23396.46823415092</v>
       </c>
       <c r="K134" t="n">
-        <v>23112.8605931872</v>
+        <v>23113.71243249917</v>
       </c>
     </row>
     <row r="135">
@@ -29238,19 +29238,19 @@
         <v>129.04</v>
       </c>
       <c r="G135" t="n">
-        <v>-281.6569154459612</v>
+        <v>-279.2741103660228</v>
       </c>
       <c r="H135" t="n">
         <v>22987.67</v>
       </c>
       <c r="I135" t="n">
-        <v>23497.95691544596</v>
+        <v>23495.57411036602</v>
       </c>
       <c r="J135" t="n">
-        <v>23377.40400056704</v>
+        <v>23374.22218578044</v>
       </c>
       <c r="K135" t="n">
-        <v>23108.22291487892</v>
+        <v>23109.02192458558</v>
       </c>
     </row>
     <row r="136">
@@ -29264,19 +29264,19 @@
         <v>128.94</v>
       </c>
       <c r="G136" t="n">
-        <v>-366.5492609512694</v>
+        <v>-364.2753266067375</v>
       </c>
       <c r="H136" t="n">
         <v>22987.56</v>
       </c>
       <c r="I136" t="n">
-        <v>23472.94926095127</v>
+        <v>23470.67532660674</v>
       </c>
       <c r="J136" t="n">
-        <v>23356.7260408039</v>
+        <v>23353.70224680616</v>
       </c>
       <c r="K136" t="n">
-        <v>23103.78322014738</v>
+        <v>23104.53307980058</v>
       </c>
     </row>
     <row r="137">
@@ -29290,19 +29290,19 @@
         <v>128.84</v>
       </c>
       <c r="G137" t="n">
-        <v>-229.563016202912</v>
+        <v>-227.3900365294758</v>
       </c>
       <c r="H137" t="n">
         <v>22987.44</v>
       </c>
       <c r="I137" t="n">
-        <v>23449.76301620291</v>
+        <v>23447.59003652948</v>
       </c>
       <c r="J137" t="n">
-        <v>23337.63917793881</v>
+        <v>23334.76211746976</v>
       </c>
       <c r="K137" t="n">
-        <v>23099.5638382641</v>
+        <v>23100.26791905971</v>
       </c>
     </row>
     <row r="138">
@@ -29316,19 +29316,19 @@
         <v>128.74</v>
       </c>
       <c r="G138" t="n">
-        <v>665.6912586924664</v>
+        <v>667.7704537643549</v>
       </c>
       <c r="H138" t="n">
         <v>22987</v>
       </c>
       <c r="I138" t="n">
-        <v>23427.90874130753</v>
+        <v>23425.82954623564</v>
       </c>
       <c r="J138" t="n">
-        <v>23319.67009028258</v>
+        <v>23316.92949988413</v>
       </c>
       <c r="K138" t="n">
-        <v>23095.23865102496</v>
+        <v>23095.90004635152</v>
       </c>
     </row>
     <row r="139">
@@ -29342,19 +29342,19 @@
         <v>128.64</v>
       </c>
       <c r="G139" t="n">
-        <v>-1028.218852166268</v>
+        <v>-1026.226935319213</v>
       </c>
       <c r="H139" t="n">
         <v>22986.83</v>
       </c>
       <c r="I139" t="n">
-        <v>23407.81885216627</v>
+        <v>23405.82693531921</v>
       </c>
       <c r="J139" t="n">
-        <v>23303.26592087301</v>
+        <v>23300.65245153834</v>
       </c>
       <c r="K139" t="n">
-        <v>23091.38293129325</v>
+        <v>23092.00448378087</v>
       </c>
     </row>
     <row r="140">
@@ -29368,19 +29368,19 @@
         <v>128.54</v>
       </c>
       <c r="G140" t="n">
-        <v>283.4755458749423</v>
+        <v>285.3860995988725</v>
       </c>
       <c r="H140" t="n">
         <v>22986.8</v>
       </c>
       <c r="I140" t="n">
-        <v>23389.22445412506</v>
+        <v>23387.31390040113</v>
       </c>
       <c r="J140" t="n">
-        <v>23288.17125327876</v>
+        <v>23285.67637403752</v>
       </c>
       <c r="K140" t="n">
-        <v>23087.85320084629</v>
+        <v>23088.43752636361</v>
       </c>
     </row>
     <row r="141">
@@ -29394,19 +29394,19 @@
         <v>128.44</v>
       </c>
       <c r="G141" t="n">
-        <v>-693.4727047300548</v>
+        <v>-691.6381265538548</v>
       </c>
       <c r="H141" t="n">
         <v>22986.68</v>
       </c>
       <c r="I141" t="n">
-        <v>23371.77270473005</v>
+        <v>23369.93812655385</v>
       </c>
       <c r="J141" t="n">
-        <v>23274.0455998925</v>
+        <v>23271.66151275637</v>
       </c>
       <c r="K141" t="n">
-        <v>23084.40710483756</v>
+        <v>23084.95661379748</v>
       </c>
     </row>
     <row r="142">
@@ -29420,19 +29420,19 @@
         <v>128.34</v>
       </c>
       <c r="G142" t="n">
-        <v>-429.9846054284499</v>
+        <v>-428.2210864861736</v>
       </c>
       <c r="H142" t="n">
         <v>22986.8</v>
       </c>
       <c r="I142" t="n">
-        <v>23355.68460542845</v>
+        <v>23353.92108648617</v>
       </c>
       <c r="J142" t="n">
-        <v>23261.12130513534</v>
+        <v>23258.84086999814</v>
       </c>
       <c r="K142" t="n">
-        <v>23081.36330029311</v>
+        <v>23081.88021648803</v>
       </c>
     </row>
     <row r="143">
@@ -29446,19 +29446,19 @@
         <v>128.24</v>
       </c>
       <c r="G143" t="n">
-        <v>-105.9431417994456</v>
+        <v>-104.2461868975806</v>
       </c>
       <c r="H143" t="n">
         <v>22986.74</v>
       </c>
       <c r="I143" t="n">
-        <v>23340.44314179945</v>
+        <v>23338.74618689758</v>
       </c>
       <c r="J143" t="n">
-        <v>23248.89178654662</v>
+        <v>23246.70845479656</v>
       </c>
       <c r="K143" t="n">
-        <v>23078.29135525283</v>
+        <v>23078.77773210102</v>
       </c>
     </row>
     <row r="144">
@@ -29472,19 +29472,19 @@
         <v>128.14</v>
       </c>
       <c r="G144" t="n">
-        <v>-116.1417039455846</v>
+        <v>-114.5071928483922</v>
       </c>
       <c r="H144" t="n">
         <v>22986.58</v>
       </c>
       <c r="I144" t="n">
-        <v>23326.04170394559</v>
+        <v>23324.40719284839</v>
       </c>
       <c r="J144" t="n">
-        <v>23237.36005255457</v>
+        <v>23235.26780830902</v>
       </c>
       <c r="K144" t="n">
-        <v>23075.26165139101</v>
+        <v>23075.71938453937</v>
       </c>
     </row>
     <row r="145">
@@ -29498,19 +29498,19 @@
         <v>128.04</v>
       </c>
       <c r="G145" t="n">
-        <v>-353.4927182983593</v>
+        <v>-351.9168591079797</v>
       </c>
       <c r="H145" t="n">
         <v>22986.51</v>
       </c>
       <c r="I145" t="n">
-        <v>23312.59271829836</v>
+        <v>23311.01685910798</v>
       </c>
       <c r="J145" t="n">
-        <v>23226.64744799358</v>
+        <v>23224.64075600392</v>
       </c>
       <c r="K145" t="n">
-        <v>23072.45527030478</v>
+        <v>23072.88610310406</v>
       </c>
     </row>
     <row r="146">
@@ -29524,19 +29524,19 @@
         <v>127.94</v>
       </c>
       <c r="G146" t="n">
-        <v>-95.04639573340683</v>
+        <v>-93.52566800864952</v>
       </c>
       <c r="H146" t="n">
         <v>22986.45</v>
       </c>
       <c r="I146" t="n">
-        <v>23299.94639573341</v>
+        <v>23298.42566800865</v>
       </c>
       <c r="J146" t="n">
-        <v>23216.61258801366</v>
+        <v>23214.68634741063</v>
       </c>
       <c r="K146" t="n">
-        <v>23069.78380771975</v>
+        <v>23070.18932059802</v>
       </c>
     </row>
     <row r="147">
@@ -29550,19 +29550,19 @@
         <v>127.84</v>
       </c>
       <c r="G147" t="n">
-        <v>-529.0894203028147</v>
+        <v>-527.6204879848301</v>
       </c>
       <c r="H147" t="n">
         <v>22986.45</v>
       </c>
       <c r="I147" t="n">
-        <v>23288.08942030281</v>
+        <v>23286.62048798483</v>
       </c>
       <c r="J147" t="n">
-        <v>23207.25044855774</v>
+        <v>23205.39995171546</v>
       </c>
       <c r="K147" t="n">
-        <v>23067.28897174507</v>
+        <v>23067.67053626937</v>
       </c>
     </row>
     <row r="148">
@@ -29576,19 +29576,19 @@
         <v>127.74</v>
       </c>
       <c r="G148" t="n">
-        <v>-58.20322546597527</v>
+        <v>-56.78278556512669</v>
       </c>
       <c r="H148" t="n">
         <v>22986.45</v>
       </c>
       <c r="I148" t="n">
-        <v>23276.90322546598</v>
+        <v>23275.48278556513</v>
       </c>
       <c r="J148" t="n">
-        <v>23198.45158753587</v>
+        <v>23196.67248342709</v>
       </c>
       <c r="K148" t="n">
-        <v>23064.9016379301</v>
+        <v>23065.26030213803</v>
       </c>
     </row>
     <row r="149">
@@ -29602,19 +29602,19 @@
         <v>127.64</v>
       </c>
       <c r="G149" t="n">
-        <v>120.3788005073147</v>
+        <v>121.7542768264793</v>
       </c>
       <c r="H149" t="n">
         <v>22986.24</v>
       </c>
       <c r="I149" t="n">
-        <v>23266.12119949269</v>
+        <v>23264.74572317352</v>
       </c>
       <c r="J149" t="n">
-        <v>23189.96147556073</v>
+        <v>23188.24973705802</v>
       </c>
       <c r="K149" t="n">
-        <v>23062.39972393196</v>
+        <v>23062.73598611551</v>
       </c>
     </row>
     <row r="150">
@@ -29628,19 +29628,19 @@
         <v>127.54</v>
       </c>
       <c r="G150" t="n">
-        <v>-71.20378832824645</v>
+        <v>-69.86912938257228</v>
       </c>
       <c r="H150" t="n">
         <v>22986.04</v>
       </c>
       <c r="I150" t="n">
-        <v>23255.90378832825</v>
+        <v>23254.56912938257</v>
       </c>
       <c r="J150" t="n">
-        <v>23181.95991889593</v>
+        <v>23180.31181354455</v>
       </c>
       <c r="K150" t="n">
-        <v>23059.98386943232</v>
+        <v>23060.29731583803</v>
       </c>
     </row>
     <row r="151">
@@ -29654,19 +29654,19 @@
         <v>127.44</v>
       </c>
       <c r="G151" t="n">
-        <v>-260.3303051530347</v>
+        <v>-259.0312307123058</v>
       </c>
       <c r="H151" t="n">
         <v>22687</v>
       </c>
       <c r="I151" t="n">
-        <v>22947.33030515303</v>
+        <v>22946.03123071231</v>
       </c>
       <c r="J151" t="n">
-        <v>22875.56056031285</v>
+        <v>22873.9726241627</v>
       </c>
       <c r="K151" t="n">
-        <v>22758.76974484019</v>
+        <v>22759.05860654961</v>
       </c>
     </row>
     <row r="152">
@@ -29680,19 +29680,19 @@
         <v>127.34</v>
       </c>
       <c r="G152" t="n">
-        <v>-251.1869073770322</v>
+        <v>-249.9167647831891</v>
       </c>
       <c r="H152" t="n">
         <v>22924.4</v>
       </c>
       <c r="I152" t="n">
-        <v>23175.58690737703</v>
+        <v>23174.31676478319</v>
       </c>
       <c r="J152" t="n">
-        <v>23106.01044601092</v>
+        <v>23104.47946014835</v>
       </c>
       <c r="K152" t="n">
-        <v>22993.97646136611</v>
+        <v>22994.23730463484</v>
       </c>
     </row>
     <row r="153">
@@ -29706,19 +29706,19 @@
         <v>127.24</v>
       </c>
       <c r="G153" t="n">
-        <v>-242.3023919428779</v>
+        <v>-241.0533125144248</v>
       </c>
       <c r="H153" t="n">
         <v>22643.1</v>
       </c>
       <c r="I153" t="n">
-        <v>22885.40239194288</v>
+        <v>22884.15331251442</v>
       </c>
       <c r="J153" t="n">
-        <v>22818.13964875335</v>
+        <v>22816.66261821941</v>
       </c>
       <c r="K153" t="n">
-        <v>22710.36274318953</v>
+        <v>22710.59069429501</v>
       </c>
     </row>
     <row r="154">
@@ -29732,19 +29732,19 @@
         <v>127.14</v>
       </c>
       <c r="G154" t="n">
-        <v>-233.4973612586837</v>
+        <v>-232.2614557650086</v>
       </c>
       <c r="H154" t="n">
         <v>22647.9</v>
       </c>
       <c r="I154" t="n">
-        <v>22881.39736125869</v>
+        <v>22880.16145576501</v>
       </c>
       <c r="J154" t="n">
-        <v>22816.72093899763</v>
+        <v>22815.29507381935</v>
       </c>
       <c r="K154" t="n">
-        <v>22712.57642226106</v>
+        <v>22712.76638194566</v>
       </c>
     </row>
     <row r="155">
@@ -29758,19 +29758,19 @@
         <v>127.04</v>
       </c>
       <c r="G155" t="n">
-        <v>-224.5465114769722</v>
+        <v>-223.3182177874187</v>
       </c>
       <c r="H155" t="n">
         <v>23050.9</v>
       </c>
       <c r="I155" t="n">
-        <v>23275.44651147697</v>
+        <v>23274.21821778742</v>
       </c>
       <c r="J155" t="n">
-        <v>23213.82949713346</v>
+        <v>23212.45219522879</v>
       </c>
       <c r="K155" t="n">
-        <v>23112.51701434351</v>
+        <v>23112.66602255863</v>
       </c>
     </row>
     <row r="156">
@@ -29784,19 +29784,19 @@
         <v>126.94</v>
       </c>
       <c r="G156" t="n">
-        <v>-215.2048468971334</v>
+        <v>-213.9838722157838</v>
       </c>
       <c r="H156" t="n">
         <v>22933.5</v>
       </c>
       <c r="I156" t="n">
-        <v>23148.70484689713</v>
+        <v>23147.48387221578</v>
       </c>
       <c r="J156" t="n">
-        <v>23090.84266103509</v>
+        <v>23089.51149278137</v>
       </c>
       <c r="K156" t="n">
-        <v>22991.36218586204</v>
+        <v>22991.47237943441</v>
       </c>
     </row>
     <row r="157">
@@ -29810,19 +29810,19 @@
         <v>126.84</v>
       </c>
       <c r="G157" t="n">
-        <v>-205.2625245969066</v>
+        <v>-204.0559797875139</v>
       </c>
       <c r="H157" t="n">
         <v>23251.9</v>
       </c>
       <c r="I157" t="n">
-        <v>23457.16252459691</v>
+        <v>23455.95597978752</v>
       </c>
       <c r="J157" t="n">
-        <v>23403.93970403015</v>
+        <v>23402.65239830776</v>
       </c>
       <c r="K157" t="n">
-        <v>23305.12282056676</v>
+        <v>23305.20358147976</v>
       </c>
     </row>
     <row r="158">
@@ -29836,19 +29836,19 @@
         <v>126.74</v>
       </c>
       <c r="G158" t="n">
-        <v>-194.6188575488595</v>
+        <v>-193.4408743680942</v>
       </c>
       <c r="H158" t="n">
         <v>22359.8</v>
       </c>
       <c r="I158" t="n">
-        <v>22554.41885754886</v>
+        <v>22553.24087436809</v>
       </c>
       <c r="J158" t="n">
-        <v>22506.801639086</v>
+        <v>22505.55607061418</v>
       </c>
       <c r="K158" t="n">
-        <v>22407.41721846286</v>
+        <v>22407.48480375391</v>
       </c>
     </row>
     <row r="159">
@@ -29862,19 +29862,19 @@
         <v>126.64</v>
       </c>
       <c r="G159" t="n">
-        <v>-183.3493465563515</v>
+        <v>-182.2172953856134</v>
       </c>
       <c r="H159" t="n">
         <v>23047.9</v>
       </c>
       <c r="I159" t="n">
-        <v>23231.24934655635</v>
+        <v>23230.11729538561</v>
       </c>
       <c r="J159" t="n">
-        <v>23190.11104540298</v>
+        <v>23188.90522313495</v>
       </c>
       <c r="K159" t="n">
-        <v>23089.03830115337</v>
+        <v>23089.11207225067</v>
       </c>
     </row>
     <row r="160">
@@ -29888,19 +29888,19 @@
         <v>126.54</v>
       </c>
       <c r="G160" t="n">
-        <v>-171.7316649862914</v>
+        <v>-170.6599249189348</v>
       </c>
       <c r="H160" t="n">
         <v>22819.4</v>
       </c>
       <c r="I160" t="n">
-        <v>22991.13166498629</v>
+        <v>22990.05992491894</v>
       </c>
       <c r="J160" t="n">
-        <v>22957.05191314525</v>
+        <v>22955.88396925636</v>
       </c>
       <c r="K160" t="n">
-        <v>22853.47975184105</v>
+        <v>22853.57595566257</v>
       </c>
     </row>
     <row r="161">
@@ -29914,19 +29914,19 @@
         <v>126.44</v>
       </c>
       <c r="G161" t="n">
-        <v>-163.0601213604386</v>
+        <v>-162.0421531267566</v>
       </c>
       <c r="H161" t="n">
         <v>22415.3</v>
       </c>
       <c r="I161" t="n">
-        <v>22578.36012136044</v>
+        <v>22577.34215312676</v>
       </c>
       <c r="J161" t="n">
-        <v>22548.60949882276</v>
+        <v>22547.47767704415</v>
       </c>
       <c r="K161" t="n">
-        <v>22445.05062253768</v>
+        <v>22445.16447608261</v>
       </c>
     </row>
     <row r="162">
@@ -29940,19 +29940,19 @@
         <v>126.34</v>
       </c>
       <c r="G162" t="n">
-        <v>-158.9207945682174</v>
+        <v>-157.9372879602197</v>
       </c>
       <c r="H162" t="n">
         <v>23032.4</v>
       </c>
       <c r="I162" t="n">
-        <v>23191.32079456822</v>
+        <v>23190.33728796022</v>
       </c>
       <c r="J162" t="n">
-        <v>23161.57017203054</v>
+        <v>23160.47281187761</v>
       </c>
       <c r="K162" t="n">
-        <v>23062.15062253768</v>
+        <v>23062.26447608261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>